<commit_message>
Increase minimum capacity for new builds to 5,000
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{36759349-8019-4983-9923-73CF152A9F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB99D16-7B86-4A50-BB95-B95934A1AD4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31095" yWindow="4725" windowWidth="20670" windowHeight="15600" activeTab="2" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" activeTab="2" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -665,7 +665,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,7 +683,7 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>1000</v>
+        <v>5000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to share of profitable capacity built
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB99D16-7B86-4A50-BB95-B95934A1AD4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CF85F1-A5A5-43BC-AFA6-1EE4A04D0A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" activeTab="2" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" activeTab="3" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -664,7 +664,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -698,8 +698,8 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B18:AE25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,94 +807,94 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -902,94 +902,94 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
@@ -997,94 +997,94 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
@@ -1092,94 +1092,94 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
@@ -1187,94 +1187,94 @@
         <v>14</v>
       </c>
       <c r="B6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
@@ -1282,94 +1282,94 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE7">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
@@ -1377,94 +1377,94 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
@@ -1472,94 +1472,94 @@
         <v>17</v>
       </c>
       <c r="B9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
@@ -1567,94 +1567,94 @@
         <v>18</v>
       </c>
       <c r="B10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
@@ -1662,94 +1662,94 @@
         <v>19</v>
       </c>
       <c r="B11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
@@ -1757,94 +1757,94 @@
         <v>20</v>
       </c>
       <c r="B12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
@@ -1852,94 +1852,94 @@
         <v>21</v>
       </c>
       <c r="B13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
@@ -1947,94 +1947,94 @@
         <v>22</v>
       </c>
       <c r="B14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
@@ -2042,94 +2042,94 @@
         <v>23</v>
       </c>
       <c r="B15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
@@ -2327,94 +2327,94 @@
         <v>26</v>
       </c>
       <c r="B18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
@@ -2422,94 +2422,94 @@
         <v>27</v>
       </c>
       <c r="B19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
@@ -2517,94 +2517,94 @@
         <v>28</v>
       </c>
       <c r="B20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
@@ -2612,94 +2612,94 @@
         <v>29</v>
       </c>
       <c r="B21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
@@ -2707,94 +2707,94 @@
         <v>30</v>
       </c>
       <c r="B22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
@@ -2802,94 +2802,94 @@
         <v>31</v>
       </c>
       <c r="B23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
@@ -2897,94 +2897,94 @@
         <v>32</v>
       </c>
       <c r="B24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
@@ -2992,94 +2992,94 @@
         <v>33</v>
       </c>
       <c r="B25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data tweaks for calibration
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CF85F1-A5A5-43BC-AFA6-1EE4A04D0A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8248DB4-6E2E-435A-8D3A-C7FBE3A7900C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" activeTab="3" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
+    <workbookView xWindow="13575" yWindow="10755" windowWidth="21840" windowHeight="9120" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="CSL-CSCCCMvSoECBtY" sheetId="2" r:id="rId2"/>
-    <sheet name="CSL-CSCMBCfPTwNEC" sheetId="3" r:id="rId3"/>
-    <sheet name="CSL-CSCSoCECBiaSY" sheetId="4" r:id="rId4"/>
+    <sheet name="CSC-CSCCCMvSoECBtY" sheetId="2" r:id="rId2"/>
+    <sheet name="CSC-CSCMBCfPTwNEC" sheetId="3" r:id="rId3"/>
+    <sheet name="CSC-CSCSoCECBiaSY" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,15 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
-    <t>CSL Capacity Supply Curve Capacity Cost Multiplier vs Share of Existing Capacity Built this Year</t>
-  </si>
-  <si>
-    <t>CSL Capacity Supply Curve Minimum Buildable Capacity for Plant Types with No Existing Capacity</t>
-  </si>
-  <si>
-    <t>CSL Capacity Supply Curve Share of Cost Effective Capacity Built in a Single Year</t>
-  </si>
-  <si>
     <t xml:space="preserve">Source: </t>
   </si>
   <si>
@@ -141,6 +132,15 @@
   </si>
   <si>
     <t>(MW)</t>
+  </si>
+  <si>
+    <t>CSC Capacity Supply Curve Capacity Cost Multiplier vs Share of Existing Capacity Built this Year</t>
+  </si>
+  <si>
+    <t>CSC Capacity Supply Curve Minimum Buildable Capacity for Plant Types with No Existing Capacity</t>
+  </si>
+  <si>
+    <t>CSC Capacity Supply Curve Share of Cost Effective Capacity Built in a Single Year</t>
   </si>
 </sst>
 </file>
@@ -503,38 +503,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3D2DEE-686E-48A0-AC3D-0F54DEA5D0EC}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -550,7 +550,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,7 +560,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -607,7 +607,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -675,12 +675,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>5000</v>
@@ -698,7 +698,7 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B25" sqref="B18:AE25"/>
     </sheetView>
   </sheetViews>
@@ -709,7 +709,7 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B1">
         <v>2021</v>
@@ -804,1337 +804,1337 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="C2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="D2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="E2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="F2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="G2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="H2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="I2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="J2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="K2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="L2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="M2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="N2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="O2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="P2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Q2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="R2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="S2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="T2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="U2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="V2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="W2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="X2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Y2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Z2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AA2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AB2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AC2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AD2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AE2">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="C3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="D3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="E3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="F3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="G3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="H3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="I3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="J3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="K3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="L3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="M3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="N3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="O3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="P3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Q3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="R3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="S3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="T3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="U3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="V3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="W3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="X3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Y3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Z3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AA3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AB3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AC3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AD3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AE3">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="C4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="D4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="E4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="F4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="G4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="H4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="I4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="J4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="K4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="L4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="M4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="N4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="O4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="P4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Q4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="R4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="S4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="T4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="U4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="V4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="W4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="X4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Y4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Z4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AA4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AB4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AC4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AD4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AE4">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="C5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="D5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="E5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="F5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="G5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="H5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="I5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="J5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="K5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="L5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="M5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="N5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="O5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="P5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Q5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="R5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="S5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="T5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="U5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="V5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="W5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="X5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Y5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Z5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AA5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AB5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AC5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AD5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AE5">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="C6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="D6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="E6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="F6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="G6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="H6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="I6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="J6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="K6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="L6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="M6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="N6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="O6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="P6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Q6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="R6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="S6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="T6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="U6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="V6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="W6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="X6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Y6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Z6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AA6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AB6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AC6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AD6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AE6">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="C7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="D7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="E7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="F7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="G7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="H7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="I7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="J7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="K7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="L7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="M7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="N7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="O7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="P7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Q7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="R7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="S7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="T7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="U7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="V7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="W7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="X7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Y7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Z7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AA7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AB7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AC7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AD7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AE7">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="C8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="D8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="E8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="F8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="G8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="H8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="I8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="J8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="K8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="L8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="M8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="N8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="O8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="P8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Q8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="R8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="S8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="T8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="U8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="V8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="W8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="X8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Y8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Z8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AA8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AB8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AC8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AD8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AE8">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="C9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="D9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="E9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="F9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="G9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="H9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="I9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="J9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="K9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="L9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="M9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="N9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="O9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="P9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Q9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="R9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="S9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="T9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="U9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="V9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="W9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="X9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Y9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Z9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AA9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AB9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AC9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AD9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AE9">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="C10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="D10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="E10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="F10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="G10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="H10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="I10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="J10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="K10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="L10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="M10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="N10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="O10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="P10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Q10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="R10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="S10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="T10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="U10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="V10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="W10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="X10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Y10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Z10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AA10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AB10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AC10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AD10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AE10">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="C11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="D11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="E11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="F11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="G11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="H11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="I11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="J11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="K11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="L11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="M11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="N11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="O11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="P11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Q11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="R11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="S11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="T11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="U11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="V11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="W11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="X11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Y11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Z11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AA11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AB11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AC11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AD11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AE11">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="C12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="D12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="E12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="F12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="G12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="H12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="I12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="J12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="K12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="L12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="M12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="N12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="O12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="P12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Q12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="R12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="S12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="T12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="U12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="V12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="W12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="X12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Y12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Z12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AA12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AB12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AC12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AD12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AE12">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="C13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="D13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="E13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="F13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="G13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="H13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="I13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="J13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="K13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="L13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="M13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="N13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="O13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="P13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Q13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="R13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="S13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="T13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="U13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="V13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="W13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="X13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Y13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Z13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AA13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AB13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AC13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AD13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AE13">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="C14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="D14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="E14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="F14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="G14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="H14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="I14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="J14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="K14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="L14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="M14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="N14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="O14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="P14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Q14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="R14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="S14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="T14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="U14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="V14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="W14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="X14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Y14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Z14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AA14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AB14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AC14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AD14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AE14">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="C15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="D15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="E15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="F15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="G15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="H15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="I15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="J15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="K15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="L15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="M15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="N15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="O15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="P15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Q15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="R15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="S15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="T15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="U15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="V15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="W15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="X15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Y15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Z15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AA15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AB15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AC15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AD15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AE15">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -2229,7 +2229,7 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -2324,762 +2324,762 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="C18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="D18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="E18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="F18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="G18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="H18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="I18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="J18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="K18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="L18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="M18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="N18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="O18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="P18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Q18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="R18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="S18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="T18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="U18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="V18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="W18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="X18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Y18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Z18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AA18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AB18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AC18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AD18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AE18">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="C19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="D19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="E19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="F19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="G19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="H19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="I19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="J19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="K19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="L19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="M19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="N19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="O19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="P19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Q19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="R19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="S19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="T19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="U19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="V19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="W19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="X19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Y19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Z19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AA19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AB19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AC19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AD19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AE19">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="C20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="D20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="E20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="F20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="G20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="H20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="I20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="J20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="K20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="L20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="M20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="N20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="O20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="P20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Q20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="R20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="S20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="T20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="U20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="V20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="W20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="X20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Y20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Z20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AA20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AB20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AC20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AD20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AE20">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="C21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="D21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="E21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="F21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="G21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="H21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="I21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="J21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="K21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="L21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="M21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="N21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="O21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="P21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Q21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="R21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="S21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="T21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="U21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="V21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="W21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="X21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Y21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Z21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AA21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AB21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AC21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AD21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AE21">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="C22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="D22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="E22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="F22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="G22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="H22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="I22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="J22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="K22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="L22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="M22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="N22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="O22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="P22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Q22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="R22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="S22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="T22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="U22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="V22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="W22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="X22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Y22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Z22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AA22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AB22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AC22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AD22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AE22">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="C23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="D23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="E23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="F23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="G23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="H23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="I23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="J23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="K23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="L23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="M23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="N23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="O23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="P23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Q23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="R23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="S23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="T23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="U23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="V23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="W23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="X23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Y23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Z23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AA23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AB23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AC23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AD23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AE23">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="C24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="D24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="E24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="F24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="G24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="H24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="I24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="J24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="K24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="L24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="M24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="N24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="O24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="P24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Q24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="R24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="S24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="T24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="U24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="V24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="W24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="X24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Y24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Z24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AA24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AB24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AC24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AD24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AE24">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="C25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="D25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="E25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="F25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="G25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="H25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="I25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="J25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="K25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="L25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="M25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="N25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="O25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="P25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Q25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="R25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="S25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="T25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="U25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="V25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="W25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="X25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Y25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="Z25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AA25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AB25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AC25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AD25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
       <c r="AE25">
-        <v>0.4</v>
+        <v>0.33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Calibrate electricity sector results against ReEDS
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\CSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8248DB4-6E2E-435A-8D3A-C7FBE3A7900C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B22D3C2-F9E7-4EEF-AC87-E83AA2134C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13575" yWindow="10755" windowWidth="21840" windowHeight="9120" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -503,7 +503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3D2DEE-686E-48A0-AC3D-0F54DEA5D0EC}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -698,8 +698,8 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B25" sqref="B18:AE25"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:AE7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1282,94 +1282,94 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="C7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="D7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="E7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="F7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="G7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="H7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="I7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="J7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="K7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="L7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="M7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="N7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="O7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="P7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="Q7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="R7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="S7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="T7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="U7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="V7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="W7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="X7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="Y7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="Z7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="AA7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="AB7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="AC7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="AD7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
       <c r="AE7">
-        <v>0.33</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Calibration edit for onshore wind
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B22D3C2-F9E7-4EEF-AC87-E83AA2134C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AFB3CF2-6E68-4D18-8816-1C722F510090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -205,9 +205,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -245,7 +245,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -351,7 +351,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -493,7 +493,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -698,7 +698,7 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7:AE7"/>
     </sheetView>
   </sheetViews>
@@ -1282,94 +1282,94 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="C7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="D7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="E7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="F7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="G7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="H7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="I7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="J7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="K7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="L7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="M7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="N7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="O7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="P7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="Q7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="R7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="S7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="T7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="U7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="V7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="W7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="X7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="Y7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="Z7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="AA7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="AB7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="AC7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="AD7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
       <c r="AE7">
-        <v>0.2</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Calibration update for onshore wind deployment
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AFB3CF2-6E68-4D18-8816-1C722F510090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56B2E26-E825-4AA4-9109-2ABC21ED5332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -698,7 +698,7 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7:AE7"/>
     </sheetView>
   </sheetViews>
@@ -1282,94 +1282,94 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="C7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="D7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="E7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="F7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="G7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="H7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="I7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="J7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="K7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="L7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="M7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="N7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="O7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="P7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="Q7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="R7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="S7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="T7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="U7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="V7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="W7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="X7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="Y7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="Z7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="AA7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="AB7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="AC7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="AD7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="AE7">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Edit to solar pv capacity supply curve
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56B2E26-E825-4AA4-9109-2ABC21ED5332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E686583-1FEC-4314-9011-6556A4E44EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
@@ -698,8 +698,8 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:AE7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="AF8" sqref="AF8:AG8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1377,94 +1377,94 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="C8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="D8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="E8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="F8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="G8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="H8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="I8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="J8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="K8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="L8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="M8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="N8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="O8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="P8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="Q8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="R8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="S8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="T8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="U8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="V8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="W8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="X8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="Y8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="Z8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="AA8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="AB8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="AC8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="AD8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
       <c r="AE8">
-        <v>0.33</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated CSC variables for calibration.
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\CSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD76A592-12DE-4015-BD9D-7A2A20F160AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F590ED6-1E27-4DF7-B728-C8F586A49182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="3" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -507,24 +507,24 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,7 +532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -550,15 +550,15 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C3" sqref="C3:N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -605,7 +605,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -613,40 +613,40 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1.1000000000000001</v>
+        <v>1.1427461300794932</v>
       </c>
       <c r="D2">
-        <v>1.3</v>
+        <v>1.4438453988846189</v>
       </c>
       <c r="E2">
-        <v>1.6</v>
+        <v>1.9309364276944523</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>2.6390158215457884</v>
       </c>
       <c r="G2">
-        <v>2.5</v>
+        <v>3.6067497647680336</v>
       </c>
       <c r="H2">
-        <v>3.1</v>
+        <v>4.8742339619263264</v>
       </c>
       <c r="I2">
-        <v>3.8</v>
+        <v>6.4818210260626374</v>
       </c>
       <c r="J2">
-        <v>4.5999999999999996</v>
+        <v>8.4695622497729151</v>
       </c>
       <c r="K2">
-        <v>5.5</v>
+        <v>10.876965857390774</v>
       </c>
       <c r="L2">
-        <v>6.5</v>
+        <v>13.742909902417514</v>
       </c>
       <c r="M2">
-        <v>7.6</v>
+        <v>17.105628240207455</v>
       </c>
       <c r="N2">
-        <v>8.8000000000000007</v>
+        <v>21.002729596824665</v>
       </c>
       <c r="O2">
         <v>1000</v>
@@ -668,17 +668,17 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -698,16 +698,16 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:AE8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:AE7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -802,1337 +802,1337 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="C2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="D2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="E2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="F2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="G2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="H2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="I2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="J2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="K2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="L2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="M2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="N2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="O2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="P2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Q2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="R2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="S2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="T2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="U2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="V2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="W2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="X2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Y2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Z2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AA2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AB2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AC2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AD2">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AE2">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="C3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="D3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="E3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="F3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="G3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="H3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="I3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="J3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="K3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="L3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="M3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="N3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="O3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="P3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Q3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="R3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="S3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="T3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="U3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="V3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="W3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="X3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Y3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Z3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AA3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AB3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AC3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AD3">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AE3">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="C4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="D4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="E4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="F4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="G4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="H4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="I4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="J4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="K4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="L4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="M4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="N4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="O4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="P4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Q4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="R4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="S4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="T4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="U4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="V4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="W4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="X4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Y4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Z4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AA4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AB4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AC4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AD4">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AE4">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="C5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="D5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="E5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="F5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="G5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="H5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="I5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="J5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="K5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="L5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="M5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="N5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="O5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="P5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Q5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="R5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="S5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="T5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="U5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="V5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="W5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="X5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Y5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Z5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AA5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AB5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AC5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AD5">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AE5">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="C6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="D6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="E6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="F6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="G6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="H6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="I6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="J6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="K6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="L6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="M6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="N6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="O6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="P6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Q6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="R6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="S6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="T6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="U6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="V6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="W6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="X6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Y6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Z6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AA6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AB6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AC6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AD6">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AE6">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="C7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="D7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="E7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="F7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="G7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="H7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="I7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="J7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="K7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="L7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="M7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="N7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="O7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="P7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="Q7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="R7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="S7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="T7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="U7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="V7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="W7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="X7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="Y7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="Z7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="AA7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="AB7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="AC7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="AD7">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="AE7">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
       <c r="B8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="C8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="D8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="E8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="F8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="G8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="H8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="I8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="J8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="K8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="L8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="M8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="N8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="O8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="P8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Q8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="R8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="S8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="T8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="U8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="V8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="W8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="X8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Y8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Z8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AA8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AB8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AC8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AD8">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AE8">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="C9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="D9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="E9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="F9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="G9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="H9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="I9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="J9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="K9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="L9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="M9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="N9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="O9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="P9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Q9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="R9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="S9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="T9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="U9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="V9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="W9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="X9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Y9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Z9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AA9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AB9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AC9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AD9">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AE9">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="B10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="C10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="D10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="E10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="F10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="G10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="H10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="I10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="J10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="K10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="L10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="M10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="N10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="O10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="P10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Q10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="R10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="S10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="T10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="U10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="V10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="W10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="X10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Y10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Z10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AA10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AB10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AC10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AD10">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AE10">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
       <c r="B11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="C11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="D11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="E11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="F11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="G11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="H11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="I11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="J11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="K11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="L11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="M11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="N11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="O11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="P11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Q11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="R11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="S11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="T11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="U11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="V11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="W11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="X11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Y11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Z11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AA11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AB11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AC11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AD11">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AE11">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
       <c r="B12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="C12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="D12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="E12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="F12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="G12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="H12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="I12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="J12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="K12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="L12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="M12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="N12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="O12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="P12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Q12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="R12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="S12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="T12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="U12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="V12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="W12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="X12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Y12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Z12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AA12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AB12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AC12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AD12">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AE12">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
       <c r="B13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="C13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="D13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="E13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="F13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="G13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="H13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="I13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="J13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="K13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="L13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="M13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="N13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="O13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="P13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Q13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="R13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="S13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="T13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="U13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="V13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="W13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="X13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Y13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Z13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AA13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AB13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AC13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AD13">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AE13">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>19</v>
       </c>
       <c r="B14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="C14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="D14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="E14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="F14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="G14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="H14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="I14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="J14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="K14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="L14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="M14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="N14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="O14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="P14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Q14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="R14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="S14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="T14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="U14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="V14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="W14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="X14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Y14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Z14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AA14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AB14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AC14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AD14">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AE14">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
       <c r="B15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="C15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="D15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="E15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="F15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="G15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="H15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="I15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="J15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="K15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="L15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="M15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="N15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="O15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="P15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Q15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="R15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="S15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="T15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="U15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="V15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="W15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="X15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Y15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Z15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AA15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AB15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AC15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AD15">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AE15">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -2227,7 +2227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -2322,764 +2322,764 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>23</v>
       </c>
       <c r="B18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="C18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="D18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="E18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="F18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="G18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="H18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="I18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="J18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="K18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="L18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="M18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="N18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="O18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="P18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Q18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="R18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="S18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="T18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="U18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="V18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="W18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="X18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Y18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Z18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AA18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AB18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AC18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AD18">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AE18">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>24</v>
       </c>
       <c r="B19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="C19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="D19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="E19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="F19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="G19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="H19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="I19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="J19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="K19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="L19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="M19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="N19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="O19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="P19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Q19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="R19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="S19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="T19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="U19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="V19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="W19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="X19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Y19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Z19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AA19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AB19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AC19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AD19">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AE19">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>25</v>
       </c>
       <c r="B20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="C20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="D20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="E20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="F20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="G20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="H20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="I20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="J20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="K20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="L20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="M20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="N20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="O20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="P20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Q20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="R20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="S20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="T20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="U20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="V20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="W20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="X20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Y20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Z20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AA20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AB20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AC20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AD20">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AE20">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>26</v>
       </c>
       <c r="B21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="C21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="D21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="E21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="F21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="G21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="H21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="I21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="J21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="K21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="L21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="M21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="N21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="O21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="P21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Q21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="R21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="S21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="T21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="U21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="V21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="W21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="X21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Y21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Z21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AA21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AB21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AC21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AD21">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AE21">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>27</v>
       </c>
       <c r="B22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="C22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="D22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="E22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="F22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="G22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="H22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="I22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="J22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="K22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="L22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="M22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="N22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="O22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="P22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Q22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="R22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="S22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="T22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="U22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="V22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="W22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="X22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Y22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Z22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AA22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AB22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AC22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AD22">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AE22">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>28</v>
       </c>
       <c r="B23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="C23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="D23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="E23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="F23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="G23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="H23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="I23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="J23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="K23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="L23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="M23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="N23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="O23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="P23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Q23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="R23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="S23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="T23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="U23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="V23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="W23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="X23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Y23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Z23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AA23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AB23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AC23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AD23">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AE23">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>29</v>
       </c>
       <c r="B24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="C24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="D24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="E24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="F24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="G24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="H24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="I24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="J24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="K24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="L24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="M24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="N24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="O24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="P24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Q24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="R24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="S24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="T24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="U24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="V24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="W24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="X24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Y24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Z24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AA24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AB24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AC24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AD24">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AE24">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>30</v>
       </c>
       <c r="B25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="C25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="D25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="E25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="F25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="G25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="H25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="I25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="J25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="K25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="L25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="M25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="N25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="O25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="P25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Q25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="R25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="S25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="T25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="U25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="V25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="W25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="X25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Y25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="Z25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AA25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AB25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AC25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AD25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="AE25">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to BS to align IRA phaseout with power sector timeline; Recalibrated power sector CSC values. Recalibrated CSC values (reverted to old curve data and upped share of profitable capacity that is built)
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F590ED6-1E27-4DF7-B728-C8F586A49182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D3FC31-7262-4D54-B6B5-CC60CDAB4540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="3" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -503,7 +503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3D2DEE-686E-48A0-AC3D-0F54DEA5D0EC}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -550,7 +550,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:N3"/>
+      <selection activeCell="O7" sqref="C3:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -613,40 +613,40 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1.1427461300794932</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D2">
-        <v>1.4438453988846189</v>
+        <v>1.3</v>
       </c>
       <c r="E2">
-        <v>1.9309364276944523</v>
+        <v>1.6</v>
       </c>
       <c r="F2">
-        <v>2.6390158215457884</v>
+        <v>2</v>
       </c>
       <c r="G2">
-        <v>3.6067497647680336</v>
+        <v>2.5</v>
       </c>
       <c r="H2">
-        <v>4.8742339619263264</v>
+        <v>3.1</v>
       </c>
       <c r="I2">
-        <v>6.4818210260626374</v>
+        <v>3.8</v>
       </c>
       <c r="J2">
-        <v>8.4695622497729151</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="K2">
-        <v>10.876965857390774</v>
+        <v>5.5</v>
       </c>
       <c r="L2">
-        <v>13.742909902417514</v>
+        <v>6.4999999999999991</v>
       </c>
       <c r="M2">
-        <v>17.105628240207455</v>
+        <v>7.5999999999999979</v>
       </c>
       <c r="N2">
-        <v>21.002729596824665</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="O2">
         <v>1000</v>
@@ -698,8 +698,8 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:AE7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B18:AE25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -807,94 +807,94 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.35">
@@ -902,94 +902,94 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.35">
@@ -997,94 +997,94 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE4">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.35">
@@ -1092,94 +1092,94 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE5">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.35">
@@ -1187,94 +1187,94 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE6">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.35">
@@ -1282,94 +1282,94 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="C7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="D7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="E7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="F7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="G7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="H7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="I7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="J7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="K7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="L7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="M7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="N7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="O7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="P7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="Q7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="R7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="S7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="T7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="U7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="V7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="W7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="X7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="Y7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="Z7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="AA7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="AB7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="AC7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="AD7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="AE7">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.35">
@@ -1377,94 +1377,94 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE8">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.35">
@@ -1472,94 +1472,94 @@
         <v>14</v>
       </c>
       <c r="B9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE9">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.35">
@@ -1567,94 +1567,94 @@
         <v>15</v>
       </c>
       <c r="B10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.35">
@@ -1662,94 +1662,94 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.35">
@@ -1757,94 +1757,94 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE12">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.35">
@@ -1852,94 +1852,94 @@
         <v>18</v>
       </c>
       <c r="B13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE13">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.35">
@@ -1947,94 +1947,94 @@
         <v>19</v>
       </c>
       <c r="B14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE14">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.35">
@@ -2042,94 +2042,94 @@
         <v>20</v>
       </c>
       <c r="B15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE15">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.35">
@@ -2327,94 +2327,94 @@
         <v>23</v>
       </c>
       <c r="B18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE18">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.35">
@@ -2422,94 +2422,94 @@
         <v>24</v>
       </c>
       <c r="B19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE19">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.35">
@@ -2517,94 +2517,94 @@
         <v>25</v>
       </c>
       <c r="B20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE20">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.35">
@@ -2612,94 +2612,94 @@
         <v>26</v>
       </c>
       <c r="B21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE21">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.35">
@@ -2707,94 +2707,94 @@
         <v>27</v>
       </c>
       <c r="B22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE22">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.35">
@@ -2802,94 +2802,94 @@
         <v>28</v>
       </c>
       <c r="B23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE23">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.35">
@@ -2897,94 +2897,94 @@
         <v>29</v>
       </c>
       <c r="B24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE24">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.35">
@@ -2992,94 +2992,94 @@
         <v>30</v>
       </c>
       <c r="B25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="F25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="G25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="H25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="I25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="J25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="K25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="M25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="N25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="O25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="P25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Q25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="R25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="S25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="T25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="U25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="V25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="W25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="X25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Y25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="Z25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AB25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AC25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AD25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AE25">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to CSC. Change the structure to better represent the diminishing marginal return of incremantal profitability for new capacity.
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D3FC31-7262-4D54-B6B5-CC60CDAB4540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3641FE2-2A3A-4F0D-A056-1DE04A6E46AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
@@ -504,7 +504,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="AU56" sqref="AU56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -550,7 +550,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O7" sqref="C3:O7"/>
+      <selection activeCell="P14" sqref="A4:P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -566,43 +566,56 @@
         <v>0</v>
       </c>
       <c r="C1">
+        <f>0.25^(1/B2)</f>
         <v>0.25</v>
       </c>
       <c r="D1">
+        <f t="shared" ref="D1:O1" si="0">0.25^(1/C2)</f>
+        <v>0.32987697769322361</v>
+      </c>
+      <c r="E1">
+        <f t="shared" si="0"/>
+        <v>0.3968502629920499</v>
+      </c>
+      <c r="F1">
+        <f t="shared" si="0"/>
+        <v>0.45286183213195336</v>
+      </c>
+      <c r="G1">
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="E1">
-        <v>0.75</v>
-      </c>
-      <c r="F1">
-        <v>1</v>
-      </c>
-      <c r="G1">
-        <v>1.25</v>
-      </c>
       <c r="H1">
-        <v>1.5</v>
+        <f t="shared" si="0"/>
+        <v>0.54002986944615305</v>
       </c>
       <c r="I1">
-        <v>1.75</v>
+        <f t="shared" si="0"/>
+        <v>0.57434917749851755</v>
       </c>
       <c r="J1">
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>0.60404472220222361</v>
       </c>
       <c r="K1">
-        <v>2.25</v>
+        <f t="shared" si="0"/>
+        <v>0.6299605249474366</v>
       </c>
       <c r="L1">
-        <v>2.5</v>
+        <f t="shared" si="0"/>
+        <v>0.65275584885490479</v>
       </c>
       <c r="M1">
-        <v>2.75</v>
+        <f t="shared" si="0"/>
+        <v>0.67295009631617808</v>
       </c>
       <c r="N1">
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>0.690956439983888</v>
       </c>
       <c r="O1">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>0.70710678118654757</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
@@ -613,40 +626,40 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1.1000000000000001</v>
+        <v>1.25</v>
       </c>
       <c r="D2">
-        <v>1.3</v>
+        <v>1.5</v>
       </c>
       <c r="E2">
-        <v>1.6</v>
+        <v>1.75</v>
       </c>
       <c r="F2">
         <v>2</v>
       </c>
       <c r="G2">
+        <v>2.25</v>
+      </c>
+      <c r="H2">
         <v>2.5</v>
       </c>
-      <c r="H2">
-        <v>3.1</v>
-      </c>
       <c r="I2">
-        <v>3.8</v>
+        <v>2.75</v>
       </c>
       <c r="J2">
-        <v>4.5999999999999996</v>
+        <v>3</v>
       </c>
       <c r="K2">
-        <v>5.5</v>
+        <v>3.25</v>
       </c>
       <c r="L2">
-        <v>6.4999999999999991</v>
+        <v>3.5</v>
       </c>
       <c r="M2">
-        <v>7.5999999999999979</v>
+        <v>3.75</v>
       </c>
       <c r="N2">
-        <v>8.8000000000000007</v>
+        <v>4</v>
       </c>
       <c r="O2">
         <v>1000</v>
@@ -807,94 +820,94 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="C2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="E2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="F2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="G2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="H2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="I2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="J2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="K2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="L2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="M2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="N2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="O2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="P2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Q2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="R2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="S2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="T2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="U2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="V2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="W2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="X2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Y2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Z2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AA2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AB2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AC2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AD2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AE2">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.35">
@@ -902,94 +915,94 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="C3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="E3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="F3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="G3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="H3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="I3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="J3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="K3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="L3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="M3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="N3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="O3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="P3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Q3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="R3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="S3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="T3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="U3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="V3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="W3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="X3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Y3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Z3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AA3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AB3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AC3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AD3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AE3">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.35">
@@ -997,94 +1010,94 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="C4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="E4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="F4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="G4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="H4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="I4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="J4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="K4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="L4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="M4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="N4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="O4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="P4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Q4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="R4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="S4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="T4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="U4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="V4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="W4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="X4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Y4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Z4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AA4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AB4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AC4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AD4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AE4">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.35">
@@ -1092,94 +1105,94 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="C5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="E5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="F5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="G5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="H5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="I5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="J5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="K5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="L5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="M5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="N5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="O5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="P5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Q5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="R5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="S5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="T5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="U5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="V5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="W5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="X5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Y5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Z5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AA5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AB5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AC5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AD5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AE5">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.35">
@@ -1187,94 +1200,94 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="C6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="E6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="F6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="G6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="H6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="I6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="J6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="K6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="L6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="M6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="N6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="O6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="P6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Q6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="R6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="S6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="T6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="U6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="V6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="W6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="X6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Y6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Z6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AA6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AB6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AC6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AD6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AE6">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.35">
@@ -1282,94 +1295,94 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="C7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="E7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="F7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="G7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="H7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="I7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="J7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="K7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="L7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="M7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="N7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="O7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="P7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Q7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="R7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="S7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="T7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="U7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="V7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="W7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="X7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Y7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Z7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AA7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AB7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AC7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AD7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AE7">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.35">
@@ -1377,94 +1390,94 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="C8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="E8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="F8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="G8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="H8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="I8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="J8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="K8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="L8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="M8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="N8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="O8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="P8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Q8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="R8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="S8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="T8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="U8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="V8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="W8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="X8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Y8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Z8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AA8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AB8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AC8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AD8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AE8">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.35">
@@ -1472,94 +1485,94 @@
         <v>14</v>
       </c>
       <c r="B9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="C9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="E9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="F9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="G9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="H9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="I9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="J9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="K9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="L9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="M9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="N9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="O9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="P9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Q9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="R9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="S9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="T9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="U9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="V9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="W9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="X9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Y9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Z9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AA9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AB9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AC9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AD9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AE9">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.35">
@@ -1567,94 +1580,94 @@
         <v>15</v>
       </c>
       <c r="B10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="C10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="E10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="F10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="G10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="H10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="I10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="J10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="K10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="L10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="M10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="N10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="O10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="P10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Q10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="R10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="S10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="T10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="U10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="V10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="W10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="X10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Y10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Z10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AA10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AB10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AC10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AD10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AE10">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.35">
@@ -1662,94 +1675,94 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="C11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="E11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="F11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="G11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="H11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="I11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="J11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="K11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="L11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="M11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="N11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="O11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="P11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Q11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="R11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="S11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="T11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="U11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="V11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="W11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="X11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Y11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Z11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AA11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AB11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AC11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AD11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AE11">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.35">
@@ -1757,94 +1770,94 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="C12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="E12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="F12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="G12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="H12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="I12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="J12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="K12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="L12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="M12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="N12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="O12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="P12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Q12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="R12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="S12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="T12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="U12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="V12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="W12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="X12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Y12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Z12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AA12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AB12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AC12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AD12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AE12">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.35">
@@ -1852,94 +1865,94 @@
         <v>18</v>
       </c>
       <c r="B13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="C13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="E13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="F13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="G13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="H13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="I13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="J13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="K13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="L13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="M13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="N13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="O13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="P13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Q13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="R13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="S13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="T13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="U13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="V13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="W13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="X13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Y13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Z13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AA13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AB13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AC13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AD13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AE13">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.35">
@@ -1947,94 +1960,94 @@
         <v>19</v>
       </c>
       <c r="B14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="C14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="E14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="F14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="G14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="H14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="I14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="J14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="K14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="L14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="M14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="N14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="O14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="P14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Q14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="R14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="S14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="T14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="U14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="V14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="W14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="X14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Y14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Z14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AA14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AB14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AC14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AD14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AE14">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.35">
@@ -2042,94 +2055,94 @@
         <v>20</v>
       </c>
       <c r="B15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="C15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="E15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="F15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="G15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="H15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="I15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="J15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="K15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="L15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="M15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="N15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="O15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="P15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Q15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="R15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="S15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="T15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="U15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="V15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="W15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="X15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Y15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Z15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AA15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AB15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AC15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AD15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AE15">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.35">
@@ -2327,94 +2340,94 @@
         <v>23</v>
       </c>
       <c r="B18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="C18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="E18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="F18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="G18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="H18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="I18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="J18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="K18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="L18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="M18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="N18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="O18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="P18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Q18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="R18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="S18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="T18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="U18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="V18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="W18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="X18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Y18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Z18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AA18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AB18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AC18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AD18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AE18">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.35">
@@ -2422,94 +2435,94 @@
         <v>24</v>
       </c>
       <c r="B19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="C19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="E19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="F19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="G19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="H19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="I19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="J19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="K19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="L19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="M19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="N19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="O19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="P19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Q19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="R19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="S19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="T19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="U19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="V19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="W19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="X19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Y19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Z19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AA19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AB19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AC19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AD19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AE19">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.35">
@@ -2517,94 +2530,94 @@
         <v>25</v>
       </c>
       <c r="B20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="C20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="E20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="F20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="G20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="H20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="I20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="J20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="K20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="L20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="M20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="N20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="O20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="P20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Q20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="R20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="S20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="T20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="U20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="V20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="W20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="X20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Y20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Z20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AA20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AB20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AC20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AD20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AE20">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.35">
@@ -2612,94 +2625,94 @@
         <v>26</v>
       </c>
       <c r="B21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="C21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="E21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="F21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="G21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="H21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="I21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="J21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="K21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="L21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="M21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="N21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="O21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="P21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Q21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="R21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="S21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="T21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="U21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="V21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="W21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="X21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Y21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Z21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AA21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AB21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AC21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AD21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AE21">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.35">
@@ -2707,94 +2720,94 @@
         <v>27</v>
       </c>
       <c r="B22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="C22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="E22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="F22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="G22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="H22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="I22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="J22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="K22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="L22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="M22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="N22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="O22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="P22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Q22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="R22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="S22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="T22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="U22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="V22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="W22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="X22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Y22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Z22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AA22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AB22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AC22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AD22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AE22">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.35">
@@ -2802,94 +2815,94 @@
         <v>28</v>
       </c>
       <c r="B23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="C23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="E23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="F23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="G23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="H23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="I23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="J23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="K23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="L23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="M23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="N23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="O23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="P23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Q23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="R23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="S23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="T23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="U23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="V23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="W23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="X23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Y23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Z23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AA23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AB23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AC23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AD23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AE23">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.35">
@@ -2897,94 +2910,94 @@
         <v>29</v>
       </c>
       <c r="B24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="C24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="E24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="F24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="G24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="H24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="I24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="J24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="K24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="L24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="M24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="N24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="O24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="P24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Q24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="R24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="S24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="T24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="U24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="V24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="W24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="X24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Y24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Z24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AA24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AB24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AC24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AD24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AE24">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.35">
@@ -2992,94 +3005,94 @@
         <v>30</v>
       </c>
       <c r="B25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="C25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="D25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="E25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="F25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="G25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="H25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="I25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="J25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="K25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="L25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="M25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="N25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="O25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="P25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Q25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="R25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="S25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="T25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="U25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="V25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="W25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="X25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Y25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="Z25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AA25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AB25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AC25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AD25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="AE25">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fix for calculating achieved capcaity factors for resources with no prior capacity. We now use calculated hypothetical capcaity factors in every year except the start year for least cost dispatch resources to avoid data discontinuities.
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15A7CD0-8D3E-480B-B2B3-5FB600AFD681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B071AECB-8889-4455-998A-0AB359C98300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1830" yWindow="2880" windowWidth="25230" windowHeight="15465" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
+    <workbookView xWindow="9210" yWindow="2970" windowWidth="23505" windowHeight="17385" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -2821,94 +2821,94 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="P2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="V2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE2">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -2916,94 +2916,94 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="P3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="V3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE3">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
@@ -3011,94 +3011,94 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="P4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="V4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE4">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
@@ -3106,94 +3106,94 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="P5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="V5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE5">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
@@ -3201,94 +3201,94 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="P6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="V6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE6">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
@@ -3296,94 +3296,94 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="P7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="V7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE7">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
@@ -3391,94 +3391,94 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="P8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="V8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE8">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
@@ -3486,94 +3486,94 @@
         <v>14</v>
       </c>
       <c r="B9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="P9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="V9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE9">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
@@ -3581,94 +3581,94 @@
         <v>15</v>
       </c>
       <c r="B10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="P10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="V10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE10">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
@@ -3676,94 +3676,94 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="P11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="V11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE11">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
@@ -3771,94 +3771,94 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="P12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="V12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE12">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
@@ -3866,94 +3866,94 @@
         <v>18</v>
       </c>
       <c r="B13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="P13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="V13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE13">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
@@ -3961,94 +3961,94 @@
         <v>19</v>
       </c>
       <c r="B14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="P14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="V14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE14">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
@@ -4056,94 +4056,94 @@
         <v>20</v>
       </c>
       <c r="B15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="P15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="V15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE15">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
@@ -4151,94 +4151,94 @@
         <v>21</v>
       </c>
       <c r="B16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="P16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="V16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE16">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
@@ -4246,94 +4246,94 @@
         <v>22</v>
       </c>
       <c r="B17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="P17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="V17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE17">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
@@ -4341,94 +4341,94 @@
         <v>23</v>
       </c>
       <c r="B18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="P18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="V18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
@@ -4436,94 +4436,94 @@
         <v>24</v>
       </c>
       <c r="B19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="P19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="V19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE19">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
@@ -4531,94 +4531,94 @@
         <v>25</v>
       </c>
       <c r="B20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="P20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="V20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE20">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
@@ -4626,94 +4626,94 @@
         <v>26</v>
       </c>
       <c r="B21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="P21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="V21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE21">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
@@ -4721,94 +4721,94 @@
         <v>27</v>
       </c>
       <c r="B22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="P22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="V22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE22">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
@@ -4816,94 +4816,94 @@
         <v>28</v>
       </c>
       <c r="B23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="P23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="V23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE23">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
@@ -4911,94 +4911,94 @@
         <v>29</v>
       </c>
       <c r="B24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="P24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="V24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE24">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
@@ -5006,94 +5006,94 @@
         <v>30</v>
       </c>
       <c r="B25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="C25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="E25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="F25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="G25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="H25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="I25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="K25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="L25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="M25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="N25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="O25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="P25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Q25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="R25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="S25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="T25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="U25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="V25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="W25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Y25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="Z25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AA25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AB25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AC25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AD25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="AE25">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to electricity calibration
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B071AECB-8889-4455-998A-0AB359C98300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE42316-798B-464A-961F-6C11136F8CE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9210" yWindow="2970" windowWidth="23505" windowHeight="17385" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
+    <workbookView xWindow="23430" yWindow="3990" windowWidth="23505" windowHeight="17385" activeTab="3" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -2470,8 +2470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3D2DEE-686E-48A0-AC3D-0F54DEA5D0EC}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2712,7 +2712,7 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:AE25"/>
     </sheetView>
   </sheetViews>
@@ -2821,94 +2821,94 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="C2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="D2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="E2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="F2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="H2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="I2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="J2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="K2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="M2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="N2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="O2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="P2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Q2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="R2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="S2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="T2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="U2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="V2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="W2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="X2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Y2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Z2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AA2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AB2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AC2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AD2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AE2">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -2916,94 +2916,94 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="C3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="D3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="E3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="F3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="H3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="I3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="J3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="K3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="M3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="N3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="O3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="P3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Q3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="R3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="S3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="T3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="U3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="V3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="W3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="X3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Y3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Z3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AA3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AB3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AC3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AD3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AE3">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
@@ -3011,94 +3011,94 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="C4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="D4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="E4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="F4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="H4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="I4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="J4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="K4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="M4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="N4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="O4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="P4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Q4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="R4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="S4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="T4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="U4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="V4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="W4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="X4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Y4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Z4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AA4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AB4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AC4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AD4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AE4">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
@@ -3106,94 +3106,94 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="C5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="D5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="E5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="F5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="H5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="I5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="J5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="K5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="M5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="N5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="O5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="P5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Q5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="R5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="S5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="T5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="U5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="V5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="W5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="X5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Y5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Z5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AA5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AB5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AC5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AD5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AE5">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
@@ -3201,94 +3201,94 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="C6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="D6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="E6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="F6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="H6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="I6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="J6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="K6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="M6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="N6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="O6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="P6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Q6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="R6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="S6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="T6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="U6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="V6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="W6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="X6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Y6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Z6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AA6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AB6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AC6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AD6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AE6">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
@@ -3296,94 +3296,94 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="C7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="D7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="E7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="F7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="H7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="I7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="J7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="K7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="M7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="N7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="O7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="P7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Q7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="R7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="S7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="T7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="U7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="V7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="W7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="X7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Y7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Z7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AA7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AB7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AC7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AD7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AE7">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
@@ -3391,94 +3391,94 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="C8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="D8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="E8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="F8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="H8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="I8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="J8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="K8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="M8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="N8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="O8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="P8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Q8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="R8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="S8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="T8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="U8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="V8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="W8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="X8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Y8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Z8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AA8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AB8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AC8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AD8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AE8">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
@@ -3486,94 +3486,94 @@
         <v>14</v>
       </c>
       <c r="B9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="C9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="D9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="E9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="F9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="H9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="I9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="J9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="K9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="M9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="N9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="O9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="P9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Q9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="R9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="S9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="T9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="U9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="V9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="W9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="X9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Y9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Z9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AA9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AB9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AC9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AD9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AE9">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
@@ -3581,94 +3581,94 @@
         <v>15</v>
       </c>
       <c r="B10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="C10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="D10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="E10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="F10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="H10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="I10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="J10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="K10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="M10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="N10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="O10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="P10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Q10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="R10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="S10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="T10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="U10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="V10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="W10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="X10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Y10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Z10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AA10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AB10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AC10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AD10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AE10">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
@@ -3676,94 +3676,94 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="C11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="D11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="E11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="F11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="H11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="I11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="J11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="K11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="M11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="N11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="O11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="P11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Q11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="R11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="S11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="T11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="U11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="V11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="W11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="X11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Y11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Z11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AA11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AB11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AC11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AD11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AE11">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
@@ -3771,94 +3771,94 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="C12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="D12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="E12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="F12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="H12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="I12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="J12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="K12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="M12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="N12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="O12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="P12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Q12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="R12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="S12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="T12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="U12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="V12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="W12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="X12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Y12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Z12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AA12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AB12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AC12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AD12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AE12">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
@@ -3866,94 +3866,94 @@
         <v>18</v>
       </c>
       <c r="B13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="C13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="D13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="E13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="F13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="H13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="I13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="J13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="K13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="M13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="N13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="O13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="P13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Q13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="R13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="S13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="T13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="U13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="V13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="W13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="X13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Y13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Z13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AA13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AB13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AC13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AD13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AE13">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
@@ -3961,94 +3961,94 @@
         <v>19</v>
       </c>
       <c r="B14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="C14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="D14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="E14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="F14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="H14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="I14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="J14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="K14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="M14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="N14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="O14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="P14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Q14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="R14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="S14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="T14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="U14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="V14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="W14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="X14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Y14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Z14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AA14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AB14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AC14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AD14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AE14">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
@@ -4056,94 +4056,94 @@
         <v>20</v>
       </c>
       <c r="B15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="C15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="D15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="E15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="F15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="H15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="I15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="J15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="K15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="M15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="N15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="O15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="P15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Q15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="R15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="S15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="T15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="U15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="V15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="W15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="X15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Y15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Z15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AA15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AB15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AC15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AD15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AE15">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
@@ -4151,94 +4151,94 @@
         <v>21</v>
       </c>
       <c r="B16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="C16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="D16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="E16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="F16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="H16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="I16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="J16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="K16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="M16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="N16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="O16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="P16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Q16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="R16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="S16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="T16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="U16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="V16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="W16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="X16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Y16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Z16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AA16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AB16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AC16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AD16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AE16">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
@@ -4246,94 +4246,94 @@
         <v>22</v>
       </c>
       <c r="B17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="C17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="D17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="E17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="F17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="H17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="I17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="J17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="K17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="M17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="N17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="O17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="P17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Q17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="R17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="S17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="T17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="U17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="V17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="W17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="X17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Y17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Z17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AA17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AB17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AC17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AD17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AE17">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
@@ -4341,94 +4341,94 @@
         <v>23</v>
       </c>
       <c r="B18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="C18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="D18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="E18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="F18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="H18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="I18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="J18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="K18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="M18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="N18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="O18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="P18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Q18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="R18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="S18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="T18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="U18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="V18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="W18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="X18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Y18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Z18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AA18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AB18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AC18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AD18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AE18">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
@@ -4436,94 +4436,94 @@
         <v>24</v>
       </c>
       <c r="B19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="C19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="D19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="E19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="F19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="H19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="I19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="J19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="K19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="M19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="N19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="O19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="P19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Q19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="R19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="S19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="T19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="U19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="V19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="W19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="X19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Y19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Z19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AA19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AB19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AC19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AD19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AE19">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
@@ -4531,94 +4531,94 @@
         <v>25</v>
       </c>
       <c r="B20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="C20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="D20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="E20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="F20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="H20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="I20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="J20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="K20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="M20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="N20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="O20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="P20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Q20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="R20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="S20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="T20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="U20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="V20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="W20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="X20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Y20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Z20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AA20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AB20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AC20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AD20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AE20">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
@@ -4626,94 +4626,94 @@
         <v>26</v>
       </c>
       <c r="B21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="C21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="D21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="E21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="F21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="H21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="I21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="J21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="K21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="M21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="N21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="O21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="P21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Q21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="R21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="S21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="T21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="U21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="V21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="W21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="X21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Y21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Z21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AA21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AB21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AC21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AD21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AE21">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
@@ -4721,94 +4721,94 @@
         <v>27</v>
       </c>
       <c r="B22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="C22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="D22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="E22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="F22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="H22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="I22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="J22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="K22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="M22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="N22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="O22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="P22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Q22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="R22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="S22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="T22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="U22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="V22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="W22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="X22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Y22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Z22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AA22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AB22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AC22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AD22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AE22">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
@@ -4816,94 +4816,94 @@
         <v>28</v>
       </c>
       <c r="B23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="C23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="D23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="E23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="F23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="H23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="I23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="J23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="K23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="M23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="N23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="O23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="P23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Q23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="R23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="S23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="T23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="U23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="V23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="W23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="X23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Y23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Z23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AA23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AB23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AC23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AD23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AE23">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
@@ -4911,94 +4911,94 @@
         <v>29</v>
       </c>
       <c r="B24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="C24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="D24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="E24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="F24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="H24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="I24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="J24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="K24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="M24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="N24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="O24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="P24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Q24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="R24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="S24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="T24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="U24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="V24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="W24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="X24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Y24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Z24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AA24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AB24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AC24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AD24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AE24">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
@@ -5006,94 +5006,94 @@
         <v>30</v>
       </c>
       <c r="B25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="C25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="D25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="E25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="F25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="G25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="H25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="I25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="J25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="K25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="L25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="M25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="N25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="O25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="P25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Q25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="R25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="S25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="T25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="U25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="V25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="W25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="X25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Y25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="Z25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AA25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AB25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AC25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AD25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
       <c r="AE25">
-        <v>0.55000000000000004</v>
+        <v>0.66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edit CSC value for onshore wind to represent higher siting constraints compared to solar
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\CSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C110F7-550A-49C7-9993-BC93998675E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0D785E-3678-4517-A5F6-3A839C381C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="3" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -2470,31 +2470,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3D2DEE-686E-48A0-AC3D-0F54DEA5D0EC}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="88.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="88.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -2502,17 +2502,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>1.45</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -2553,12 +2553,12 @@
       <selection activeCell="B1" sqref="B1:N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2682,17 +2682,17 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2712,16 +2712,16 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AE25"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:AE7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3101,7 +3101,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -3291,102 +3291,102 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="C7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="D7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="E7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="F7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="G7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="H7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="I7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="J7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="K7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="L7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="M7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="N7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="O7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="P7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="Q7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="R7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="S7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="T7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="U7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="V7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="W7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="X7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="Y7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="Z7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="AA7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="AB7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="AC7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="AD7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="AE7">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -3671,7 +3671,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -3956,7 +3956,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -4051,7 +4051,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -4146,7 +4146,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -4241,7 +4241,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -4336,7 +4336,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -4431,7 +4431,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -4621,7 +4621,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -4716,7 +4716,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -4811,7 +4811,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -4906,7 +4906,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -5001,7 +5001,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Add CSC file for hybrid power plants
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0D785E-3678-4517-A5F6-3A839C381C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EA3E01-597B-419B-939D-70FB58155BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="3" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="CSC-CSCCCMvSoECBtY" sheetId="2" r:id="rId2"/>
     <sheet name="CSC-CSCMBCfPTwNEC" sheetId="3" r:id="rId3"/>
     <sheet name="CSC-CSCSoCECBiaSY" sheetId="4" r:id="rId4"/>
+    <sheet name="CSC-CSCSoCEHCBiaSY" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
   <si>
     <t xml:space="preserve">Source: </t>
   </si>
@@ -153,6 +154,9 @@
   </si>
   <si>
     <t>Max share of existing capacity buildable</t>
+  </si>
+  <si>
+    <t>CSC Capacity Supply Curve Share of Cost Effective Hybrid Capacity Built in a Single Year</t>
   </si>
 </sst>
 </file>
@@ -2093,13 +2097,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>4572000</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2468,71 +2472,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3D2DEE-686E-48A0-AC3D-0F54DEA5D0EC}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="88.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="88.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>35</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>1.45</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>38</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>36</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>3</v>
       </c>
     </row>
@@ -2553,12 +2562,12 @@
       <selection activeCell="B1" sqref="B1:N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2566,59 +2575,59 @@
         <v>0</v>
       </c>
       <c r="C1">
-        <f>2*(1/(1+EXP(-(C2-1)/(About!$B$11-1)*About!$B$13))-0.5)*About!$B$12</f>
+        <f>2*(1/(1+EXP(-(C2-1)/(About!$B$12-1)*About!$B$14))-0.5)*About!$B$13</f>
         <v>8.2570206462314721E-2</v>
       </c>
       <c r="D1">
-        <f>2*(1/(1+EXP(-(D2-1)/(About!$B$11-1)*About!$B$13))-0.5)*About!$B$12</f>
+        <f>2*(1/(1+EXP(-(D2-1)/(About!$B$12-1)*About!$B$14))-0.5)*About!$B$13</f>
         <v>0.16075636876581723</v>
       </c>
       <c r="E1">
-        <f>2*(1/(1+EXP(-(E2-1)/(About!$B$11-1)*About!$B$13))-0.5)*About!$B$12</f>
+        <f>2*(1/(1+EXP(-(E2-1)/(About!$B$12-1)*About!$B$14))-0.5)*About!$B$13</f>
         <v>0.23105857863000479</v>
       </c>
       <c r="F1">
-        <f>2*(1/(1+EXP(-(F2-1)/(About!$B$11-1)*About!$B$13))-0.5)*About!$B$12</f>
+        <f>2*(1/(1+EXP(-(F2-1)/(About!$B$12-1)*About!$B$14))-0.5)*About!$B$13</f>
         <v>0.29139147267395504</v>
       </c>
       <c r="G1">
-        <f>2*(1/(1+EXP(-(G2-1)/(About!$B$11-1)*About!$B$13))-0.5)*About!$B$12</f>
+        <f>2*(1/(1+EXP(-(G2-1)/(About!$B$12-1)*About!$B$14))-0.5)*About!$B$13</f>
         <v>0.3411308951190849</v>
       </c>
       <c r="H1">
-        <f>2*(1/(1+EXP(-(H2-1)/(About!$B$11-1)*About!$B$13))-0.5)*About!$B$12</f>
+        <f>2*(1/(1+EXP(-(H2-1)/(About!$B$12-1)*About!$B$14))-0.5)*About!$B$13</f>
         <v>0.38079707797788254</v>
       </c>
       <c r="I1">
-        <f>2*(1/(1+EXP(-(I2-1)/(About!$B$11-1)*About!$B$13))-0.5)*About!$B$12</f>
+        <f>2*(1/(1+EXP(-(I2-1)/(About!$B$12-1)*About!$B$14))-0.5)*About!$B$13</f>
         <v>0.41160032279294168</v>
       </c>
       <c r="J1">
-        <f>2*(1/(1+EXP(-(J2-1)/(About!$B$11-1)*About!$B$13))-0.5)*About!$B$12</f>
+        <f>2*(1/(1+EXP(-(J2-1)/(About!$B$12-1)*About!$B$14))-0.5)*About!$B$13</f>
         <v>0.43503083087133598</v>
       </c>
       <c r="K1">
-        <f>2*(1/(1+EXP(-(K2-1)/(About!$B$11-1)*About!$B$13))-0.5)*About!$B$12</f>
+        <f>2*(1/(1+EXP(-(K2-1)/(About!$B$12-1)*About!$B$14))-0.5)*About!$B$13</f>
         <v>0.45257412682243336</v>
       </c>
       <c r="L1">
-        <f>2*(1/(1+EXP(-(L2-1)/(About!$B$11-1)*About!$B$13))-0.5)*About!$B$12</f>
+        <f>2*(1/(1+EXP(-(L2-1)/(About!$B$12-1)*About!$B$14))-0.5)*About!$B$13</f>
         <v>0.46555480433378893</v>
       </c>
       <c r="M1">
-        <f>2*(1/(1+EXP(-(M2-1)/(About!$B$11-1)*About!$B$13))-0.5)*About!$B$12</f>
+        <f>2*(1/(1+EXP(-(M2-1)/(About!$B$12-1)*About!$B$14))-0.5)*About!$B$13</f>
         <v>0.47507557335288597</v>
       </c>
       <c r="N1">
-        <f>2*(1/(1+EXP(-(N2-1)/(About!$B$11-1)*About!$B$13))-0.5)*About!$B$12</f>
+        <f>2*(1/(1+EXP(-(N2-1)/(About!$B$12-1)*About!$B$14))-0.5)*About!$B$13</f>
         <v>0.48201379003790845</v>
       </c>
       <c r="O1">
-        <f>About!$B$12</f>
+        <f>About!$B$13</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2682,17 +2691,17 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -2712,16 +2721,16 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7:AE7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2816,7 +2825,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -2911,7 +2920,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -3006,7 +3015,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -3101,7 +3110,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -3196,7 +3205,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -3291,7 +3300,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -3386,7 +3395,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -3481,7 +3490,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -3576,7 +3585,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -3671,7 +3680,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -3766,7 +3775,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -3861,7 +3870,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -3956,7 +3965,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -4051,7 +4060,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -4146,7 +4155,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -4241,7 +4250,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -4336,7 +4345,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -4431,7 +4440,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -4526,7 +4535,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -4621,7 +4630,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -4716,7 +4725,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -4811,7 +4820,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -4906,7 +4915,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -5001,7 +5010,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -5094,6 +5103,2402 @@
       </c>
       <c r="AE25">
         <v>0.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2C5DFE4-6336-427D-B509-77FBC5D5DDAF}">
+  <sheetPr>
+    <tabColor rgb="FF002060"/>
+  </sheetPr>
+  <dimension ref="A1:AE25"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:AE8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1">
+        <v>2021</v>
+      </c>
+      <c r="C1">
+        <v>2022</v>
+      </c>
+      <c r="D1">
+        <v>2023</v>
+      </c>
+      <c r="E1">
+        <v>2024</v>
+      </c>
+      <c r="F1">
+        <v>2025</v>
+      </c>
+      <c r="G1">
+        <v>2026</v>
+      </c>
+      <c r="H1">
+        <v>2027</v>
+      </c>
+      <c r="I1">
+        <v>2028</v>
+      </c>
+      <c r="J1">
+        <v>2029</v>
+      </c>
+      <c r="K1">
+        <v>2030</v>
+      </c>
+      <c r="L1">
+        <v>2031</v>
+      </c>
+      <c r="M1">
+        <v>2032</v>
+      </c>
+      <c r="N1">
+        <v>2033</v>
+      </c>
+      <c r="O1">
+        <v>2034</v>
+      </c>
+      <c r="P1">
+        <v>2035</v>
+      </c>
+      <c r="Q1">
+        <v>2036</v>
+      </c>
+      <c r="R1">
+        <v>2037</v>
+      </c>
+      <c r="S1">
+        <v>2038</v>
+      </c>
+      <c r="T1">
+        <v>2039</v>
+      </c>
+      <c r="U1">
+        <v>2040</v>
+      </c>
+      <c r="V1">
+        <v>2041</v>
+      </c>
+      <c r="W1">
+        <v>2042</v>
+      </c>
+      <c r="X1">
+        <v>2043</v>
+      </c>
+      <c r="Y1">
+        <v>2044</v>
+      </c>
+      <c r="Z1">
+        <v>2045</v>
+      </c>
+      <c r="AA1">
+        <v>2046</v>
+      </c>
+      <c r="AB1">
+        <v>2047</v>
+      </c>
+      <c r="AC1">
+        <v>2048</v>
+      </c>
+      <c r="AD1">
+        <v>2049</v>
+      </c>
+      <c r="AE1">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>0.05</v>
+      </c>
+      <c r="C7">
+        <v>0.05</v>
+      </c>
+      <c r="D7">
+        <v>0.05</v>
+      </c>
+      <c r="E7">
+        <v>0.05</v>
+      </c>
+      <c r="F7">
+        <v>0.05</v>
+      </c>
+      <c r="G7">
+        <v>0.05</v>
+      </c>
+      <c r="H7">
+        <v>0.05</v>
+      </c>
+      <c r="I7">
+        <v>0.05</v>
+      </c>
+      <c r="J7">
+        <v>0.05</v>
+      </c>
+      <c r="K7">
+        <v>0.05</v>
+      </c>
+      <c r="L7">
+        <v>0.05</v>
+      </c>
+      <c r="M7">
+        <v>0.05</v>
+      </c>
+      <c r="N7">
+        <v>0.05</v>
+      </c>
+      <c r="O7">
+        <v>0.05</v>
+      </c>
+      <c r="P7">
+        <v>0.05</v>
+      </c>
+      <c r="Q7">
+        <v>0.05</v>
+      </c>
+      <c r="R7">
+        <v>0.05</v>
+      </c>
+      <c r="S7">
+        <v>0.05</v>
+      </c>
+      <c r="T7">
+        <v>0.05</v>
+      </c>
+      <c r="U7">
+        <v>0.05</v>
+      </c>
+      <c r="V7">
+        <v>0.05</v>
+      </c>
+      <c r="W7">
+        <v>0.05</v>
+      </c>
+      <c r="X7">
+        <v>0.05</v>
+      </c>
+      <c r="Y7">
+        <v>0.05</v>
+      </c>
+      <c r="Z7">
+        <v>0.05</v>
+      </c>
+      <c r="AA7">
+        <v>0.05</v>
+      </c>
+      <c r="AB7">
+        <v>0.05</v>
+      </c>
+      <c r="AC7">
+        <v>0.05</v>
+      </c>
+      <c r="AD7">
+        <v>0.05</v>
+      </c>
+      <c r="AE7">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>0.05</v>
+      </c>
+      <c r="C8">
+        <v>0.05</v>
+      </c>
+      <c r="D8">
+        <v>0.05</v>
+      </c>
+      <c r="E8">
+        <v>0.05</v>
+      </c>
+      <c r="F8">
+        <v>0.05</v>
+      </c>
+      <c r="G8">
+        <v>0.05</v>
+      </c>
+      <c r="H8">
+        <v>0.05</v>
+      </c>
+      <c r="I8">
+        <v>0.05</v>
+      </c>
+      <c r="J8">
+        <v>0.05</v>
+      </c>
+      <c r="K8">
+        <v>0.05</v>
+      </c>
+      <c r="L8">
+        <v>0.05</v>
+      </c>
+      <c r="M8">
+        <v>0.05</v>
+      </c>
+      <c r="N8">
+        <v>0.05</v>
+      </c>
+      <c r="O8">
+        <v>0.05</v>
+      </c>
+      <c r="P8">
+        <v>0.05</v>
+      </c>
+      <c r="Q8">
+        <v>0.05</v>
+      </c>
+      <c r="R8">
+        <v>0.05</v>
+      </c>
+      <c r="S8">
+        <v>0.05</v>
+      </c>
+      <c r="T8">
+        <v>0.05</v>
+      </c>
+      <c r="U8">
+        <v>0.05</v>
+      </c>
+      <c r="V8">
+        <v>0.05</v>
+      </c>
+      <c r="W8">
+        <v>0.05</v>
+      </c>
+      <c r="X8">
+        <v>0.05</v>
+      </c>
+      <c r="Y8">
+        <v>0.05</v>
+      </c>
+      <c r="Z8">
+        <v>0.05</v>
+      </c>
+      <c r="AA8">
+        <v>0.05</v>
+      </c>
+      <c r="AB8">
+        <v>0.05</v>
+      </c>
+      <c r="AC8">
+        <v>0.05</v>
+      </c>
+      <c r="AD8">
+        <v>0.05</v>
+      </c>
+      <c r="AE8">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+      <c r="AE9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <v>0</v>
+      </c>
+      <c r="AE12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13">
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <v>0</v>
+      </c>
+      <c r="AE13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14">
+        <v>0</v>
+      </c>
+      <c r="AD14">
+        <v>0</v>
+      </c>
+      <c r="AE14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <v>0</v>
+      </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <v>0</v>
+      </c>
+      <c r="AE16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <v>0</v>
+      </c>
+      <c r="AB17">
+        <v>0</v>
+      </c>
+      <c r="AC17">
+        <v>0</v>
+      </c>
+      <c r="AD17">
+        <v>0</v>
+      </c>
+      <c r="AE17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>0</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AB18">
+        <v>0</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>0</v>
+      </c>
+      <c r="AE18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>0</v>
+      </c>
+      <c r="AA19">
+        <v>0</v>
+      </c>
+      <c r="AB19">
+        <v>0</v>
+      </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+      <c r="AE19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Y20">
+        <v>0</v>
+      </c>
+      <c r="Z20">
+        <v>0</v>
+      </c>
+      <c r="AA20">
+        <v>0</v>
+      </c>
+      <c r="AB20">
+        <v>0</v>
+      </c>
+      <c r="AC20">
+        <v>0</v>
+      </c>
+      <c r="AD20">
+        <v>0</v>
+      </c>
+      <c r="AE20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21">
+        <v>0</v>
+      </c>
+      <c r="AA21">
+        <v>0</v>
+      </c>
+      <c r="AB21">
+        <v>0</v>
+      </c>
+      <c r="AC21">
+        <v>0</v>
+      </c>
+      <c r="AD21">
+        <v>0</v>
+      </c>
+      <c r="AE21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+      <c r="X22">
+        <v>0</v>
+      </c>
+      <c r="Y22">
+        <v>0</v>
+      </c>
+      <c r="Z22">
+        <v>0</v>
+      </c>
+      <c r="AA22">
+        <v>0</v>
+      </c>
+      <c r="AB22">
+        <v>0</v>
+      </c>
+      <c r="AC22">
+        <v>0</v>
+      </c>
+      <c r="AD22">
+        <v>0</v>
+      </c>
+      <c r="AE22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>0</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <v>0</v>
+      </c>
+      <c r="Y23">
+        <v>0</v>
+      </c>
+      <c r="Z23">
+        <v>0</v>
+      </c>
+      <c r="AA23">
+        <v>0</v>
+      </c>
+      <c r="AB23">
+        <v>0</v>
+      </c>
+      <c r="AC23">
+        <v>0</v>
+      </c>
+      <c r="AD23">
+        <v>0</v>
+      </c>
+      <c r="AE23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <v>0</v>
+      </c>
+      <c r="X24">
+        <v>0</v>
+      </c>
+      <c r="Y24">
+        <v>0</v>
+      </c>
+      <c r="Z24">
+        <v>0</v>
+      </c>
+      <c r="AA24">
+        <v>0</v>
+      </c>
+      <c r="AB24">
+        <v>0</v>
+      </c>
+      <c r="AC24">
+        <v>0</v>
+      </c>
+      <c r="AD24">
+        <v>0</v>
+      </c>
+      <c r="AE24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>0</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>0</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>0</v>
+      </c>
+      <c r="X25">
+        <v>0</v>
+      </c>
+      <c r="Y25">
+        <v>0</v>
+      </c>
+      <c r="Z25">
+        <v>0</v>
+      </c>
+      <c r="AA25">
+        <v>0</v>
+      </c>
+      <c r="AB25">
+        <v>0</v>
+      </c>
+      <c r="AC25">
+        <v>0</v>
+      </c>
+      <c r="AD25">
+        <v>0</v>
+      </c>
+      <c r="AE25">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change CSC curve shape parameter after updated electricity calibration runs
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26E14AA-AE72-4B0A-9CCA-4B50EF8636AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72F467A-16B4-4CAB-922F-945672D8DA4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -383,40 +383,40 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.30946470671195E-3</c:v>
+                  <c:v>2.9962456884000122E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.8179777849356926E-2</c:v>
+                  <c:v>2.3473206571269223E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.8751548707702217E-2</c:v>
+                  <c:v>7.4900141956719624E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.12821646039704676</c:v>
+                  <c:v>0.15966347062760222</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.21968768431511465</c:v>
+                  <c:v>0.26412705355846133</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.31606027941427894</c:v>
+                  <c:v>0.36349842917090391</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.39782928042887927</c:v>
+                  <c:v>0.43637539384532031</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.45327694490118725</c:v>
+                  <c:v>0.47696021108917119</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.482890940844167</c:v>
+                  <c:v>0.49374775762398693</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.49512081367739108</c:v>
+                  <c:v>0.4987735918534465</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.49894602254348458</c:v>
+                  <c:v>0.49983226868604874</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.49983226868604874</c:v>
+                  <c:v>0.49998457194554841</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -999,304 +999,304 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>1.8518175587234342E-5</c:v>
+                  <c:v>2.4041495616800024E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.4812620244186725E-4</c:v>
+                  <c:v>1.9229960041033944E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.9975008331248905E-4</c:v>
+                  <c:v>6.4871479274314359E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1837816304625659E-3</c:v>
+                  <c:v>1.5363275637635954E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.30946470671195E-3</c:v>
+                  <c:v>2.9962456884000122E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.9840425814696712E-3</c:v>
+                  <c:v>5.1662128652874006E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.3116761366486807E-3</c:v>
+                  <c:v>8.1787999479949192E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.3921485539219529E-3</c:v>
+                  <c:v>1.2159252732797055E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.3319379237831663E-2</c:v>
+                  <c:v>1.7223045498576117E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.8179777849356926E-2</c:v>
+                  <c:v>2.3473206571269223E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.4050478125526686E-2</c:v>
+                  <c:v>3.0997500234635322E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.0997500234635322E-2</c:v>
+                  <c:v>3.9865567220398856E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.9073899265828771E-2</c:v>
+                  <c:v>5.0126142457089129E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.8317965498893056E-2</c:v>
+                  <c:v>6.1804482243504932E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.8751548707702439E-2</c:v>
+                  <c:v>7.4900141956719901E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.0378583251537175E-2</c:v>
+                  <c:v>8.9385248244384874E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.3183892444397944E-2</c:v>
+                  <c:v>0.10520340498301078</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9.7132349063260404E-2</c:v>
+                  <c:v>0.12226935901674252</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.11216846337375413</c:v>
+                  <c:v>0.14046952920696243</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.12821646039704715</c:v>
+                  <c:v>0.15966347062760267</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.145180894219896</c:v>
+                  <c:v>0.17968630558391707</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.1629478291374219</c:v>
+                  <c:v>0.20035210607723114</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.18138659579656291</c:v>
+                  <c:v>0.22145816076288932</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.2003521060772312</c:v>
+                  <c:v>0.24279000646233656</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.21968768431511504</c:v>
+                  <c:v>0.26412705355846178</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.23922834600936815</c:v>
+                  <c:v>0.2852485900850692</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.25880442994243746</c:v>
+                  <c:v>0.30593991493344896</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.27824546734033195</c:v>
+                  <c:v>0.32599832983443455</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.29738415397127527</c:v>
+                  <c:v>0.34523871531305683</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.31606027941427933</c:v>
+                  <c:v>0.36349842917090425</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.33412446332724866</c:v>
+                  <c:v>0.38064129731528962</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.35144155218419226</c:v>
+                  <c:v>0.39656051444532991</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.36789354188345735</c:v>
+                  <c:v>0.41118033320243297</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.38338191151156198</c:v>
+                  <c:v>0.42445649053243717</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.39782928042887961</c:v>
+                  <c:v>0.43637539384532065</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.41118033320243297</c:v>
+                  <c:v>0.44695216127096254</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.42340199275076174</c:v>
+                  <c:v>0.4562276741678255</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.43448285906130646</c:v>
+                  <c:v>0.46426485100526288</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.44443196652468936</c:v>
+                  <c:v>0.47114438598562269</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.45327694490118764</c:v>
+                  <c:v>0.47696021108917142</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.46106169506614503</c:v>
+                  <c:v>0.48181493622808969</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.46784370930984587</c:v>
+                  <c:v>0.48581550032261223</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.47369117603949534</c:v>
+                  <c:v>0.48906922940547914</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.47868000988903292</c:v>
+                  <c:v>0.49168045056913828</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.48289094084416712</c:v>
+                  <c:v>0.49374775762398698</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.48640678105535029</c:v>
+                  <c:v>0.49536197077070659</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.48930996710586872</c:v>
+                  <c:v>0.49660478299595257</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.49168045056913828</c:v>
+                  <c:v>0.49754804397175195</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.49359398285198086</c:v>
+                  <c:v>0.49825360046900036</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.49512081367739114</c:v>
+                  <c:v>0.4987735918534465</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.49632479799529</c:v>
+                  <c:v>0.49915109001197139</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.49726288514031575</c:v>
+                  <c:v>0.49942097387364487</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.49798494773010005</c:v>
+                  <c:v>0.49961093758286002</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.49853389665074921</c:v>
+                  <c:v>0.49974254596131784</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.49894602254348458</c:v>
+                  <c:v>0.49983226868604874</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.49925150308587324</c:v>
+                  <c:v>0.49989244334063315</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.49947501831440388</c:v>
+                  <c:v>0.49993213530833991</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.49963642230809158</c:v>
+                  <c:v>0.49995787803925179</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.49975142770027831</c:v>
+                  <c:v>0.49997428976150043</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.49983226868604874</c:v>
+                  <c:v>0.49998457194554841</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.49988831753913909</c:v>
+                  <c:v>0.49999090089962539</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.49992663841639778</c:v>
+                  <c:v>0.4999947271831322</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.49995246989130931</c:v>
+                  <c:v>0.49999699863673219</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.49996963391561561</c:v>
+                  <c:v>0.49999832235222452</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.49998087364778804</c:v>
+                  <c:v>0.49999907941465183</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.49998812585464286</c:v>
+                  <c:v>0.49999950422675427</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.49999273554696116</c:v>
+                  <c:v>0.49999973804145276</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.49999562137938031</c:v>
+                  <c:v>0.49999986423518789</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.49999740038494733</c:v>
+                  <c:v>0.49999993100434548</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.49999848007700298</c:v>
+                  <c:v>0.49999996562752336</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.49999912505966676</c:v>
+                  <c:v>0.49999998321856143</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.49999950422675427</c:v>
+                  <c:v>0.49999999197303208</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.49999972353572192</c:v>
+                  <c:v>0.49999999623943975</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.4999998483125187</c:v>
+                  <c:v>0.49999999827492908</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.49999991813114347</c:v>
+                  <c:v>0.49999999922537869</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.49999995654402807</c:v>
+                  <c:v>0.49999999965961162</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.49999997731987417</c:v>
+                  <c:v>0.49999999985366861</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.49999998836382642</c:v>
+                  <c:v>0.49999999993847488</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.49999999413258034</c:v>
+                  <c:v>0.49999999997470734</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.49999999709290094</c:v>
+                  <c:v>0.49999999998983663</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.49999999858501537</c:v>
+                  <c:v>0.49999999999600925</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.49999999932356465</c:v>
+                  <c:v>0.49999999999846917</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.49999999968246833</c:v>
+                  <c:v>0.49999999999942651</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.49999999985366861</c:v>
+                  <c:v>0.49999999999979022</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.49999999993381172</c:v>
+                  <c:v>0.49999999999992512</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.49999999997062206</c:v>
+                  <c:v>0.49999999999997391</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.49999999998720729</c:v>
+                  <c:v>0.49999999999999112</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.49999999999453604</c:v>
+                  <c:v>0.49999999999999706</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.49999999999771144</c:v>
+                  <c:v>0.49999999999999906</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.49999999999906025</c:v>
+                  <c:v>0.49999999999999972</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.49999999999962175</c:v>
+                  <c:v>0.49999999999999989</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.49999999999985079</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.49999999999994232</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.49999999999997818</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.4999999999999919</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.49999999999999706</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.49999999999999895</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.49999999999999961</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.49999999999999989</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.49999999999999994</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="100">
                   <c:v>0.5</c:v>
@@ -1633,40 +1633,40 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.30946470671195E-3</c:v>
+                  <c:v>2.9962456884000122E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.8179777849356926E-2</c:v>
+                  <c:v>2.3473206571269223E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.8751548707702217E-2</c:v>
+                  <c:v>7.4900141956719624E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.12821646039704676</c:v>
+                  <c:v>0.15966347062760222</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.21968768431511465</c:v>
+                  <c:v>0.26412705355846133</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.31606027941427894</c:v>
+                  <c:v>0.36349842917090391</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.39782928042887927</c:v>
+                  <c:v>0.43637539384532031</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.45327694490118725</c:v>
+                  <c:v>0.47696021108917119</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.482890940844167</c:v>
+                  <c:v>0.49374775762398693</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.49512081367739108</c:v>
+                  <c:v>0.4987735918534465</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.49894602254348458</c:v>
+                  <c:v>0.49983226868604874</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.49983226868604874</c:v>
+                  <c:v>0.49998457194554841</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4013,7 +4013,7 @@
         <v>37</v>
       </c>
       <c r="B13">
-        <v>0.3</v>
+        <v>0.27500000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -4044,7 +4044,7 @@
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21">
         <f t="shared" ref="B21:B84" si="0">(1-EXP(-((C21-($B$15-0.5))/$B$13)^$B$14))*$B$12</f>
-        <v>1.8518175587234342E-5</v>
+        <v>2.4041495616800024E-5</v>
       </c>
       <c r="C21">
         <f>C20+0.01</f>
@@ -4054,7 +4054,7 @@
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>1.4812620244186725E-4</v>
+        <v>1.9229960041033944E-4</v>
       </c>
       <c r="C22">
         <f t="shared" ref="C22:C85" si="1">C21+0.01</f>
@@ -4064,7 +4064,7 @@
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>4.9975008331248905E-4</v>
+        <v>6.4871479274314359E-4</v>
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
@@ -4074,7 +4074,7 @@
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>1.1837816304625659E-3</v>
+        <v>1.5363275637635954E-3</v>
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
@@ -4084,7 +4084,7 @@
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>2.30946470671195E-3</v>
+        <v>2.9962456884000122E-3</v>
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
@@ -4094,7 +4094,7 @@
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>3.9840425814696712E-3</v>
+        <v>5.1662128652874006E-3</v>
       </c>
       <c r="C26">
         <f t="shared" si="1"/>
@@ -4104,7 +4104,7 @@
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>6.3116761366486807E-3</v>
+        <v>8.1787999479949192E-3</v>
       </c>
       <c r="C27">
         <f t="shared" si="1"/>
@@ -4114,7 +4114,7 @@
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>9.3921485539219529E-3</v>
+        <v>1.2159252732797055E-2</v>
       </c>
       <c r="C28">
         <f t="shared" si="1"/>
@@ -4124,7 +4124,7 @@
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>1.3319379237831663E-2</v>
+        <v>1.7223045498576117E-2</v>
       </c>
       <c r="C29">
         <f t="shared" si="1"/>
@@ -4134,7 +4134,7 @@
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>1.8179777849356926E-2</v>
+        <v>2.3473206571269223E-2</v>
       </c>
       <c r="C30">
         <f t="shared" si="1"/>
@@ -4144,7 +4144,7 @@
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>2.4050478125526686E-2</v>
+        <v>3.0997500234635322E-2</v>
       </c>
       <c r="C31">
         <f t="shared" si="1"/>
@@ -4154,7 +4154,7 @@
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>3.0997500234635322E-2</v>
+        <v>3.9865567220398856E-2</v>
       </c>
       <c r="C32">
         <f t="shared" si="1"/>
@@ -4164,7 +4164,7 @@
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33">
         <f t="shared" si="0"/>
-        <v>3.9073899265828771E-2</v>
+        <v>5.0126142457089129E-2</v>
       </c>
       <c r="C33">
         <f t="shared" si="1"/>
@@ -4174,7 +4174,7 @@
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34">
         <f t="shared" si="0"/>
-        <v>4.8317965498893056E-2</v>
+        <v>6.1804482243504932E-2</v>
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
@@ -4184,7 +4184,7 @@
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35">
         <f t="shared" si="0"/>
-        <v>5.8751548707702439E-2</v>
+        <v>7.4900141956719901E-2</v>
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
@@ -4194,7 +4194,7 @@
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36">
         <f t="shared" si="0"/>
-        <v>7.0378583251537175E-2</v>
+        <v>8.9385248244384874E-2</v>
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
@@ -4204,7 +4204,7 @@
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37">
         <f t="shared" si="0"/>
-        <v>8.3183892444397944E-2</v>
+        <v>0.10520340498301078</v>
       </c>
       <c r="C37">
         <f t="shared" si="1"/>
@@ -4214,7 +4214,7 @@
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38">
         <f t="shared" si="0"/>
-        <v>9.7132349063260404E-2</v>
+        <v>0.12226935901674252</v>
       </c>
       <c r="C38">
         <f t="shared" si="1"/>
@@ -4224,7 +4224,7 @@
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39">
         <f t="shared" si="0"/>
-        <v>0.11216846337375413</v>
+        <v>0.14046952920696243</v>
       </c>
       <c r="C39">
         <f t="shared" si="1"/>
@@ -4234,7 +4234,7 @@
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40">
         <f t="shared" si="0"/>
-        <v>0.12821646039704715</v>
+        <v>0.15966347062760267</v>
       </c>
       <c r="C40">
         <f t="shared" si="1"/>
@@ -4244,7 +4244,7 @@
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41">
         <f t="shared" si="0"/>
-        <v>0.145180894219896</v>
+        <v>0.17968630558391707</v>
       </c>
       <c r="C41">
         <f t="shared" si="1"/>
@@ -4254,7 +4254,7 @@
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42">
         <f t="shared" si="0"/>
-        <v>0.1629478291374219</v>
+        <v>0.20035210607723114</v>
       </c>
       <c r="C42">
         <f t="shared" si="1"/>
@@ -4264,7 +4264,7 @@
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43">
         <f t="shared" si="0"/>
-        <v>0.18138659579656291</v>
+        <v>0.22145816076288932</v>
       </c>
       <c r="C43">
         <f t="shared" si="1"/>
@@ -4274,7 +4274,7 @@
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44">
         <f t="shared" si="0"/>
-        <v>0.2003521060772312</v>
+        <v>0.24279000646233656</v>
       </c>
       <c r="C44">
         <f t="shared" si="1"/>
@@ -4284,7 +4284,7 @@
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45">
         <f t="shared" si="0"/>
-        <v>0.21968768431511504</v>
+        <v>0.26412705355846178</v>
       </c>
       <c r="C45">
         <f t="shared" si="1"/>
@@ -4294,7 +4294,7 @@
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46">
         <f t="shared" si="0"/>
-        <v>0.23922834600936815</v>
+        <v>0.2852485900850692</v>
       </c>
       <c r="C46">
         <f t="shared" si="1"/>
@@ -4304,7 +4304,7 @@
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47">
         <f t="shared" si="0"/>
-        <v>0.25880442994243746</v>
+        <v>0.30593991493344896</v>
       </c>
       <c r="C47">
         <f t="shared" si="1"/>
@@ -4314,7 +4314,7 @@
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48">
         <f t="shared" si="0"/>
-        <v>0.27824546734033195</v>
+        <v>0.32599832983443455</v>
       </c>
       <c r="C48">
         <f t="shared" si="1"/>
@@ -4324,7 +4324,7 @@
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49">
         <f t="shared" si="0"/>
-        <v>0.29738415397127527</v>
+        <v>0.34523871531305683</v>
       </c>
       <c r="C49">
         <f t="shared" si="1"/>
@@ -4334,7 +4334,7 @@
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50">
         <f t="shared" si="0"/>
-        <v>0.31606027941427933</v>
+        <v>0.36349842917090425</v>
       </c>
       <c r="C50">
         <f t="shared" si="1"/>
@@ -4344,7 +4344,7 @@
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51">
         <f t="shared" si="0"/>
-        <v>0.33412446332724866</v>
+        <v>0.38064129731528962</v>
       </c>
       <c r="C51">
         <f t="shared" si="1"/>
@@ -4354,7 +4354,7 @@
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52">
         <f t="shared" si="0"/>
-        <v>0.35144155218419226</v>
+        <v>0.39656051444532991</v>
       </c>
       <c r="C52">
         <f t="shared" si="1"/>
@@ -4364,7 +4364,7 @@
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53">
         <f t="shared" si="0"/>
-        <v>0.36789354188345735</v>
+        <v>0.41118033320243297</v>
       </c>
       <c r="C53">
         <f t="shared" si="1"/>
@@ -4374,7 +4374,7 @@
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54">
         <f t="shared" si="0"/>
-        <v>0.38338191151156198</v>
+        <v>0.42445649053243717</v>
       </c>
       <c r="C54">
         <f t="shared" si="1"/>
@@ -4384,7 +4384,7 @@
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55">
         <f t="shared" si="0"/>
-        <v>0.39782928042887961</v>
+        <v>0.43637539384532065</v>
       </c>
       <c r="C55">
         <f t="shared" si="1"/>
@@ -4394,7 +4394,7 @@
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56">
         <f t="shared" si="0"/>
-        <v>0.41118033320243297</v>
+        <v>0.44695216127096254</v>
       </c>
       <c r="C56">
         <f t="shared" si="1"/>
@@ -4404,7 +4404,7 @@
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57">
         <f t="shared" si="0"/>
-        <v>0.42340199275076174</v>
+        <v>0.4562276741678255</v>
       </c>
       <c r="C57">
         <f t="shared" si="1"/>
@@ -4414,7 +4414,7 @@
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58">
         <f t="shared" si="0"/>
-        <v>0.43448285906130646</v>
+        <v>0.46426485100526288</v>
       </c>
       <c r="C58">
         <f t="shared" si="1"/>
@@ -4424,7 +4424,7 @@
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59">
         <f t="shared" si="0"/>
-        <v>0.44443196652468936</v>
+        <v>0.47114438598562269</v>
       </c>
       <c r="C59">
         <f t="shared" si="1"/>
@@ -4434,7 +4434,7 @@
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60">
         <f t="shared" si="0"/>
-        <v>0.45327694490118764</v>
+        <v>0.47696021108917142</v>
       </c>
       <c r="C60">
         <f t="shared" si="1"/>
@@ -4444,7 +4444,7 @@
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61">
         <f t="shared" si="0"/>
-        <v>0.46106169506614503</v>
+        <v>0.48181493622808969</v>
       </c>
       <c r="C61">
         <f t="shared" si="1"/>
@@ -4454,7 +4454,7 @@
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62">
         <f t="shared" si="0"/>
-        <v>0.46784370930984587</v>
+        <v>0.48581550032261223</v>
       </c>
       <c r="C62">
         <f t="shared" si="1"/>
@@ -4464,7 +4464,7 @@
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63">
         <f t="shared" si="0"/>
-        <v>0.47369117603949534</v>
+        <v>0.48906922940547914</v>
       </c>
       <c r="C63">
         <f t="shared" si="1"/>
@@ -4474,7 +4474,7 @@
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64">
         <f t="shared" si="0"/>
-        <v>0.47868000988903292</v>
+        <v>0.49168045056913828</v>
       </c>
       <c r="C64">
         <f t="shared" si="1"/>
@@ -4484,7 +4484,7 @@
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65">
         <f t="shared" si="0"/>
-        <v>0.48289094084416712</v>
+        <v>0.49374775762398698</v>
       </c>
       <c r="C65">
         <f t="shared" si="1"/>
@@ -4494,7 +4494,7 @@
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66">
         <f t="shared" si="0"/>
-        <v>0.48640678105535029</v>
+        <v>0.49536197077070659</v>
       </c>
       <c r="C66">
         <f t="shared" si="1"/>
@@ -4504,7 +4504,7 @@
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67">
         <f t="shared" si="0"/>
-        <v>0.48930996710586872</v>
+        <v>0.49660478299595257</v>
       </c>
       <c r="C67">
         <f t="shared" si="1"/>
@@ -4514,7 +4514,7 @@
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68">
         <f t="shared" si="0"/>
-        <v>0.49168045056913828</v>
+        <v>0.49754804397175195</v>
       </c>
       <c r="C68">
         <f t="shared" si="1"/>
@@ -4524,7 +4524,7 @@
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69">
         <f t="shared" si="0"/>
-        <v>0.49359398285198086</v>
+        <v>0.49825360046900036</v>
       </c>
       <c r="C69">
         <f t="shared" si="1"/>
@@ -4534,7 +4534,7 @@
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70">
         <f t="shared" si="0"/>
-        <v>0.49512081367739114</v>
+        <v>0.4987735918534465</v>
       </c>
       <c r="C70">
         <f t="shared" si="1"/>
@@ -4544,7 +4544,7 @@
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71">
         <f t="shared" si="0"/>
-        <v>0.49632479799529</v>
+        <v>0.49915109001197139</v>
       </c>
       <c r="C71">
         <f t="shared" si="1"/>
@@ -4554,7 +4554,7 @@
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72">
         <f t="shared" si="0"/>
-        <v>0.49726288514031575</v>
+        <v>0.49942097387364487</v>
       </c>
       <c r="C72">
         <f t="shared" si="1"/>
@@ -4564,7 +4564,7 @@
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73">
         <f t="shared" si="0"/>
-        <v>0.49798494773010005</v>
+        <v>0.49961093758286002</v>
       </c>
       <c r="C73">
         <f t="shared" si="1"/>
@@ -4574,7 +4574,7 @@
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74">
         <f t="shared" si="0"/>
-        <v>0.49853389665074921</v>
+        <v>0.49974254596131784</v>
       </c>
       <c r="C74">
         <f t="shared" si="1"/>
@@ -4584,7 +4584,7 @@
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75">
         <f t="shared" si="0"/>
-        <v>0.49894602254348458</v>
+        <v>0.49983226868604874</v>
       </c>
       <c r="C75">
         <f t="shared" si="1"/>
@@ -4594,7 +4594,7 @@
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76">
         <f t="shared" si="0"/>
-        <v>0.49925150308587324</v>
+        <v>0.49989244334063315</v>
       </c>
       <c r="C76">
         <f t="shared" si="1"/>
@@ -4604,7 +4604,7 @@
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77">
         <f t="shared" si="0"/>
-        <v>0.49947501831440388</v>
+        <v>0.49993213530833991</v>
       </c>
       <c r="C77">
         <f t="shared" si="1"/>
@@ -4614,7 +4614,7 @@
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78">
         <f t="shared" si="0"/>
-        <v>0.49963642230809158</v>
+        <v>0.49995787803925179</v>
       </c>
       <c r="C78">
         <f t="shared" si="1"/>
@@ -4624,7 +4624,7 @@
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79">
         <f t="shared" si="0"/>
-        <v>0.49975142770027831</v>
+        <v>0.49997428976150043</v>
       </c>
       <c r="C79">
         <f t="shared" si="1"/>
@@ -4634,7 +4634,7 @@
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80">
         <f t="shared" si="0"/>
-        <v>0.49983226868604874</v>
+        <v>0.49998457194554841</v>
       </c>
       <c r="C80">
         <f t="shared" si="1"/>
@@ -4644,7 +4644,7 @@
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81">
         <f t="shared" si="0"/>
-        <v>0.49988831753913909</v>
+        <v>0.49999090089962539</v>
       </c>
       <c r="C81">
         <f t="shared" si="1"/>
@@ -4654,7 +4654,7 @@
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82">
         <f t="shared" si="0"/>
-        <v>0.49992663841639778</v>
+        <v>0.4999947271831322</v>
       </c>
       <c r="C82">
         <f t="shared" si="1"/>
@@ -4664,7 +4664,7 @@
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83">
         <f t="shared" si="0"/>
-        <v>0.49995246989130931</v>
+        <v>0.49999699863673219</v>
       </c>
       <c r="C83">
         <f t="shared" si="1"/>
@@ -4674,7 +4674,7 @@
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84">
         <f t="shared" si="0"/>
-        <v>0.49996963391561561</v>
+        <v>0.49999832235222452</v>
       </c>
       <c r="C84">
         <f t="shared" si="1"/>
@@ -4684,7 +4684,7 @@
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85">
         <f t="shared" ref="B85:B121" si="2">(1-EXP(-((C85-($B$15-0.5))/$B$13)^$B$14))*$B$12</f>
-        <v>0.49998087364778804</v>
+        <v>0.49999907941465183</v>
       </c>
       <c r="C85">
         <f t="shared" si="1"/>
@@ -4694,7 +4694,7 @@
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86">
         <f t="shared" si="2"/>
-        <v>0.49998812585464286</v>
+        <v>0.49999950422675427</v>
       </c>
       <c r="C86">
         <f t="shared" ref="C86:C121" si="3">C85+0.01</f>
@@ -4704,7 +4704,7 @@
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87">
         <f t="shared" si="2"/>
-        <v>0.49999273554696116</v>
+        <v>0.49999973804145276</v>
       </c>
       <c r="C87">
         <f t="shared" si="3"/>
@@ -4714,7 +4714,7 @@
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88">
         <f t="shared" si="2"/>
-        <v>0.49999562137938031</v>
+        <v>0.49999986423518789</v>
       </c>
       <c r="C88">
         <f t="shared" si="3"/>
@@ -4724,7 +4724,7 @@
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89">
         <f t="shared" si="2"/>
-        <v>0.49999740038494733</v>
+        <v>0.49999993100434548</v>
       </c>
       <c r="C89">
         <f t="shared" si="3"/>
@@ -4734,7 +4734,7 @@
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90">
         <f t="shared" si="2"/>
-        <v>0.49999848007700298</v>
+        <v>0.49999996562752336</v>
       </c>
       <c r="C90">
         <f t="shared" si="3"/>
@@ -4744,7 +4744,7 @@
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91">
         <f t="shared" si="2"/>
-        <v>0.49999912505966676</v>
+        <v>0.49999998321856143</v>
       </c>
       <c r="C91">
         <f t="shared" si="3"/>
@@ -4754,7 +4754,7 @@
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92">
         <f t="shared" si="2"/>
-        <v>0.49999950422675427</v>
+        <v>0.49999999197303208</v>
       </c>
       <c r="C92">
         <f t="shared" si="3"/>
@@ -4764,7 +4764,7 @@
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93">
         <f t="shared" si="2"/>
-        <v>0.49999972353572192</v>
+        <v>0.49999999623943975</v>
       </c>
       <c r="C93">
         <f t="shared" si="3"/>
@@ -4774,7 +4774,7 @@
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94">
         <f t="shared" si="2"/>
-        <v>0.4999998483125187</v>
+        <v>0.49999999827492908</v>
       </c>
       <c r="C94">
         <f t="shared" si="3"/>
@@ -4784,7 +4784,7 @@
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95">
         <f t="shared" si="2"/>
-        <v>0.49999991813114347</v>
+        <v>0.49999999922537869</v>
       </c>
       <c r="C95">
         <f t="shared" si="3"/>
@@ -4794,7 +4794,7 @@
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96">
         <f t="shared" si="2"/>
-        <v>0.49999995654402807</v>
+        <v>0.49999999965961162</v>
       </c>
       <c r="C96">
         <f t="shared" si="3"/>
@@ -4804,7 +4804,7 @@
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97">
         <f t="shared" si="2"/>
-        <v>0.49999997731987417</v>
+        <v>0.49999999985366861</v>
       </c>
       <c r="C97">
         <f t="shared" si="3"/>
@@ -4814,7 +4814,7 @@
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98">
         <f t="shared" si="2"/>
-        <v>0.49999998836382642</v>
+        <v>0.49999999993847488</v>
       </c>
       <c r="C98">
         <f t="shared" si="3"/>
@@ -4824,7 +4824,7 @@
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99">
         <f t="shared" si="2"/>
-        <v>0.49999999413258034</v>
+        <v>0.49999999997470734</v>
       </c>
       <c r="C99">
         <f t="shared" si="3"/>
@@ -4834,7 +4834,7 @@
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100">
         <f t="shared" si="2"/>
-        <v>0.49999999709290094</v>
+        <v>0.49999999998983663</v>
       </c>
       <c r="C100">
         <f t="shared" si="3"/>
@@ -4844,7 +4844,7 @@
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101">
         <f t="shared" si="2"/>
-        <v>0.49999999858501537</v>
+        <v>0.49999999999600925</v>
       </c>
       <c r="C101">
         <f t="shared" si="3"/>
@@ -4854,7 +4854,7 @@
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102">
         <f t="shared" si="2"/>
-        <v>0.49999999932356465</v>
+        <v>0.49999999999846917</v>
       </c>
       <c r="C102">
         <f t="shared" si="3"/>
@@ -4864,7 +4864,7 @@
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103">
         <f t="shared" si="2"/>
-        <v>0.49999999968246833</v>
+        <v>0.49999999999942651</v>
       </c>
       <c r="C103">
         <f t="shared" si="3"/>
@@ -4874,7 +4874,7 @@
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104">
         <f t="shared" si="2"/>
-        <v>0.49999999985366861</v>
+        <v>0.49999999999979022</v>
       </c>
       <c r="C104">
         <f t="shared" si="3"/>
@@ -4884,7 +4884,7 @@
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105">
         <f t="shared" si="2"/>
-        <v>0.49999999993381172</v>
+        <v>0.49999999999992512</v>
       </c>
       <c r="C105">
         <f t="shared" si="3"/>
@@ -4894,7 +4894,7 @@
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106">
         <f t="shared" si="2"/>
-        <v>0.49999999997062206</v>
+        <v>0.49999999999997391</v>
       </c>
       <c r="C106">
         <f t="shared" si="3"/>
@@ -4904,7 +4904,7 @@
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107">
         <f t="shared" si="2"/>
-        <v>0.49999999998720729</v>
+        <v>0.49999999999999112</v>
       </c>
       <c r="C107">
         <f t="shared" si="3"/>
@@ -4914,7 +4914,7 @@
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108">
         <f t="shared" si="2"/>
-        <v>0.49999999999453604</v>
+        <v>0.49999999999999706</v>
       </c>
       <c r="C108">
         <f t="shared" si="3"/>
@@ -4924,7 +4924,7 @@
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109">
         <f t="shared" si="2"/>
-        <v>0.49999999999771144</v>
+        <v>0.49999999999999906</v>
       </c>
       <c r="C109">
         <f t="shared" si="3"/>
@@ -4934,7 +4934,7 @@
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110">
         <f t="shared" si="2"/>
-        <v>0.49999999999906025</v>
+        <v>0.49999999999999972</v>
       </c>
       <c r="C110">
         <f t="shared" si="3"/>
@@ -4944,7 +4944,7 @@
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111">
         <f t="shared" si="2"/>
-        <v>0.49999999999962175</v>
+        <v>0.49999999999999989</v>
       </c>
       <c r="C111">
         <f t="shared" si="3"/>
@@ -4954,7 +4954,7 @@
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112">
         <f t="shared" si="2"/>
-        <v>0.49999999999985079</v>
+        <v>0.5</v>
       </c>
       <c r="C112">
         <f t="shared" si="3"/>
@@ -4964,7 +4964,7 @@
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113">
         <f t="shared" si="2"/>
-        <v>0.49999999999994232</v>
+        <v>0.5</v>
       </c>
       <c r="C113">
         <f t="shared" si="3"/>
@@ -4974,7 +4974,7 @@
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114">
         <f t="shared" si="2"/>
-        <v>0.49999999999997818</v>
+        <v>0.5</v>
       </c>
       <c r="C114">
         <f t="shared" si="3"/>
@@ -4984,7 +4984,7 @@
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115">
         <f t="shared" si="2"/>
-        <v>0.4999999999999919</v>
+        <v>0.5</v>
       </c>
       <c r="C115">
         <f t="shared" si="3"/>
@@ -4994,7 +4994,7 @@
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116">
         <f t="shared" si="2"/>
-        <v>0.49999999999999706</v>
+        <v>0.5</v>
       </c>
       <c r="C116">
         <f t="shared" si="3"/>
@@ -5004,7 +5004,7 @@
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117">
         <f t="shared" si="2"/>
-        <v>0.49999999999999895</v>
+        <v>0.5</v>
       </c>
       <c r="C117">
         <f t="shared" si="3"/>
@@ -5014,7 +5014,7 @@
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118">
         <f t="shared" si="2"/>
-        <v>0.49999999999999961</v>
+        <v>0.5</v>
       </c>
       <c r="C118">
         <f t="shared" si="3"/>
@@ -5024,7 +5024,7 @@
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119">
         <f t="shared" si="2"/>
-        <v>0.49999999999999989</v>
+        <v>0.5</v>
       </c>
       <c r="C119">
         <f t="shared" si="3"/>
@@ -5034,7 +5034,7 @@
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120">
         <f t="shared" si="2"/>
-        <v>0.49999999999999994</v>
+        <v>0.5</v>
       </c>
       <c r="C120">
         <f t="shared" si="3"/>
@@ -5083,51 +5083,51 @@
       </c>
       <c r="C1">
         <f>(1-EXP(-((C2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>2.30946470671195E-3</v>
+        <v>2.9962456884000122E-3</v>
       </c>
       <c r="D1">
         <f>(1-EXP(-((D2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>1.8179777849356926E-2</v>
+        <v>2.3473206571269223E-2</v>
       </c>
       <c r="E1">
         <f>(1-EXP(-((E2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>5.8751548707702217E-2</v>
+        <v>7.4900141956719624E-2</v>
       </c>
       <c r="F1">
         <f>(1-EXP(-((F2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.12821646039704676</v>
+        <v>0.15966347062760222</v>
       </c>
       <c r="G1">
         <f>(1-EXP(-((G2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.21968768431511465</v>
+        <v>0.26412705355846133</v>
       </c>
       <c r="H1">
         <f>(1-EXP(-((H2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.31606027941427894</v>
+        <v>0.36349842917090391</v>
       </c>
       <c r="I1">
         <f>(1-EXP(-((I2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.39782928042887927</v>
+        <v>0.43637539384532031</v>
       </c>
       <c r="J1">
         <f>(1-EXP(-((J2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.45327694490118725</v>
+        <v>0.47696021108917119</v>
       </c>
       <c r="K1">
         <f>(1-EXP(-((K2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.482890940844167</v>
+        <v>0.49374775762398693</v>
       </c>
       <c r="L1">
         <f>(1-EXP(-((L2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.49512081367739108</v>
+        <v>0.4987735918534465</v>
       </c>
       <c r="M1">
         <f>(1-EXP(-((M2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.49894602254348458</v>
+        <v>0.49983226868604874</v>
       </c>
       <c r="N1">
         <f>(1-EXP(-((N2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.49983226868604874</v>
+        <v>0.49998457194554841</v>
       </c>
       <c r="O1">
         <f>(1-EXP(-((O2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>

</xml_diff>

<commit_message>
Updates cost-effectiveness structure to use $/MWh profit for resrouces instead of a multiplier of revenues to costs. Updates capacity supply curve accordingly. Updates weighted average capacity fatcors for new wind, bumping them up.
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\CSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Models\US\Models\eps-us\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72F467A-16B4-4CAB-922F-945672D8DA4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A4A1CFFE-EAE2-4ED0-BAA6-8E17A86A7094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="42">
   <si>
     <t xml:space="preserve">Source: </t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Share of existing capacity</t>
-  </si>
-  <si>
-    <t>Cost multiplier</t>
   </si>
   <si>
     <t>Time (Year)</t>
@@ -161,6 +158,12 @@
   <si>
     <t>multiplier cutoff</t>
   </si>
+  <si>
+    <t>Max profitability cutoff</t>
+  </si>
+  <si>
+    <t>Incremental Revenue</t>
+  </si>
 </sst>
 </file>
 
@@ -238,398 +241,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Supply Curve Function</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'CSC-CSCCCMvSoECBtY'!$B$2:$N$2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.05</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.1000000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.1499999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.25</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.35</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.45</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.55</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'CSC-CSCCCMvSoECBtY'!$B$1:$N$1</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.9962456884000122E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.3473206571269223E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.4900141956719624E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.15966347062760222</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.26412705355846133</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.36349842917090391</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.43637539384532031</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.47696021108917119</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.49374775762398693</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.4987735918534465</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.49983226868604874</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.49998457194554841</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-908C-4D72-A67B-057BE1973861}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="589529087"/>
-        <c:axId val="589529567"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="589529087"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="589529567"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="589529567"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="589529087"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -687,307 +298,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>1.01</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.02</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.03</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.04</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.05</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.06</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.07</c:v>
+                  <c:v>1.75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.08</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0900000000000001</c:v>
+                  <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.1000000000000001</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1100000000000001</c:v>
+                  <c:v>2.75</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.1200000000000001</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.1300000000000001</c:v>
+                  <c:v>3.25</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.1400000000000001</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.1500000000000001</c:v>
+                  <c:v>3.75</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.1600000000000001</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.1700000000000002</c:v>
+                  <c:v>4.25</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.1800000000000002</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.1900000000000002</c:v>
+                  <c:v>4.75</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.2000000000000002</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.2100000000000002</c:v>
+                  <c:v>5.25</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.2200000000000002</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.2300000000000002</c:v>
+                  <c:v>5.75</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.2400000000000002</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.2500000000000002</c:v>
+                  <c:v>6.25</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.2600000000000002</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.2700000000000002</c:v>
+                  <c:v>6.75</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.2800000000000002</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.2900000000000003</c:v>
+                  <c:v>7.25</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.3000000000000003</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.3100000000000003</c:v>
+                  <c:v>7.75</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.3200000000000003</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.3300000000000003</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.3400000000000003</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.3500000000000003</c:v>
+                  <c:v>8.75</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.3600000000000003</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.3700000000000003</c:v>
+                  <c:v>9.25</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.3800000000000003</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1.3900000000000003</c:v>
+                  <c:v>9.75</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1.4000000000000004</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1.4100000000000004</c:v>
+                  <c:v>10.25</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.4200000000000004</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1.4300000000000004</c:v>
+                  <c:v>10.75</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1.4400000000000004</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.4500000000000004</c:v>
+                  <c:v>11.25</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.4600000000000004</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.4700000000000004</c:v>
+                  <c:v>11.75</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.4800000000000004</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.4900000000000004</c:v>
+                  <c:v>12.25</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1.5000000000000004</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1.5100000000000005</c:v>
+                  <c:v>12.75</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1.5200000000000005</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1.5300000000000005</c:v>
+                  <c:v>13.25</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1.5400000000000005</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1.5500000000000005</c:v>
+                  <c:v>13.75</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1.5600000000000005</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1.5700000000000005</c:v>
+                  <c:v>14.25</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1.5800000000000005</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1.5900000000000005</c:v>
+                  <c:v>14.75</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1.6000000000000005</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1.6100000000000005</c:v>
+                  <c:v>15.25</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1.6200000000000006</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>1.6300000000000006</c:v>
+                  <c:v>15.75</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1.6400000000000006</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1.6500000000000006</c:v>
+                  <c:v>16.25</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1.6600000000000006</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1.6700000000000006</c:v>
+                  <c:v>16.75</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1.6800000000000006</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>1.6900000000000006</c:v>
+                  <c:v>17.25</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>1.7000000000000006</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>1.7100000000000006</c:v>
+                  <c:v>17.75</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1.7200000000000006</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>1.7300000000000006</c:v>
+                  <c:v>18.25</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>1.7400000000000007</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>1.7500000000000007</c:v>
+                  <c:v>18.75</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>1.7600000000000007</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>1.7700000000000007</c:v>
+                  <c:v>19.25</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>1.7800000000000007</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>1.7900000000000007</c:v>
+                  <c:v>19.75</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>1.8000000000000007</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>1.8100000000000007</c:v>
+                  <c:v>20.25</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1.8200000000000007</c:v>
+                  <c:v>20.5</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>1.8300000000000007</c:v>
+                  <c:v>20.75</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>1.8400000000000007</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>1.8500000000000008</c:v>
+                  <c:v>21.25</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>1.8600000000000008</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>1.8700000000000008</c:v>
+                  <c:v>21.75</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>1.8800000000000008</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>1.8900000000000008</c:v>
+                  <c:v>22.25</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>1.9000000000000008</c:v>
+                  <c:v>22.5</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>1.9100000000000008</c:v>
+                  <c:v>22.75</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>1.9200000000000008</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>1.9300000000000008</c:v>
+                  <c:v>23.25</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>1.9400000000000008</c:v>
+                  <c:v>23.5</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>1.9500000000000008</c:v>
+                  <c:v>23.75</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>1.9600000000000009</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>1.9700000000000009</c:v>
+                  <c:v>24.25</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>1.9800000000000009</c:v>
+                  <c:v>24.5</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>1.9900000000000009</c:v>
+                  <c:v>24.75</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>2.0000000000000009</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>2.0100000000000007</c:v>
+                  <c:v>25.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -999,307 +610,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>2.4041495616800024E-5</c:v>
+                  <c:v>7.5016342843348124E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9229960041033944E-4</c:v>
+                  <c:v>6.0008572506203833E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.4871479274314359E-4</c:v>
+                  <c:v>2.024877004541181E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5363275637635954E-3</c:v>
+                  <c:v>4.7978059651185284E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.9962456884000122E-3</c:v>
+                  <c:v>9.3645930124346957E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.1662128652874006E-3</c:v>
+                  <c:v>1.6166252946983649E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.1787999479949192E-3</c:v>
+                  <c:v>2.5636530091484311E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.2159252732797055E-2</c:v>
+                  <c:v>3.8198800190648858E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.7223045498576117E-2</c:v>
+                  <c:v>5.4262470481070413E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.3473206571269223E-2</c:v>
+                  <c:v>7.4218920962914039E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.0997500234635322E-2</c:v>
+                  <c:v>9.843704293543025E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.9865567220398856E-2</c:v>
+                  <c:v>1.2725844494549809E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.0126142457089129E-2</c:v>
+                  <c:v>1.6099241101609572E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.1804482243504932E-2</c:v>
+                  <c:v>1.9991071085629669E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.4900141956719901E-2</c:v>
+                  <c:v>2.4424237610961935E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8.9385248244384874E-2</c:v>
+                  <c:v>2.9416856990439513E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.10520340498301078</c:v>
+                  <c:v>3.4981768830348287E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.12226935901674252</c:v>
+                  <c:v>4.1126084095391591E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.14046952920696243</c:v>
+                  <c:v>4.7850786355034675E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.15966347062760267</c:v>
+                  <c:v>5.5150401592329062E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.17968630558391707</c:v>
+                  <c:v>6.3012751599265338E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.20035210607723114</c:v>
+                  <c:v>7.1418805095598475E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.22145816076288932</c:v>
+                  <c:v>8.0342639254068787E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.24279000646233656</c:v>
+                  <c:v>8.9751522277932802E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.26412705355846178</c:v>
+                  <c:v>9.9606125065372003E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.2852485900850692</c:v>
+                  <c:v>0.10986086684613371</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.30593991493344896</c:v>
+                  <c:v>0.12046439605497444</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.32599832983443455</c:v>
+                  <c:v>0.13136020371072249</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.34523871531305683</c:v>
+                  <c:v>0.14248736232479842</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.36349842917090425</c:v>
+                  <c:v>0.15378137902058026</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.38064129731528962</c:v>
+                  <c:v>0.16517514727773613</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.39656051444532991</c:v>
+                  <c:v>0.17659997771015737</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.41118033320243297</c:v>
+                  <c:v>0.18798668473414495</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.42445649053243717</c:v>
+                  <c:v>0.19926670307190242</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.43637539384532065</c:v>
+                  <c:v>0.21037320593524328</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.44695216127096254</c:v>
+                  <c:v>0.22124219558999517</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.4562276741678255</c:v>
+                  <c:v>0.23181353691984963</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.46426485100526288</c:v>
+                  <c:v>0.24203190564996585</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.47114438598562269</c:v>
+                  <c:v>0.25184762506281139</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.47696021108917142</c:v>
+                  <c:v>0.26121736829143588</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.48181493622808969</c:v>
+                  <c:v>0.27010470750054377</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.48581550032261223</c:v>
+                  <c:v>0.27848049630021543</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.48906922940547914</c:v>
+                  <c:v>0.28632307736964208</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.49168045056913828</c:v>
+                  <c:v>0.29361831324963961</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.49374775762398698</c:v>
+                  <c:v>0.30035944431943007</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.49536197077070659</c:v>
+                  <c:v>0.30654678382278544</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.49660478299595257</c:v>
+                  <c:v>0.31218726517655226</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.49754804397175195</c:v>
+                  <c:v>0.31729386143083116</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.49825360046900036</c:v>
+                  <c:v>0.32188490044468793</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.4987735918534465</c:v>
+                  <c:v>0.32598330193721398</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.49915109001197139</c:v>
+                  <c:v>0.32961576397642717</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.49942097387364487</c:v>
+                  <c:v>0.33281192665098364</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.49961093758286002</c:v>
+                  <c:v>0.33560353967312706</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.49974254596131784</c:v>
+                  <c:v>0.33802365859091688</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.49983226868604874</c:v>
+                  <c:v>0.34010589130406521</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.49989244334063315</c:v>
+                  <c:v>0.34188371288438546</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.49993213530833991</c:v>
+                  <c:v>0.34338986253095471</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.49995787803925179</c:v>
+                  <c:v>0.34465583208577671</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.49997428976150043</c:v>
+                  <c:v>0.34571145113798446</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.49998457194554841</c:v>
+                  <c:v>0.34658456957417372</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.49999090089962539</c:v>
+                  <c:v>0.34730083467801665</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.4999947271831322</c:v>
+                  <c:v>0.34788355669100007</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.49999699863673219</c:v>
+                  <c:v>0.34835365421771686</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.49999832235222452</c:v>
+                  <c:v>0.34872966904405506</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.49999907941465183</c:v>
+                  <c:v>0.34902783883791444</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.49999950422675427</c:v>
+                  <c:v>0.3492622157804392</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.49999973804145276</c:v>
+                  <c:v>0.34944481935725885</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.49999986423518789</c:v>
+                  <c:v>0.3495858122245698</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.49999993100434548</c:v>
+                  <c:v>0.34969368913943127</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.49999996562752336</c:v>
+                  <c:v>0.34977547028721101</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.49999998321856143</c:v>
+                  <c:v>0.3498368918348444</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.49999999197303208</c:v>
+                  <c:v>0.34988258808023409</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.49999999623943975</c:v>
+                  <c:v>0.34991626106546403</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.49999999827492908</c:v>
+                  <c:v>0.34994083490357991</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.49999999922537869</c:v>
+                  <c:v>0.34995859328510975</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.49999999965961162</c:v>
+                  <c:v>0.34997129965097196</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.49999999985366861</c:v>
+                  <c:v>0.34998030033082916</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.49999999993847488</c:v>
+                  <c:v>0.34998661155345162</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.49999999997470734</c:v>
+                  <c:v>0.34999099165321684</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.49999999998983663</c:v>
+                  <c:v>0.34999400004761355</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.49999999999600925</c:v>
+                  <c:v>0.34999604467238488</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.49999999999846917</c:v>
+                  <c:v>0.34999741956325225</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.49999999999942651</c:v>
+                  <c:v>0.34999833419476295</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.49999999999979022</c:v>
+                  <c:v>0.34999893605390209</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.49999999999992512</c:v>
+                  <c:v>0.34999932776119835</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.49999999999997391</c:v>
+                  <c:v>0.34999957987335761</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.49999999999999112</c:v>
+                  <c:v>0.34999974032286191</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.49999999999999706</c:v>
+                  <c:v>0.34999984128126099</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.49999999999999906</c:v>
+                  <c:v>0.3499999040802943</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.49999999999999972</c:v>
+                  <c:v>0.3499999426918004</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.49999999999999989</c:v>
+                  <c:v>0.34999996615464019</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.5</c:v>
+                  <c:v>0.34999998024399626</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.5</c:v>
+                  <c:v>0.34999998860378051</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.5</c:v>
+                  <c:v>0.34999999350426342</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.5</c:v>
+                  <c:v>0.34999999634198026</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.5</c:v>
+                  <c:v>0.34999999796503062</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.5</c:v>
+                  <c:v>0.34999999888182948</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.5</c:v>
+                  <c:v>0.34999999939320681</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.5</c:v>
+                  <c:v>0.3499999996748378</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.5</c:v>
+                  <c:v>0.34999999982795971</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.5</c:v>
+                  <c:v>0.34999999991013819</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1498,6 +1109,541 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'CSC-CSCCCMvSoECBtY'!$B$2:$AP$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.75</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.75</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.75</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7.25</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7.75</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8.25</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8.75</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9.25</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9.75</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'CSC-CSCCCMvSoECBtY'!$B$1:$AP$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="41"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.5016342843348124E-6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0008572506203833E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.024877004541181E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.7978059651185284E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.3645930124346957E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6166252946983649E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5636530091484311E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.8198800190648858E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.4262470481070413E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.4218920962914039E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.843704293543025E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2725844494549809E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.6099241101609572E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.9991071085629669E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.4424237610961935E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.9416856990439513E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.4981768830348287E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.1126084095391591E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.7850786355034675E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.5150401592329062E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.3012751599265338E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7.1418805095598475E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.0342639254068787E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.9751522277932802E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.9606125065372003E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.10986086684613371</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.12046439605497444</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.13136020371072249</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.14248736232479842</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.15378137902058026</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.16517514727773613</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.17659997771015737</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.18798668473414495</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.19926670307190242</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.21037320593524328</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.22124219558999517</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.23181353691984963</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.24203190564996585</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.25184762506281139</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.26121736829143588</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5E3E-4506-B7FF-2865DFAAB582}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1627802751"/>
+        <c:axId val="1627803711"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1627802751"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1627803711"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1627803711"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1627802751"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -1577,96 +1723,264 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'CSC-CSCCCMvSoECBtY'!$B$2:$N$2</c:f>
+              <c:f>'CSC-CSCCCMvSoECBtY'!$B$2:$AP$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.05</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.1000000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.1499999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.35</c:v>
+                  <c:v>1.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.45</c:v>
+                  <c:v>2.25</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.5</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.55</c:v>
+                  <c:v>2.75</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.6</c:v>
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.75</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.75</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>6.25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6.75</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7.25</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7.75</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8.25</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8.75</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>9.25</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>9.75</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'CSC-CSCCCMvSoECBtY'!$B$1:$N$1</c:f>
+              <c:f>'CSC-CSCCCMvSoECBtY'!$B$1:$AP$1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="41"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.9962456884000122E-3</c:v>
+                  <c:v>7.5016342843348124E-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3473206571269223E-2</c:v>
+                  <c:v>6.0008572506203833E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.4900141956719624E-2</c:v>
+                  <c:v>2.024877004541181E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.15966347062760222</c:v>
+                  <c:v>4.7978059651185284E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.26412705355846133</c:v>
+                  <c:v>9.3645930124346957E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.36349842917090391</c:v>
+                  <c:v>1.6166252946983649E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.43637539384532031</c:v>
+                  <c:v>2.5636530091484311E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.47696021108917119</c:v>
+                  <c:v>3.8198800190648858E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.49374775762398693</c:v>
+                  <c:v>5.4262470481070413E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.4987735918534465</c:v>
+                  <c:v>7.4218920962914039E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.49983226868604874</c:v>
+                  <c:v>9.843704293543025E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.49998457194554841</c:v>
+                  <c:v>1.2725844494549809E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.6099241101609572E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.9991071085629669E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.4424237610961935E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.9416856990439513E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.4981768830348287E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.1126084095391591E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.7850786355034675E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.5150401592329062E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.3012751599265338E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7.1418805095598475E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8.0342639254068787E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8.9751522277932802E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9.9606125065372003E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.10986086684613371</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.12046439605497444</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.13136020371072249</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.14248736232479842</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.15378137902058026</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.16517514727773613</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.17659997771015737</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.18798668473414495</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.19926670307190242</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.21037320593524328</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.22124219558999517</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.23181353691984963</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.24203190564996585</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.25184762506281139</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.26121736829143588</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3538,51 +3852,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>4445</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>4572000</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>74295</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C8AEA8B-FF98-4BE8-BCDC-8A0B95A3B297}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>447675</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>4572000</xdr:colOff>
+      <xdr:colOff>5019675</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>132080</xdr:rowOff>
     </xdr:to>
@@ -3603,6 +3879,44 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>5210175</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12E5539E-DC92-4633-8C32-ACBC3A592645}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
@@ -3616,16 +3930,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3952,8 +4266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3D2DEE-686E-48A0-AC3D-0F54DEA5D0EC}">
   <dimension ref="A1:C121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C56" sqref="B56:C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3964,22 +4278,22 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3997,28 +4311,28 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12">
-        <v>0.5</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13">
-        <v>0.27500000000000002</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -4026,1029 +4340,1037 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>40</v>
       </c>
-      <c r="B15">
-        <v>1.5</v>
+      <c r="B16">
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20">
-        <f>(1-EXP(-((C20-($B$15-0.5))/$B$13)^$B$14))*$B$12</f>
+        <f>(1-EXP(-((C20/$B$16-($B$15-0.5))/$B$13)^$B$14))*$B$12</f>
         <v>0</v>
       </c>
       <c r="C20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21">
-        <f t="shared" ref="B21:B84" si="0">(1-EXP(-((C21-($B$15-0.5))/$B$13)^$B$14))*$B$12</f>
-        <v>2.4041495616800024E-5</v>
+        <f t="shared" ref="B21:B84" si="0">(1-EXP(-((C21/$B$16-($B$15-0.5))/$B$13)^$B$14))*$B$12</f>
+        <v>7.5016342843348124E-6</v>
       </c>
       <c r="C21">
-        <f>C20+0.01</f>
-        <v>1.01</v>
+        <f>C20+0.25</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>1.9229960041033944E-4</v>
+        <v>6.0008572506203833E-5</v>
       </c>
       <c r="C22">
-        <f t="shared" ref="C22:C85" si="1">C21+0.01</f>
-        <v>1.02</v>
+        <f t="shared" ref="C22:C85" si="1">C21+0.25</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>6.4871479274314359E-4</v>
+        <v>2.024877004541181E-4</v>
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
-        <v>1.03</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>1.5363275637635954E-3</v>
+        <v>4.7978059651185284E-4</v>
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
-        <v>1.04</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>2.9962456884000122E-3</v>
+        <v>9.3645930124346957E-4</v>
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
-        <v>1.05</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>5.1662128652874006E-3</v>
+        <v>1.6166252946983649E-3</v>
       </c>
       <c r="C26">
         <f t="shared" si="1"/>
-        <v>1.06</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>8.1787999479949192E-3</v>
+        <v>2.5636530091484311E-3</v>
       </c>
       <c r="C27">
         <f t="shared" si="1"/>
-        <v>1.07</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>1.2159252732797055E-2</v>
+        <v>3.8198800190648858E-3</v>
       </c>
       <c r="C28">
         <f t="shared" si="1"/>
-        <v>1.08</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>1.7223045498576117E-2</v>
+        <v>5.4262470481070413E-3</v>
       </c>
       <c r="C29">
         <f t="shared" si="1"/>
-        <v>1.0900000000000001</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>2.3473206571269223E-2</v>
+        <v>7.4218920962914039E-3</v>
       </c>
       <c r="C30">
         <f t="shared" si="1"/>
-        <v>1.1000000000000001</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>3.0997500234635322E-2</v>
+        <v>9.843704293543025E-3</v>
       </c>
       <c r="C31">
         <f t="shared" si="1"/>
-        <v>1.1100000000000001</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>3.9865567220398856E-2</v>
+        <v>1.2725844494549809E-2</v>
       </c>
       <c r="C32">
         <f t="shared" si="1"/>
-        <v>1.1200000000000001</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33">
         <f t="shared" si="0"/>
-        <v>5.0126142457089129E-2</v>
+        <v>1.6099241101609572E-2</v>
       </c>
       <c r="C33">
         <f t="shared" si="1"/>
-        <v>1.1300000000000001</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34">
         <f t="shared" si="0"/>
-        <v>6.1804482243504932E-2</v>
+        <v>1.9991071085629669E-2</v>
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
-        <v>1.1400000000000001</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35">
         <f t="shared" si="0"/>
-        <v>7.4900141956719901E-2</v>
+        <v>2.4424237610961935E-2</v>
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
-        <v>1.1500000000000001</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36">
         <f t="shared" si="0"/>
-        <v>8.9385248244384874E-2</v>
+        <v>2.9416856990439513E-2</v>
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
-        <v>1.1600000000000001</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37">
         <f t="shared" si="0"/>
-        <v>0.10520340498301078</v>
+        <v>3.4981768830348287E-2</v>
       </c>
       <c r="C37">
         <f t="shared" si="1"/>
-        <v>1.1700000000000002</v>
+        <v>4.25</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38">
         <f t="shared" si="0"/>
-        <v>0.12226935901674252</v>
+        <v>4.1126084095391591E-2</v>
       </c>
       <c r="C38">
         <f t="shared" si="1"/>
-        <v>1.1800000000000002</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39">
         <f t="shared" si="0"/>
-        <v>0.14046952920696243</v>
+        <v>4.7850786355034675E-2</v>
       </c>
       <c r="C39">
         <f t="shared" si="1"/>
-        <v>1.1900000000000002</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40">
         <f t="shared" si="0"/>
-        <v>0.15966347062760267</v>
+        <v>5.5150401592329062E-2</v>
       </c>
       <c r="C40">
         <f t="shared" si="1"/>
-        <v>1.2000000000000002</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41">
         <f t="shared" si="0"/>
-        <v>0.17968630558391707</v>
+        <v>6.3012751599265338E-2</v>
       </c>
       <c r="C41">
         <f t="shared" si="1"/>
-        <v>1.2100000000000002</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42">
         <f t="shared" si="0"/>
-        <v>0.20035210607723114</v>
+        <v>7.1418805095598475E-2</v>
       </c>
       <c r="C42">
         <f t="shared" si="1"/>
-        <v>1.2200000000000002</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43">
         <f t="shared" si="0"/>
-        <v>0.22145816076288932</v>
+        <v>8.0342639254068787E-2</v>
       </c>
       <c r="C43">
         <f t="shared" si="1"/>
-        <v>1.2300000000000002</v>
+        <v>5.75</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44">
         <f t="shared" si="0"/>
-        <v>0.24279000646233656</v>
+        <v>8.9751522277932802E-2</v>
       </c>
       <c r="C44">
         <f t="shared" si="1"/>
-        <v>1.2400000000000002</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45">
         <f t="shared" si="0"/>
-        <v>0.26412705355846178</v>
+        <v>9.9606125065372003E-2</v>
       </c>
       <c r="C45">
         <f t="shared" si="1"/>
-        <v>1.2500000000000002</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46">
         <f t="shared" si="0"/>
-        <v>0.2852485900850692</v>
+        <v>0.10986086684613371</v>
       </c>
       <c r="C46">
         <f t="shared" si="1"/>
-        <v>1.2600000000000002</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47">
         <f t="shared" si="0"/>
-        <v>0.30593991493344896</v>
+        <v>0.12046439605497444</v>
       </c>
       <c r="C47">
         <f t="shared" si="1"/>
-        <v>1.2700000000000002</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48">
         <f t="shared" si="0"/>
-        <v>0.32599832983443455</v>
+        <v>0.13136020371072249</v>
       </c>
       <c r="C48">
         <f t="shared" si="1"/>
-        <v>1.2800000000000002</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49">
         <f t="shared" si="0"/>
-        <v>0.34523871531305683</v>
+        <v>0.14248736232479842</v>
       </c>
       <c r="C49">
         <f t="shared" si="1"/>
-        <v>1.2900000000000003</v>
+        <v>7.25</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50">
         <f t="shared" si="0"/>
-        <v>0.36349842917090425</v>
+        <v>0.15378137902058026</v>
       </c>
       <c r="C50">
         <f t="shared" si="1"/>
-        <v>1.3000000000000003</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51">
         <f t="shared" si="0"/>
-        <v>0.38064129731528962</v>
+        <v>0.16517514727773613</v>
       </c>
       <c r="C51">
         <f t="shared" si="1"/>
-        <v>1.3100000000000003</v>
+        <v>7.75</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52">
         <f t="shared" si="0"/>
-        <v>0.39656051444532991</v>
+        <v>0.17659997771015737</v>
       </c>
       <c r="C52">
         <f t="shared" si="1"/>
-        <v>1.3200000000000003</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53">
         <f t="shared" si="0"/>
-        <v>0.41118033320243297</v>
+        <v>0.18798668473414495</v>
       </c>
       <c r="C53">
         <f t="shared" si="1"/>
-        <v>1.3300000000000003</v>
+        <v>8.25</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54">
         <f t="shared" si="0"/>
-        <v>0.42445649053243717</v>
+        <v>0.19926670307190242</v>
       </c>
       <c r="C54">
         <f t="shared" si="1"/>
-        <v>1.3400000000000003</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55">
         <f t="shared" si="0"/>
-        <v>0.43637539384532065</v>
+        <v>0.21037320593524328</v>
       </c>
       <c r="C55">
         <f t="shared" si="1"/>
-        <v>1.3500000000000003</v>
+        <v>8.75</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56">
         <f t="shared" si="0"/>
-        <v>0.44695216127096254</v>
+        <v>0.22124219558999517</v>
       </c>
       <c r="C56">
         <f t="shared" si="1"/>
-        <v>1.3600000000000003</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57">
         <f t="shared" si="0"/>
-        <v>0.4562276741678255</v>
+        <v>0.23181353691984963</v>
       </c>
       <c r="C57">
         <f t="shared" si="1"/>
-        <v>1.3700000000000003</v>
+        <v>9.25</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58">
         <f t="shared" si="0"/>
-        <v>0.46426485100526288</v>
+        <v>0.24203190564996585</v>
       </c>
       <c r="C58">
         <f t="shared" si="1"/>
-        <v>1.3800000000000003</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59">
         <f t="shared" si="0"/>
-        <v>0.47114438598562269</v>
+        <v>0.25184762506281139</v>
       </c>
       <c r="C59">
         <f t="shared" si="1"/>
-        <v>1.3900000000000003</v>
+        <v>9.75</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60">
         <f t="shared" si="0"/>
-        <v>0.47696021108917142</v>
+        <v>0.26121736829143588</v>
       </c>
       <c r="C60">
         <f t="shared" si="1"/>
-        <v>1.4000000000000004</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61">
         <f t="shared" si="0"/>
-        <v>0.48181493622808969</v>
+        <v>0.27010470750054377</v>
       </c>
       <c r="C61">
         <f t="shared" si="1"/>
-        <v>1.4100000000000004</v>
+        <v>10.25</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62">
         <f t="shared" si="0"/>
-        <v>0.48581550032261223</v>
+        <v>0.27848049630021543</v>
       </c>
       <c r="C62">
         <f t="shared" si="1"/>
-        <v>1.4200000000000004</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63">
         <f t="shared" si="0"/>
-        <v>0.48906922940547914</v>
+        <v>0.28632307736964208</v>
       </c>
       <c r="C63">
         <f t="shared" si="1"/>
-        <v>1.4300000000000004</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64">
         <f t="shared" si="0"/>
-        <v>0.49168045056913828</v>
+        <v>0.29361831324963961</v>
       </c>
       <c r="C64">
         <f t="shared" si="1"/>
-        <v>1.4400000000000004</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65">
         <f t="shared" si="0"/>
-        <v>0.49374775762398698</v>
+        <v>0.30035944431943007</v>
       </c>
       <c r="C65">
         <f t="shared" si="1"/>
-        <v>1.4500000000000004</v>
+        <v>11.25</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66">
         <f t="shared" si="0"/>
-        <v>0.49536197077070659</v>
+        <v>0.30654678382278544</v>
       </c>
       <c r="C66">
         <f t="shared" si="1"/>
-        <v>1.4600000000000004</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67">
         <f t="shared" si="0"/>
-        <v>0.49660478299595257</v>
+        <v>0.31218726517655226</v>
       </c>
       <c r="C67">
         <f t="shared" si="1"/>
-        <v>1.4700000000000004</v>
+        <v>11.75</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68">
         <f t="shared" si="0"/>
-        <v>0.49754804397175195</v>
+        <v>0.31729386143083116</v>
       </c>
       <c r="C68">
         <f t="shared" si="1"/>
-        <v>1.4800000000000004</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69">
         <f t="shared" si="0"/>
-        <v>0.49825360046900036</v>
+        <v>0.32188490044468793</v>
       </c>
       <c r="C69">
         <f t="shared" si="1"/>
-        <v>1.4900000000000004</v>
+        <v>12.25</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70">
         <f t="shared" si="0"/>
-        <v>0.4987735918534465</v>
+        <v>0.32598330193721398</v>
       </c>
       <c r="C70">
         <f t="shared" si="1"/>
-        <v>1.5000000000000004</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71">
         <f t="shared" si="0"/>
-        <v>0.49915109001197139</v>
+        <v>0.32961576397642717</v>
       </c>
       <c r="C71">
         <f t="shared" si="1"/>
-        <v>1.5100000000000005</v>
+        <v>12.75</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72">
         <f t="shared" si="0"/>
-        <v>0.49942097387364487</v>
+        <v>0.33281192665098364</v>
       </c>
       <c r="C72">
         <f t="shared" si="1"/>
-        <v>1.5200000000000005</v>
+        <v>13</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73">
         <f t="shared" si="0"/>
-        <v>0.49961093758286002</v>
+        <v>0.33560353967312706</v>
       </c>
       <c r="C73">
         <f t="shared" si="1"/>
-        <v>1.5300000000000005</v>
+        <v>13.25</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74">
         <f t="shared" si="0"/>
-        <v>0.49974254596131784</v>
+        <v>0.33802365859091688</v>
       </c>
       <c r="C74">
         <f t="shared" si="1"/>
-        <v>1.5400000000000005</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75">
         <f t="shared" si="0"/>
-        <v>0.49983226868604874</v>
+        <v>0.34010589130406521</v>
       </c>
       <c r="C75">
         <f t="shared" si="1"/>
-        <v>1.5500000000000005</v>
+        <v>13.75</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76">
         <f t="shared" si="0"/>
-        <v>0.49989244334063315</v>
+        <v>0.34188371288438546</v>
       </c>
       <c r="C76">
         <f t="shared" si="1"/>
-        <v>1.5600000000000005</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77">
         <f t="shared" si="0"/>
-        <v>0.49993213530833991</v>
+        <v>0.34338986253095471</v>
       </c>
       <c r="C77">
         <f t="shared" si="1"/>
-        <v>1.5700000000000005</v>
+        <v>14.25</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78">
         <f t="shared" si="0"/>
-        <v>0.49995787803925179</v>
+        <v>0.34465583208577671</v>
       </c>
       <c r="C78">
         <f t="shared" si="1"/>
-        <v>1.5800000000000005</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79">
         <f t="shared" si="0"/>
-        <v>0.49997428976150043</v>
+        <v>0.34571145113798446</v>
       </c>
       <c r="C79">
         <f t="shared" si="1"/>
-        <v>1.5900000000000005</v>
+        <v>14.75</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80">
         <f t="shared" si="0"/>
-        <v>0.49998457194554841</v>
+        <v>0.34658456957417372</v>
       </c>
       <c r="C80">
         <f t="shared" si="1"/>
-        <v>1.6000000000000005</v>
+        <v>15</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81">
         <f t="shared" si="0"/>
-        <v>0.49999090089962539</v>
+        <v>0.34730083467801665</v>
       </c>
       <c r="C81">
         <f t="shared" si="1"/>
-        <v>1.6100000000000005</v>
+        <v>15.25</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82">
         <f t="shared" si="0"/>
-        <v>0.4999947271831322</v>
+        <v>0.34788355669100007</v>
       </c>
       <c r="C82">
         <f t="shared" si="1"/>
-        <v>1.6200000000000006</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83">
         <f t="shared" si="0"/>
-        <v>0.49999699863673219</v>
+        <v>0.34835365421771686</v>
       </c>
       <c r="C83">
         <f t="shared" si="1"/>
-        <v>1.6300000000000006</v>
+        <v>15.75</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84">
         <f t="shared" si="0"/>
-        <v>0.49999832235222452</v>
+        <v>0.34872966904405506</v>
       </c>
       <c r="C84">
         <f t="shared" si="1"/>
-        <v>1.6400000000000006</v>
+        <v>16</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85">
-        <f t="shared" ref="B85:B121" si="2">(1-EXP(-((C85-($B$15-0.5))/$B$13)^$B$14))*$B$12</f>
-        <v>0.49999907941465183</v>
+        <f t="shared" ref="B85:B121" si="2">(1-EXP(-((C85/$B$16-($B$15-0.5))/$B$13)^$B$14))*$B$12</f>
+        <v>0.34902783883791444</v>
       </c>
       <c r="C85">
         <f t="shared" si="1"/>
-        <v>1.6500000000000006</v>
+        <v>16.25</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86">
         <f t="shared" si="2"/>
-        <v>0.49999950422675427</v>
+        <v>0.3492622157804392</v>
       </c>
       <c r="C86">
-        <f t="shared" ref="C86:C121" si="3">C85+0.01</f>
-        <v>1.6600000000000006</v>
+        <f t="shared" ref="C86:C121" si="3">C85+0.25</f>
+        <v>16.5</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87">
         <f t="shared" si="2"/>
-        <v>0.49999973804145276</v>
+        <v>0.34944481935725885</v>
       </c>
       <c r="C87">
         <f t="shared" si="3"/>
-        <v>1.6700000000000006</v>
+        <v>16.75</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88">
         <f t="shared" si="2"/>
-        <v>0.49999986423518789</v>
+        <v>0.3495858122245698</v>
       </c>
       <c r="C88">
         <f t="shared" si="3"/>
-        <v>1.6800000000000006</v>
+        <v>17</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89">
         <f t="shared" si="2"/>
-        <v>0.49999993100434548</v>
+        <v>0.34969368913943127</v>
       </c>
       <c r="C89">
         <f t="shared" si="3"/>
-        <v>1.6900000000000006</v>
+        <v>17.25</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90">
         <f t="shared" si="2"/>
-        <v>0.49999996562752336</v>
+        <v>0.34977547028721101</v>
       </c>
       <c r="C90">
         <f t="shared" si="3"/>
-        <v>1.7000000000000006</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91">
         <f t="shared" si="2"/>
-        <v>0.49999998321856143</v>
+        <v>0.3498368918348444</v>
       </c>
       <c r="C91">
         <f t="shared" si="3"/>
-        <v>1.7100000000000006</v>
+        <v>17.75</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92">
         <f t="shared" si="2"/>
-        <v>0.49999999197303208</v>
+        <v>0.34988258808023409</v>
       </c>
       <c r="C92">
         <f t="shared" si="3"/>
-        <v>1.7200000000000006</v>
+        <v>18</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93">
         <f t="shared" si="2"/>
-        <v>0.49999999623943975</v>
+        <v>0.34991626106546403</v>
       </c>
       <c r="C93">
         <f t="shared" si="3"/>
-        <v>1.7300000000000006</v>
+        <v>18.25</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94">
         <f t="shared" si="2"/>
-        <v>0.49999999827492908</v>
+        <v>0.34994083490357991</v>
       </c>
       <c r="C94">
         <f t="shared" si="3"/>
-        <v>1.7400000000000007</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95">
         <f t="shared" si="2"/>
-        <v>0.49999999922537869</v>
+        <v>0.34995859328510975</v>
       </c>
       <c r="C95">
         <f t="shared" si="3"/>
-        <v>1.7500000000000007</v>
+        <v>18.75</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96">
         <f t="shared" si="2"/>
-        <v>0.49999999965961162</v>
+        <v>0.34997129965097196</v>
       </c>
       <c r="C96">
         <f t="shared" si="3"/>
-        <v>1.7600000000000007</v>
+        <v>19</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97">
         <f t="shared" si="2"/>
-        <v>0.49999999985366861</v>
+        <v>0.34998030033082916</v>
       </c>
       <c r="C97">
         <f t="shared" si="3"/>
-        <v>1.7700000000000007</v>
+        <v>19.25</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98">
         <f t="shared" si="2"/>
-        <v>0.49999999993847488</v>
+        <v>0.34998661155345162</v>
       </c>
       <c r="C98">
         <f t="shared" si="3"/>
-        <v>1.7800000000000007</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99">
         <f t="shared" si="2"/>
-        <v>0.49999999997470734</v>
+        <v>0.34999099165321684</v>
       </c>
       <c r="C99">
         <f t="shared" si="3"/>
-        <v>1.7900000000000007</v>
+        <v>19.75</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100">
         <f t="shared" si="2"/>
-        <v>0.49999999998983663</v>
+        <v>0.34999400004761355</v>
       </c>
       <c r="C100">
         <f t="shared" si="3"/>
-        <v>1.8000000000000007</v>
+        <v>20</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101">
         <f t="shared" si="2"/>
-        <v>0.49999999999600925</v>
+        <v>0.34999604467238488</v>
       </c>
       <c r="C101">
         <f t="shared" si="3"/>
-        <v>1.8100000000000007</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102">
         <f t="shared" si="2"/>
-        <v>0.49999999999846917</v>
+        <v>0.34999741956325225</v>
       </c>
       <c r="C102">
         <f t="shared" si="3"/>
-        <v>1.8200000000000007</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103">
         <f t="shared" si="2"/>
-        <v>0.49999999999942651</v>
+        <v>0.34999833419476295</v>
       </c>
       <c r="C103">
         <f t="shared" si="3"/>
-        <v>1.8300000000000007</v>
+        <v>20.75</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104">
         <f t="shared" si="2"/>
-        <v>0.49999999999979022</v>
+        <v>0.34999893605390209</v>
       </c>
       <c r="C104">
         <f t="shared" si="3"/>
-        <v>1.8400000000000007</v>
+        <v>21</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105">
         <f t="shared" si="2"/>
-        <v>0.49999999999992512</v>
+        <v>0.34999932776119835</v>
       </c>
       <c r="C105">
         <f t="shared" si="3"/>
-        <v>1.8500000000000008</v>
+        <v>21.25</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106">
         <f t="shared" si="2"/>
-        <v>0.49999999999997391</v>
+        <v>0.34999957987335761</v>
       </c>
       <c r="C106">
         <f t="shared" si="3"/>
-        <v>1.8600000000000008</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107">
         <f t="shared" si="2"/>
-        <v>0.49999999999999112</v>
+        <v>0.34999974032286191</v>
       </c>
       <c r="C107">
         <f t="shared" si="3"/>
-        <v>1.8700000000000008</v>
+        <v>21.75</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108">
         <f t="shared" si="2"/>
-        <v>0.49999999999999706</v>
+        <v>0.34999984128126099</v>
       </c>
       <c r="C108">
         <f t="shared" si="3"/>
-        <v>1.8800000000000008</v>
+        <v>22</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109">
         <f t="shared" si="2"/>
-        <v>0.49999999999999906</v>
+        <v>0.3499999040802943</v>
       </c>
       <c r="C109">
         <f t="shared" si="3"/>
-        <v>1.8900000000000008</v>
+        <v>22.25</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110">
         <f t="shared" si="2"/>
-        <v>0.49999999999999972</v>
+        <v>0.3499999426918004</v>
       </c>
       <c r="C110">
         <f t="shared" si="3"/>
-        <v>1.9000000000000008</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111">
         <f t="shared" si="2"/>
-        <v>0.49999999999999989</v>
+        <v>0.34999996615464019</v>
       </c>
       <c r="C111">
         <f t="shared" si="3"/>
-        <v>1.9100000000000008</v>
+        <v>22.75</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.34999998024399626</v>
       </c>
       <c r="C112">
         <f t="shared" si="3"/>
-        <v>1.9200000000000008</v>
+        <v>23</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.34999998860378051</v>
       </c>
       <c r="C113">
         <f t="shared" si="3"/>
-        <v>1.9300000000000008</v>
+        <v>23.25</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.34999999350426342</v>
       </c>
       <c r="C114">
         <f t="shared" si="3"/>
-        <v>1.9400000000000008</v>
+        <v>23.5</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.34999999634198026</v>
       </c>
       <c r="C115">
         <f t="shared" si="3"/>
-        <v>1.9500000000000008</v>
+        <v>23.75</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.34999999796503062</v>
       </c>
       <c r="C116">
         <f t="shared" si="3"/>
-        <v>1.9600000000000009</v>
+        <v>24</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.34999999888182948</v>
       </c>
       <c r="C117">
         <f t="shared" si="3"/>
-        <v>1.9700000000000009</v>
+        <v>24.25</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.34999999939320681</v>
       </c>
       <c r="C118">
         <f t="shared" si="3"/>
-        <v>1.9800000000000009</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.3499999996748378</v>
       </c>
       <c r="C119">
         <f t="shared" si="3"/>
-        <v>1.9900000000000009</v>
+        <v>24.75</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.34999999982795971</v>
       </c>
       <c r="C120">
         <f t="shared" si="3"/>
-        <v>2.0000000000000009</v>
+        <v>25</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>0.34999999991013819</v>
       </c>
       <c r="C121">
         <f t="shared" si="3"/>
-        <v>2.0100000000000007</v>
+        <v>25.25</v>
       </c>
     </row>
   </sheetData>
@@ -5062,10 +5384,10 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:BK2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:O1"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:BK2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5074,110 +5396,507 @@
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:63" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1">
+        <f>(1-EXP(-((B2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
         <v>0</v>
       </c>
       <c r="C1">
-        <f>(1-EXP(-((C2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>2.9962456884000122E-3</v>
+        <f>(1-EXP(-((C2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>7.5016342843348124E-6</v>
       </c>
       <c r="D1">
-        <f>(1-EXP(-((D2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>2.3473206571269223E-2</v>
+        <f>(1-EXP(-((D2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>6.0008572506203833E-5</v>
       </c>
       <c r="E1">
-        <f>(1-EXP(-((E2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>7.4900141956719624E-2</v>
+        <f>(1-EXP(-((E2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>2.024877004541181E-4</v>
       </c>
       <c r="F1">
-        <f>(1-EXP(-((F2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.15966347062760222</v>
+        <f>(1-EXP(-((F2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>4.7978059651185284E-4</v>
       </c>
       <c r="G1">
-        <f>(1-EXP(-((G2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.26412705355846133</v>
+        <f>(1-EXP(-((G2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>9.3645930124346957E-4</v>
       </c>
       <c r="H1">
-        <f>(1-EXP(-((H2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.36349842917090391</v>
+        <f>(1-EXP(-((H2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>1.6166252946983649E-3</v>
       </c>
       <c r="I1">
-        <f>(1-EXP(-((I2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.43637539384532031</v>
+        <f>(1-EXP(-((I2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>2.5636530091484311E-3</v>
       </c>
       <c r="J1">
-        <f>(1-EXP(-((J2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.47696021108917119</v>
+        <f>(1-EXP(-((J2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>3.8198800190648858E-3</v>
       </c>
       <c r="K1">
-        <f>(1-EXP(-((K2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.49374775762398693</v>
+        <f>(1-EXP(-((K2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>5.4262470481070413E-3</v>
       </c>
       <c r="L1">
-        <f>(1-EXP(-((L2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.4987735918534465</v>
+        <f>(1-EXP(-((L2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>7.4218920962914039E-3</v>
       </c>
       <c r="M1">
-        <f>(1-EXP(-((M2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.49983226868604874</v>
+        <f>(1-EXP(-((M2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>9.843704293543025E-3</v>
       </c>
       <c r="N1">
-        <f>(1-EXP(-((N2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.49998457194554841</v>
+        <f>(1-EXP(-((N2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>1.2725844494549809E-2</v>
       </c>
       <c r="O1">
-        <f>(1-EXP(-((O2-1)/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((O2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>1.6099241101609572E-2</v>
+      </c>
+      <c r="P1">
+        <f>(1-EXP(-((P2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>1.9991071085629669E-2</v>
+      </c>
+      <c r="Q1">
+        <f>(1-EXP(-((Q2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>2.4424237610961935E-2</v>
+      </c>
+      <c r="R1">
+        <f>(1-EXP(-((R2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>2.9416856990439513E-2</v>
+      </c>
+      <c r="S1">
+        <f>(1-EXP(-((S2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>3.4981768830348287E-2</v>
+      </c>
+      <c r="T1">
+        <f>(1-EXP(-((T2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>4.1126084095391591E-2</v>
+      </c>
+      <c r="U1">
+        <f>(1-EXP(-((U2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>4.7850786355034675E-2</v>
+      </c>
+      <c r="V1">
+        <f>(1-EXP(-((V2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>5.5150401592329062E-2</v>
+      </c>
+      <c r="W1">
+        <f>(1-EXP(-((W2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>6.3012751599265338E-2</v>
+      </c>
+      <c r="X1">
+        <f>(1-EXP(-((X2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>7.1418805095598475E-2</v>
+      </c>
+      <c r="Y1">
+        <f>(1-EXP(-((Y2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>8.0342639254068787E-2</v>
+      </c>
+      <c r="Z1">
+        <f>(1-EXP(-((Z2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>8.9751522277932802E-2</v>
+      </c>
+      <c r="AA1">
+        <f>(1-EXP(-((AA2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>9.9606125065372003E-2</v>
+      </c>
+      <c r="AB1">
+        <f>(1-EXP(-((AB2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.10986086684613371</v>
+      </c>
+      <c r="AC1">
+        <f>(1-EXP(-((AC2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.12046439605497444</v>
+      </c>
+      <c r="AD1">
+        <f>(1-EXP(-((AD2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.13136020371072249</v>
+      </c>
+      <c r="AE1">
+        <f>(1-EXP(-((AE2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.14248736232479842</v>
+      </c>
+      <c r="AF1">
+        <f>(1-EXP(-((AF2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.15378137902058026</v>
+      </c>
+      <c r="AG1">
+        <f>(1-EXP(-((AG2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.16517514727773613</v>
+      </c>
+      <c r="AH1">
+        <f>(1-EXP(-((AH2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.17659997771015737</v>
+      </c>
+      <c r="AI1">
+        <f>(1-EXP(-((AI2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.18798668473414495</v>
+      </c>
+      <c r="AJ1">
+        <f>(1-EXP(-((AJ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.19926670307190242</v>
+      </c>
+      <c r="AK1">
+        <f>(1-EXP(-((AK2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.21037320593524328</v>
+      </c>
+      <c r="AL1">
+        <f>(1-EXP(-((AL2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.22124219558999517</v>
+      </c>
+      <c r="AM1">
+        <f>(1-EXP(-((AM2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.23181353691984963</v>
+      </c>
+      <c r="AN1">
+        <f>(1-EXP(-((AN2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.24203190564996585</v>
+      </c>
+      <c r="AO1">
+        <f>(1-EXP(-((AO2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.25184762506281139</v>
+      </c>
+      <c r="AP1">
+        <f>(1-EXP(-((AP2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.26121736829143588</v>
+      </c>
+      <c r="AQ1">
+        <f>(1-EXP(-((AQ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.27010470750054377</v>
+      </c>
+      <c r="AR1">
+        <f>(1-EXP(-((AR2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.27848049630021543</v>
+      </c>
+      <c r="AS1">
+        <f>(1-EXP(-((AS2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.28632307736964208</v>
+      </c>
+      <c r="AT1">
+        <f>(1-EXP(-((AT2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.29361831324963961</v>
+      </c>
+      <c r="AU1">
+        <f>(1-EXP(-((AU2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.30035944431943007</v>
+      </c>
+      <c r="AV1">
+        <f>(1-EXP(-((AV2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.30654678382278544</v>
+      </c>
+      <c r="AW1">
+        <f>(1-EXP(-((AW2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.31218726517655226</v>
+      </c>
+      <c r="AX1">
+        <f>(1-EXP(-((AX2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.31729386143083116</v>
+      </c>
+      <c r="AY1">
+        <f>(1-EXP(-((AY2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.32188490044468793</v>
+      </c>
+      <c r="AZ1">
+        <f>(1-EXP(-((AZ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.32598330193721398</v>
+      </c>
+      <c r="BA1">
+        <f>(1-EXP(-((BA2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.32961576397642717</v>
+      </c>
+      <c r="BB1">
+        <f>(1-EXP(-((BB2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.33281192665098364</v>
+      </c>
+      <c r="BC1">
+        <f>(1-EXP(-((BC2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.33560353967312706</v>
+      </c>
+      <c r="BD1">
+        <f>(1-EXP(-((BD2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.33802365859091688</v>
+      </c>
+      <c r="BE1">
+        <f>(1-EXP(-((BE2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.34010589130406521</v>
+      </c>
+      <c r="BF1">
+        <f>(1-EXP(-((BF2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.34188371288438546</v>
+      </c>
+      <c r="BG1">
+        <f>(1-EXP(-((BG2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.34338986253095471</v>
+      </c>
+      <c r="BH1">
+        <f>(1-EXP(-((BH2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.34465583208577671</v>
+      </c>
+      <c r="BI1">
+        <f>(1-EXP(-((BI2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.34571145113798446</v>
+      </c>
+      <c r="BJ1">
+        <f>(1-EXP(-((BJ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.34658456957417372</v>
+      </c>
+      <c r="BK1">
+        <f>(1-EXP(-((BK2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <f>B2+0.25</f>
+        <v>0.25</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:AI2" si="0">C2+0.25</f>
         <v>0.5</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E2">
+        <f t="shared" si="0"/>
+        <v>0.75</v>
+      </c>
+      <c r="F2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+      <c r="H2">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="I2">
+        <f t="shared" si="0"/>
+        <v>1.75</v>
+      </c>
+      <c r="J2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <f t="shared" si="0"/>
+        <v>2.25</v>
+      </c>
+      <c r="L2">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="M2">
+        <f t="shared" si="0"/>
+        <v>2.75</v>
+      </c>
+      <c r="N2">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="O2">
+        <f t="shared" si="0"/>
+        <v>3.25</v>
+      </c>
+      <c r="P2">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="Q2">
+        <f t="shared" si="0"/>
+        <v>3.75</v>
+      </c>
+      <c r="R2">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1.05</v>
-      </c>
-      <c r="D2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E2">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="F2">
-        <v>1.2</v>
-      </c>
-      <c r="G2">
-        <v>1.25</v>
-      </c>
-      <c r="H2">
-        <v>1.3</v>
-      </c>
-      <c r="I2">
-        <v>1.35</v>
-      </c>
-      <c r="J2">
-        <v>1.4</v>
-      </c>
-      <c r="K2">
-        <v>1.45</v>
-      </c>
-      <c r="L2">
-        <v>1.5</v>
-      </c>
-      <c r="M2">
-        <v>1.55</v>
-      </c>
-      <c r="N2">
-        <v>1.6</v>
-      </c>
-      <c r="O2">
+      <c r="S2">
+        <f t="shared" si="0"/>
+        <v>4.25</v>
+      </c>
+      <c r="T2">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="U2">
+        <f t="shared" si="0"/>
+        <v>4.75</v>
+      </c>
+      <c r="V2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="W2">
+        <f t="shared" si="0"/>
+        <v>5.25</v>
+      </c>
+      <c r="X2">
+        <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
+      <c r="Y2">
+        <f t="shared" si="0"/>
+        <v>5.75</v>
+      </c>
+      <c r="Z2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AA2">
+        <f t="shared" si="0"/>
+        <v>6.25</v>
+      </c>
+      <c r="AB2">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="AC2">
+        <f t="shared" si="0"/>
+        <v>6.75</v>
+      </c>
+      <c r="AD2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="AE2">
+        <f t="shared" si="0"/>
+        <v>7.25</v>
+      </c>
+      <c r="AF2">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="AG2">
+        <f t="shared" si="0"/>
+        <v>7.75</v>
+      </c>
+      <c r="AH2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="AI2">
+        <f t="shared" si="0"/>
+        <v>8.25</v>
+      </c>
+      <c r="AJ2">
+        <f>AI2+0.25</f>
+        <v>8.5</v>
+      </c>
+      <c r="AK2">
+        <f t="shared" ref="AK2:AO2" si="1">AJ2+0.25</f>
+        <v>8.75</v>
+      </c>
+      <c r="AL2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="AM2">
+        <f t="shared" si="1"/>
+        <v>9.25</v>
+      </c>
+      <c r="AN2">
+        <f t="shared" si="1"/>
+        <v>9.5</v>
+      </c>
+      <c r="AO2">
+        <f t="shared" si="1"/>
+        <v>9.75</v>
+      </c>
+      <c r="AP2">
+        <f>AO2+0.25</f>
+        <v>10</v>
+      </c>
+      <c r="AQ2">
+        <f t="shared" ref="AQ2:BJ2" si="2">AP2+0.25</f>
+        <v>10.25</v>
+      </c>
+      <c r="AR2">
+        <f t="shared" si="2"/>
+        <v>10.5</v>
+      </c>
+      <c r="AS2">
+        <f t="shared" si="2"/>
+        <v>10.75</v>
+      </c>
+      <c r="AT2">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="AU2">
+        <f t="shared" si="2"/>
+        <v>11.25</v>
+      </c>
+      <c r="AV2">
+        <f t="shared" si="2"/>
+        <v>11.5</v>
+      </c>
+      <c r="AW2">
+        <f t="shared" si="2"/>
+        <v>11.75</v>
+      </c>
+      <c r="AX2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="AY2">
+        <f t="shared" si="2"/>
+        <v>12.25</v>
+      </c>
+      <c r="AZ2">
+        <f t="shared" si="2"/>
+        <v>12.5</v>
+      </c>
+      <c r="BA2">
+        <f t="shared" si="2"/>
+        <v>12.75</v>
+      </c>
+      <c r="BB2">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="BC2">
+        <f t="shared" si="2"/>
+        <v>13.25</v>
+      </c>
+      <c r="BD2">
+        <f t="shared" si="2"/>
+        <v>13.5</v>
+      </c>
+      <c r="BE2">
+        <f t="shared" si="2"/>
+        <v>13.75</v>
+      </c>
+      <c r="BF2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="BG2">
+        <f t="shared" si="2"/>
+        <v>14.25</v>
+      </c>
+      <c r="BH2">
+        <f t="shared" si="2"/>
+        <v>14.5</v>
+      </c>
+      <c r="BI2">
+        <f t="shared" si="2"/>
+        <v>14.75</v>
+      </c>
+      <c r="BJ2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="BK2">
         <v>1000</v>
       </c>
     </row>
@@ -5205,12 +5924,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2">
         <v>0.02</v>
@@ -5239,7 +5958,7 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1">
         <v>2021</v>
@@ -5334,7 +6053,7 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5429,7 +6148,7 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -5524,7 +6243,7 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -5619,7 +6338,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -5714,7 +6433,7 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -5809,7 +6528,7 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -5904,7 +6623,7 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -5999,7 +6718,7 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -6094,7 +6813,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -6189,7 +6908,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -6284,7 +7003,7 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -6379,7 +7098,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -6474,7 +7193,7 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -6569,7 +7288,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -6664,7 +7383,7 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -6759,7 +7478,7 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -6854,7 +7573,7 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -6949,7 +7668,7 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -7044,7 +7763,7 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -7139,7 +7858,7 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -7234,7 +7953,7 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -7329,7 +8048,7 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -7424,7 +8143,7 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -7519,7 +8238,7 @@
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -7635,7 +8354,7 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1">
         <v>2021</v>
@@ -7730,7 +8449,7 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -7825,7 +8544,7 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -7920,7 +8639,7 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -8015,7 +8734,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -8110,7 +8829,7 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -8205,7 +8924,7 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>0.05</v>
@@ -8300,7 +9019,7 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>0.05</v>
@@ -8395,7 +9114,7 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -8490,7 +9209,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -8585,7 +9304,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -8680,7 +9399,7 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -8775,7 +9494,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -8870,7 +9589,7 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -8965,7 +9684,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -9060,7 +9779,7 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -9155,7 +9874,7 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -9250,7 +9969,7 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -9345,7 +10064,7 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -9440,7 +10159,7 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -9535,7 +10254,7 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -9630,7 +10349,7 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -9725,7 +10444,7 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -9820,7 +10539,7 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -9915,7 +10634,7 @@
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25">
         <v>0</v>

</xml_diff>

<commit_message>
Updates calculation methodology for electricity rates by collecting capacity market revenues over ten years and collecing all other non amortized costs on an annual basis. Updates CSC parameters for calibration.
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Models\US\Models\eps-us\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A4A1CFFE-EAE2-4ED0-BAA6-8E17A86A7094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C8E4E65-C83F-455C-8258-12FE5751306F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
@@ -610,307 +610,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>7.5016342843348124E-6</c:v>
+                  <c:v>2.7126613468153591E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0008572506203833E-5</c:v>
+                  <c:v>2.1700603990693067E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.024877004541181E-4</c:v>
+                  <c:v>7.3233247530835044E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.7978059651185284E-4</c:v>
+                  <c:v>1.7356088610352981E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.3645930124346957E-4</c:v>
+                  <c:v>3.3889264340773994E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6166252946983649E-3</c:v>
+                  <c:v>5.853656677573426E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.5636530091484311E-3</c:v>
+                  <c:v>9.2900565297051587E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.8198800190648858E-3</c:v>
+                  <c:v>1.3856788240271701E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.4262470481070413E-3</c:v>
+                  <c:v>1.9710355922915369E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.4218920962914039E-3</c:v>
+                  <c:v>2.700446163192427E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.843704293543025E-3</c:v>
+                  <c:v>3.5889284688606191E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.2725844494549809E-2</c:v>
+                  <c:v>4.651068898377464E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.6099241101609572E-2</c:v>
+                  <c:v>5.9009364077483913E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.9991071085629669E-2</c:v>
+                  <c:v>7.3519907089534368E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.4424237610961935E-2</c:v>
+                  <c:v>9.0169853605967954E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.9416856990439513E-2</c:v>
+                  <c:v>1.0907866709614121E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.4981768830348287E-2</c:v>
+                  <c:v>1.303566976172048E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.1126084095391591E-2</c:v>
+                  <c:v>1.5410412185000931E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.7850786355034675E-2</c:v>
+                  <c:v>1.8040987773186055E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.5150401592329062E-2</c:v>
+                  <c:v>2.0935060809395944E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6.3012751599265338E-2</c:v>
+                  <c:v>2.4098962873959361E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.1418805095598475E-2</c:v>
+                  <c:v>2.7537593727665208E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>8.0342639254068787E-2</c:v>
+                  <c:v>3.1254327970773217E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>8.9751522277932802E-2</c:v>
+                  <c:v>3.5250929224621363E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>9.9606125065372003E-2</c:v>
+                  <c:v>3.9527473603179493E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.10986086684613371</c:v>
+                  <c:v>4.4082284233117663E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.12046439605497444</c:v>
+                  <c:v>4.8911878539958133E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.13136020371072249</c:v>
+                  <c:v>5.4010929942227434E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.14248736232479842</c:v>
+                  <c:v>5.9372245483401073E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.15378137902058026</c:v>
+                  <c:v>6.4986760781754541E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.16517514727773613</c:v>
+                  <c:v>7.0843553490771954E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.17659997771015737</c:v>
+                  <c:v>7.6929876238228126E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.18798668473414495</c:v>
+                  <c:v>8.3231209752196347E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.19926670307190242</c:v>
+                  <c:v>8.973133658987105E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.21037320593524328</c:v>
+                  <c:v>9.641243556416082E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.22124219558999517</c:v>
+                  <c:v>0.10325519661854952</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.23181353691984963</c:v>
+                  <c:v>0.11023895553883063</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.24203190564996585</c:v>
+                  <c:v>0.11734184751806659</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.25184762506281139</c:v>
+                  <c:v>0.12454097821643233</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.26121736829143588</c:v>
+                  <c:v>0.13181261058906879</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.27010470750054377</c:v>
+                  <c:v>0.13913236540178756</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.27848049630021543</c:v>
+                  <c:v>0.14647543302575003</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.28632307736964208</c:v>
+                  <c:v>0.15381679380738991</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.29361831324963961</c:v>
+                  <c:v>0.16113144405783855</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.30035944431943007</c:v>
+                  <c:v>0.16839462450529405</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.30654678382278544</c:v>
+                  <c:v>0.17558204791159163</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.31218726517655226</c:v>
+                  <c:v>0.18267012247688577</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.31729386143083116</c:v>
+                  <c:v>0.18963616764856731</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.32188490044468793</c:v>
+                  <c:v>0.19645861901529907</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.32598330193721398</c:v>
+                  <c:v>0.20311721910542085</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.32961576397642717</c:v>
+                  <c:v>0.20959319111996269</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.33281192665098364</c:v>
+                  <c:v>0.21586939291098117</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.33560353967312706</c:v>
+                  <c:v>0.22193044886066229</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.33802365859091688</c:v>
+                  <c:v>0.2277628577183255</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.34010589130406521</c:v>
+                  <c:v>0.23335507490195029</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.34188371288438546</c:v>
+                  <c:v>0.23869756825732752</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.34338986253095471</c:v>
+                  <c:v>0.24378284677925793</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.34465583208577671</c:v>
+                  <c:v>0.24860546232227976</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.34571145113798446</c:v>
+                  <c:v>0.25316198484953234</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.34658456957417372</c:v>
+                  <c:v>0.25745095227379722</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.34730083467801665</c:v>
+                  <c:v>0.26147279642109311</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.34788355669100007</c:v>
+                  <c:v>0.26522974708186364</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.34835365421771686</c:v>
+                  <c:v>0.26872571649646854</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.34872966904405506</c:v>
+                  <c:v>0.27196616694071241</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.34902783883791444</c:v>
+                  <c:v>0.27495796432585551</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.3492622157804392</c:v>
+                  <c:v>0.27770922090054417</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.34944481935725885</c:v>
+                  <c:v>0.28022913023639223</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.3495858122245698</c:v>
+                  <c:v>0.28252779769408043</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.34969368913943127</c:v>
+                  <c:v>0.2846160695048362</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.34977547028721101</c:v>
+                  <c:v>0.28650536346742178</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.3498368918348444</c:v>
+                  <c:v>0.28820750405985879</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.34988258808023409</c:v>
+                  <c:v>0.2897345645065002</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.34991626106546403</c:v>
+                  <c:v>0.29109871803469367</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.34994083490357991</c:v>
+                  <c:v>0.29231210021223275</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.34995859328510975</c:v>
+                  <c:v>0.29338668388880529</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.34997129965097196</c:v>
+                  <c:v>0.29433416788367545</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.34998030033082916</c:v>
+                  <c:v>0.29516588017958978</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.34998661155345162</c:v>
+                  <c:v>0.29589269601045221</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.34999099165321684</c:v>
+                  <c:v>0.29652497087771895</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.34999400004761355</c:v>
+                  <c:v>0.29707248820643462</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.34999604467238488</c:v>
+                  <c:v>0.2975444210635308</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.34999741956325225</c:v>
+                  <c:v>0.29794930711385315</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.34999833419476295</c:v>
+                  <c:v>0.29829503578700706</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.34999893605390209</c:v>
+                  <c:v>0.29858884647232875</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.34999932776119835</c:v>
+                  <c:v>0.29883733645020727</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.34999957987335761</c:v>
+                  <c:v>0.29904647720411548</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.34999974032286191</c:v>
+                  <c:v>0.29922163773619626</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.34999984128126099</c:v>
+                  <c:v>0.29936761352609076</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.3499999040802943</c:v>
+                  <c:v>0.29948865982299966</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.3499999426918004</c:v>
+                  <c:v>0.29958852803926317</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.34999996615464019</c:v>
+                  <c:v>0.29967050411421003</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.34999998024399626</c:v>
+                  <c:v>0.29973744783379824</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.34999998860378051</c:v>
+                  <c:v>0.29979183221893801</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.34999999350426342</c:v>
+                  <c:v>0.29983578222801444</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.34999999634198026</c:v>
+                  <c:v>0.29987111215221296</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.34999999796503062</c:v>
+                  <c:v>0.29989936121162925</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.34999999888182948</c:v>
+                  <c:v>0.29992182698238479</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.34999999939320681</c:v>
+                  <c:v>0.29993959639739087</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.3499999996748378</c:v>
+                  <c:v>0.29995357416407437</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.34999999982795971</c:v>
+                  <c:v>0.2999645085300941</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.34999999991013819</c:v>
+                  <c:v>0.29997301440226942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1328,124 +1328,124 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.5016342843348124E-6</c:v>
+                  <c:v>2.7126613468153591E-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.0008572506203833E-5</c:v>
+                  <c:v>2.1700603990693067E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.024877004541181E-4</c:v>
+                  <c:v>7.3233247530835044E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.7978059651185284E-4</c:v>
+                  <c:v>1.7356088610352981E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.3645930124346957E-4</c:v>
+                  <c:v>3.3889264340773994E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.6166252946983649E-3</c:v>
+                  <c:v>5.853656677573426E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5636530091484311E-3</c:v>
+                  <c:v>9.2900565297051587E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.8198800190648858E-3</c:v>
+                  <c:v>1.3856788240271701E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.4262470481070413E-3</c:v>
+                  <c:v>1.9710355922915369E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.4218920962914039E-3</c:v>
+                  <c:v>2.700446163192427E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.843704293543025E-3</c:v>
+                  <c:v>3.5889284688606191E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.2725844494549809E-2</c:v>
+                  <c:v>4.651068898377464E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.6099241101609572E-2</c:v>
+                  <c:v>5.9009364077483913E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.9991071085629669E-2</c:v>
+                  <c:v>7.3519907089534368E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.4424237610961935E-2</c:v>
+                  <c:v>9.0169853605967954E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.9416856990439513E-2</c:v>
+                  <c:v>1.0907866709614121E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.4981768830348287E-2</c:v>
+                  <c:v>1.303566976172048E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.1126084095391591E-2</c:v>
+                  <c:v>1.5410412185000931E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.7850786355034675E-2</c:v>
+                  <c:v>1.8040987773186055E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.5150401592329062E-2</c:v>
+                  <c:v>2.0935060809395944E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>6.3012751599265338E-2</c:v>
+                  <c:v>2.4098962873959361E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.1418805095598475E-2</c:v>
+                  <c:v>2.7537593727665208E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>8.0342639254068787E-2</c:v>
+                  <c:v>3.1254327970773217E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8.9751522277932802E-2</c:v>
+                  <c:v>3.5250929224621363E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9.9606125065372003E-2</c:v>
+                  <c:v>3.9527473603179493E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.10986086684613371</c:v>
+                  <c:v>4.4082284233117663E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.12046439605497444</c:v>
+                  <c:v>4.8911878539958133E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.13136020371072249</c:v>
+                  <c:v>5.4010929942227434E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.14248736232479842</c:v>
+                  <c:v>5.9372245483401073E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.15378137902058026</c:v>
+                  <c:v>6.4986760781754541E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.16517514727773613</c:v>
+                  <c:v>7.0843553490771954E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.17659997771015737</c:v>
+                  <c:v>7.6929876238228126E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.18798668473414495</c:v>
+                  <c:v>8.3231209752196347E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.19926670307190242</c:v>
+                  <c:v>8.973133658987105E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.21037320593524328</c:v>
+                  <c:v>9.641243556416082E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.22124219558999517</c:v>
+                  <c:v>0.10325519661854952</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.23181353691984963</c:v>
+                  <c:v>0.11023895553883063</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.24203190564996585</c:v>
+                  <c:v>0.11734184751806659</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.25184762506281139</c:v>
+                  <c:v>0.12454097821643233</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.26121736829143588</c:v>
+                  <c:v>0.13181261058906879</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1863,124 +1863,124 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.5016342843348124E-6</c:v>
+                  <c:v>2.7126613468153591E-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.0008572506203833E-5</c:v>
+                  <c:v>2.1700603990693067E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.024877004541181E-4</c:v>
+                  <c:v>7.3233247530835044E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.7978059651185284E-4</c:v>
+                  <c:v>1.7356088610352981E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.3645930124346957E-4</c:v>
+                  <c:v>3.3889264340773994E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.6166252946983649E-3</c:v>
+                  <c:v>5.853656677573426E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.5636530091484311E-3</c:v>
+                  <c:v>9.2900565297051587E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.8198800190648858E-3</c:v>
+                  <c:v>1.3856788240271701E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.4262470481070413E-3</c:v>
+                  <c:v>1.9710355922915369E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.4218920962914039E-3</c:v>
+                  <c:v>2.700446163192427E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.843704293543025E-3</c:v>
+                  <c:v>3.5889284688606191E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.2725844494549809E-2</c:v>
+                  <c:v>4.651068898377464E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.6099241101609572E-2</c:v>
+                  <c:v>5.9009364077483913E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.9991071085629669E-2</c:v>
+                  <c:v>7.3519907089534368E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.4424237610961935E-2</c:v>
+                  <c:v>9.0169853605967954E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.9416856990439513E-2</c:v>
+                  <c:v>1.0907866709614121E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.4981768830348287E-2</c:v>
+                  <c:v>1.303566976172048E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.1126084095391591E-2</c:v>
+                  <c:v>1.5410412185000931E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.7850786355034675E-2</c:v>
+                  <c:v>1.8040987773186055E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.5150401592329062E-2</c:v>
+                  <c:v>2.0935060809395944E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>6.3012751599265338E-2</c:v>
+                  <c:v>2.4098962873959361E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.1418805095598475E-2</c:v>
+                  <c:v>2.7537593727665208E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>8.0342639254068787E-2</c:v>
+                  <c:v>3.1254327970773217E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8.9751522277932802E-2</c:v>
+                  <c:v>3.5250929224621363E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9.9606125065372003E-2</c:v>
+                  <c:v>3.9527473603179493E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.10986086684613371</c:v>
+                  <c:v>4.4082284233117663E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.12046439605497444</c:v>
+                  <c:v>4.8911878539958133E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.13136020371072249</c:v>
+                  <c:v>5.4010929942227434E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.14248736232479842</c:v>
+                  <c:v>5.9372245483401073E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.15378137902058026</c:v>
+                  <c:v>6.4986760781754541E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.16517514727773613</c:v>
+                  <c:v>7.0843553490771954E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.17659997771015737</c:v>
+                  <c:v>7.6929876238228126E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.18798668473414495</c:v>
+                  <c:v>8.3231209752196347E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.19926670307190242</c:v>
+                  <c:v>8.973133658987105E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.21037320593524328</c:v>
+                  <c:v>9.641243556416082E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.22124219558999517</c:v>
+                  <c:v>0.10325519661854952</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.23181353691984963</c:v>
+                  <c:v>0.11023895553883063</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.24203190564996585</c:v>
+                  <c:v>0.11734184751806659</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.25184762506281139</c:v>
+                  <c:v>0.12454097821643233</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.26121736829143588</c:v>
+                  <c:v>0.13181261058906879</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4266,8 +4266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3D2DEE-686E-48A0-AC3D-0F54DEA5D0EC}">
   <dimension ref="A1:C121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C56" sqref="B56:C56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4319,7 +4319,7 @@
         <v>38</v>
       </c>
       <c r="B12">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -4351,7 +4351,7 @@
         <v>40</v>
       </c>
       <c r="B16">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -4366,7 +4366,7 @@
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21">
         <f t="shared" ref="B21:B84" si="0">(1-EXP(-((C21/$B$16-($B$15-0.5))/$B$13)^$B$14))*$B$12</f>
-        <v>7.5016342843348124E-6</v>
+        <v>2.7126613468153591E-6</v>
       </c>
       <c r="C21">
         <f>C20+0.25</f>
@@ -4376,7 +4376,7 @@
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>6.0008572506203833E-5</v>
+        <v>2.1700603990693067E-5</v>
       </c>
       <c r="C22">
         <f t="shared" ref="C22:C85" si="1">C21+0.25</f>
@@ -4386,7 +4386,7 @@
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>2.024877004541181E-4</v>
+        <v>7.3233247530835044E-5</v>
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
@@ -4396,7 +4396,7 @@
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>4.7978059651185284E-4</v>
+        <v>1.7356088610352981E-4</v>
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
@@ -4406,7 +4406,7 @@
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>9.3645930124346957E-4</v>
+        <v>3.3889264340773994E-4</v>
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
@@ -4416,7 +4416,7 @@
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>1.6166252946983649E-3</v>
+        <v>5.853656677573426E-4</v>
       </c>
       <c r="C26">
         <f t="shared" si="1"/>
@@ -4426,7 +4426,7 @@
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>2.5636530091484311E-3</v>
+        <v>9.2900565297051587E-4</v>
       </c>
       <c r="C27">
         <f t="shared" si="1"/>
@@ -4436,7 +4436,7 @@
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>3.8198800190648858E-3</v>
+        <v>1.3856788240271701E-3</v>
       </c>
       <c r="C28">
         <f t="shared" si="1"/>
@@ -4446,7 +4446,7 @@
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>5.4262470481070413E-3</v>
+        <v>1.9710355922915369E-3</v>
       </c>
       <c r="C29">
         <f t="shared" si="1"/>
@@ -4456,7 +4456,7 @@
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>7.4218920962914039E-3</v>
+        <v>2.700446163192427E-3</v>
       </c>
       <c r="C30">
         <f t="shared" si="1"/>
@@ -4466,7 +4466,7 @@
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>9.843704293543025E-3</v>
+        <v>3.5889284688606191E-3</v>
       </c>
       <c r="C31">
         <f t="shared" si="1"/>
@@ -4476,7 +4476,7 @@
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>1.2725844494549809E-2</v>
+        <v>4.651068898377464E-3</v>
       </c>
       <c r="C32">
         <f t="shared" si="1"/>
@@ -4486,7 +4486,7 @@
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33">
         <f t="shared" si="0"/>
-        <v>1.6099241101609572E-2</v>
+        <v>5.9009364077483913E-3</v>
       </c>
       <c r="C33">
         <f t="shared" si="1"/>
@@ -4496,7 +4496,7 @@
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34">
         <f t="shared" si="0"/>
-        <v>1.9991071085629669E-2</v>
+        <v>7.3519907089534368E-3</v>
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
@@ -4506,7 +4506,7 @@
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35">
         <f t="shared" si="0"/>
-        <v>2.4424237610961935E-2</v>
+        <v>9.0169853605967954E-3</v>
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
@@ -4516,7 +4516,7 @@
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36">
         <f t="shared" si="0"/>
-        <v>2.9416856990439513E-2</v>
+        <v>1.0907866709614121E-2</v>
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
@@ -4526,7 +4526,7 @@
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37">
         <f t="shared" si="0"/>
-        <v>3.4981768830348287E-2</v>
+        <v>1.303566976172048E-2</v>
       </c>
       <c r="C37">
         <f t="shared" si="1"/>
@@ -4536,7 +4536,7 @@
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38">
         <f t="shared" si="0"/>
-        <v>4.1126084095391591E-2</v>
+        <v>1.5410412185000931E-2</v>
       </c>
       <c r="C38">
         <f t="shared" si="1"/>
@@ -4546,7 +4546,7 @@
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39">
         <f t="shared" si="0"/>
-        <v>4.7850786355034675E-2</v>
+        <v>1.8040987773186055E-2</v>
       </c>
       <c r="C39">
         <f t="shared" si="1"/>
@@ -4556,7 +4556,7 @@
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40">
         <f t="shared" si="0"/>
-        <v>5.5150401592329062E-2</v>
+        <v>2.0935060809395944E-2</v>
       </c>
       <c r="C40">
         <f t="shared" si="1"/>
@@ -4566,7 +4566,7 @@
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41">
         <f t="shared" si="0"/>
-        <v>6.3012751599265338E-2</v>
+        <v>2.4098962873959361E-2</v>
       </c>
       <c r="C41">
         <f t="shared" si="1"/>
@@ -4576,7 +4576,7 @@
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42">
         <f t="shared" si="0"/>
-        <v>7.1418805095598475E-2</v>
+        <v>2.7537593727665208E-2</v>
       </c>
       <c r="C42">
         <f t="shared" si="1"/>
@@ -4586,7 +4586,7 @@
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43">
         <f t="shared" si="0"/>
-        <v>8.0342639254068787E-2</v>
+        <v>3.1254327970773217E-2</v>
       </c>
       <c r="C43">
         <f t="shared" si="1"/>
@@ -4596,7 +4596,7 @@
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44">
         <f t="shared" si="0"/>
-        <v>8.9751522277932802E-2</v>
+        <v>3.5250929224621363E-2</v>
       </c>
       <c r="C44">
         <f t="shared" si="1"/>
@@ -4606,7 +4606,7 @@
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45">
         <f t="shared" si="0"/>
-        <v>9.9606125065372003E-2</v>
+        <v>3.9527473603179493E-2</v>
       </c>
       <c r="C45">
         <f t="shared" si="1"/>
@@ -4616,7 +4616,7 @@
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46">
         <f t="shared" si="0"/>
-        <v>0.10986086684613371</v>
+        <v>4.4082284233117663E-2</v>
       </c>
       <c r="C46">
         <f t="shared" si="1"/>
@@ -4626,7 +4626,7 @@
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47">
         <f t="shared" si="0"/>
-        <v>0.12046439605497444</v>
+        <v>4.8911878539958133E-2</v>
       </c>
       <c r="C47">
         <f t="shared" si="1"/>
@@ -4636,7 +4636,7 @@
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48">
         <f t="shared" si="0"/>
-        <v>0.13136020371072249</v>
+        <v>5.4010929942227434E-2</v>
       </c>
       <c r="C48">
         <f t="shared" si="1"/>
@@ -4646,7 +4646,7 @@
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49">
         <f t="shared" si="0"/>
-        <v>0.14248736232479842</v>
+        <v>5.9372245483401073E-2</v>
       </c>
       <c r="C49">
         <f t="shared" si="1"/>
@@ -4656,7 +4656,7 @@
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50">
         <f t="shared" si="0"/>
-        <v>0.15378137902058026</v>
+        <v>6.4986760781754541E-2</v>
       </c>
       <c r="C50">
         <f t="shared" si="1"/>
@@ -4666,7 +4666,7 @@
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51">
         <f t="shared" si="0"/>
-        <v>0.16517514727773613</v>
+        <v>7.0843553490771954E-2</v>
       </c>
       <c r="C51">
         <f t="shared" si="1"/>
@@ -4676,7 +4676,7 @@
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52">
         <f t="shared" si="0"/>
-        <v>0.17659997771015737</v>
+        <v>7.6929876238228126E-2</v>
       </c>
       <c r="C52">
         <f t="shared" si="1"/>
@@ -4686,7 +4686,7 @@
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53">
         <f t="shared" si="0"/>
-        <v>0.18798668473414495</v>
+        <v>8.3231209752196347E-2</v>
       </c>
       <c r="C53">
         <f t="shared" si="1"/>
@@ -4696,7 +4696,7 @@
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54">
         <f t="shared" si="0"/>
-        <v>0.19926670307190242</v>
+        <v>8.973133658987105E-2</v>
       </c>
       <c r="C54">
         <f t="shared" si="1"/>
@@ -4706,7 +4706,7 @@
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55">
         <f t="shared" si="0"/>
-        <v>0.21037320593524328</v>
+        <v>9.641243556416082E-2</v>
       </c>
       <c r="C55">
         <f t="shared" si="1"/>
@@ -4716,7 +4716,7 @@
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56">
         <f t="shared" si="0"/>
-        <v>0.22124219558999517</v>
+        <v>0.10325519661854952</v>
       </c>
       <c r="C56">
         <f t="shared" si="1"/>
@@ -4726,7 +4726,7 @@
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57">
         <f t="shared" si="0"/>
-        <v>0.23181353691984963</v>
+        <v>0.11023895553883063</v>
       </c>
       <c r="C57">
         <f t="shared" si="1"/>
@@ -4736,7 +4736,7 @@
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58">
         <f t="shared" si="0"/>
-        <v>0.24203190564996585</v>
+        <v>0.11734184751806659</v>
       </c>
       <c r="C58">
         <f t="shared" si="1"/>
@@ -4746,7 +4746,7 @@
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59">
         <f t="shared" si="0"/>
-        <v>0.25184762506281139</v>
+        <v>0.12454097821643233</v>
       </c>
       <c r="C59">
         <f t="shared" si="1"/>
@@ -4756,7 +4756,7 @@
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60">
         <f t="shared" si="0"/>
-        <v>0.26121736829143588</v>
+        <v>0.13181261058906879</v>
       </c>
       <c r="C60">
         <f t="shared" si="1"/>
@@ -4766,7 +4766,7 @@
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61">
         <f t="shared" si="0"/>
-        <v>0.27010470750054377</v>
+        <v>0.13913236540178756</v>
       </c>
       <c r="C61">
         <f t="shared" si="1"/>
@@ -4776,7 +4776,7 @@
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62">
         <f t="shared" si="0"/>
-        <v>0.27848049630021543</v>
+        <v>0.14647543302575003</v>
       </c>
       <c r="C62">
         <f t="shared" si="1"/>
@@ -4786,7 +4786,7 @@
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63">
         <f t="shared" si="0"/>
-        <v>0.28632307736964208</v>
+        <v>0.15381679380738991</v>
       </c>
       <c r="C63">
         <f t="shared" si="1"/>
@@ -4796,7 +4796,7 @@
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64">
         <f t="shared" si="0"/>
-        <v>0.29361831324963961</v>
+        <v>0.16113144405783855</v>
       </c>
       <c r="C64">
         <f t="shared" si="1"/>
@@ -4806,7 +4806,7 @@
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65">
         <f t="shared" si="0"/>
-        <v>0.30035944431943007</v>
+        <v>0.16839462450529405</v>
       </c>
       <c r="C65">
         <f t="shared" si="1"/>
@@ -4816,7 +4816,7 @@
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66">
         <f t="shared" si="0"/>
-        <v>0.30654678382278544</v>
+        <v>0.17558204791159163</v>
       </c>
       <c r="C66">
         <f t="shared" si="1"/>
@@ -4826,7 +4826,7 @@
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67">
         <f t="shared" si="0"/>
-        <v>0.31218726517655226</v>
+        <v>0.18267012247688577</v>
       </c>
       <c r="C67">
         <f t="shared" si="1"/>
@@ -4836,7 +4836,7 @@
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68">
         <f t="shared" si="0"/>
-        <v>0.31729386143083116</v>
+        <v>0.18963616764856731</v>
       </c>
       <c r="C68">
         <f t="shared" si="1"/>
@@ -4846,7 +4846,7 @@
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69">
         <f t="shared" si="0"/>
-        <v>0.32188490044468793</v>
+        <v>0.19645861901529907</v>
       </c>
       <c r="C69">
         <f t="shared" si="1"/>
@@ -4856,7 +4856,7 @@
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70">
         <f t="shared" si="0"/>
-        <v>0.32598330193721398</v>
+        <v>0.20311721910542085</v>
       </c>
       <c r="C70">
         <f t="shared" si="1"/>
@@ -4866,7 +4866,7 @@
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71">
         <f t="shared" si="0"/>
-        <v>0.32961576397642717</v>
+        <v>0.20959319111996269</v>
       </c>
       <c r="C71">
         <f t="shared" si="1"/>
@@ -4876,7 +4876,7 @@
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72">
         <f t="shared" si="0"/>
-        <v>0.33281192665098364</v>
+        <v>0.21586939291098117</v>
       </c>
       <c r="C72">
         <f t="shared" si="1"/>
@@ -4886,7 +4886,7 @@
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73">
         <f t="shared" si="0"/>
-        <v>0.33560353967312706</v>
+        <v>0.22193044886066229</v>
       </c>
       <c r="C73">
         <f t="shared" si="1"/>
@@ -4896,7 +4896,7 @@
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74">
         <f t="shared" si="0"/>
-        <v>0.33802365859091688</v>
+        <v>0.2277628577183255</v>
       </c>
       <c r="C74">
         <f t="shared" si="1"/>
@@ -4906,7 +4906,7 @@
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75">
         <f t="shared" si="0"/>
-        <v>0.34010589130406521</v>
+        <v>0.23335507490195029</v>
       </c>
       <c r="C75">
         <f t="shared" si="1"/>
@@ -4916,7 +4916,7 @@
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76">
         <f t="shared" si="0"/>
-        <v>0.34188371288438546</v>
+        <v>0.23869756825732752</v>
       </c>
       <c r="C76">
         <f t="shared" si="1"/>
@@ -4926,7 +4926,7 @@
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77">
         <f t="shared" si="0"/>
-        <v>0.34338986253095471</v>
+        <v>0.24378284677925793</v>
       </c>
       <c r="C77">
         <f t="shared" si="1"/>
@@ -4936,7 +4936,7 @@
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78">
         <f t="shared" si="0"/>
-        <v>0.34465583208577671</v>
+        <v>0.24860546232227976</v>
       </c>
       <c r="C78">
         <f t="shared" si="1"/>
@@ -4946,7 +4946,7 @@
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79">
         <f t="shared" si="0"/>
-        <v>0.34571145113798446</v>
+        <v>0.25316198484953234</v>
       </c>
       <c r="C79">
         <f t="shared" si="1"/>
@@ -4956,7 +4956,7 @@
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80">
         <f t="shared" si="0"/>
-        <v>0.34658456957417372</v>
+        <v>0.25745095227379722</v>
       </c>
       <c r="C80">
         <f t="shared" si="1"/>
@@ -4966,7 +4966,7 @@
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81">
         <f t="shared" si="0"/>
-        <v>0.34730083467801665</v>
+        <v>0.26147279642109311</v>
       </c>
       <c r="C81">
         <f t="shared" si="1"/>
@@ -4976,7 +4976,7 @@
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82">
         <f t="shared" si="0"/>
-        <v>0.34788355669100007</v>
+        <v>0.26522974708186364</v>
       </c>
       <c r="C82">
         <f t="shared" si="1"/>
@@ -4986,7 +4986,7 @@
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83">
         <f t="shared" si="0"/>
-        <v>0.34835365421771686</v>
+        <v>0.26872571649646854</v>
       </c>
       <c r="C83">
         <f t="shared" si="1"/>
@@ -4996,7 +4996,7 @@
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84">
         <f t="shared" si="0"/>
-        <v>0.34872966904405506</v>
+        <v>0.27196616694071241</v>
       </c>
       <c r="C84">
         <f t="shared" si="1"/>
@@ -5006,7 +5006,7 @@
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85">
         <f t="shared" ref="B85:B121" si="2">(1-EXP(-((C85/$B$16-($B$15-0.5))/$B$13)^$B$14))*$B$12</f>
-        <v>0.34902783883791444</v>
+        <v>0.27495796432585551</v>
       </c>
       <c r="C85">
         <f t="shared" si="1"/>
@@ -5016,7 +5016,7 @@
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86">
         <f t="shared" si="2"/>
-        <v>0.3492622157804392</v>
+        <v>0.27770922090054417</v>
       </c>
       <c r="C86">
         <f t="shared" ref="C86:C121" si="3">C85+0.25</f>
@@ -5026,7 +5026,7 @@
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87">
         <f t="shared" si="2"/>
-        <v>0.34944481935725885</v>
+        <v>0.28022913023639223</v>
       </c>
       <c r="C87">
         <f t="shared" si="3"/>
@@ -5036,7 +5036,7 @@
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88">
         <f t="shared" si="2"/>
-        <v>0.3495858122245698</v>
+        <v>0.28252779769408043</v>
       </c>
       <c r="C88">
         <f t="shared" si="3"/>
@@ -5046,7 +5046,7 @@
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89">
         <f t="shared" si="2"/>
-        <v>0.34969368913943127</v>
+        <v>0.2846160695048362</v>
       </c>
       <c r="C89">
         <f t="shared" si="3"/>
@@ -5056,7 +5056,7 @@
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90">
         <f t="shared" si="2"/>
-        <v>0.34977547028721101</v>
+        <v>0.28650536346742178</v>
       </c>
       <c r="C90">
         <f t="shared" si="3"/>
@@ -5066,7 +5066,7 @@
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91">
         <f t="shared" si="2"/>
-        <v>0.3498368918348444</v>
+        <v>0.28820750405985879</v>
       </c>
       <c r="C91">
         <f t="shared" si="3"/>
@@ -5076,7 +5076,7 @@
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92">
         <f t="shared" si="2"/>
-        <v>0.34988258808023409</v>
+        <v>0.2897345645065002</v>
       </c>
       <c r="C92">
         <f t="shared" si="3"/>
@@ -5086,7 +5086,7 @@
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93">
         <f t="shared" si="2"/>
-        <v>0.34991626106546403</v>
+        <v>0.29109871803469367</v>
       </c>
       <c r="C93">
         <f t="shared" si="3"/>
@@ -5096,7 +5096,7 @@
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94">
         <f t="shared" si="2"/>
-        <v>0.34994083490357991</v>
+        <v>0.29231210021223275</v>
       </c>
       <c r="C94">
         <f t="shared" si="3"/>
@@ -5106,7 +5106,7 @@
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95">
         <f t="shared" si="2"/>
-        <v>0.34995859328510975</v>
+        <v>0.29338668388880529</v>
       </c>
       <c r="C95">
         <f t="shared" si="3"/>
@@ -5116,7 +5116,7 @@
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96">
         <f t="shared" si="2"/>
-        <v>0.34997129965097196</v>
+        <v>0.29433416788367545</v>
       </c>
       <c r="C96">
         <f t="shared" si="3"/>
@@ -5126,7 +5126,7 @@
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97">
         <f t="shared" si="2"/>
-        <v>0.34998030033082916</v>
+        <v>0.29516588017958978</v>
       </c>
       <c r="C97">
         <f t="shared" si="3"/>
@@ -5136,7 +5136,7 @@
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98">
         <f t="shared" si="2"/>
-        <v>0.34998661155345162</v>
+        <v>0.29589269601045221</v>
       </c>
       <c r="C98">
         <f t="shared" si="3"/>
@@ -5146,7 +5146,7 @@
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99">
         <f t="shared" si="2"/>
-        <v>0.34999099165321684</v>
+        <v>0.29652497087771895</v>
       </c>
       <c r="C99">
         <f t="shared" si="3"/>
@@ -5156,7 +5156,7 @@
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100">
         <f t="shared" si="2"/>
-        <v>0.34999400004761355</v>
+        <v>0.29707248820643462</v>
       </c>
       <c r="C100">
         <f t="shared" si="3"/>
@@ -5166,7 +5166,7 @@
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101">
         <f t="shared" si="2"/>
-        <v>0.34999604467238488</v>
+        <v>0.2975444210635308</v>
       </c>
       <c r="C101">
         <f t="shared" si="3"/>
@@ -5176,7 +5176,7 @@
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102">
         <f t="shared" si="2"/>
-        <v>0.34999741956325225</v>
+        <v>0.29794930711385315</v>
       </c>
       <c r="C102">
         <f t="shared" si="3"/>
@@ -5186,7 +5186,7 @@
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103">
         <f t="shared" si="2"/>
-        <v>0.34999833419476295</v>
+        <v>0.29829503578700706</v>
       </c>
       <c r="C103">
         <f t="shared" si="3"/>
@@ -5196,7 +5196,7 @@
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104">
         <f t="shared" si="2"/>
-        <v>0.34999893605390209</v>
+        <v>0.29858884647232875</v>
       </c>
       <c r="C104">
         <f t="shared" si="3"/>
@@ -5206,7 +5206,7 @@
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105">
         <f t="shared" si="2"/>
-        <v>0.34999932776119835</v>
+        <v>0.29883733645020727</v>
       </c>
       <c r="C105">
         <f t="shared" si="3"/>
@@ -5216,7 +5216,7 @@
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106">
         <f t="shared" si="2"/>
-        <v>0.34999957987335761</v>
+        <v>0.29904647720411548</v>
       </c>
       <c r="C106">
         <f t="shared" si="3"/>
@@ -5226,7 +5226,7 @@
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107">
         <f t="shared" si="2"/>
-        <v>0.34999974032286191</v>
+        <v>0.29922163773619626</v>
       </c>
       <c r="C107">
         <f t="shared" si="3"/>
@@ -5236,7 +5236,7 @@
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108">
         <f t="shared" si="2"/>
-        <v>0.34999984128126099</v>
+        <v>0.29936761352609076</v>
       </c>
       <c r="C108">
         <f t="shared" si="3"/>
@@ -5246,7 +5246,7 @@
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109">
         <f t="shared" si="2"/>
-        <v>0.3499999040802943</v>
+        <v>0.29948865982299966</v>
       </c>
       <c r="C109">
         <f t="shared" si="3"/>
@@ -5256,7 +5256,7 @@
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110">
         <f t="shared" si="2"/>
-        <v>0.3499999426918004</v>
+        <v>0.29958852803926317</v>
       </c>
       <c r="C110">
         <f t="shared" si="3"/>
@@ -5266,7 +5266,7 @@
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111">
         <f t="shared" si="2"/>
-        <v>0.34999996615464019</v>
+        <v>0.29967050411421003</v>
       </c>
       <c r="C111">
         <f t="shared" si="3"/>
@@ -5276,7 +5276,7 @@
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112">
         <f t="shared" si="2"/>
-        <v>0.34999998024399626</v>
+        <v>0.29973744783379824</v>
       </c>
       <c r="C112">
         <f t="shared" si="3"/>
@@ -5286,7 +5286,7 @@
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113">
         <f t="shared" si="2"/>
-        <v>0.34999998860378051</v>
+        <v>0.29979183221893801</v>
       </c>
       <c r="C113">
         <f t="shared" si="3"/>
@@ -5296,7 +5296,7 @@
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114">
         <f t="shared" si="2"/>
-        <v>0.34999999350426342</v>
+        <v>0.29983578222801444</v>
       </c>
       <c r="C114">
         <f t="shared" si="3"/>
@@ -5306,7 +5306,7 @@
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115">
         <f t="shared" si="2"/>
-        <v>0.34999999634198026</v>
+        <v>0.29987111215221296</v>
       </c>
       <c r="C115">
         <f t="shared" si="3"/>
@@ -5316,7 +5316,7 @@
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116">
         <f t="shared" si="2"/>
-        <v>0.34999999796503062</v>
+        <v>0.29989936121162925</v>
       </c>
       <c r="C116">
         <f t="shared" si="3"/>
@@ -5326,7 +5326,7 @@
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117">
         <f t="shared" si="2"/>
-        <v>0.34999999888182948</v>
+        <v>0.29992182698238479</v>
       </c>
       <c r="C117">
         <f t="shared" si="3"/>
@@ -5336,7 +5336,7 @@
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118">
         <f t="shared" si="2"/>
-        <v>0.34999999939320681</v>
+        <v>0.29993959639739087</v>
       </c>
       <c r="C118">
         <f t="shared" si="3"/>
@@ -5346,7 +5346,7 @@
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119">
         <f t="shared" si="2"/>
-        <v>0.3499999996748378</v>
+        <v>0.29995357416407437</v>
       </c>
       <c r="C119">
         <f t="shared" si="3"/>
@@ -5356,7 +5356,7 @@
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120">
         <f t="shared" si="2"/>
-        <v>0.34999999982795971</v>
+        <v>0.2999645085300941</v>
       </c>
       <c r="C120">
         <f t="shared" si="3"/>
@@ -5366,7 +5366,7 @@
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121">
         <f t="shared" si="2"/>
-        <v>0.34999999991013819</v>
+        <v>0.29997301440226942</v>
       </c>
       <c r="C121">
         <f t="shared" si="3"/>
@@ -5384,10 +5384,10 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:BK2"/>
+  <dimension ref="A1:CE2"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:BK2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5396,7 +5396,7 @@
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -5406,250 +5406,330 @@
       </c>
       <c r="C1">
         <f>(1-EXP(-((C2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>7.5016342843348124E-6</v>
+        <v>2.7126613468153591E-6</v>
       </c>
       <c r="D1">
         <f>(1-EXP(-((D2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>6.0008572506203833E-5</v>
+        <v>2.1700603990693067E-5</v>
       </c>
       <c r="E1">
         <f>(1-EXP(-((E2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>2.024877004541181E-4</v>
+        <v>7.3233247530835044E-5</v>
       </c>
       <c r="F1">
         <f>(1-EXP(-((F2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>4.7978059651185284E-4</v>
+        <v>1.7356088610352981E-4</v>
       </c>
       <c r="G1">
         <f>(1-EXP(-((G2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>9.3645930124346957E-4</v>
+        <v>3.3889264340773994E-4</v>
       </c>
       <c r="H1">
         <f>(1-EXP(-((H2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>1.6166252946983649E-3</v>
+        <v>5.853656677573426E-4</v>
       </c>
       <c r="I1">
         <f>(1-EXP(-((I2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>2.5636530091484311E-3</v>
+        <v>9.2900565297051587E-4</v>
       </c>
       <c r="J1">
         <f>(1-EXP(-((J2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>3.8198800190648858E-3</v>
+        <v>1.3856788240271701E-3</v>
       </c>
       <c r="K1">
         <f>(1-EXP(-((K2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>5.4262470481070413E-3</v>
+        <v>1.9710355922915369E-3</v>
       </c>
       <c r="L1">
         <f>(1-EXP(-((L2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>7.4218920962914039E-3</v>
+        <v>2.700446163192427E-3</v>
       </c>
       <c r="M1">
         <f>(1-EXP(-((M2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>9.843704293543025E-3</v>
+        <v>3.5889284688606191E-3</v>
       </c>
       <c r="N1">
         <f>(1-EXP(-((N2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>1.2725844494549809E-2</v>
+        <v>4.651068898377464E-3</v>
       </c>
       <c r="O1">
         <f>(1-EXP(-((O2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>1.6099241101609572E-2</v>
+        <v>5.9009364077483913E-3</v>
       </c>
       <c r="P1">
         <f>(1-EXP(-((P2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>1.9991071085629669E-2</v>
+        <v>7.3519907089534368E-3</v>
       </c>
       <c r="Q1">
         <f>(1-EXP(-((Q2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>2.4424237610961935E-2</v>
+        <v>9.0169853605967954E-3</v>
       </c>
       <c r="R1">
         <f>(1-EXP(-((R2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>2.9416856990439513E-2</v>
+        <v>1.0907866709614121E-2</v>
       </c>
       <c r="S1">
         <f>(1-EXP(-((S2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>3.4981768830348287E-2</v>
+        <v>1.303566976172048E-2</v>
       </c>
       <c r="T1">
         <f>(1-EXP(-((T2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>4.1126084095391591E-2</v>
+        <v>1.5410412185000931E-2</v>
       </c>
       <c r="U1">
         <f>(1-EXP(-((U2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>4.7850786355034675E-2</v>
+        <v>1.8040987773186055E-2</v>
       </c>
       <c r="V1">
         <f>(1-EXP(-((V2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>5.5150401592329062E-2</v>
+        <v>2.0935060809395944E-2</v>
       </c>
       <c r="W1">
         <f>(1-EXP(-((W2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>6.3012751599265338E-2</v>
+        <v>2.4098962873959361E-2</v>
       </c>
       <c r="X1">
         <f>(1-EXP(-((X2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>7.1418805095598475E-2</v>
+        <v>2.7537593727665208E-2</v>
       </c>
       <c r="Y1">
         <f>(1-EXP(-((Y2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>8.0342639254068787E-2</v>
+        <v>3.1254327970773217E-2</v>
       </c>
       <c r="Z1">
         <f>(1-EXP(-((Z2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>8.9751522277932802E-2</v>
+        <v>3.5250929224621363E-2</v>
       </c>
       <c r="AA1">
         <f>(1-EXP(-((AA2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>9.9606125065372003E-2</v>
+        <v>3.9527473603179493E-2</v>
       </c>
       <c r="AB1">
         <f>(1-EXP(-((AB2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.10986086684613371</v>
+        <v>4.4082284233117663E-2</v>
       </c>
       <c r="AC1">
         <f>(1-EXP(-((AC2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.12046439605497444</v>
+        <v>4.8911878539958133E-2</v>
       </c>
       <c r="AD1">
         <f>(1-EXP(-((AD2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.13136020371072249</v>
+        <v>5.4010929942227434E-2</v>
       </c>
       <c r="AE1">
         <f>(1-EXP(-((AE2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.14248736232479842</v>
+        <v>5.9372245483401073E-2</v>
       </c>
       <c r="AF1">
         <f>(1-EXP(-((AF2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.15378137902058026</v>
+        <v>6.4986760781754541E-2</v>
       </c>
       <c r="AG1">
         <f>(1-EXP(-((AG2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.16517514727773613</v>
+        <v>7.0843553490771954E-2</v>
       </c>
       <c r="AH1">
         <f>(1-EXP(-((AH2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.17659997771015737</v>
+        <v>7.6929876238228126E-2</v>
       </c>
       <c r="AI1">
         <f>(1-EXP(-((AI2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.18798668473414495</v>
+        <v>8.3231209752196347E-2</v>
       </c>
       <c r="AJ1">
         <f>(1-EXP(-((AJ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.19926670307190242</v>
+        <v>8.973133658987105E-2</v>
       </c>
       <c r="AK1">
         <f>(1-EXP(-((AK2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.21037320593524328</v>
+        <v>9.641243556416082E-2</v>
       </c>
       <c r="AL1">
         <f>(1-EXP(-((AL2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.22124219558999517</v>
+        <v>0.10325519661854952</v>
       </c>
       <c r="AM1">
         <f>(1-EXP(-((AM2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.23181353691984963</v>
+        <v>0.11023895553883063</v>
       </c>
       <c r="AN1">
         <f>(1-EXP(-((AN2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.24203190564996585</v>
+        <v>0.11734184751806659</v>
       </c>
       <c r="AO1">
         <f>(1-EXP(-((AO2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.25184762506281139</v>
+        <v>0.12454097821643233</v>
       </c>
       <c r="AP1">
         <f>(1-EXP(-((AP2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.26121736829143588</v>
+        <v>0.13181261058906879</v>
       </c>
       <c r="AQ1">
         <f>(1-EXP(-((AQ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.27010470750054377</v>
+        <v>0.13913236540178756</v>
       </c>
       <c r="AR1">
         <f>(1-EXP(-((AR2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.27848049630021543</v>
+        <v>0.14647543302575003</v>
       </c>
       <c r="AS1">
         <f>(1-EXP(-((AS2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.28632307736964208</v>
+        <v>0.15381679380738991</v>
       </c>
       <c r="AT1">
         <f>(1-EXP(-((AT2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.29361831324963961</v>
+        <v>0.16113144405783855</v>
       </c>
       <c r="AU1">
         <f>(1-EXP(-((AU2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.30035944431943007</v>
+        <v>0.16839462450529405</v>
       </c>
       <c r="AV1">
         <f>(1-EXP(-((AV2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.30654678382278544</v>
+        <v>0.17558204791159163</v>
       </c>
       <c r="AW1">
         <f>(1-EXP(-((AW2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.31218726517655226</v>
+        <v>0.18267012247688577</v>
       </c>
       <c r="AX1">
         <f>(1-EXP(-((AX2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.31729386143083116</v>
+        <v>0.18963616764856731</v>
       </c>
       <c r="AY1">
         <f>(1-EXP(-((AY2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.32188490044468793</v>
+        <v>0.19645861901529907</v>
       </c>
       <c r="AZ1">
         <f>(1-EXP(-((AZ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.32598330193721398</v>
+        <v>0.20311721910542085</v>
       </c>
       <c r="BA1">
         <f>(1-EXP(-((BA2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.32961576397642717</v>
+        <v>0.20959319111996269</v>
       </c>
       <c r="BB1">
         <f>(1-EXP(-((BB2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.33281192665098364</v>
+        <v>0.21586939291098117</v>
       </c>
       <c r="BC1">
         <f>(1-EXP(-((BC2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.33560353967312706</v>
+        <v>0.22193044886066229</v>
       </c>
       <c r="BD1">
         <f>(1-EXP(-((BD2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.33802365859091688</v>
+        <v>0.2277628577183255</v>
       </c>
       <c r="BE1">
         <f>(1-EXP(-((BE2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.34010589130406521</v>
+        <v>0.23335507490195029</v>
       </c>
       <c r="BF1">
         <f>(1-EXP(-((BF2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.34188371288438546</v>
+        <v>0.23869756825732752</v>
       </c>
       <c r="BG1">
         <f>(1-EXP(-((BG2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.34338986253095471</v>
+        <v>0.24378284677925793</v>
       </c>
       <c r="BH1">
         <f>(1-EXP(-((BH2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.34465583208577671</v>
+        <v>0.24860546232227976</v>
       </c>
       <c r="BI1">
         <f>(1-EXP(-((BI2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.34571145113798446</v>
+        <v>0.25316198484953234</v>
       </c>
       <c r="BJ1">
         <f>(1-EXP(-((BJ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.34658456957417372</v>
+        <v>0.25745095227379722</v>
       </c>
       <c r="BK1">
         <f>(1-EXP(-((BK2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
+        <v>0.26147279642109311</v>
+      </c>
+      <c r="BL1">
+        <f>(1-EXP(-((BL2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.26522974708186364</v>
+      </c>
+      <c r="BM1">
+        <f>(1-EXP(-((BM2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.26872571649646854</v>
+      </c>
+      <c r="BN1">
+        <f>(1-EXP(-((BN2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.27196616694071241</v>
+      </c>
+      <c r="BO1">
+        <f>(1-EXP(-((BO2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.27495796432585551</v>
+      </c>
+      <c r="BP1">
+        <f>(1-EXP(-((BP2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.27770922090054417</v>
+      </c>
+      <c r="BQ1">
+        <f>(1-EXP(-((BQ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.28022913023639223</v>
+      </c>
+      <c r="BR1">
+        <f>(1-EXP(-((BR2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.28252779769408043</v>
+      </c>
+      <c r="BS1">
+        <f>(1-EXP(-((BS2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.2846160695048362</v>
+      </c>
+      <c r="BT1">
+        <f>(1-EXP(-((BT2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.28650536346742178</v>
+      </c>
+      <c r="BU1">
+        <f>(1-EXP(-((BU2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.28820750405985879</v>
+      </c>
+      <c r="BV1">
+        <f>(1-EXP(-((BV2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.2897345645065002</v>
+      </c>
+      <c r="BW1">
+        <f>(1-EXP(-((BW2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.29109871803469367</v>
+      </c>
+      <c r="BX1">
+        <f>(1-EXP(-((BX2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.29231210021223275</v>
+      </c>
+      <c r="BY1">
+        <f>(1-EXP(-((BY2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.29338668388880529</v>
+      </c>
+      <c r="BZ1">
+        <f>(1-EXP(-((BZ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.29433416788367545</v>
+      </c>
+      <c r="CA1">
+        <f>(1-EXP(-((CA2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.29516588017958978</v>
+      </c>
+      <c r="CB1">
+        <f>(1-EXP(-((CB2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.29589269601045221</v>
+      </c>
+      <c r="CC1">
+        <f>(1-EXP(-((CC2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.29652497087771895</v>
+      </c>
+      <c r="CD1">
+        <f>(1-EXP(-((CD2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.29707248820643462</v>
+      </c>
+      <c r="CE1">
+        <f>(1-EXP(-((CE2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -5897,6 +5977,86 @@
         <v>15</v>
       </c>
       <c r="BK2">
+        <f t="shared" ref="BK2" si="3">BJ2+0.25</f>
+        <v>15.25</v>
+      </c>
+      <c r="BL2">
+        <f t="shared" ref="BL2" si="4">BK2+0.25</f>
+        <v>15.5</v>
+      </c>
+      <c r="BM2">
+        <f t="shared" ref="BM2" si="5">BL2+0.25</f>
+        <v>15.75</v>
+      </c>
+      <c r="BN2">
+        <f t="shared" ref="BN2" si="6">BM2+0.25</f>
+        <v>16</v>
+      </c>
+      <c r="BO2">
+        <f t="shared" ref="BO2" si="7">BN2+0.25</f>
+        <v>16.25</v>
+      </c>
+      <c r="BP2">
+        <f t="shared" ref="BP2" si="8">BO2+0.25</f>
+        <v>16.5</v>
+      </c>
+      <c r="BQ2">
+        <f t="shared" ref="BQ2" si="9">BP2+0.25</f>
+        <v>16.75</v>
+      </c>
+      <c r="BR2">
+        <f t="shared" ref="BR2" si="10">BQ2+0.25</f>
+        <v>17</v>
+      </c>
+      <c r="BS2">
+        <f t="shared" ref="BS2" si="11">BR2+0.25</f>
+        <v>17.25</v>
+      </c>
+      <c r="BT2">
+        <f t="shared" ref="BT2" si="12">BS2+0.25</f>
+        <v>17.5</v>
+      </c>
+      <c r="BU2">
+        <f t="shared" ref="BU2" si="13">BT2+0.25</f>
+        <v>17.75</v>
+      </c>
+      <c r="BV2">
+        <f t="shared" ref="BV2" si="14">BU2+0.25</f>
+        <v>18</v>
+      </c>
+      <c r="BW2">
+        <f t="shared" ref="BW2" si="15">BV2+0.25</f>
+        <v>18.25</v>
+      </c>
+      <c r="BX2">
+        <f t="shared" ref="BX2" si="16">BW2+0.25</f>
+        <v>18.5</v>
+      </c>
+      <c r="BY2">
+        <f t="shared" ref="BY2" si="17">BX2+0.25</f>
+        <v>18.75</v>
+      </c>
+      <c r="BZ2">
+        <f t="shared" ref="BZ2" si="18">BY2+0.25</f>
+        <v>19</v>
+      </c>
+      <c r="CA2">
+        <f t="shared" ref="CA2" si="19">BZ2+0.25</f>
+        <v>19.25</v>
+      </c>
+      <c r="CB2">
+        <f t="shared" ref="CB2" si="20">CA2+0.25</f>
+        <v>19.5</v>
+      </c>
+      <c r="CC2">
+        <f t="shared" ref="CC2:CE2" si="21">CB2+0.25</f>
+        <v>19.75</v>
+      </c>
+      <c r="CD2">
+        <f t="shared" ref="CD2" si="22">CC2+0.25</f>
+        <v>20</v>
+      </c>
+      <c r="CE2">
         <v>1000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update max cost driven retirements data included in BCRbQ file and update CSC to adjust calibration
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CD896B-2370-44DD-9731-7CCF4C2E9B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55974A76-ACCE-4EEE-8FAE-8F68F7567405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
@@ -609,307 +609,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>2.2605511223461328E-6</c:v>
+                  <c:v>2.9387164590499728E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.808383665891089E-5</c:v>
+                  <c:v>2.3508987656584158E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.102770627569587E-5</c:v>
+                  <c:v>7.9336018158404631E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4463407175294152E-4</c:v>
+                  <c:v>1.8802429327882398E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.8241053617311662E-4</c:v>
+                  <c:v>3.6713369702505162E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.8780472313111889E-4</c:v>
+                  <c:v>6.3414614007045462E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.7417137747542997E-4</c:v>
+                  <c:v>1.006422790718059E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.154732353355975E-3</c:v>
+                  <c:v>1.5011520593627675E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.6425296602429473E-3</c:v>
+                  <c:v>2.1352885583158314E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.2503718026603559E-3</c:v>
+                  <c:v>2.9254833434584626E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.9907737240505161E-3</c:v>
+                  <c:v>3.8880058412656712E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.8758907486478866E-3</c:v>
+                  <c:v>5.0386579732422526E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.9174470064569931E-3</c:v>
+                  <c:v>6.3926811083940913E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.1266589241278646E-3</c:v>
+                  <c:v>7.9646566013662247E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.514154467163997E-3</c:v>
+                  <c:v>9.7684008073131972E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.0898889246784353E-3</c:v>
+                  <c:v>1.1816855602081967E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.0863058134767067E-2</c:v>
+                  <c:v>1.4121975575197189E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.2842010154167444E-2</c:v>
+                  <c:v>1.6694613200417676E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.5034156477655047E-2</c:v>
+                  <c:v>1.9544403420951564E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.7445884007829954E-2</c:v>
+                  <c:v>2.267964921017894E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.0082469061632802E-2</c:v>
+                  <c:v>2.6107209780122643E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.2947994773054342E-2</c:v>
+                  <c:v>2.9832393204970647E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.6045273308977684E-2</c:v>
+                  <c:v>3.3858855301670994E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.9375774353851136E-2</c:v>
+                  <c:v>3.8188506660006477E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.2939561335982914E-2</c:v>
+                  <c:v>4.2821429736777793E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.6735236860931386E-2</c:v>
+                  <c:v>4.7755807919210802E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4.0759898783298443E-2</c:v>
+                  <c:v>5.2987868418287974E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.5009108285189531E-2</c:v>
+                  <c:v>5.8511840770746393E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4.9476871236167563E-2</c:v>
+                  <c:v>6.4319932607017835E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5.4155633984795448E-2</c:v>
+                  <c:v>7.040232418023408E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>5.90362945756433E-2</c:v>
+                  <c:v>7.6747182948336296E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>6.4108230198523436E-2</c:v>
+                  <c:v>8.3340699258080464E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>6.935934146016362E-2</c:v>
+                  <c:v>9.0167143898212704E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>7.4776113824892548E-2</c:v>
+                  <c:v>9.7208947972360321E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8.0343696303467355E-2</c:v>
+                  <c:v>0.10444680519450757</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>8.6045997182124606E-2</c:v>
+                  <c:v>0.11185979633676199</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>9.1865796282358858E-2</c:v>
+                  <c:v>0.11942553516706651</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>9.7784872931722167E-2</c:v>
+                  <c:v>0.12712033481123883</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.10378414851369361</c:v>
+                  <c:v>0.13491939306780171</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.10984384215755733</c:v>
+                  <c:v>0.14279699480482452</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.11594363783482298</c:v>
+                  <c:v>0.15072672918526989</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.1220628608547917</c:v>
+                  <c:v>0.15868171911122922</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.12818066150615826</c:v>
+                  <c:v>0.16663485995800573</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.13427620338153212</c:v>
+                  <c:v>0.17455906439599175</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.1403288537544117</c:v>
+                  <c:v>0.18242750988073522</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.14631837325965968</c:v>
+                  <c:v>0.19021388523755758</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.15222510206407147</c:v>
+                  <c:v>0.19789263268329291</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.15803013970713942</c:v>
+                  <c:v>0.20543918161928124</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.16371551584608257</c:v>
+                  <c:v>0.21283017059990736</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.16926434925451739</c:v>
+                  <c:v>0.22004365403087262</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.17466099259996892</c:v>
+                  <c:v>0.22705929037995962</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.17989116075915099</c:v>
+                  <c:v>0.23385850898689628</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.18494204071721859</c:v>
+                  <c:v>0.24042465293238419</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.18980238143193792</c:v>
+                  <c:v>0.2467430958615193</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.19446256241829191</c:v>
+                  <c:v>0.25280133114377951</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.19891464021443961</c:v>
+                  <c:v>0.2585890322787715</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.2031523723160483</c:v>
+                  <c:v>0.26409808401086282</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.2071712186018998</c:v>
+                  <c:v>0.26932258418246974</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.21096832070794364</c:v>
+                  <c:v>0.27425881692032672</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.21454246022816437</c:v>
+                  <c:v>0.2789051982966137</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.21789399701757761</c:v>
+                  <c:v>0.28326219612285092</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.22102478923488639</c:v>
+                  <c:v>0.2873322260053523</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.22393809708039045</c:v>
+                  <c:v>0.29111952620450759</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.22663847245059368</c:v>
+                  <c:v>0.29463001418577178</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.22913163693821295</c:v>
+                  <c:v>0.29787112801967686</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.23142435075045348</c:v>
+                  <c:v>0.30085165597558955</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.23352427519699354</c:v>
+                  <c:v>0.30358155775609158</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.23543983141173369</c:v>
+                  <c:v>0.30607178083525383</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.23718005792069682</c:v>
+                  <c:v>0.30833407529690587</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.23875446955618485</c:v>
+                  <c:v>0.31038081042304033</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.24017292004988233</c:v>
+                  <c:v>0.31222479606484704</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.2414454704220835</c:v>
+                  <c:v>0.31387911154870857</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.24258226502891142</c:v>
+                  <c:v>0.31535694453758484</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.24359341684352731</c:v>
+                  <c:v>0.31667144189658553</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.24448890324067107</c:v>
+                  <c:v>0.3178355742128724</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.24527847323639623</c:v>
+                  <c:v>0.31886201520731511</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.24597156681632482</c:v>
+                  <c:v>0.31976303686122226</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.24657724667537687</c:v>
+                  <c:v>0.32055042067798994</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.24710414239809914</c:v>
+                  <c:v>0.32123538511752886</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.24756040683869554</c:v>
+                  <c:v>0.32182852889030422</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.24795368421960901</c:v>
+                  <c:v>0.32233978948549169</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.24829108926154431</c:v>
+                  <c:v>0.32277841604000762</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.24857919648917257</c:v>
+                  <c:v>0.32315295543592437</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.24882403872694062</c:v>
+                  <c:v>0.32347125034502283</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.24903111370850606</c:v>
+                  <c:v>0.32374044782105788</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.24920539767009622</c:v>
+                  <c:v>0.32396701697112512</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.24935136478016356</c:v>
+                  <c:v>0.32415677421421263</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.24947301127174229</c:v>
+                  <c:v>0.32431491465326501</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.24957388318583304</c:v>
+                  <c:v>0.32444604814158295</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.24965710669938598</c:v>
+                  <c:v>0.3245542387092018</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.24972542009517504</c:v>
+                  <c:v>0.32464304612372757</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.24978120652816521</c:v>
+                  <c:v>0.32471556848661476</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.24982652684911502</c:v>
+                  <c:v>0.32477448490384953</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.24986315185667871</c:v>
+                  <c:v>0.32482209741368234</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.24989259346017748</c:v>
+                  <c:v>0.32486037149823072</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.24991613434302437</c:v>
+                  <c:v>0.3248909746459317</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.24993485581865399</c:v>
+                  <c:v>0.32491531256425021</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.24994966366449239</c:v>
+                  <c:v>0.32493456276384014</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.24996131180339531</c:v>
+                  <c:v>0.32494970534441392</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.24997042377507842</c:v>
+                  <c:v>0.32496155090760193</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.24997751200189119</c:v>
+                  <c:v>0.32497076560245858</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1327,124 +1327,124 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2605511223461328E-6</c:v>
+                  <c:v>2.9387164590499728E-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.808383665891089E-5</c:v>
+                  <c:v>2.3508987656584158E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.102770627569587E-5</c:v>
+                  <c:v>7.9336018158404631E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4463407175294152E-4</c:v>
+                  <c:v>1.8802429327882398E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.8241053617311662E-4</c:v>
+                  <c:v>3.6713369702505162E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.8780472313111889E-4</c:v>
+                  <c:v>6.3414614007045462E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.7417137747542997E-4</c:v>
+                  <c:v>1.006422790718059E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.154732353355975E-3</c:v>
+                  <c:v>1.5011520593627675E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.6425296602429473E-3</c:v>
+                  <c:v>2.1352885583158314E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.2503718026603559E-3</c:v>
+                  <c:v>2.9254833434584626E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.9907737240505161E-3</c:v>
+                  <c:v>3.8880058412656712E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.8758907486478866E-3</c:v>
+                  <c:v>5.0386579732422526E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.9174470064569931E-3</c:v>
+                  <c:v>6.3926811083940913E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.1266589241278646E-3</c:v>
+                  <c:v>7.9646566013662247E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.514154467163997E-3</c:v>
+                  <c:v>9.7684008073131972E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.0898889246784353E-3</c:v>
+                  <c:v>1.1816855602081967E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.0863058134767067E-2</c:v>
+                  <c:v>1.4121975575197189E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.2842010154167444E-2</c:v>
+                  <c:v>1.6694613200417676E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.5034156477655047E-2</c:v>
+                  <c:v>1.9544403420951564E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.7445884007829954E-2</c:v>
+                  <c:v>2.267964921017894E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.0082469061632802E-2</c:v>
+                  <c:v>2.6107209780122643E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.2947994773054342E-2</c:v>
+                  <c:v>2.9832393204970647E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.6045273308977684E-2</c:v>
+                  <c:v>3.3858855301670994E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.9375774353851136E-2</c:v>
+                  <c:v>3.8188506660006477E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.2939561335982914E-2</c:v>
+                  <c:v>4.2821429736777793E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.6735236860931386E-2</c:v>
+                  <c:v>4.7755807919210802E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.0759898783298443E-2</c:v>
+                  <c:v>5.2987868418287974E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4.5009108285189531E-2</c:v>
+                  <c:v>5.8511840770746393E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4.9476871236167563E-2</c:v>
+                  <c:v>6.4319932607017835E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>5.4155633984795448E-2</c:v>
+                  <c:v>7.040232418023408E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>5.90362945756433E-2</c:v>
+                  <c:v>7.6747182948336296E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>6.4108230198523436E-2</c:v>
+                  <c:v>8.3340699258080464E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>6.935934146016362E-2</c:v>
+                  <c:v>9.0167143898212704E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>7.4776113824892548E-2</c:v>
+                  <c:v>9.7208947972360321E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>8.0343696303467355E-2</c:v>
+                  <c:v>0.10444680519450757</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>8.6045997182124606E-2</c:v>
+                  <c:v>0.11185979633676199</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>9.1865796282358858E-2</c:v>
+                  <c:v>0.11942553516706651</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>9.7784872931722167E-2</c:v>
+                  <c:v>0.12712033481123883</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.10378414851369361</c:v>
+                  <c:v>0.13491939306780171</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.10984384215755733</c:v>
+                  <c:v>0.14279699480482452</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1862,124 +1862,124 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2605511223461328E-6</c:v>
+                  <c:v>2.9387164590499728E-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.808383665891089E-5</c:v>
+                  <c:v>2.3508987656584158E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.102770627569587E-5</c:v>
+                  <c:v>7.9336018158404631E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4463407175294152E-4</c:v>
+                  <c:v>1.8802429327882398E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.8241053617311662E-4</c:v>
+                  <c:v>3.6713369702505162E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.8780472313111889E-4</c:v>
+                  <c:v>6.3414614007045462E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.7417137747542997E-4</c:v>
+                  <c:v>1.006422790718059E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.154732353355975E-3</c:v>
+                  <c:v>1.5011520593627675E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.6425296602429473E-3</c:v>
+                  <c:v>2.1352885583158314E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.2503718026603559E-3</c:v>
+                  <c:v>2.9254833434584626E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.9907737240505161E-3</c:v>
+                  <c:v>3.8880058412656712E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.8758907486478866E-3</c:v>
+                  <c:v>5.0386579732422526E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.9174470064569931E-3</c:v>
+                  <c:v>6.3926811083940913E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6.1266589241278646E-3</c:v>
+                  <c:v>7.9646566013662247E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.514154467163997E-3</c:v>
+                  <c:v>9.7684008073131972E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.0898889246784353E-3</c:v>
+                  <c:v>1.1816855602081967E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.0863058134767067E-2</c:v>
+                  <c:v>1.4121975575197189E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.2842010154167444E-2</c:v>
+                  <c:v>1.6694613200417676E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.5034156477655047E-2</c:v>
+                  <c:v>1.9544403420951564E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.7445884007829954E-2</c:v>
+                  <c:v>2.267964921017894E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.0082469061632802E-2</c:v>
+                  <c:v>2.6107209780122643E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.2947994773054342E-2</c:v>
+                  <c:v>2.9832393204970647E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.6045273308977684E-2</c:v>
+                  <c:v>3.3858855301670994E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.9375774353851136E-2</c:v>
+                  <c:v>3.8188506660006477E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.2939561335982914E-2</c:v>
+                  <c:v>4.2821429736777793E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.6735236860931386E-2</c:v>
+                  <c:v>4.7755807919210802E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.0759898783298443E-2</c:v>
+                  <c:v>5.2987868418287974E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4.5009108285189531E-2</c:v>
+                  <c:v>5.8511840770746393E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4.9476871236167563E-2</c:v>
+                  <c:v>6.4319932607017835E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>5.4155633984795448E-2</c:v>
+                  <c:v>7.040232418023408E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>5.90362945756433E-2</c:v>
+                  <c:v>7.6747182948336296E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>6.4108230198523436E-2</c:v>
+                  <c:v>8.3340699258080464E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>6.935934146016362E-2</c:v>
+                  <c:v>9.0167143898212704E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>7.4776113824892548E-2</c:v>
+                  <c:v>9.7208947972360321E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>8.0343696303467355E-2</c:v>
+                  <c:v>0.10444680519450757</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>8.6045997182124606E-2</c:v>
+                  <c:v>0.11185979633676199</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>9.1865796282358858E-2</c:v>
+                  <c:v>0.11942553516706651</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>9.7784872931722167E-2</c:v>
+                  <c:v>0.12712033481123883</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.10378414851369361</c:v>
+                  <c:v>0.13491939306780171</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.10984384215755733</c:v>
+                  <c:v>0.14279699480482452</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4318,7 +4318,7 @@
         <v>38</v>
       </c>
       <c r="B12">
-        <v>0.25</v>
+        <v>0.32500000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -4365,7 +4365,7 @@
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21">
         <f t="shared" ref="B21:B84" si="0">(1-EXP(-((C21/$B$16-($B$15-0.5))/$B$13)^$B$14))*$B$12</f>
-        <v>2.2605511223461328E-6</v>
+        <v>2.9387164590499728E-6</v>
       </c>
       <c r="C21">
         <f>C20+0.25</f>
@@ -4375,7 +4375,7 @@
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>1.808383665891089E-5</v>
+        <v>2.3508987656584158E-5</v>
       </c>
       <c r="C22">
         <f t="shared" ref="C22:C85" si="1">C21+0.25</f>
@@ -4385,7 +4385,7 @@
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>6.102770627569587E-5</v>
+        <v>7.9336018158404631E-5</v>
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
@@ -4395,7 +4395,7 @@
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>1.4463407175294152E-4</v>
+        <v>1.8802429327882398E-4</v>
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
@@ -4405,7 +4405,7 @@
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>2.8241053617311662E-4</v>
+        <v>3.6713369702505162E-4</v>
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
@@ -4415,7 +4415,7 @@
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>4.8780472313111889E-4</v>
+        <v>6.3414614007045462E-4</v>
       </c>
       <c r="C26">
         <f t="shared" si="1"/>
@@ -4425,7 +4425,7 @@
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>7.7417137747542997E-4</v>
+        <v>1.006422790718059E-3</v>
       </c>
       <c r="C27">
         <f t="shared" si="1"/>
@@ -4435,7 +4435,7 @@
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>1.154732353355975E-3</v>
+        <v>1.5011520593627675E-3</v>
       </c>
       <c r="C28">
         <f t="shared" si="1"/>
@@ -4445,7 +4445,7 @@
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>1.6425296602429473E-3</v>
+        <v>2.1352885583158314E-3</v>
       </c>
       <c r="C29">
         <f t="shared" si="1"/>
@@ -4455,7 +4455,7 @@
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>2.2503718026603559E-3</v>
+        <v>2.9254833434584626E-3</v>
       </c>
       <c r="C30">
         <f t="shared" si="1"/>
@@ -4465,7 +4465,7 @@
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>2.9907737240505161E-3</v>
+        <v>3.8880058412656712E-3</v>
       </c>
       <c r="C31">
         <f t="shared" si="1"/>
@@ -4475,7 +4475,7 @@
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>3.8758907486478866E-3</v>
+        <v>5.0386579732422526E-3</v>
       </c>
       <c r="C32">
         <f t="shared" si="1"/>
@@ -4485,7 +4485,7 @@
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33">
         <f t="shared" si="0"/>
-        <v>4.9174470064569931E-3</v>
+        <v>6.3926811083940913E-3</v>
       </c>
       <c r="C33">
         <f t="shared" si="1"/>
@@ -4495,7 +4495,7 @@
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34">
         <f t="shared" si="0"/>
-        <v>6.1266589241278646E-3</v>
+        <v>7.9646566013662247E-3</v>
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
@@ -4505,7 +4505,7 @@
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35">
         <f t="shared" si="0"/>
-        <v>7.514154467163997E-3</v>
+        <v>9.7684008073131972E-3</v>
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
@@ -4515,7 +4515,7 @@
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36">
         <f t="shared" si="0"/>
-        <v>9.0898889246784353E-3</v>
+        <v>1.1816855602081967E-2</v>
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
@@ -4525,7 +4525,7 @@
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37">
         <f t="shared" si="0"/>
-        <v>1.0863058134767067E-2</v>
+        <v>1.4121975575197189E-2</v>
       </c>
       <c r="C37">
         <f t="shared" si="1"/>
@@ -4535,7 +4535,7 @@
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38">
         <f t="shared" si="0"/>
-        <v>1.2842010154167444E-2</v>
+        <v>1.6694613200417676E-2</v>
       </c>
       <c r="C38">
         <f t="shared" si="1"/>
@@ -4545,7 +4545,7 @@
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39">
         <f t="shared" si="0"/>
-        <v>1.5034156477655047E-2</v>
+        <v>1.9544403420951564E-2</v>
       </c>
       <c r="C39">
         <f t="shared" si="1"/>
@@ -4555,7 +4555,7 @@
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40">
         <f t="shared" si="0"/>
-        <v>1.7445884007829954E-2</v>
+        <v>2.267964921017894E-2</v>
       </c>
       <c r="C40">
         <f t="shared" si="1"/>
@@ -4565,7 +4565,7 @@
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41">
         <f t="shared" si="0"/>
-        <v>2.0082469061632802E-2</v>
+        <v>2.6107209780122643E-2</v>
       </c>
       <c r="C41">
         <f t="shared" si="1"/>
@@ -4575,7 +4575,7 @@
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42">
         <f t="shared" si="0"/>
-        <v>2.2947994773054342E-2</v>
+        <v>2.9832393204970647E-2</v>
       </c>
       <c r="C42">
         <f t="shared" si="1"/>
@@ -4585,7 +4585,7 @@
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43">
         <f t="shared" si="0"/>
-        <v>2.6045273308977684E-2</v>
+        <v>3.3858855301670994E-2</v>
       </c>
       <c r="C43">
         <f t="shared" si="1"/>
@@ -4595,7 +4595,7 @@
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44">
         <f t="shared" si="0"/>
-        <v>2.9375774353851136E-2</v>
+        <v>3.8188506660006477E-2</v>
       </c>
       <c r="C44">
         <f t="shared" si="1"/>
@@ -4605,7 +4605,7 @@
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45">
         <f t="shared" si="0"/>
-        <v>3.2939561335982914E-2</v>
+        <v>4.2821429736777793E-2</v>
       </c>
       <c r="C45">
         <f t="shared" si="1"/>
@@ -4615,7 +4615,7 @@
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46">
         <f t="shared" si="0"/>
-        <v>3.6735236860931386E-2</v>
+        <v>4.7755807919210802E-2</v>
       </c>
       <c r="C46">
         <f t="shared" si="1"/>
@@ -4625,7 +4625,7 @@
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47">
         <f t="shared" si="0"/>
-        <v>4.0759898783298443E-2</v>
+        <v>5.2987868418287974E-2</v>
       </c>
       <c r="C47">
         <f t="shared" si="1"/>
@@ -4635,7 +4635,7 @@
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48">
         <f t="shared" si="0"/>
-        <v>4.5009108285189531E-2</v>
+        <v>5.8511840770746393E-2</v>
       </c>
       <c r="C48">
         <f t="shared" si="1"/>
@@ -4645,7 +4645,7 @@
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49">
         <f t="shared" si="0"/>
-        <v>4.9476871236167563E-2</v>
+        <v>6.4319932607017835E-2</v>
       </c>
       <c r="C49">
         <f t="shared" si="1"/>
@@ -4655,7 +4655,7 @@
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50">
         <f t="shared" si="0"/>
-        <v>5.4155633984795448E-2</v>
+        <v>7.040232418023408E-2</v>
       </c>
       <c r="C50">
         <f t="shared" si="1"/>
@@ -4665,7 +4665,7 @@
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51">
         <f t="shared" si="0"/>
-        <v>5.90362945756433E-2</v>
+        <v>7.6747182948336296E-2</v>
       </c>
       <c r="C51">
         <f t="shared" si="1"/>
@@ -4675,7 +4675,7 @@
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52">
         <f t="shared" si="0"/>
-        <v>6.4108230198523436E-2</v>
+        <v>8.3340699258080464E-2</v>
       </c>
       <c r="C52">
         <f t="shared" si="1"/>
@@ -4685,7 +4685,7 @@
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53">
         <f t="shared" si="0"/>
-        <v>6.935934146016362E-2</v>
+        <v>9.0167143898212704E-2</v>
       </c>
       <c r="C53">
         <f t="shared" si="1"/>
@@ -4695,7 +4695,7 @@
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54">
         <f t="shared" si="0"/>
-        <v>7.4776113824892548E-2</v>
+        <v>9.7208947972360321E-2</v>
       </c>
       <c r="C54">
         <f t="shared" si="1"/>
@@ -4705,7 +4705,7 @@
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55">
         <f t="shared" si="0"/>
-        <v>8.0343696303467355E-2</v>
+        <v>0.10444680519450757</v>
       </c>
       <c r="C55">
         <f t="shared" si="1"/>
@@ -4715,7 +4715,7 @@
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56">
         <f t="shared" si="0"/>
-        <v>8.6045997182124606E-2</v>
+        <v>0.11185979633676199</v>
       </c>
       <c r="C56">
         <f t="shared" si="1"/>
@@ -4725,7 +4725,7 @@
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57">
         <f t="shared" si="0"/>
-        <v>9.1865796282358858E-2</v>
+        <v>0.11942553516706651</v>
       </c>
       <c r="C57">
         <f t="shared" si="1"/>
@@ -4735,7 +4735,7 @@
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58">
         <f t="shared" si="0"/>
-        <v>9.7784872931722167E-2</v>
+        <v>0.12712033481123883</v>
       </c>
       <c r="C58">
         <f t="shared" si="1"/>
@@ -4745,7 +4745,7 @@
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59">
         <f t="shared" si="0"/>
-        <v>0.10378414851369361</v>
+        <v>0.13491939306780171</v>
       </c>
       <c r="C59">
         <f t="shared" si="1"/>
@@ -4755,7 +4755,7 @@
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60">
         <f t="shared" si="0"/>
-        <v>0.10984384215755733</v>
+        <v>0.14279699480482452</v>
       </c>
       <c r="C60">
         <f t="shared" si="1"/>
@@ -4765,7 +4765,7 @@
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61">
         <f t="shared" si="0"/>
-        <v>0.11594363783482298</v>
+        <v>0.15072672918526989</v>
       </c>
       <c r="C61">
         <f t="shared" si="1"/>
@@ -4775,7 +4775,7 @@
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62">
         <f t="shared" si="0"/>
-        <v>0.1220628608547917</v>
+        <v>0.15868171911122922</v>
       </c>
       <c r="C62">
         <f t="shared" si="1"/>
@@ -4785,7 +4785,7 @@
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63">
         <f t="shared" si="0"/>
-        <v>0.12818066150615826</v>
+        <v>0.16663485995800573</v>
       </c>
       <c r="C63">
         <f t="shared" si="1"/>
@@ -4795,7 +4795,7 @@
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64">
         <f t="shared" si="0"/>
-        <v>0.13427620338153212</v>
+        <v>0.17455906439599175</v>
       </c>
       <c r="C64">
         <f t="shared" si="1"/>
@@ -4805,7 +4805,7 @@
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65">
         <f t="shared" si="0"/>
-        <v>0.1403288537544117</v>
+        <v>0.18242750988073522</v>
       </c>
       <c r="C65">
         <f t="shared" si="1"/>
@@ -4815,7 +4815,7 @@
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66">
         <f t="shared" si="0"/>
-        <v>0.14631837325965968</v>
+        <v>0.19021388523755758</v>
       </c>
       <c r="C66">
         <f t="shared" si="1"/>
@@ -4825,7 +4825,7 @@
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67">
         <f t="shared" si="0"/>
-        <v>0.15222510206407147</v>
+        <v>0.19789263268329291</v>
       </c>
       <c r="C67">
         <f t="shared" si="1"/>
@@ -4835,7 +4835,7 @@
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68">
         <f t="shared" si="0"/>
-        <v>0.15803013970713942</v>
+        <v>0.20543918161928124</v>
       </c>
       <c r="C68">
         <f t="shared" si="1"/>
@@ -4845,7 +4845,7 @@
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69">
         <f t="shared" si="0"/>
-        <v>0.16371551584608257</v>
+        <v>0.21283017059990736</v>
       </c>
       <c r="C69">
         <f t="shared" si="1"/>
@@ -4855,7 +4855,7 @@
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70">
         <f t="shared" si="0"/>
-        <v>0.16926434925451739</v>
+        <v>0.22004365403087262</v>
       </c>
       <c r="C70">
         <f t="shared" si="1"/>
@@ -4865,7 +4865,7 @@
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71">
         <f t="shared" si="0"/>
-        <v>0.17466099259996892</v>
+        <v>0.22705929037995962</v>
       </c>
       <c r="C71">
         <f t="shared" si="1"/>
@@ -4875,7 +4875,7 @@
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72">
         <f t="shared" si="0"/>
-        <v>0.17989116075915099</v>
+        <v>0.23385850898689628</v>
       </c>
       <c r="C72">
         <f t="shared" si="1"/>
@@ -4885,7 +4885,7 @@
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73">
         <f t="shared" si="0"/>
-        <v>0.18494204071721859</v>
+        <v>0.24042465293238419</v>
       </c>
       <c r="C73">
         <f t="shared" si="1"/>
@@ -4895,7 +4895,7 @@
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74">
         <f t="shared" si="0"/>
-        <v>0.18980238143193792</v>
+        <v>0.2467430958615193</v>
       </c>
       <c r="C74">
         <f t="shared" si="1"/>
@@ -4905,7 +4905,7 @@
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75">
         <f t="shared" si="0"/>
-        <v>0.19446256241829191</v>
+        <v>0.25280133114377951</v>
       </c>
       <c r="C75">
         <f t="shared" si="1"/>
@@ -4915,7 +4915,7 @@
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76">
         <f t="shared" si="0"/>
-        <v>0.19891464021443961</v>
+        <v>0.2585890322787715</v>
       </c>
       <c r="C76">
         <f t="shared" si="1"/>
@@ -4925,7 +4925,7 @@
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77">
         <f t="shared" si="0"/>
-        <v>0.2031523723160483</v>
+        <v>0.26409808401086282</v>
       </c>
       <c r="C77">
         <f t="shared" si="1"/>
@@ -4935,7 +4935,7 @@
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78">
         <f t="shared" si="0"/>
-        <v>0.2071712186018998</v>
+        <v>0.26932258418246974</v>
       </c>
       <c r="C78">
         <f t="shared" si="1"/>
@@ -4945,7 +4945,7 @@
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79">
         <f t="shared" si="0"/>
-        <v>0.21096832070794364</v>
+        <v>0.27425881692032672</v>
       </c>
       <c r="C79">
         <f t="shared" si="1"/>
@@ -4955,7 +4955,7 @@
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80">
         <f t="shared" si="0"/>
-        <v>0.21454246022816437</v>
+        <v>0.2789051982966137</v>
       </c>
       <c r="C80">
         <f t="shared" si="1"/>
@@ -4965,7 +4965,7 @@
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81">
         <f t="shared" si="0"/>
-        <v>0.21789399701757761</v>
+        <v>0.28326219612285092</v>
       </c>
       <c r="C81">
         <f t="shared" si="1"/>
@@ -4975,7 +4975,7 @@
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82">
         <f t="shared" si="0"/>
-        <v>0.22102478923488639</v>
+        <v>0.2873322260053523</v>
       </c>
       <c r="C82">
         <f t="shared" si="1"/>
@@ -4985,7 +4985,7 @@
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83">
         <f t="shared" si="0"/>
-        <v>0.22393809708039045</v>
+        <v>0.29111952620450759</v>
       </c>
       <c r="C83">
         <f t="shared" si="1"/>
@@ -4995,7 +4995,7 @@
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84">
         <f t="shared" si="0"/>
-        <v>0.22663847245059368</v>
+        <v>0.29463001418577178</v>
       </c>
       <c r="C84">
         <f t="shared" si="1"/>
@@ -5005,7 +5005,7 @@
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85">
         <f t="shared" ref="B85:B121" si="2">(1-EXP(-((C85/$B$16-($B$15-0.5))/$B$13)^$B$14))*$B$12</f>
-        <v>0.22913163693821295</v>
+        <v>0.29787112801967686</v>
       </c>
       <c r="C85">
         <f t="shared" si="1"/>
@@ -5015,7 +5015,7 @@
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86">
         <f t="shared" si="2"/>
-        <v>0.23142435075045348</v>
+        <v>0.30085165597558955</v>
       </c>
       <c r="C86">
         <f t="shared" ref="C86:C121" si="3">C85+0.25</f>
@@ -5025,7 +5025,7 @@
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87">
         <f t="shared" si="2"/>
-        <v>0.23352427519699354</v>
+        <v>0.30358155775609158</v>
       </c>
       <c r="C87">
         <f t="shared" si="3"/>
@@ -5035,7 +5035,7 @@
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88">
         <f t="shared" si="2"/>
-        <v>0.23543983141173369</v>
+        <v>0.30607178083525383</v>
       </c>
       <c r="C88">
         <f t="shared" si="3"/>
@@ -5045,7 +5045,7 @@
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89">
         <f t="shared" si="2"/>
-        <v>0.23718005792069682</v>
+        <v>0.30833407529690587</v>
       </c>
       <c r="C89">
         <f t="shared" si="3"/>
@@ -5055,7 +5055,7 @@
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90">
         <f t="shared" si="2"/>
-        <v>0.23875446955618485</v>
+        <v>0.31038081042304033</v>
       </c>
       <c r="C90">
         <f t="shared" si="3"/>
@@ -5065,7 +5065,7 @@
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91">
         <f t="shared" si="2"/>
-        <v>0.24017292004988233</v>
+        <v>0.31222479606484704</v>
       </c>
       <c r="C91">
         <f t="shared" si="3"/>
@@ -5075,7 +5075,7 @@
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92">
         <f t="shared" si="2"/>
-        <v>0.2414454704220835</v>
+        <v>0.31387911154870857</v>
       </c>
       <c r="C92">
         <f t="shared" si="3"/>
@@ -5085,7 +5085,7 @@
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93">
         <f t="shared" si="2"/>
-        <v>0.24258226502891142</v>
+        <v>0.31535694453758484</v>
       </c>
       <c r="C93">
         <f t="shared" si="3"/>
@@ -5095,7 +5095,7 @@
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94">
         <f t="shared" si="2"/>
-        <v>0.24359341684352731</v>
+        <v>0.31667144189658553</v>
       </c>
       <c r="C94">
         <f t="shared" si="3"/>
@@ -5105,7 +5105,7 @@
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95">
         <f t="shared" si="2"/>
-        <v>0.24448890324067107</v>
+        <v>0.3178355742128724</v>
       </c>
       <c r="C95">
         <f t="shared" si="3"/>
@@ -5115,7 +5115,7 @@
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96">
         <f t="shared" si="2"/>
-        <v>0.24527847323639623</v>
+        <v>0.31886201520731511</v>
       </c>
       <c r="C96">
         <f t="shared" si="3"/>
@@ -5125,7 +5125,7 @@
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97">
         <f t="shared" si="2"/>
-        <v>0.24597156681632482</v>
+        <v>0.31976303686122226</v>
       </c>
       <c r="C97">
         <f t="shared" si="3"/>
@@ -5135,7 +5135,7 @@
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98">
         <f t="shared" si="2"/>
-        <v>0.24657724667537687</v>
+        <v>0.32055042067798994</v>
       </c>
       <c r="C98">
         <f t="shared" si="3"/>
@@ -5145,7 +5145,7 @@
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99">
         <f t="shared" si="2"/>
-        <v>0.24710414239809914</v>
+        <v>0.32123538511752886</v>
       </c>
       <c r="C99">
         <f t="shared" si="3"/>
@@ -5155,7 +5155,7 @@
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100">
         <f t="shared" si="2"/>
-        <v>0.24756040683869554</v>
+        <v>0.32182852889030422</v>
       </c>
       <c r="C100">
         <f t="shared" si="3"/>
@@ -5165,7 +5165,7 @@
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101">
         <f t="shared" si="2"/>
-        <v>0.24795368421960901</v>
+        <v>0.32233978948549169</v>
       </c>
       <c r="C101">
         <f t="shared" si="3"/>
@@ -5175,7 +5175,7 @@
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102">
         <f t="shared" si="2"/>
-        <v>0.24829108926154431</v>
+        <v>0.32277841604000762</v>
       </c>
       <c r="C102">
         <f t="shared" si="3"/>
@@ -5185,7 +5185,7 @@
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103">
         <f t="shared" si="2"/>
-        <v>0.24857919648917257</v>
+        <v>0.32315295543592437</v>
       </c>
       <c r="C103">
         <f t="shared" si="3"/>
@@ -5195,7 +5195,7 @@
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104">
         <f t="shared" si="2"/>
-        <v>0.24882403872694062</v>
+        <v>0.32347125034502283</v>
       </c>
       <c r="C104">
         <f t="shared" si="3"/>
@@ -5205,7 +5205,7 @@
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105">
         <f t="shared" si="2"/>
-        <v>0.24903111370850606</v>
+        <v>0.32374044782105788</v>
       </c>
       <c r="C105">
         <f t="shared" si="3"/>
@@ -5215,7 +5215,7 @@
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106">
         <f t="shared" si="2"/>
-        <v>0.24920539767009622</v>
+        <v>0.32396701697112512</v>
       </c>
       <c r="C106">
         <f t="shared" si="3"/>
@@ -5225,7 +5225,7 @@
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107">
         <f t="shared" si="2"/>
-        <v>0.24935136478016356</v>
+        <v>0.32415677421421263</v>
       </c>
       <c r="C107">
         <f t="shared" si="3"/>
@@ -5235,7 +5235,7 @@
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108">
         <f t="shared" si="2"/>
-        <v>0.24947301127174229</v>
+        <v>0.32431491465326501</v>
       </c>
       <c r="C108">
         <f t="shared" si="3"/>
@@ -5245,7 +5245,7 @@
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109">
         <f t="shared" si="2"/>
-        <v>0.24957388318583304</v>
+        <v>0.32444604814158295</v>
       </c>
       <c r="C109">
         <f t="shared" si="3"/>
@@ -5255,7 +5255,7 @@
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110">
         <f t="shared" si="2"/>
-        <v>0.24965710669938598</v>
+        <v>0.3245542387092018</v>
       </c>
       <c r="C110">
         <f t="shared" si="3"/>
@@ -5265,7 +5265,7 @@
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111">
         <f t="shared" si="2"/>
-        <v>0.24972542009517504</v>
+        <v>0.32464304612372757</v>
       </c>
       <c r="C111">
         <f t="shared" si="3"/>
@@ -5275,7 +5275,7 @@
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112">
         <f t="shared" si="2"/>
-        <v>0.24978120652816521</v>
+        <v>0.32471556848661476</v>
       </c>
       <c r="C112">
         <f t="shared" si="3"/>
@@ -5285,7 +5285,7 @@
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113">
         <f t="shared" si="2"/>
-        <v>0.24982652684911502</v>
+        <v>0.32477448490384953</v>
       </c>
       <c r="C113">
         <f t="shared" si="3"/>
@@ -5295,7 +5295,7 @@
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114">
         <f t="shared" si="2"/>
-        <v>0.24986315185667871</v>
+        <v>0.32482209741368234</v>
       </c>
       <c r="C114">
         <f t="shared" si="3"/>
@@ -5305,7 +5305,7 @@
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115">
         <f t="shared" si="2"/>
-        <v>0.24989259346017748</v>
+        <v>0.32486037149823072</v>
       </c>
       <c r="C115">
         <f t="shared" si="3"/>
@@ -5315,7 +5315,7 @@
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116">
         <f t="shared" si="2"/>
-        <v>0.24991613434302437</v>
+        <v>0.3248909746459317</v>
       </c>
       <c r="C116">
         <f t="shared" si="3"/>
@@ -5325,7 +5325,7 @@
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117">
         <f t="shared" si="2"/>
-        <v>0.24993485581865399</v>
+        <v>0.32491531256425021</v>
       </c>
       <c r="C117">
         <f t="shared" si="3"/>
@@ -5335,7 +5335,7 @@
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118">
         <f t="shared" si="2"/>
-        <v>0.24994966366449239</v>
+        <v>0.32493456276384014</v>
       </c>
       <c r="C118">
         <f t="shared" si="3"/>
@@ -5345,7 +5345,7 @@
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119">
         <f t="shared" si="2"/>
-        <v>0.24996131180339531</v>
+        <v>0.32494970534441392</v>
       </c>
       <c r="C119">
         <f t="shared" si="3"/>
@@ -5355,7 +5355,7 @@
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120">
         <f t="shared" si="2"/>
-        <v>0.24997042377507842</v>
+        <v>0.32496155090760193</v>
       </c>
       <c r="C120">
         <f t="shared" si="3"/>
@@ -5365,7 +5365,7 @@
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121">
         <f t="shared" si="2"/>
-        <v>0.24997751200189119</v>
+        <v>0.32497076560245858</v>
       </c>
       <c r="C121">
         <f t="shared" si="3"/>
@@ -5405,327 +5405,327 @@
       </c>
       <c r="C1">
         <f>(1-EXP(-((C2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>2.2605511223461328E-6</v>
+        <v>2.9387164590499728E-6</v>
       </c>
       <c r="D1">
         <f>(1-EXP(-((D2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>1.808383665891089E-5</v>
+        <v>2.3508987656584158E-5</v>
       </c>
       <c r="E1">
         <f>(1-EXP(-((E2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>6.102770627569587E-5</v>
+        <v>7.9336018158404631E-5</v>
       </c>
       <c r="F1">
         <f>(1-EXP(-((F2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>1.4463407175294152E-4</v>
+        <v>1.8802429327882398E-4</v>
       </c>
       <c r="G1">
         <f>(1-EXP(-((G2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>2.8241053617311662E-4</v>
+        <v>3.6713369702505162E-4</v>
       </c>
       <c r="H1">
         <f>(1-EXP(-((H2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>4.8780472313111889E-4</v>
+        <v>6.3414614007045462E-4</v>
       </c>
       <c r="I1">
         <f>(1-EXP(-((I2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>7.7417137747542997E-4</v>
+        <v>1.006422790718059E-3</v>
       </c>
       <c r="J1">
         <f>(1-EXP(-((J2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>1.154732353355975E-3</v>
+        <v>1.5011520593627675E-3</v>
       </c>
       <c r="K1">
         <f>(1-EXP(-((K2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>1.6425296602429473E-3</v>
+        <v>2.1352885583158314E-3</v>
       </c>
       <c r="L1">
         <f>(1-EXP(-((L2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>2.2503718026603559E-3</v>
+        <v>2.9254833434584626E-3</v>
       </c>
       <c r="M1">
         <f>(1-EXP(-((M2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>2.9907737240505161E-3</v>
+        <v>3.8880058412656712E-3</v>
       </c>
       <c r="N1">
         <f>(1-EXP(-((N2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>3.8758907486478866E-3</v>
+        <v>5.0386579732422526E-3</v>
       </c>
       <c r="O1">
         <f>(1-EXP(-((O2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>4.9174470064569931E-3</v>
+        <v>6.3926811083940913E-3</v>
       </c>
       <c r="P1">
         <f>(1-EXP(-((P2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>6.1266589241278646E-3</v>
+        <v>7.9646566013662247E-3</v>
       </c>
       <c r="Q1">
         <f>(1-EXP(-((Q2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>7.514154467163997E-3</v>
+        <v>9.7684008073131972E-3</v>
       </c>
       <c r="R1">
         <f>(1-EXP(-((R2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>9.0898889246784353E-3</v>
+        <v>1.1816855602081967E-2</v>
       </c>
       <c r="S1">
         <f>(1-EXP(-((S2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>1.0863058134767067E-2</v>
+        <v>1.4121975575197189E-2</v>
       </c>
       <c r="T1">
         <f>(1-EXP(-((T2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>1.2842010154167444E-2</v>
+        <v>1.6694613200417676E-2</v>
       </c>
       <c r="U1">
         <f>(1-EXP(-((U2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>1.5034156477655047E-2</v>
+        <v>1.9544403420951564E-2</v>
       </c>
       <c r="V1">
         <f>(1-EXP(-((V2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>1.7445884007829954E-2</v>
+        <v>2.267964921017894E-2</v>
       </c>
       <c r="W1">
         <f>(1-EXP(-((W2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>2.0082469061632802E-2</v>
+        <v>2.6107209780122643E-2</v>
       </c>
       <c r="X1">
         <f>(1-EXP(-((X2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>2.2947994773054342E-2</v>
+        <v>2.9832393204970647E-2</v>
       </c>
       <c r="Y1">
         <f>(1-EXP(-((Y2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>2.6045273308977684E-2</v>
+        <v>3.3858855301670994E-2</v>
       </c>
       <c r="Z1">
         <f>(1-EXP(-((Z2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>2.9375774353851136E-2</v>
+        <v>3.8188506660006477E-2</v>
       </c>
       <c r="AA1">
         <f>(1-EXP(-((AA2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>3.2939561335982914E-2</v>
+        <v>4.2821429736777793E-2</v>
       </c>
       <c r="AB1">
         <f>(1-EXP(-((AB2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>3.6735236860931386E-2</v>
+        <v>4.7755807919210802E-2</v>
       </c>
       <c r="AC1">
         <f>(1-EXP(-((AC2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>4.0759898783298443E-2</v>
+        <v>5.2987868418287974E-2</v>
       </c>
       <c r="AD1">
         <f>(1-EXP(-((AD2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>4.5009108285189531E-2</v>
+        <v>5.8511840770746393E-2</v>
       </c>
       <c r="AE1">
         <f>(1-EXP(-((AE2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>4.9476871236167563E-2</v>
+        <v>6.4319932607017835E-2</v>
       </c>
       <c r="AF1">
         <f>(1-EXP(-((AF2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>5.4155633984795448E-2</v>
+        <v>7.040232418023408E-2</v>
       </c>
       <c r="AG1">
         <f>(1-EXP(-((AG2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>5.90362945756433E-2</v>
+        <v>7.6747182948336296E-2</v>
       </c>
       <c r="AH1">
         <f>(1-EXP(-((AH2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>6.4108230198523436E-2</v>
+        <v>8.3340699258080464E-2</v>
       </c>
       <c r="AI1">
         <f>(1-EXP(-((AI2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>6.935934146016362E-2</v>
+        <v>9.0167143898212704E-2</v>
       </c>
       <c r="AJ1">
         <f>(1-EXP(-((AJ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>7.4776113824892548E-2</v>
+        <v>9.7208947972360321E-2</v>
       </c>
       <c r="AK1">
         <f>(1-EXP(-((AK2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>8.0343696303467355E-2</v>
+        <v>0.10444680519450757</v>
       </c>
       <c r="AL1">
         <f>(1-EXP(-((AL2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>8.6045997182124606E-2</v>
+        <v>0.11185979633676199</v>
       </c>
       <c r="AM1">
         <f>(1-EXP(-((AM2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>9.1865796282358858E-2</v>
+        <v>0.11942553516706651</v>
       </c>
       <c r="AN1">
         <f>(1-EXP(-((AN2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>9.7784872931722167E-2</v>
+        <v>0.12712033481123883</v>
       </c>
       <c r="AO1">
         <f>(1-EXP(-((AO2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.10378414851369361</v>
+        <v>0.13491939306780171</v>
       </c>
       <c r="AP1">
         <f>(1-EXP(-((AP2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.10984384215755733</v>
+        <v>0.14279699480482452</v>
       </c>
       <c r="AQ1">
         <f>(1-EXP(-((AQ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.11594363783482298</v>
+        <v>0.15072672918526989</v>
       </c>
       <c r="AR1">
         <f>(1-EXP(-((AR2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.1220628608547917</v>
+        <v>0.15868171911122922</v>
       </c>
       <c r="AS1">
         <f>(1-EXP(-((AS2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.12818066150615826</v>
+        <v>0.16663485995800573</v>
       </c>
       <c r="AT1">
         <f>(1-EXP(-((AT2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.13427620338153212</v>
+        <v>0.17455906439599175</v>
       </c>
       <c r="AU1">
         <f>(1-EXP(-((AU2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.1403288537544117</v>
+        <v>0.18242750988073522</v>
       </c>
       <c r="AV1">
         <f>(1-EXP(-((AV2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.14631837325965968</v>
+        <v>0.19021388523755758</v>
       </c>
       <c r="AW1">
         <f>(1-EXP(-((AW2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.15222510206407147</v>
+        <v>0.19789263268329291</v>
       </c>
       <c r="AX1">
         <f>(1-EXP(-((AX2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.15803013970713942</v>
+        <v>0.20543918161928124</v>
       </c>
       <c r="AY1">
         <f>(1-EXP(-((AY2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.16371551584608257</v>
+        <v>0.21283017059990736</v>
       </c>
       <c r="AZ1">
         <f>(1-EXP(-((AZ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.16926434925451739</v>
+        <v>0.22004365403087262</v>
       </c>
       <c r="BA1">
         <f>(1-EXP(-((BA2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.17466099259996892</v>
+        <v>0.22705929037995962</v>
       </c>
       <c r="BB1">
         <f>(1-EXP(-((BB2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.17989116075915099</v>
+        <v>0.23385850898689628</v>
       </c>
       <c r="BC1">
         <f>(1-EXP(-((BC2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.18494204071721859</v>
+        <v>0.24042465293238419</v>
       </c>
       <c r="BD1">
         <f>(1-EXP(-((BD2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.18980238143193792</v>
+        <v>0.2467430958615193</v>
       </c>
       <c r="BE1">
         <f>(1-EXP(-((BE2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.19446256241829191</v>
+        <v>0.25280133114377951</v>
       </c>
       <c r="BF1">
         <f>(1-EXP(-((BF2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.19891464021443961</v>
+        <v>0.2585890322787715</v>
       </c>
       <c r="BG1">
         <f>(1-EXP(-((BG2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.2031523723160483</v>
+        <v>0.26409808401086282</v>
       </c>
       <c r="BH1">
         <f>(1-EXP(-((BH2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.2071712186018998</v>
+        <v>0.26932258418246974</v>
       </c>
       <c r="BI1">
         <f>(1-EXP(-((BI2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.21096832070794364</v>
+        <v>0.27425881692032672</v>
       </c>
       <c r="BJ1">
         <f>(1-EXP(-((BJ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.21454246022816437</v>
+        <v>0.2789051982966137</v>
       </c>
       <c r="BK1">
         <f>(1-EXP(-((BK2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.21789399701757761</v>
+        <v>0.28326219612285092</v>
       </c>
       <c r="BL1">
         <f>(1-EXP(-((BL2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.22102478923488639</v>
+        <v>0.2873322260053523</v>
       </c>
       <c r="BM1">
         <f>(1-EXP(-((BM2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.22393809708039045</v>
+        <v>0.29111952620450759</v>
       </c>
       <c r="BN1">
         <f>(1-EXP(-((BN2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.22663847245059368</v>
+        <v>0.29463001418577178</v>
       </c>
       <c r="BO1">
         <f>(1-EXP(-((BO2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.22913163693821295</v>
+        <v>0.29787112801967686</v>
       </c>
       <c r="BP1">
         <f>(1-EXP(-((BP2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.23142435075045348</v>
+        <v>0.30085165597558955</v>
       </c>
       <c r="BQ1">
         <f>(1-EXP(-((BQ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.23352427519699354</v>
+        <v>0.30358155775609158</v>
       </c>
       <c r="BR1">
         <f>(1-EXP(-((BR2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.23543983141173369</v>
+        <v>0.30607178083525383</v>
       </c>
       <c r="BS1">
         <f>(1-EXP(-((BS2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.23718005792069682</v>
+        <v>0.30833407529690587</v>
       </c>
       <c r="BT1">
         <f>(1-EXP(-((BT2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.23875446955618485</v>
+        <v>0.31038081042304033</v>
       </c>
       <c r="BU1">
         <f>(1-EXP(-((BU2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.24017292004988233</v>
+        <v>0.31222479606484704</v>
       </c>
       <c r="BV1">
         <f>(1-EXP(-((BV2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.2414454704220835</v>
+        <v>0.31387911154870857</v>
       </c>
       <c r="BW1">
         <f>(1-EXP(-((BW2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.24258226502891142</v>
+        <v>0.31535694453758484</v>
       </c>
       <c r="BX1">
         <f>(1-EXP(-((BX2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.24359341684352731</v>
+        <v>0.31667144189658553</v>
       </c>
       <c r="BY1">
         <f>(1-EXP(-((BY2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.24448890324067107</v>
+        <v>0.3178355742128724</v>
       </c>
       <c r="BZ1">
         <f>(1-EXP(-((BZ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.24527847323639623</v>
+        <v>0.31886201520731511</v>
       </c>
       <c r="CA1">
         <f>(1-EXP(-((CA2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.24597156681632482</v>
+        <v>0.31976303686122226</v>
       </c>
       <c r="CB1">
         <f>(1-EXP(-((CB2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.24657724667537687</v>
+        <v>0.32055042067798994</v>
       </c>
       <c r="CC1">
         <f>(1-EXP(-((CC2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.24710414239809914</v>
+        <v>0.32123538511752886</v>
       </c>
       <c r="CD1">
         <f>(1-EXP(-((CD2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.24756040683869554</v>
+        <v>0.32182852889030422</v>
       </c>
       <c r="CE1">
         <f>(1-EXP(-((CE2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.25</v>
+        <v>0.32500000000000001</v>
       </c>
     </row>
     <row r="2" spans="1:83" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Correct CSC curve parameters
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B3885D-EC63-427F-94FA-9191017FDCC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279403AA-B43E-4A1C-9142-BC3BE82C1B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
+    <workbookView xWindow="-24120" yWindow="6690" windowWidth="24240" windowHeight="13020" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -609,307 +609,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>1.1302755611730664E-6</c:v>
+                  <c:v>1.3563306734076795E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.041918329455445E-6</c:v>
+                  <c:v>1.0850301995346534E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0513853137847935E-5</c:v>
+                  <c:v>3.6616623765417522E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.2317035876470759E-5</c:v>
+                  <c:v>8.6780443051764905E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4120526808655831E-4</c:v>
+                  <c:v>1.6944632170386997E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.4390236156555944E-4</c:v>
+                  <c:v>2.926828338786713E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.8708568873771498E-4</c:v>
+                  <c:v>4.6450282648525794E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.7736617667798751E-4</c:v>
+                  <c:v>6.9283941201358503E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.2126483012147367E-4</c:v>
+                  <c:v>9.8551779614576844E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.1251859013301779E-3</c:v>
+                  <c:v>1.3502230815962135E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.4953868620252581E-3</c:v>
+                  <c:v>1.7944642344303095E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.9379453743239433E-3</c:v>
+                  <c:v>2.325534449188732E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.4587235032284965E-3</c:v>
+                  <c:v>2.9504682038741957E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.0633294620639323E-3</c:v>
+                  <c:v>3.6759953544767184E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.7570772335819985E-3</c:v>
+                  <c:v>4.5084926802983977E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.5449444623392177E-3</c:v>
+                  <c:v>5.4539333548070607E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.4315290673835337E-3</c:v>
+                  <c:v>6.5178348808602399E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.4210050770837218E-3</c:v>
+                  <c:v>7.7052060925004657E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.5170782388275237E-3</c:v>
+                  <c:v>9.0204938865930274E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.7229420039149769E-3</c:v>
+                  <c:v>1.0467530404697972E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.0041234530816401E-2</c:v>
+                  <c:v>1.2049481436979681E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.1473997386527171E-2</c:v>
+                  <c:v>1.3768796863832604E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.3022636654488842E-2</c:v>
+                  <c:v>1.5627163985386609E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.4687887176925568E-2</c:v>
+                  <c:v>1.7625464612310682E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.6469780667991457E-2</c:v>
+                  <c:v>1.9763736801589746E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.8367618430465693E-2</c:v>
+                  <c:v>2.2041142116558832E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.0379949391649221E-2</c:v>
+                  <c:v>2.4455939269979066E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.2504554142594765E-2</c:v>
+                  <c:v>2.7005464971113717E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.4738435618083782E-2</c:v>
+                  <c:v>2.9686122741700537E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.7077816992397724E-2</c:v>
+                  <c:v>3.249338039087727E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.951814728782165E-2</c:v>
+                  <c:v>3.5421776745385977E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.2054115099261718E-2</c:v>
+                  <c:v>3.8464938119114063E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.467967073008181E-2</c:v>
+                  <c:v>4.1615604876098174E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.7388056912446274E-2</c:v>
+                  <c:v>4.4865668294935525E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4.0171848151733677E-2</c:v>
+                  <c:v>4.820621778208041E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.3022998591062303E-2</c:v>
+                  <c:v>5.1627598309274762E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.5932898141179429E-2</c:v>
+                  <c:v>5.5119477769415316E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.8892436465861083E-2</c:v>
+                  <c:v>5.8670923759033294E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>5.1892074256846804E-2</c:v>
+                  <c:v>6.2270489108216164E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>5.4921921078778663E-2</c:v>
+                  <c:v>6.5906305294534395E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>5.7971818917411488E-2</c:v>
+                  <c:v>6.9566182700893778E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>6.1031430427395852E-2</c:v>
+                  <c:v>7.3237716512875015E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>6.4090330753079128E-2</c:v>
+                  <c:v>7.6908396903694956E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>6.7138101690766061E-2</c:v>
+                  <c:v>8.0565722028919276E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>7.0164426877205852E-2</c:v>
+                  <c:v>8.4197312252647025E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>7.3159186629829842E-2</c:v>
+                  <c:v>8.7791023955795813E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>7.6112551032035736E-2</c:v>
+                  <c:v>9.1335061238442886E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>7.9015069853569708E-2</c:v>
+                  <c:v>9.4818083824283653E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>8.1857757923041286E-2</c:v>
+                  <c:v>9.8229309507649534E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>8.4632174627258694E-2</c:v>
+                  <c:v>0.10155860955271043</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>8.7330496299984461E-2</c:v>
+                  <c:v>0.10479659555998135</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>8.9945580379575493E-2</c:v>
+                  <c:v>0.10793469645549059</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>9.2471020358609296E-2</c:v>
+                  <c:v>0.11096522443033115</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>9.4901190715968961E-2</c:v>
+                  <c:v>0.11388142885916275</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>9.7231281209145953E-2</c:v>
+                  <c:v>0.11667753745097514</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>9.9457320107219804E-2</c:v>
+                  <c:v>0.11934878412866376</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.10157618615802415</c:v>
+                  <c:v>0.12189142338962897</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.1035856093009499</c:v>
+                  <c:v>0.12430273116113988</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.10548416035397182</c:v>
+                  <c:v>0.12658099242476617</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.10727123011408218</c:v>
+                  <c:v>0.12872547613689861</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.10894699850878881</c:v>
+                  <c:v>0.13073639821054656</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.11051239461744319</c:v>
+                  <c:v>0.13261487354093182</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.11196904854019522</c:v>
+                  <c:v>0.13436285824823427</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.11331923622529684</c:v>
+                  <c:v>0.1359830834703562</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.11456581846910648</c:v>
+                  <c:v>0.13747898216292775</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.11571217537522674</c:v>
+                  <c:v>0.13885461045027209</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.11676213759849677</c:v>
+                  <c:v>0.14011456511819612</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.11771991570586685</c:v>
+                  <c:v>0.14126389884704021</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.11859002896034841</c:v>
+                  <c:v>0.1423080347524181</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.11937723477809242</c:v>
+                  <c:v>0.14325268173371089</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.12008646002494117</c:v>
+                  <c:v>0.14410375202992939</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.12072273521104175</c:v>
+                  <c:v>0.1448672822532501</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.12129113251445571</c:v>
+                  <c:v>0.14554935901734684</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.12179670842176366</c:v>
+                  <c:v>0.14615605010611638</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.12224445162033554</c:v>
+                  <c:v>0.14669334194440264</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.12263923661819812</c:v>
+                  <c:v>0.14716708394183772</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.12298578340816241</c:v>
+                  <c:v>0.14758294008979489</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.12328862333768843</c:v>
+                  <c:v>0.1479463480052261</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.12355207119904957</c:v>
+                  <c:v>0.14826248543885948</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.12378020341934777</c:v>
+                  <c:v>0.14853624410321731</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.1239768421098045</c:v>
+                  <c:v>0.1487722105317654</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.12414554463077215</c:v>
+                  <c:v>0.14897465355692657</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.12428959824458628</c:v>
+                  <c:v>0.14914751789350353</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.12441201936347031</c:v>
+                  <c:v>0.14929442323616438</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.12451555685425303</c:v>
+                  <c:v>0.14941866822510363</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.12460269883504811</c:v>
+                  <c:v>0.14952323860205774</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.12467568239008178</c:v>
+                  <c:v>0.14961081886809813</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.12473650563587114</c:v>
+                  <c:v>0.14968380676304538</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.12478694159291652</c:v>
+                  <c:v>0.14974432991149983</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.12482855334969299</c:v>
+                  <c:v>0.14979426401963158</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.12486271004758752</c:v>
+                  <c:v>0.14983525205710502</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.12489060326408261</c:v>
+                  <c:v>0.14986872391689912</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.12491326342455751</c:v>
+                  <c:v>0.14989591610946901</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.12493157592833935</c:v>
+                  <c:v>0.14991789111400722</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.12494629673008874</c:v>
+                  <c:v>0.14993555607610648</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.12495806717151219</c:v>
+                  <c:v>0.14994968060581462</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.12496742790932699</c:v>
+                  <c:v>0.14996091349119239</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.1249748318322462</c:v>
+                  <c:v>0.14996979819869544</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.12498065590169766</c:v>
+                  <c:v>0.14997678708203718</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.12498521188753921</c:v>
+                  <c:v>0.14998225426504705</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.1249887560009456</c:v>
+                  <c:v>0.14998650720113471</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1327,124 +1327,124 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1302755611730664E-6</c:v>
+                  <c:v>1.3563306734076795E-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.041918329455445E-6</c:v>
+                  <c:v>1.0850301995346534E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0513853137847935E-5</c:v>
+                  <c:v>3.6616623765417522E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.2317035876470759E-5</c:v>
+                  <c:v>8.6780443051764905E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4120526808655831E-4</c:v>
+                  <c:v>1.6944632170386997E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.4390236156555944E-4</c:v>
+                  <c:v>2.926828338786713E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.8708568873771498E-4</c:v>
+                  <c:v>4.6450282648525794E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.7736617667798751E-4</c:v>
+                  <c:v>6.9283941201358503E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.2126483012147367E-4</c:v>
+                  <c:v>9.8551779614576844E-4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1251859013301779E-3</c:v>
+                  <c:v>1.3502230815962135E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.4953868620252581E-3</c:v>
+                  <c:v>1.7944642344303095E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.9379453743239433E-3</c:v>
+                  <c:v>2.325534449188732E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.4587235032284965E-3</c:v>
+                  <c:v>2.9504682038741957E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.0633294620639323E-3</c:v>
+                  <c:v>3.6759953544767184E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.7570772335819985E-3</c:v>
+                  <c:v>4.5084926802983977E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.5449444623392177E-3</c:v>
+                  <c:v>5.4539333548070607E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.4315290673835337E-3</c:v>
+                  <c:v>6.5178348808602399E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.4210050770837218E-3</c:v>
+                  <c:v>7.7052060925004657E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.5170782388275237E-3</c:v>
+                  <c:v>9.0204938865930274E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8.7229420039149769E-3</c:v>
+                  <c:v>1.0467530404697972E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.0041234530816401E-2</c:v>
+                  <c:v>1.2049481436979681E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.1473997386527171E-2</c:v>
+                  <c:v>1.3768796863832604E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.3022636654488842E-2</c:v>
+                  <c:v>1.5627163985386609E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.4687887176925568E-2</c:v>
+                  <c:v>1.7625464612310682E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.6469780667991457E-2</c:v>
+                  <c:v>1.9763736801589746E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.8367618430465693E-2</c:v>
+                  <c:v>2.2041142116558832E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.0379949391649221E-2</c:v>
+                  <c:v>2.4455939269979066E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.2504554142594765E-2</c:v>
+                  <c:v>2.7005464971113717E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.4738435618083782E-2</c:v>
+                  <c:v>2.9686122741700537E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.7077816992397724E-2</c:v>
+                  <c:v>3.249338039087727E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.951814728782165E-2</c:v>
+                  <c:v>3.5421776745385977E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.2054115099261718E-2</c:v>
+                  <c:v>3.8464938119114063E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.467967073008181E-2</c:v>
+                  <c:v>4.1615604876098174E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.7388056912446274E-2</c:v>
+                  <c:v>4.4865668294935525E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.0171848151733677E-2</c:v>
+                  <c:v>4.820621778208041E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.3022998591062303E-2</c:v>
+                  <c:v>5.1627598309274762E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.5932898141179429E-2</c:v>
+                  <c:v>5.5119477769415316E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4.8892436465861083E-2</c:v>
+                  <c:v>5.8670923759033294E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>5.1892074256846804E-2</c:v>
+                  <c:v>6.2270489108216164E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>5.4921921078778663E-2</c:v>
+                  <c:v>6.5906305294534395E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1862,124 +1862,124 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1302755611730664E-6</c:v>
+                  <c:v>1.3563306734076795E-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.041918329455445E-6</c:v>
+                  <c:v>1.0850301995346534E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.0513853137847935E-5</c:v>
+                  <c:v>3.6616623765417522E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.2317035876470759E-5</c:v>
+                  <c:v>8.6780443051764905E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4120526808655831E-4</c:v>
+                  <c:v>1.6944632170386997E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.4390236156555944E-4</c:v>
+                  <c:v>2.926828338786713E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.8708568873771498E-4</c:v>
+                  <c:v>4.6450282648525794E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.7736617667798751E-4</c:v>
+                  <c:v>6.9283941201358503E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.2126483012147367E-4</c:v>
+                  <c:v>9.8551779614576844E-4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1251859013301779E-3</c:v>
+                  <c:v>1.3502230815962135E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.4953868620252581E-3</c:v>
+                  <c:v>1.7944642344303095E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.9379453743239433E-3</c:v>
+                  <c:v>2.325534449188732E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.4587235032284965E-3</c:v>
+                  <c:v>2.9504682038741957E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.0633294620639323E-3</c:v>
+                  <c:v>3.6759953544767184E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.7570772335819985E-3</c:v>
+                  <c:v>4.5084926802983977E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.5449444623392177E-3</c:v>
+                  <c:v>5.4539333548070607E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.4315290673835337E-3</c:v>
+                  <c:v>6.5178348808602399E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.4210050770837218E-3</c:v>
+                  <c:v>7.7052060925004657E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.5170782388275237E-3</c:v>
+                  <c:v>9.0204938865930274E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8.7229420039149769E-3</c:v>
+                  <c:v>1.0467530404697972E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.0041234530816401E-2</c:v>
+                  <c:v>1.2049481436979681E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.1473997386527171E-2</c:v>
+                  <c:v>1.3768796863832604E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.3022636654488842E-2</c:v>
+                  <c:v>1.5627163985386609E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.4687887176925568E-2</c:v>
+                  <c:v>1.7625464612310682E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.6469780667991457E-2</c:v>
+                  <c:v>1.9763736801589746E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.8367618430465693E-2</c:v>
+                  <c:v>2.2041142116558832E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.0379949391649221E-2</c:v>
+                  <c:v>2.4455939269979066E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.2504554142594765E-2</c:v>
+                  <c:v>2.7005464971113717E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.4738435618083782E-2</c:v>
+                  <c:v>2.9686122741700537E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.7077816992397724E-2</c:v>
+                  <c:v>3.249338039087727E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.951814728782165E-2</c:v>
+                  <c:v>3.5421776745385977E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.2054115099261718E-2</c:v>
+                  <c:v>3.8464938119114063E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.467967073008181E-2</c:v>
+                  <c:v>4.1615604876098174E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.7388056912446274E-2</c:v>
+                  <c:v>4.4865668294935525E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.0171848151733677E-2</c:v>
+                  <c:v>4.820621778208041E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.3022998591062303E-2</c:v>
+                  <c:v>5.1627598309274762E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.5932898141179429E-2</c:v>
+                  <c:v>5.5119477769415316E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4.8892436465861083E-2</c:v>
+                  <c:v>5.8670923759033294E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>5.1892074256846804E-2</c:v>
+                  <c:v>6.2270489108216164E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>5.4921921078778663E-2</c:v>
+                  <c:v>6.5906305294534395E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4266,7 +4266,7 @@
   <dimension ref="A1:C121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B12" sqref="B12:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4318,7 +4318,7 @@
         <v>38</v>
       </c>
       <c r="B12">
-        <v>0.125</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -4365,7 +4365,7 @@
     <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B21">
         <f t="shared" ref="B21:B84" si="0">(1-EXP(-((C21/$B$16-($B$15-0.5))/$B$13)^$B$14))*$B$12</f>
-        <v>1.1302755611730664E-6</v>
+        <v>1.3563306734076795E-6</v>
       </c>
       <c r="C21">
         <f>C20+0.25</f>
@@ -4375,7 +4375,7 @@
     <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>9.041918329455445E-6</v>
+        <v>1.0850301995346534E-5</v>
       </c>
       <c r="C22">
         <f t="shared" ref="C22:C85" si="1">C21+0.25</f>
@@ -4385,7 +4385,7 @@
     <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>3.0513853137847935E-5</v>
+        <v>3.6616623765417522E-5</v>
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
@@ -4395,7 +4395,7 @@
     <row r="24" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>7.2317035876470759E-5</v>
+        <v>8.6780443051764905E-5</v>
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
@@ -4405,7 +4405,7 @@
     <row r="25" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>1.4120526808655831E-4</v>
+        <v>1.6944632170386997E-4</v>
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
@@ -4415,7 +4415,7 @@
     <row r="26" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>2.4390236156555944E-4</v>
+        <v>2.926828338786713E-4</v>
       </c>
       <c r="C26">
         <f t="shared" si="1"/>
@@ -4425,7 +4425,7 @@
     <row r="27" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>3.8708568873771498E-4</v>
+        <v>4.6450282648525794E-4</v>
       </c>
       <c r="C27">
         <f t="shared" si="1"/>
@@ -4435,7 +4435,7 @@
     <row r="28" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>5.7736617667798751E-4</v>
+        <v>6.9283941201358503E-4</v>
       </c>
       <c r="C28">
         <f t="shared" si="1"/>
@@ -4445,7 +4445,7 @@
     <row r="29" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>8.2126483012147367E-4</v>
+        <v>9.8551779614576844E-4</v>
       </c>
       <c r="C29">
         <f t="shared" si="1"/>
@@ -4455,7 +4455,7 @@
     <row r="30" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>1.1251859013301779E-3</v>
+        <v>1.3502230815962135E-3</v>
       </c>
       <c r="C30">
         <f t="shared" si="1"/>
@@ -4465,7 +4465,7 @@
     <row r="31" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>1.4953868620252581E-3</v>
+        <v>1.7944642344303095E-3</v>
       </c>
       <c r="C31">
         <f t="shared" si="1"/>
@@ -4475,7 +4475,7 @@
     <row r="32" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>1.9379453743239433E-3</v>
+        <v>2.325534449188732E-3</v>
       </c>
       <c r="C32">
         <f t="shared" si="1"/>
@@ -4485,7 +4485,7 @@
     <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B33">
         <f t="shared" si="0"/>
-        <v>2.4587235032284965E-3</v>
+        <v>2.9504682038741957E-3</v>
       </c>
       <c r="C33">
         <f t="shared" si="1"/>
@@ -4495,7 +4495,7 @@
     <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34">
         <f t="shared" si="0"/>
-        <v>3.0633294620639323E-3</v>
+        <v>3.6759953544767184E-3</v>
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
@@ -4505,7 +4505,7 @@
     <row r="35" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B35">
         <f t="shared" si="0"/>
-        <v>3.7570772335819985E-3</v>
+        <v>4.5084926802983977E-3</v>
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
@@ -4515,7 +4515,7 @@
     <row r="36" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B36">
         <f t="shared" si="0"/>
-        <v>4.5449444623392177E-3</v>
+        <v>5.4539333548070607E-3</v>
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
@@ -4525,7 +4525,7 @@
     <row r="37" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B37">
         <f t="shared" si="0"/>
-        <v>5.4315290673835337E-3</v>
+        <v>6.5178348808602399E-3</v>
       </c>
       <c r="C37">
         <f t="shared" si="1"/>
@@ -4535,7 +4535,7 @@
     <row r="38" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B38">
         <f t="shared" si="0"/>
-        <v>6.4210050770837218E-3</v>
+        <v>7.7052060925004657E-3</v>
       </c>
       <c r="C38">
         <f t="shared" si="1"/>
@@ -4545,7 +4545,7 @@
     <row r="39" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B39">
         <f t="shared" si="0"/>
-        <v>7.5170782388275237E-3</v>
+        <v>9.0204938865930274E-3</v>
       </c>
       <c r="C39">
         <f t="shared" si="1"/>
@@ -4555,7 +4555,7 @@
     <row r="40" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B40">
         <f t="shared" si="0"/>
-        <v>8.7229420039149769E-3</v>
+        <v>1.0467530404697972E-2</v>
       </c>
       <c r="C40">
         <f t="shared" si="1"/>
@@ -4565,7 +4565,7 @@
     <row r="41" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B41">
         <f t="shared" si="0"/>
-        <v>1.0041234530816401E-2</v>
+        <v>1.2049481436979681E-2</v>
       </c>
       <c r="C41">
         <f t="shared" si="1"/>
@@ -4575,7 +4575,7 @@
     <row r="42" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B42">
         <f t="shared" si="0"/>
-        <v>1.1473997386527171E-2</v>
+        <v>1.3768796863832604E-2</v>
       </c>
       <c r="C42">
         <f t="shared" si="1"/>
@@ -4585,7 +4585,7 @@
     <row r="43" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B43">
         <f t="shared" si="0"/>
-        <v>1.3022636654488842E-2</v>
+        <v>1.5627163985386609E-2</v>
       </c>
       <c r="C43">
         <f t="shared" si="1"/>
@@ -4595,7 +4595,7 @@
     <row r="44" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B44">
         <f t="shared" si="0"/>
-        <v>1.4687887176925568E-2</v>
+        <v>1.7625464612310682E-2</v>
       </c>
       <c r="C44">
         <f t="shared" si="1"/>
@@ -4605,7 +4605,7 @@
     <row r="45" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B45">
         <f t="shared" si="0"/>
-        <v>1.6469780667991457E-2</v>
+        <v>1.9763736801589746E-2</v>
       </c>
       <c r="C45">
         <f t="shared" si="1"/>
@@ -4615,7 +4615,7 @@
     <row r="46" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B46">
         <f t="shared" si="0"/>
-        <v>1.8367618430465693E-2</v>
+        <v>2.2041142116558832E-2</v>
       </c>
       <c r="C46">
         <f t="shared" si="1"/>
@@ -4625,7 +4625,7 @@
     <row r="47" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B47">
         <f t="shared" si="0"/>
-        <v>2.0379949391649221E-2</v>
+        <v>2.4455939269979066E-2</v>
       </c>
       <c r="C47">
         <f t="shared" si="1"/>
@@ -4635,7 +4635,7 @@
     <row r="48" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B48">
         <f t="shared" si="0"/>
-        <v>2.2504554142594765E-2</v>
+        <v>2.7005464971113717E-2</v>
       </c>
       <c r="C48">
         <f t="shared" si="1"/>
@@ -4645,7 +4645,7 @@
     <row r="49" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B49">
         <f t="shared" si="0"/>
-        <v>2.4738435618083782E-2</v>
+        <v>2.9686122741700537E-2</v>
       </c>
       <c r="C49">
         <f t="shared" si="1"/>
@@ -4655,7 +4655,7 @@
     <row r="50" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B50">
         <f t="shared" si="0"/>
-        <v>2.7077816992397724E-2</v>
+        <v>3.249338039087727E-2</v>
       </c>
       <c r="C50">
         <f t="shared" si="1"/>
@@ -4665,7 +4665,7 @@
     <row r="51" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B51">
         <f t="shared" si="0"/>
-        <v>2.951814728782165E-2</v>
+        <v>3.5421776745385977E-2</v>
       </c>
       <c r="C51">
         <f t="shared" si="1"/>
@@ -4675,7 +4675,7 @@
     <row r="52" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B52">
         <f t="shared" si="0"/>
-        <v>3.2054115099261718E-2</v>
+        <v>3.8464938119114063E-2</v>
       </c>
       <c r="C52">
         <f t="shared" si="1"/>
@@ -4685,7 +4685,7 @@
     <row r="53" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B53">
         <f t="shared" si="0"/>
-        <v>3.467967073008181E-2</v>
+        <v>4.1615604876098174E-2</v>
       </c>
       <c r="C53">
         <f t="shared" si="1"/>
@@ -4695,7 +4695,7 @@
     <row r="54" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B54">
         <f t="shared" si="0"/>
-        <v>3.7388056912446274E-2</v>
+        <v>4.4865668294935525E-2</v>
       </c>
       <c r="C54">
         <f t="shared" si="1"/>
@@ -4705,7 +4705,7 @@
     <row r="55" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B55">
         <f t="shared" si="0"/>
-        <v>4.0171848151733677E-2</v>
+        <v>4.820621778208041E-2</v>
       </c>
       <c r="C55">
         <f t="shared" si="1"/>
@@ -4715,7 +4715,7 @@
     <row r="56" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B56">
         <f t="shared" si="0"/>
-        <v>4.3022998591062303E-2</v>
+        <v>5.1627598309274762E-2</v>
       </c>
       <c r="C56">
         <f t="shared" si="1"/>
@@ -4725,7 +4725,7 @@
     <row r="57" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B57">
         <f t="shared" si="0"/>
-        <v>4.5932898141179429E-2</v>
+        <v>5.5119477769415316E-2</v>
       </c>
       <c r="C57">
         <f t="shared" si="1"/>
@@ -4735,7 +4735,7 @@
     <row r="58" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B58">
         <f t="shared" si="0"/>
-        <v>4.8892436465861083E-2</v>
+        <v>5.8670923759033294E-2</v>
       </c>
       <c r="C58">
         <f t="shared" si="1"/>
@@ -4745,7 +4745,7 @@
     <row r="59" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B59">
         <f t="shared" si="0"/>
-        <v>5.1892074256846804E-2</v>
+        <v>6.2270489108216164E-2</v>
       </c>
       <c r="C59">
         <f t="shared" si="1"/>
@@ -4755,7 +4755,7 @@
     <row r="60" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B60">
         <f t="shared" si="0"/>
-        <v>5.4921921078778663E-2</v>
+        <v>6.5906305294534395E-2</v>
       </c>
       <c r="C60">
         <f t="shared" si="1"/>
@@ -4765,7 +4765,7 @@
     <row r="61" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B61">
         <f t="shared" si="0"/>
-        <v>5.7971818917411488E-2</v>
+        <v>6.9566182700893778E-2</v>
       </c>
       <c r="C61">
         <f t="shared" si="1"/>
@@ -4775,7 +4775,7 @@
     <row r="62" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B62">
         <f t="shared" si="0"/>
-        <v>6.1031430427395852E-2</v>
+        <v>7.3237716512875015E-2</v>
       </c>
       <c r="C62">
         <f t="shared" si="1"/>
@@ -4785,7 +4785,7 @@
     <row r="63" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B63">
         <f t="shared" si="0"/>
-        <v>6.4090330753079128E-2</v>
+        <v>7.6908396903694956E-2</v>
       </c>
       <c r="C63">
         <f t="shared" si="1"/>
@@ -4795,7 +4795,7 @@
     <row r="64" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B64">
         <f t="shared" si="0"/>
-        <v>6.7138101690766061E-2</v>
+        <v>8.0565722028919276E-2</v>
       </c>
       <c r="C64">
         <f t="shared" si="1"/>
@@ -4805,7 +4805,7 @@
     <row r="65" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B65">
         <f t="shared" si="0"/>
-        <v>7.0164426877205852E-2</v>
+        <v>8.4197312252647025E-2</v>
       </c>
       <c r="C65">
         <f t="shared" si="1"/>
@@ -4815,7 +4815,7 @@
     <row r="66" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B66">
         <f t="shared" si="0"/>
-        <v>7.3159186629829842E-2</v>
+        <v>8.7791023955795813E-2</v>
       </c>
       <c r="C66">
         <f t="shared" si="1"/>
@@ -4825,7 +4825,7 @@
     <row r="67" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B67">
         <f t="shared" si="0"/>
-        <v>7.6112551032035736E-2</v>
+        <v>9.1335061238442886E-2</v>
       </c>
       <c r="C67">
         <f t="shared" si="1"/>
@@ -4835,7 +4835,7 @@
     <row r="68" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B68">
         <f t="shared" si="0"/>
-        <v>7.9015069853569708E-2</v>
+        <v>9.4818083824283653E-2</v>
       </c>
       <c r="C68">
         <f t="shared" si="1"/>
@@ -4845,7 +4845,7 @@
     <row r="69" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B69">
         <f t="shared" si="0"/>
-        <v>8.1857757923041286E-2</v>
+        <v>9.8229309507649534E-2</v>
       </c>
       <c r="C69">
         <f t="shared" si="1"/>
@@ -4855,7 +4855,7 @@
     <row r="70" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B70">
         <f t="shared" si="0"/>
-        <v>8.4632174627258694E-2</v>
+        <v>0.10155860955271043</v>
       </c>
       <c r="C70">
         <f t="shared" si="1"/>
@@ -4865,7 +4865,7 @@
     <row r="71" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B71">
         <f t="shared" si="0"/>
-        <v>8.7330496299984461E-2</v>
+        <v>0.10479659555998135</v>
       </c>
       <c r="C71">
         <f t="shared" si="1"/>
@@ -4875,7 +4875,7 @@
     <row r="72" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B72">
         <f t="shared" si="0"/>
-        <v>8.9945580379575493E-2</v>
+        <v>0.10793469645549059</v>
       </c>
       <c r="C72">
         <f t="shared" si="1"/>
@@ -4885,7 +4885,7 @@
     <row r="73" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B73">
         <f t="shared" si="0"/>
-        <v>9.2471020358609296E-2</v>
+        <v>0.11096522443033115</v>
       </c>
       <c r="C73">
         <f t="shared" si="1"/>
@@ -4895,7 +4895,7 @@
     <row r="74" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B74">
         <f t="shared" si="0"/>
-        <v>9.4901190715968961E-2</v>
+        <v>0.11388142885916275</v>
       </c>
       <c r="C74">
         <f t="shared" si="1"/>
@@ -4905,7 +4905,7 @@
     <row r="75" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B75">
         <f t="shared" si="0"/>
-        <v>9.7231281209145953E-2</v>
+        <v>0.11667753745097514</v>
       </c>
       <c r="C75">
         <f t="shared" si="1"/>
@@ -4915,7 +4915,7 @@
     <row r="76" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B76">
         <f t="shared" si="0"/>
-        <v>9.9457320107219804E-2</v>
+        <v>0.11934878412866376</v>
       </c>
       <c r="C76">
         <f t="shared" si="1"/>
@@ -4925,7 +4925,7 @@
     <row r="77" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B77">
         <f t="shared" si="0"/>
-        <v>0.10157618615802415</v>
+        <v>0.12189142338962897</v>
       </c>
       <c r="C77">
         <f t="shared" si="1"/>
@@ -4935,7 +4935,7 @@
     <row r="78" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B78">
         <f t="shared" si="0"/>
-        <v>0.1035856093009499</v>
+        <v>0.12430273116113988</v>
       </c>
       <c r="C78">
         <f t="shared" si="1"/>
@@ -4945,7 +4945,7 @@
     <row r="79" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B79">
         <f t="shared" si="0"/>
-        <v>0.10548416035397182</v>
+        <v>0.12658099242476617</v>
       </c>
       <c r="C79">
         <f t="shared" si="1"/>
@@ -4955,7 +4955,7 @@
     <row r="80" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B80">
         <f t="shared" si="0"/>
-        <v>0.10727123011408218</v>
+        <v>0.12872547613689861</v>
       </c>
       <c r="C80">
         <f t="shared" si="1"/>
@@ -4965,7 +4965,7 @@
     <row r="81" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B81">
         <f t="shared" si="0"/>
-        <v>0.10894699850878881</v>
+        <v>0.13073639821054656</v>
       </c>
       <c r="C81">
         <f t="shared" si="1"/>
@@ -4975,7 +4975,7 @@
     <row r="82" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B82">
         <f t="shared" si="0"/>
-        <v>0.11051239461744319</v>
+        <v>0.13261487354093182</v>
       </c>
       <c r="C82">
         <f t="shared" si="1"/>
@@ -4985,7 +4985,7 @@
     <row r="83" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B83">
         <f t="shared" si="0"/>
-        <v>0.11196904854019522</v>
+        <v>0.13436285824823427</v>
       </c>
       <c r="C83">
         <f t="shared" si="1"/>
@@ -4995,7 +4995,7 @@
     <row r="84" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B84">
         <f t="shared" si="0"/>
-        <v>0.11331923622529684</v>
+        <v>0.1359830834703562</v>
       </c>
       <c r="C84">
         <f t="shared" si="1"/>
@@ -5005,7 +5005,7 @@
     <row r="85" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B85">
         <f t="shared" ref="B85:B121" si="2">(1-EXP(-((C85/$B$16-($B$15-0.5))/$B$13)^$B$14))*$B$12</f>
-        <v>0.11456581846910648</v>
+        <v>0.13747898216292775</v>
       </c>
       <c r="C85">
         <f t="shared" si="1"/>
@@ -5015,7 +5015,7 @@
     <row r="86" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B86">
         <f t="shared" si="2"/>
-        <v>0.11571217537522674</v>
+        <v>0.13885461045027209</v>
       </c>
       <c r="C86">
         <f t="shared" ref="C86:C121" si="3">C85+0.25</f>
@@ -5025,7 +5025,7 @@
     <row r="87" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B87">
         <f t="shared" si="2"/>
-        <v>0.11676213759849677</v>
+        <v>0.14011456511819612</v>
       </c>
       <c r="C87">
         <f t="shared" si="3"/>
@@ -5035,7 +5035,7 @@
     <row r="88" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B88">
         <f t="shared" si="2"/>
-        <v>0.11771991570586685</v>
+        <v>0.14126389884704021</v>
       </c>
       <c r="C88">
         <f t="shared" si="3"/>
@@ -5045,7 +5045,7 @@
     <row r="89" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B89">
         <f t="shared" si="2"/>
-        <v>0.11859002896034841</v>
+        <v>0.1423080347524181</v>
       </c>
       <c r="C89">
         <f t="shared" si="3"/>
@@ -5055,7 +5055,7 @@
     <row r="90" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B90">
         <f t="shared" si="2"/>
-        <v>0.11937723477809242</v>
+        <v>0.14325268173371089</v>
       </c>
       <c r="C90">
         <f t="shared" si="3"/>
@@ -5065,7 +5065,7 @@
     <row r="91" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B91">
         <f t="shared" si="2"/>
-        <v>0.12008646002494117</v>
+        <v>0.14410375202992939</v>
       </c>
       <c r="C91">
         <f t="shared" si="3"/>
@@ -5075,7 +5075,7 @@
     <row r="92" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B92">
         <f t="shared" si="2"/>
-        <v>0.12072273521104175</v>
+        <v>0.1448672822532501</v>
       </c>
       <c r="C92">
         <f t="shared" si="3"/>
@@ -5085,7 +5085,7 @@
     <row r="93" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B93">
         <f t="shared" si="2"/>
-        <v>0.12129113251445571</v>
+        <v>0.14554935901734684</v>
       </c>
       <c r="C93">
         <f t="shared" si="3"/>
@@ -5095,7 +5095,7 @@
     <row r="94" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B94">
         <f t="shared" si="2"/>
-        <v>0.12179670842176366</v>
+        <v>0.14615605010611638</v>
       </c>
       <c r="C94">
         <f t="shared" si="3"/>
@@ -5105,7 +5105,7 @@
     <row r="95" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B95">
         <f t="shared" si="2"/>
-        <v>0.12224445162033554</v>
+        <v>0.14669334194440264</v>
       </c>
       <c r="C95">
         <f t="shared" si="3"/>
@@ -5115,7 +5115,7 @@
     <row r="96" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B96">
         <f t="shared" si="2"/>
-        <v>0.12263923661819812</v>
+        <v>0.14716708394183772</v>
       </c>
       <c r="C96">
         <f t="shared" si="3"/>
@@ -5125,7 +5125,7 @@
     <row r="97" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B97">
         <f t="shared" si="2"/>
-        <v>0.12298578340816241</v>
+        <v>0.14758294008979489</v>
       </c>
       <c r="C97">
         <f t="shared" si="3"/>
@@ -5135,7 +5135,7 @@
     <row r="98" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B98">
         <f t="shared" si="2"/>
-        <v>0.12328862333768843</v>
+        <v>0.1479463480052261</v>
       </c>
       <c r="C98">
         <f t="shared" si="3"/>
@@ -5145,7 +5145,7 @@
     <row r="99" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B99">
         <f t="shared" si="2"/>
-        <v>0.12355207119904957</v>
+        <v>0.14826248543885948</v>
       </c>
       <c r="C99">
         <f t="shared" si="3"/>
@@ -5155,7 +5155,7 @@
     <row r="100" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B100">
         <f t="shared" si="2"/>
-        <v>0.12378020341934777</v>
+        <v>0.14853624410321731</v>
       </c>
       <c r="C100">
         <f t="shared" si="3"/>
@@ -5165,7 +5165,7 @@
     <row r="101" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B101">
         <f t="shared" si="2"/>
-        <v>0.1239768421098045</v>
+        <v>0.1487722105317654</v>
       </c>
       <c r="C101">
         <f t="shared" si="3"/>
@@ -5175,7 +5175,7 @@
     <row r="102" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B102">
         <f t="shared" si="2"/>
-        <v>0.12414554463077215</v>
+        <v>0.14897465355692657</v>
       </c>
       <c r="C102">
         <f t="shared" si="3"/>
@@ -5185,7 +5185,7 @@
     <row r="103" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B103">
         <f t="shared" si="2"/>
-        <v>0.12428959824458628</v>
+        <v>0.14914751789350353</v>
       </c>
       <c r="C103">
         <f t="shared" si="3"/>
@@ -5195,7 +5195,7 @@
     <row r="104" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B104">
         <f t="shared" si="2"/>
-        <v>0.12441201936347031</v>
+        <v>0.14929442323616438</v>
       </c>
       <c r="C104">
         <f t="shared" si="3"/>
@@ -5205,7 +5205,7 @@
     <row r="105" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B105">
         <f t="shared" si="2"/>
-        <v>0.12451555685425303</v>
+        <v>0.14941866822510363</v>
       </c>
       <c r="C105">
         <f t="shared" si="3"/>
@@ -5215,7 +5215,7 @@
     <row r="106" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B106">
         <f t="shared" si="2"/>
-        <v>0.12460269883504811</v>
+        <v>0.14952323860205774</v>
       </c>
       <c r="C106">
         <f t="shared" si="3"/>
@@ -5225,7 +5225,7 @@
     <row r="107" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B107">
         <f t="shared" si="2"/>
-        <v>0.12467568239008178</v>
+        <v>0.14961081886809813</v>
       </c>
       <c r="C107">
         <f t="shared" si="3"/>
@@ -5235,7 +5235,7 @@
     <row r="108" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B108">
         <f t="shared" si="2"/>
-        <v>0.12473650563587114</v>
+        <v>0.14968380676304538</v>
       </c>
       <c r="C108">
         <f t="shared" si="3"/>
@@ -5245,7 +5245,7 @@
     <row r="109" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B109">
         <f t="shared" si="2"/>
-        <v>0.12478694159291652</v>
+        <v>0.14974432991149983</v>
       </c>
       <c r="C109">
         <f t="shared" si="3"/>
@@ -5255,7 +5255,7 @@
     <row r="110" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B110">
         <f t="shared" si="2"/>
-        <v>0.12482855334969299</v>
+        <v>0.14979426401963158</v>
       </c>
       <c r="C110">
         <f t="shared" si="3"/>
@@ -5265,7 +5265,7 @@
     <row r="111" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B111">
         <f t="shared" si="2"/>
-        <v>0.12486271004758752</v>
+        <v>0.14983525205710502</v>
       </c>
       <c r="C111">
         <f t="shared" si="3"/>
@@ -5275,7 +5275,7 @@
     <row r="112" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B112">
         <f t="shared" si="2"/>
-        <v>0.12489060326408261</v>
+        <v>0.14986872391689912</v>
       </c>
       <c r="C112">
         <f t="shared" si="3"/>
@@ -5285,7 +5285,7 @@
     <row r="113" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B113">
         <f t="shared" si="2"/>
-        <v>0.12491326342455751</v>
+        <v>0.14989591610946901</v>
       </c>
       <c r="C113">
         <f t="shared" si="3"/>
@@ -5295,7 +5295,7 @@
     <row r="114" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B114">
         <f t="shared" si="2"/>
-        <v>0.12493157592833935</v>
+        <v>0.14991789111400722</v>
       </c>
       <c r="C114">
         <f t="shared" si="3"/>
@@ -5305,7 +5305,7 @@
     <row r="115" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B115">
         <f t="shared" si="2"/>
-        <v>0.12494629673008874</v>
+        <v>0.14993555607610648</v>
       </c>
       <c r="C115">
         <f t="shared" si="3"/>
@@ -5315,7 +5315,7 @@
     <row r="116" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B116">
         <f t="shared" si="2"/>
-        <v>0.12495806717151219</v>
+        <v>0.14994968060581462</v>
       </c>
       <c r="C116">
         <f t="shared" si="3"/>
@@ -5325,7 +5325,7 @@
     <row r="117" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B117">
         <f t="shared" si="2"/>
-        <v>0.12496742790932699</v>
+        <v>0.14996091349119239</v>
       </c>
       <c r="C117">
         <f t="shared" si="3"/>
@@ -5335,7 +5335,7 @@
     <row r="118" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B118">
         <f t="shared" si="2"/>
-        <v>0.1249748318322462</v>
+        <v>0.14996979819869544</v>
       </c>
       <c r="C118">
         <f t="shared" si="3"/>
@@ -5345,7 +5345,7 @@
     <row r="119" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B119">
         <f t="shared" si="2"/>
-        <v>0.12498065590169766</v>
+        <v>0.14997678708203718</v>
       </c>
       <c r="C119">
         <f t="shared" si="3"/>
@@ -5355,7 +5355,7 @@
     <row r="120" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B120">
         <f t="shared" si="2"/>
-        <v>0.12498521188753921</v>
+        <v>0.14998225426504705</v>
       </c>
       <c r="C120">
         <f t="shared" si="3"/>
@@ -5365,7 +5365,7 @@
     <row r="121" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B121">
         <f t="shared" si="2"/>
-        <v>0.1249887560009456</v>
+        <v>0.14998650720113471</v>
       </c>
       <c r="C121">
         <f t="shared" si="3"/>
@@ -5405,327 +5405,327 @@
       </c>
       <c r="C1">
         <f>(1-EXP(-((C2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>1.1302755611730664E-6</v>
+        <v>1.3563306734076795E-6</v>
       </c>
       <c r="D1">
         <f>(1-EXP(-((D2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>9.041918329455445E-6</v>
+        <v>1.0850301995346534E-5</v>
       </c>
       <c r="E1">
         <f>(1-EXP(-((E2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>3.0513853137847935E-5</v>
+        <v>3.6616623765417522E-5</v>
       </c>
       <c r="F1">
         <f>(1-EXP(-((F2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>7.2317035876470759E-5</v>
+        <v>8.6780443051764905E-5</v>
       </c>
       <c r="G1">
         <f>(1-EXP(-((G2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>1.4120526808655831E-4</v>
+        <v>1.6944632170386997E-4</v>
       </c>
       <c r="H1">
         <f>(1-EXP(-((H2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>2.4390236156555944E-4</v>
+        <v>2.926828338786713E-4</v>
       </c>
       <c r="I1">
         <f>(1-EXP(-((I2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>3.8708568873771498E-4</v>
+        <v>4.6450282648525794E-4</v>
       </c>
       <c r="J1">
         <f>(1-EXP(-((J2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>5.7736617667798751E-4</v>
+        <v>6.9283941201358503E-4</v>
       </c>
       <c r="K1">
         <f>(1-EXP(-((K2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>8.2126483012147367E-4</v>
+        <v>9.8551779614576844E-4</v>
       </c>
       <c r="L1">
         <f>(1-EXP(-((L2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>1.1251859013301779E-3</v>
+        <v>1.3502230815962135E-3</v>
       </c>
       <c r="M1">
         <f>(1-EXP(-((M2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>1.4953868620252581E-3</v>
+        <v>1.7944642344303095E-3</v>
       </c>
       <c r="N1">
         <f>(1-EXP(-((N2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>1.9379453743239433E-3</v>
+        <v>2.325534449188732E-3</v>
       </c>
       <c r="O1">
         <f>(1-EXP(-((O2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>2.4587235032284965E-3</v>
+        <v>2.9504682038741957E-3</v>
       </c>
       <c r="P1">
         <f>(1-EXP(-((P2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>3.0633294620639323E-3</v>
+        <v>3.6759953544767184E-3</v>
       </c>
       <c r="Q1">
         <f>(1-EXP(-((Q2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>3.7570772335819985E-3</v>
+        <v>4.5084926802983977E-3</v>
       </c>
       <c r="R1">
         <f>(1-EXP(-((R2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>4.5449444623392177E-3</v>
+        <v>5.4539333548070607E-3</v>
       </c>
       <c r="S1">
         <f>(1-EXP(-((S2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>5.4315290673835337E-3</v>
+        <v>6.5178348808602399E-3</v>
       </c>
       <c r="T1">
         <f>(1-EXP(-((T2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>6.4210050770837218E-3</v>
+        <v>7.7052060925004657E-3</v>
       </c>
       <c r="U1">
         <f>(1-EXP(-((U2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>7.5170782388275237E-3</v>
+        <v>9.0204938865930274E-3</v>
       </c>
       <c r="V1">
         <f>(1-EXP(-((V2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>8.7229420039149769E-3</v>
+        <v>1.0467530404697972E-2</v>
       </c>
       <c r="W1">
         <f>(1-EXP(-((W2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>1.0041234530816401E-2</v>
+        <v>1.2049481436979681E-2</v>
       </c>
       <c r="X1">
         <f>(1-EXP(-((X2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>1.1473997386527171E-2</v>
+        <v>1.3768796863832604E-2</v>
       </c>
       <c r="Y1">
         <f>(1-EXP(-((Y2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>1.3022636654488842E-2</v>
+        <v>1.5627163985386609E-2</v>
       </c>
       <c r="Z1">
         <f>(1-EXP(-((Z2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>1.4687887176925568E-2</v>
+        <v>1.7625464612310682E-2</v>
       </c>
       <c r="AA1">
         <f>(1-EXP(-((AA2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>1.6469780667991457E-2</v>
+        <v>1.9763736801589746E-2</v>
       </c>
       <c r="AB1">
         <f>(1-EXP(-((AB2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>1.8367618430465693E-2</v>
+        <v>2.2041142116558832E-2</v>
       </c>
       <c r="AC1">
         <f>(1-EXP(-((AC2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>2.0379949391649221E-2</v>
+        <v>2.4455939269979066E-2</v>
       </c>
       <c r="AD1">
         <f>(1-EXP(-((AD2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>2.2504554142594765E-2</v>
+        <v>2.7005464971113717E-2</v>
       </c>
       <c r="AE1">
         <f>(1-EXP(-((AE2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>2.4738435618083782E-2</v>
+        <v>2.9686122741700537E-2</v>
       </c>
       <c r="AF1">
         <f>(1-EXP(-((AF2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>2.7077816992397724E-2</v>
+        <v>3.249338039087727E-2</v>
       </c>
       <c r="AG1">
         <f>(1-EXP(-((AG2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>2.951814728782165E-2</v>
+        <v>3.5421776745385977E-2</v>
       </c>
       <c r="AH1">
         <f>(1-EXP(-((AH2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>3.2054115099261718E-2</v>
+        <v>3.8464938119114063E-2</v>
       </c>
       <c r="AI1">
         <f>(1-EXP(-((AI2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>3.467967073008181E-2</v>
+        <v>4.1615604876098174E-2</v>
       </c>
       <c r="AJ1">
         <f>(1-EXP(-((AJ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>3.7388056912446274E-2</v>
+        <v>4.4865668294935525E-2</v>
       </c>
       <c r="AK1">
         <f>(1-EXP(-((AK2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>4.0171848151733677E-2</v>
+        <v>4.820621778208041E-2</v>
       </c>
       <c r="AL1">
         <f>(1-EXP(-((AL2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>4.3022998591062303E-2</v>
+        <v>5.1627598309274762E-2</v>
       </c>
       <c r="AM1">
         <f>(1-EXP(-((AM2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>4.5932898141179429E-2</v>
+        <v>5.5119477769415316E-2</v>
       </c>
       <c r="AN1">
         <f>(1-EXP(-((AN2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>4.8892436465861083E-2</v>
+        <v>5.8670923759033294E-2</v>
       </c>
       <c r="AO1">
         <f>(1-EXP(-((AO2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>5.1892074256846804E-2</v>
+        <v>6.2270489108216164E-2</v>
       </c>
       <c r="AP1">
         <f>(1-EXP(-((AP2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>5.4921921078778663E-2</v>
+        <v>6.5906305294534395E-2</v>
       </c>
       <c r="AQ1">
         <f>(1-EXP(-((AQ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>5.7971818917411488E-2</v>
+        <v>6.9566182700893778E-2</v>
       </c>
       <c r="AR1">
         <f>(1-EXP(-((AR2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>6.1031430427395852E-2</v>
+        <v>7.3237716512875015E-2</v>
       </c>
       <c r="AS1">
         <f>(1-EXP(-((AS2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>6.4090330753079128E-2</v>
+        <v>7.6908396903694956E-2</v>
       </c>
       <c r="AT1">
         <f>(1-EXP(-((AT2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>6.7138101690766061E-2</v>
+        <v>8.0565722028919276E-2</v>
       </c>
       <c r="AU1">
         <f>(1-EXP(-((AU2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>7.0164426877205852E-2</v>
+        <v>8.4197312252647025E-2</v>
       </c>
       <c r="AV1">
         <f>(1-EXP(-((AV2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>7.3159186629829842E-2</v>
+        <v>8.7791023955795813E-2</v>
       </c>
       <c r="AW1">
         <f>(1-EXP(-((AW2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>7.6112551032035736E-2</v>
+        <v>9.1335061238442886E-2</v>
       </c>
       <c r="AX1">
         <f>(1-EXP(-((AX2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>7.9015069853569708E-2</v>
+        <v>9.4818083824283653E-2</v>
       </c>
       <c r="AY1">
         <f>(1-EXP(-((AY2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>8.1857757923041286E-2</v>
+        <v>9.8229309507649534E-2</v>
       </c>
       <c r="AZ1">
         <f>(1-EXP(-((AZ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>8.4632174627258694E-2</v>
+        <v>0.10155860955271043</v>
       </c>
       <c r="BA1">
         <f>(1-EXP(-((BA2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>8.7330496299984461E-2</v>
+        <v>0.10479659555998135</v>
       </c>
       <c r="BB1">
         <f>(1-EXP(-((BB2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>8.9945580379575493E-2</v>
+        <v>0.10793469645549059</v>
       </c>
       <c r="BC1">
         <f>(1-EXP(-((BC2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>9.2471020358609296E-2</v>
+        <v>0.11096522443033115</v>
       </c>
       <c r="BD1">
         <f>(1-EXP(-((BD2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>9.4901190715968961E-2</v>
+        <v>0.11388142885916275</v>
       </c>
       <c r="BE1">
         <f>(1-EXP(-((BE2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>9.7231281209145953E-2</v>
+        <v>0.11667753745097514</v>
       </c>
       <c r="BF1">
         <f>(1-EXP(-((BF2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>9.9457320107219804E-2</v>
+        <v>0.11934878412866376</v>
       </c>
       <c r="BG1">
         <f>(1-EXP(-((BG2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.10157618615802415</v>
+        <v>0.12189142338962897</v>
       </c>
       <c r="BH1">
         <f>(1-EXP(-((BH2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.1035856093009499</v>
+        <v>0.12430273116113988</v>
       </c>
       <c r="BI1">
         <f>(1-EXP(-((BI2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.10548416035397182</v>
+        <v>0.12658099242476617</v>
       </c>
       <c r="BJ1">
         <f>(1-EXP(-((BJ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.10727123011408218</v>
+        <v>0.12872547613689861</v>
       </c>
       <c r="BK1">
         <f>(1-EXP(-((BK2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.10894699850878881</v>
+        <v>0.13073639821054656</v>
       </c>
       <c r="BL1">
         <f>(1-EXP(-((BL2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.11051239461744319</v>
+        <v>0.13261487354093182</v>
       </c>
       <c r="BM1">
         <f>(1-EXP(-((BM2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.11196904854019522</v>
+        <v>0.13436285824823427</v>
       </c>
       <c r="BN1">
         <f>(1-EXP(-((BN2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.11331923622529684</v>
+        <v>0.1359830834703562</v>
       </c>
       <c r="BO1">
         <f>(1-EXP(-((BO2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.11456581846910648</v>
+        <v>0.13747898216292775</v>
       </c>
       <c r="BP1">
         <f>(1-EXP(-((BP2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.11571217537522674</v>
+        <v>0.13885461045027209</v>
       </c>
       <c r="BQ1">
         <f>(1-EXP(-((BQ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.11676213759849677</v>
+        <v>0.14011456511819612</v>
       </c>
       <c r="BR1">
         <f>(1-EXP(-((BR2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.11771991570586685</v>
+        <v>0.14126389884704021</v>
       </c>
       <c r="BS1">
         <f>(1-EXP(-((BS2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.11859002896034841</v>
+        <v>0.1423080347524181</v>
       </c>
       <c r="BT1">
         <f>(1-EXP(-((BT2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.11937723477809242</v>
+        <v>0.14325268173371089</v>
       </c>
       <c r="BU1">
         <f>(1-EXP(-((BU2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.12008646002494117</v>
+        <v>0.14410375202992939</v>
       </c>
       <c r="BV1">
         <f>(1-EXP(-((BV2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.12072273521104175</v>
+        <v>0.1448672822532501</v>
       </c>
       <c r="BW1">
         <f>(1-EXP(-((BW2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.12129113251445571</v>
+        <v>0.14554935901734684</v>
       </c>
       <c r="BX1">
         <f>(1-EXP(-((BX2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.12179670842176366</v>
+        <v>0.14615605010611638</v>
       </c>
       <c r="BY1">
         <f>(1-EXP(-((BY2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.12224445162033554</v>
+        <v>0.14669334194440264</v>
       </c>
       <c r="BZ1">
         <f>(1-EXP(-((BZ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.12263923661819812</v>
+        <v>0.14716708394183772</v>
       </c>
       <c r="CA1">
         <f>(1-EXP(-((CA2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.12298578340816241</v>
+        <v>0.14758294008979489</v>
       </c>
       <c r="CB1">
         <f>(1-EXP(-((CB2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.12328862333768843</v>
+        <v>0.1479463480052261</v>
       </c>
       <c r="CC1">
         <f>(1-EXP(-((CC2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.12355207119904957</v>
+        <v>0.14826248543885948</v>
       </c>
       <c r="CD1">
         <f>(1-EXP(-((CD2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.12378020341934777</v>
+        <v>0.14853624410321731</v>
       </c>
       <c r="CE1">
         <f>(1-EXP(-((CE2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
-        <v>0.125</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="2" spans="1:83" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Fix csv file that had been incorrectly exported
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279403AA-B43E-4A1C-9142-BC3BE82C1B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF55D05-AAEC-4547-8908-FD5E1D83DFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="6690" windowWidth="24240" windowHeight="13020" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t xml:space="preserve">Source: </t>
   </si>
@@ -135,9 +135,6 @@
   </si>
   <si>
     <t>Supply Curve Parameters</t>
-  </si>
-  <si>
-    <t>CSC Capacity Supply Curve Share of Cost Effective Hybrid Capacity Built in a Single Year</t>
   </si>
   <si>
     <t>% of total installed capacity</t>
@@ -292,7 +289,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>About!$C$21:$C$121</c:f>
+              <c:f>About!$C$20:$C$120</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
@@ -604,7 +601,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>About!$B$21:$B$121</c:f>
+              <c:f>About!$B$20:$B$120</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
@@ -3852,13 +3849,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>151130</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>138430</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3888,13 +3885,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>638175</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>5210175</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4263,10 +4260,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3D2DEE-686E-48A0-AC3D-0F54DEA5D0EC}">
-  <dimension ref="A1:C121"/>
+  <dimension ref="A1:C120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4290,35 +4287,38 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>32</v>
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11">
+        <v>0.15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B12">
-        <v>0.15</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -4326,15 +4326,15 @@
         <v>36</v>
       </c>
       <c r="B13">
-        <v>0.6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -4342,1032 +4342,1024 @@
         <v>39</v>
       </c>
       <c r="B15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16">
         <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B19">
+        <f>(1-EXP(-((C19/$B$15-($B$14-0.5))/$B$12)^$B$13))*$B$11</f>
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B20">
-        <f>(1-EXP(-((C20/$B$16-($B$15-0.5))/$B$13)^$B$14))*$B$12</f>
-        <v>0</v>
+        <f t="shared" ref="B20:B83" si="0">(1-EXP(-((C20/$B$15-($B$14-0.5))/$B$12)^$B$13))*$B$11</f>
+        <v>1.3563306734076795E-6</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <f>C19+0.25</f>
+        <v>0.25</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B21">
-        <f t="shared" ref="B21:B84" si="0">(1-EXP(-((C21/$B$16-($B$15-0.5))/$B$13)^$B$14))*$B$12</f>
-        <v>1.3563306734076795E-6</v>
+        <f t="shared" si="0"/>
+        <v>1.0850301995346534E-5</v>
       </c>
       <c r="C21">
-        <f>C20+0.25</f>
-        <v>0.25</v>
+        <f t="shared" ref="C21:C84" si="1">C20+0.25</f>
+        <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>1.0850301995346534E-5</v>
+        <v>3.6616623765417522E-5</v>
       </c>
       <c r="C22">
-        <f t="shared" ref="C22:C85" si="1">C21+0.25</f>
-        <v>0.5</v>
+        <f t="shared" si="1"/>
+        <v>0.75</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>3.6616623765417522E-5</v>
+        <v>8.6780443051764905E-5</v>
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>8.6780443051764905E-5</v>
+        <v>1.6944632170386997E-4</v>
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.25</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>1.6944632170386997E-4</v>
+        <v>2.926828338786713E-4</v>
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>2.926828338786713E-4</v>
+        <v>4.6450282648525794E-4</v>
       </c>
       <c r="C26">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>4.6450282648525794E-4</v>
+        <v>6.9283941201358503E-4</v>
       </c>
       <c r="C27">
         <f t="shared" si="1"/>
-        <v>1.75</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>6.9283941201358503E-4</v>
+        <v>9.8551779614576844E-4</v>
       </c>
       <c r="C28">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>9.8551779614576844E-4</v>
+        <v>1.3502230815962135E-3</v>
       </c>
       <c r="C29">
         <f t="shared" si="1"/>
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>1.3502230815962135E-3</v>
+        <v>1.7944642344303095E-3</v>
       </c>
       <c r="C30">
         <f t="shared" si="1"/>
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>1.7944642344303095E-3</v>
+        <v>2.325534449188732E-3</v>
       </c>
       <c r="C31">
         <f t="shared" si="1"/>
-        <v>2.75</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>2.325534449188732E-3</v>
+        <v>2.9504682038741957E-3</v>
       </c>
       <c r="C32">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>3.25</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B33">
         <f t="shared" si="0"/>
-        <v>2.9504682038741957E-3</v>
+        <v>3.6759953544767184E-3</v>
       </c>
       <c r="C33">
         <f t="shared" si="1"/>
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34">
         <f t="shared" si="0"/>
-        <v>3.6759953544767184E-3</v>
+        <v>4.5084926802983977E-3</v>
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B35">
         <f t="shared" si="0"/>
-        <v>4.5084926802983977E-3</v>
+        <v>5.4539333548070607E-3</v>
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
-        <v>3.75</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B36">
         <f t="shared" si="0"/>
-        <v>5.4539333548070607E-3</v>
+        <v>6.5178348808602399E-3</v>
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>4.25</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B37">
         <f t="shared" si="0"/>
-        <v>6.5178348808602399E-3</v>
+        <v>7.7052060925004657E-3</v>
       </c>
       <c r="C37">
         <f t="shared" si="1"/>
-        <v>4.25</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B38">
         <f t="shared" si="0"/>
-        <v>7.7052060925004657E-3</v>
+        <v>9.0204938865930274E-3</v>
       </c>
       <c r="C38">
         <f t="shared" si="1"/>
-        <v>4.5</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B39">
         <f t="shared" si="0"/>
-        <v>9.0204938865930274E-3</v>
+        <v>1.0467530404697972E-2</v>
       </c>
       <c r="C39">
         <f t="shared" si="1"/>
-        <v>4.75</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B40">
         <f t="shared" si="0"/>
-        <v>1.0467530404697972E-2</v>
+        <v>1.2049481436979681E-2</v>
       </c>
       <c r="C40">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B41">
         <f t="shared" si="0"/>
-        <v>1.2049481436979681E-2</v>
+        <v>1.3768796863832604E-2</v>
       </c>
       <c r="C41">
         <f t="shared" si="1"/>
-        <v>5.25</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B42">
         <f t="shared" si="0"/>
-        <v>1.3768796863832604E-2</v>
+        <v>1.5627163985386609E-2</v>
       </c>
       <c r="C42">
         <f t="shared" si="1"/>
-        <v>5.5</v>
+        <v>5.75</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B43">
         <f t="shared" si="0"/>
-        <v>1.5627163985386609E-2</v>
+        <v>1.7625464612310682E-2</v>
       </c>
       <c r="C43">
         <f t="shared" si="1"/>
-        <v>5.75</v>
+        <v>6</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B44">
         <f t="shared" si="0"/>
-        <v>1.7625464612310682E-2</v>
+        <v>1.9763736801589746E-2</v>
       </c>
       <c r="C44">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B45">
         <f t="shared" si="0"/>
-        <v>1.9763736801589746E-2</v>
+        <v>2.2041142116558832E-2</v>
       </c>
       <c r="C45">
         <f t="shared" si="1"/>
-        <v>6.25</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B46">
         <f t="shared" si="0"/>
-        <v>2.2041142116558832E-2</v>
+        <v>2.4455939269979066E-2</v>
       </c>
       <c r="C46">
         <f t="shared" si="1"/>
-        <v>6.5</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B47">
         <f t="shared" si="0"/>
-        <v>2.4455939269979066E-2</v>
+        <v>2.7005464971113717E-2</v>
       </c>
       <c r="C47">
         <f t="shared" si="1"/>
-        <v>6.75</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B48">
         <f t="shared" si="0"/>
-        <v>2.7005464971113717E-2</v>
+        <v>2.9686122741700537E-2</v>
       </c>
       <c r="C48">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>7.25</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B49">
         <f t="shared" si="0"/>
-        <v>2.9686122741700537E-2</v>
+        <v>3.249338039087727E-2</v>
       </c>
       <c r="C49">
         <f t="shared" si="1"/>
-        <v>7.25</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B50">
         <f t="shared" si="0"/>
-        <v>3.249338039087727E-2</v>
+        <v>3.5421776745385977E-2</v>
       </c>
       <c r="C50">
         <f t="shared" si="1"/>
-        <v>7.5</v>
+        <v>7.75</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B51">
         <f t="shared" si="0"/>
-        <v>3.5421776745385977E-2</v>
+        <v>3.8464938119114063E-2</v>
       </c>
       <c r="C51">
         <f t="shared" si="1"/>
-        <v>7.75</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B52">
         <f t="shared" si="0"/>
-        <v>3.8464938119114063E-2</v>
+        <v>4.1615604876098174E-2</v>
       </c>
       <c r="C52">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>8.25</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B53">
         <f t="shared" si="0"/>
-        <v>4.1615604876098174E-2</v>
+        <v>4.4865668294935525E-2</v>
       </c>
       <c r="C53">
         <f t="shared" si="1"/>
-        <v>8.25</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B54">
         <f t="shared" si="0"/>
-        <v>4.4865668294935525E-2</v>
+        <v>4.820621778208041E-2</v>
       </c>
       <c r="C54">
         <f t="shared" si="1"/>
-        <v>8.5</v>
+        <v>8.75</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B55">
         <f t="shared" si="0"/>
-        <v>4.820621778208041E-2</v>
+        <v>5.1627598309274762E-2</v>
       </c>
       <c r="C55">
         <f t="shared" si="1"/>
-        <v>8.75</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B56">
         <f t="shared" si="0"/>
-        <v>5.1627598309274762E-2</v>
+        <v>5.5119477769415316E-2</v>
       </c>
       <c r="C56">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>9.25</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B57">
         <f t="shared" si="0"/>
-        <v>5.5119477769415316E-2</v>
+        <v>5.8670923759033294E-2</v>
       </c>
       <c r="C57">
         <f t="shared" si="1"/>
-        <v>9.25</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B58">
         <f t="shared" si="0"/>
-        <v>5.8670923759033294E-2</v>
+        <v>6.2270489108216164E-2</v>
       </c>
       <c r="C58">
         <f t="shared" si="1"/>
-        <v>9.5</v>
+        <v>9.75</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B59">
         <f t="shared" si="0"/>
-        <v>6.2270489108216164E-2</v>
+        <v>6.5906305294534395E-2</v>
       </c>
       <c r="C59">
         <f t="shared" si="1"/>
-        <v>9.75</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B60">
         <f t="shared" si="0"/>
-        <v>6.5906305294534395E-2</v>
+        <v>6.9566182700893778E-2</v>
       </c>
       <c r="C60">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>10.25</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B61">
         <f t="shared" si="0"/>
-        <v>6.9566182700893778E-2</v>
+        <v>7.3237716512875015E-2</v>
       </c>
       <c r="C61">
         <f t="shared" si="1"/>
-        <v>10.25</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B62">
         <f t="shared" si="0"/>
-        <v>7.3237716512875015E-2</v>
+        <v>7.6908396903694956E-2</v>
       </c>
       <c r="C62">
         <f t="shared" si="1"/>
-        <v>10.5</v>
+        <v>10.75</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B63">
         <f t="shared" si="0"/>
-        <v>7.6908396903694956E-2</v>
+        <v>8.0565722028919276E-2</v>
       </c>
       <c r="C63">
         <f t="shared" si="1"/>
-        <v>10.75</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B64">
         <f t="shared" si="0"/>
-        <v>8.0565722028919276E-2</v>
+        <v>8.4197312252647025E-2</v>
       </c>
       <c r="C64">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>11.25</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B65">
         <f t="shared" si="0"/>
-        <v>8.4197312252647025E-2</v>
+        <v>8.7791023955795813E-2</v>
       </c>
       <c r="C65">
         <f t="shared" si="1"/>
-        <v>11.25</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B66">
         <f t="shared" si="0"/>
-        <v>8.7791023955795813E-2</v>
+        <v>9.1335061238442886E-2</v>
       </c>
       <c r="C66">
         <f t="shared" si="1"/>
-        <v>11.5</v>
+        <v>11.75</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B67">
         <f t="shared" si="0"/>
-        <v>9.1335061238442886E-2</v>
+        <v>9.4818083824283653E-2</v>
       </c>
       <c r="C67">
         <f t="shared" si="1"/>
-        <v>11.75</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B68">
         <f t="shared" si="0"/>
-        <v>9.4818083824283653E-2</v>
+        <v>9.8229309507649534E-2</v>
       </c>
       <c r="C68">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>12.25</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B69">
         <f t="shared" si="0"/>
-        <v>9.8229309507649534E-2</v>
+        <v>0.10155860955271043</v>
       </c>
       <c r="C69">
         <f t="shared" si="1"/>
-        <v>12.25</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B70">
         <f t="shared" si="0"/>
-        <v>0.10155860955271043</v>
+        <v>0.10479659555998135</v>
       </c>
       <c r="C70">
         <f t="shared" si="1"/>
-        <v>12.5</v>
+        <v>12.75</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B71">
         <f t="shared" si="0"/>
-        <v>0.10479659555998135</v>
+        <v>0.10793469645549059</v>
       </c>
       <c r="C71">
         <f t="shared" si="1"/>
-        <v>12.75</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B72">
         <f t="shared" si="0"/>
-        <v>0.10793469645549059</v>
+        <v>0.11096522443033115</v>
       </c>
       <c r="C72">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>13.25</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B73">
         <f t="shared" si="0"/>
-        <v>0.11096522443033115</v>
+        <v>0.11388142885916275</v>
       </c>
       <c r="C73">
         <f t="shared" si="1"/>
-        <v>13.25</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B74">
         <f t="shared" si="0"/>
-        <v>0.11388142885916275</v>
+        <v>0.11667753745097514</v>
       </c>
       <c r="C74">
         <f t="shared" si="1"/>
-        <v>13.5</v>
+        <v>13.75</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B75">
         <f t="shared" si="0"/>
-        <v>0.11667753745097514</v>
+        <v>0.11934878412866376</v>
       </c>
       <c r="C75">
         <f t="shared" si="1"/>
-        <v>13.75</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B76">
         <f t="shared" si="0"/>
-        <v>0.11934878412866376</v>
+        <v>0.12189142338962897</v>
       </c>
       <c r="C76">
         <f t="shared" si="1"/>
-        <v>14</v>
+        <v>14.25</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B77">
         <f t="shared" si="0"/>
-        <v>0.12189142338962897</v>
+        <v>0.12430273116113988</v>
       </c>
       <c r="C77">
         <f t="shared" si="1"/>
-        <v>14.25</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B78">
         <f t="shared" si="0"/>
-        <v>0.12430273116113988</v>
+        <v>0.12658099242476617</v>
       </c>
       <c r="C78">
         <f t="shared" si="1"/>
-        <v>14.5</v>
+        <v>14.75</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B79">
         <f t="shared" si="0"/>
-        <v>0.12658099242476617</v>
+        <v>0.12872547613689861</v>
       </c>
       <c r="C79">
         <f t="shared" si="1"/>
-        <v>14.75</v>
+        <v>15</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B80">
         <f t="shared" si="0"/>
-        <v>0.12872547613689861</v>
+        <v>0.13073639821054656</v>
       </c>
       <c r="C80">
         <f t="shared" si="1"/>
-        <v>15</v>
+        <v>15.25</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B81">
         <f t="shared" si="0"/>
-        <v>0.13073639821054656</v>
+        <v>0.13261487354093182</v>
       </c>
       <c r="C81">
         <f t="shared" si="1"/>
-        <v>15.25</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B82">
         <f t="shared" si="0"/>
-        <v>0.13261487354093182</v>
+        <v>0.13436285824823427</v>
       </c>
       <c r="C82">
         <f t="shared" si="1"/>
-        <v>15.5</v>
+        <v>15.75</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B83">
         <f t="shared" si="0"/>
-        <v>0.13436285824823427</v>
+        <v>0.1359830834703562</v>
       </c>
       <c r="C83">
         <f t="shared" si="1"/>
-        <v>15.75</v>
+        <v>16</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B84">
-        <f t="shared" si="0"/>
-        <v>0.1359830834703562</v>
+        <f t="shared" ref="B84:B120" si="2">(1-EXP(-((C84/$B$15-($B$14-0.5))/$B$12)^$B$13))*$B$11</f>
+        <v>0.13747898216292775</v>
       </c>
       <c r="C84">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>16.25</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B85">
-        <f t="shared" ref="B85:B121" si="2">(1-EXP(-((C85/$B$16-($B$15-0.5))/$B$13)^$B$14))*$B$12</f>
-        <v>0.13747898216292775</v>
+        <f t="shared" si="2"/>
+        <v>0.13885461045027209</v>
       </c>
       <c r="C85">
-        <f t="shared" si="1"/>
-        <v>16.25</v>
+        <f t="shared" ref="C85:C120" si="3">C84+0.25</f>
+        <v>16.5</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B86">
         <f t="shared" si="2"/>
-        <v>0.13885461045027209</v>
+        <v>0.14011456511819612</v>
       </c>
       <c r="C86">
-        <f t="shared" ref="C86:C121" si="3">C85+0.25</f>
-        <v>16.5</v>
+        <f t="shared" si="3"/>
+        <v>16.75</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B87">
         <f t="shared" si="2"/>
-        <v>0.14011456511819612</v>
+        <v>0.14126389884704021</v>
       </c>
       <c r="C87">
         <f t="shared" si="3"/>
-        <v>16.75</v>
+        <v>17</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B88">
         <f t="shared" si="2"/>
-        <v>0.14126389884704021</v>
+        <v>0.1423080347524181</v>
       </c>
       <c r="C88">
         <f t="shared" si="3"/>
-        <v>17</v>
+        <v>17.25</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B89">
         <f t="shared" si="2"/>
-        <v>0.1423080347524181</v>
+        <v>0.14325268173371089</v>
       </c>
       <c r="C89">
         <f t="shared" si="3"/>
-        <v>17.25</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B90">
         <f t="shared" si="2"/>
-        <v>0.14325268173371089</v>
+        <v>0.14410375202992939</v>
       </c>
       <c r="C90">
         <f t="shared" si="3"/>
-        <v>17.5</v>
+        <v>17.75</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B91">
         <f t="shared" si="2"/>
-        <v>0.14410375202992939</v>
+        <v>0.1448672822532501</v>
       </c>
       <c r="C91">
         <f t="shared" si="3"/>
-        <v>17.75</v>
+        <v>18</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B92">
         <f t="shared" si="2"/>
-        <v>0.1448672822532501</v>
+        <v>0.14554935901734684</v>
       </c>
       <c r="C92">
         <f t="shared" si="3"/>
-        <v>18</v>
+        <v>18.25</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B93">
         <f t="shared" si="2"/>
-        <v>0.14554935901734684</v>
+        <v>0.14615605010611638</v>
       </c>
       <c r="C93">
         <f t="shared" si="3"/>
-        <v>18.25</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B94">
         <f t="shared" si="2"/>
-        <v>0.14615605010611638</v>
+        <v>0.14669334194440264</v>
       </c>
       <c r="C94">
         <f t="shared" si="3"/>
-        <v>18.5</v>
+        <v>18.75</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B95">
         <f t="shared" si="2"/>
-        <v>0.14669334194440264</v>
+        <v>0.14716708394183772</v>
       </c>
       <c r="C95">
         <f t="shared" si="3"/>
-        <v>18.75</v>
+        <v>19</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B96">
         <f t="shared" si="2"/>
-        <v>0.14716708394183772</v>
+        <v>0.14758294008979489</v>
       </c>
       <c r="C96">
         <f t="shared" si="3"/>
-        <v>19</v>
+        <v>19.25</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B97">
         <f t="shared" si="2"/>
-        <v>0.14758294008979489</v>
+        <v>0.1479463480052261</v>
       </c>
       <c r="C97">
         <f t="shared" si="3"/>
-        <v>19.25</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B98">
         <f t="shared" si="2"/>
-        <v>0.1479463480052261</v>
+        <v>0.14826248543885948</v>
       </c>
       <c r="C98">
         <f t="shared" si="3"/>
-        <v>19.5</v>
+        <v>19.75</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B99">
         <f t="shared" si="2"/>
-        <v>0.14826248543885948</v>
+        <v>0.14853624410321731</v>
       </c>
       <c r="C99">
         <f t="shared" si="3"/>
-        <v>19.75</v>
+        <v>20</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B100">
         <f t="shared" si="2"/>
-        <v>0.14853624410321731</v>
+        <v>0.1487722105317654</v>
       </c>
       <c r="C100">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>20.25</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B101">
         <f t="shared" si="2"/>
-        <v>0.1487722105317654</v>
+        <v>0.14897465355692657</v>
       </c>
       <c r="C101">
         <f t="shared" si="3"/>
-        <v>20.25</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B102">
         <f t="shared" si="2"/>
-        <v>0.14897465355692657</v>
+        <v>0.14914751789350353</v>
       </c>
       <c r="C102">
         <f t="shared" si="3"/>
-        <v>20.5</v>
+        <v>20.75</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B103">
         <f t="shared" si="2"/>
-        <v>0.14914751789350353</v>
+        <v>0.14929442323616438</v>
       </c>
       <c r="C103">
         <f t="shared" si="3"/>
-        <v>20.75</v>
+        <v>21</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B104">
         <f t="shared" si="2"/>
-        <v>0.14929442323616438</v>
+        <v>0.14941866822510363</v>
       </c>
       <c r="C104">
         <f t="shared" si="3"/>
-        <v>21</v>
+        <v>21.25</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B105">
         <f t="shared" si="2"/>
-        <v>0.14941866822510363</v>
+        <v>0.14952323860205774</v>
       </c>
       <c r="C105">
         <f t="shared" si="3"/>
-        <v>21.25</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B106">
         <f t="shared" si="2"/>
-        <v>0.14952323860205774</v>
+        <v>0.14961081886809813</v>
       </c>
       <c r="C106">
         <f t="shared" si="3"/>
-        <v>21.5</v>
+        <v>21.75</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B107">
         <f t="shared" si="2"/>
-        <v>0.14961081886809813</v>
+        <v>0.14968380676304538</v>
       </c>
       <c r="C107">
         <f t="shared" si="3"/>
-        <v>21.75</v>
+        <v>22</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B108">
         <f t="shared" si="2"/>
-        <v>0.14968380676304538</v>
+        <v>0.14974432991149983</v>
       </c>
       <c r="C108">
         <f t="shared" si="3"/>
-        <v>22</v>
+        <v>22.25</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B109">
         <f t="shared" si="2"/>
-        <v>0.14974432991149983</v>
+        <v>0.14979426401963158</v>
       </c>
       <c r="C109">
         <f t="shared" si="3"/>
-        <v>22.25</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B110">
         <f t="shared" si="2"/>
-        <v>0.14979426401963158</v>
+        <v>0.14983525205710502</v>
       </c>
       <c r="C110">
         <f t="shared" si="3"/>
-        <v>22.5</v>
+        <v>22.75</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B111">
         <f t="shared" si="2"/>
-        <v>0.14983525205710502</v>
+        <v>0.14986872391689912</v>
       </c>
       <c r="C111">
         <f t="shared" si="3"/>
-        <v>22.75</v>
+        <v>23</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B112">
         <f t="shared" si="2"/>
-        <v>0.14986872391689912</v>
+        <v>0.14989591610946901</v>
       </c>
       <c r="C112">
         <f t="shared" si="3"/>
-        <v>23</v>
+        <v>23.25</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B113">
         <f t="shared" si="2"/>
-        <v>0.14989591610946901</v>
+        <v>0.14991789111400722</v>
       </c>
       <c r="C113">
         <f t="shared" si="3"/>
-        <v>23.25</v>
+        <v>23.5</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B114">
         <f t="shared" si="2"/>
-        <v>0.14991789111400722</v>
+        <v>0.14993555607610648</v>
       </c>
       <c r="C114">
         <f t="shared" si="3"/>
-        <v>23.5</v>
+        <v>23.75</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B115">
         <f t="shared" si="2"/>
-        <v>0.14993555607610648</v>
+        <v>0.14994968060581462</v>
       </c>
       <c r="C115">
         <f t="shared" si="3"/>
-        <v>23.75</v>
+        <v>24</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B116">
         <f t="shared" si="2"/>
-        <v>0.14994968060581462</v>
+        <v>0.14996091349119239</v>
       </c>
       <c r="C116">
         <f t="shared" si="3"/>
-        <v>24</v>
+        <v>24.25</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B117">
         <f t="shared" si="2"/>
-        <v>0.14996091349119239</v>
+        <v>0.14996979819869544</v>
       </c>
       <c r="C117">
         <f t="shared" si="3"/>
-        <v>24.25</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B118">
         <f t="shared" si="2"/>
-        <v>0.14996979819869544</v>
+        <v>0.14997678708203718</v>
       </c>
       <c r="C118">
         <f t="shared" si="3"/>
-        <v>24.5</v>
+        <v>24.75</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B119">
         <f t="shared" si="2"/>
-        <v>0.14997678708203718</v>
+        <v>0.14998225426504705</v>
       </c>
       <c r="C119">
         <f t="shared" si="3"/>
-        <v>24.75</v>
+        <v>25</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B120">
         <f t="shared" si="2"/>
-        <v>0.14998225426504705</v>
+        <v>0.14998650720113471</v>
       </c>
       <c r="C120">
-        <f t="shared" si="3"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B121">
-        <f t="shared" si="2"/>
-        <v>0.14998650720113471</v>
-      </c>
-      <c r="C121">
         <f t="shared" si="3"/>
         <v>25.25</v>
       </c>
@@ -5400,337 +5392,337 @@
         <v>3</v>
       </c>
       <c r="B1">
-        <f>(1-EXP(-((B2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((B2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0</v>
       </c>
       <c r="C1">
-        <f>(1-EXP(-((C2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((C2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>1.3563306734076795E-6</v>
       </c>
       <c r="D1">
-        <f>(1-EXP(-((D2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((D2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>1.0850301995346534E-5</v>
       </c>
       <c r="E1">
-        <f>(1-EXP(-((E2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((E2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>3.6616623765417522E-5</v>
       </c>
       <c r="F1">
-        <f>(1-EXP(-((F2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((F2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>8.6780443051764905E-5</v>
       </c>
       <c r="G1">
-        <f>(1-EXP(-((G2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((G2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>1.6944632170386997E-4</v>
       </c>
       <c r="H1">
-        <f>(1-EXP(-((H2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((H2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>2.926828338786713E-4</v>
       </c>
       <c r="I1">
-        <f>(1-EXP(-((I2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((I2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>4.6450282648525794E-4</v>
       </c>
       <c r="J1">
-        <f>(1-EXP(-((J2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((J2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>6.9283941201358503E-4</v>
       </c>
       <c r="K1">
-        <f>(1-EXP(-((K2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((K2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>9.8551779614576844E-4</v>
       </c>
       <c r="L1">
-        <f>(1-EXP(-((L2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((L2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>1.3502230815962135E-3</v>
       </c>
       <c r="M1">
-        <f>(1-EXP(-((M2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((M2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>1.7944642344303095E-3</v>
       </c>
       <c r="N1">
-        <f>(1-EXP(-((N2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((N2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>2.325534449188732E-3</v>
       </c>
       <c r="O1">
-        <f>(1-EXP(-((O2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((O2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>2.9504682038741957E-3</v>
       </c>
       <c r="P1">
-        <f>(1-EXP(-((P2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((P2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>3.6759953544767184E-3</v>
       </c>
       <c r="Q1">
-        <f>(1-EXP(-((Q2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((Q2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>4.5084926802983977E-3</v>
       </c>
       <c r="R1">
-        <f>(1-EXP(-((R2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((R2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>5.4539333548070607E-3</v>
       </c>
       <c r="S1">
-        <f>(1-EXP(-((S2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((S2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>6.5178348808602399E-3</v>
       </c>
       <c r="T1">
-        <f>(1-EXP(-((T2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((T2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>7.7052060925004657E-3</v>
       </c>
       <c r="U1">
-        <f>(1-EXP(-((U2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((U2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>9.0204938865930274E-3</v>
       </c>
       <c r="V1">
-        <f>(1-EXP(-((V2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((V2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>1.0467530404697972E-2</v>
       </c>
       <c r="W1">
-        <f>(1-EXP(-((W2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((W2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>1.2049481436979681E-2</v>
       </c>
       <c r="X1">
-        <f>(1-EXP(-((X2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((X2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>1.3768796863832604E-2</v>
       </c>
       <c r="Y1">
-        <f>(1-EXP(-((Y2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((Y2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>1.5627163985386609E-2</v>
       </c>
       <c r="Z1">
-        <f>(1-EXP(-((Z2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((Z2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>1.7625464612310682E-2</v>
       </c>
       <c r="AA1">
-        <f>(1-EXP(-((AA2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AA2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>1.9763736801589746E-2</v>
       </c>
       <c r="AB1">
-        <f>(1-EXP(-((AB2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AB2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>2.2041142116558832E-2</v>
       </c>
       <c r="AC1">
-        <f>(1-EXP(-((AC2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AC2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>2.4455939269979066E-2</v>
       </c>
       <c r="AD1">
-        <f>(1-EXP(-((AD2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AD2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>2.7005464971113717E-2</v>
       </c>
       <c r="AE1">
-        <f>(1-EXP(-((AE2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AE2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>2.9686122741700537E-2</v>
       </c>
       <c r="AF1">
-        <f>(1-EXP(-((AF2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AF2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>3.249338039087727E-2</v>
       </c>
       <c r="AG1">
-        <f>(1-EXP(-((AG2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AG2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>3.5421776745385977E-2</v>
       </c>
       <c r="AH1">
-        <f>(1-EXP(-((AH2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AH2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>3.8464938119114063E-2</v>
       </c>
       <c r="AI1">
-        <f>(1-EXP(-((AI2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AI2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>4.1615604876098174E-2</v>
       </c>
       <c r="AJ1">
-        <f>(1-EXP(-((AJ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AJ2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>4.4865668294935525E-2</v>
       </c>
       <c r="AK1">
-        <f>(1-EXP(-((AK2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AK2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>4.820621778208041E-2</v>
       </c>
       <c r="AL1">
-        <f>(1-EXP(-((AL2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AL2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>5.1627598309274762E-2</v>
       </c>
       <c r="AM1">
-        <f>(1-EXP(-((AM2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AM2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>5.5119477769415316E-2</v>
       </c>
       <c r="AN1">
-        <f>(1-EXP(-((AN2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AN2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>5.8670923759033294E-2</v>
       </c>
       <c r="AO1">
-        <f>(1-EXP(-((AO2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AO2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>6.2270489108216164E-2</v>
       </c>
       <c r="AP1">
-        <f>(1-EXP(-((AP2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AP2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>6.5906305294534395E-2</v>
       </c>
       <c r="AQ1">
-        <f>(1-EXP(-((AQ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AQ2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>6.9566182700893778E-2</v>
       </c>
       <c r="AR1">
-        <f>(1-EXP(-((AR2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AR2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>7.3237716512875015E-2</v>
       </c>
       <c r="AS1">
-        <f>(1-EXP(-((AS2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AS2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>7.6908396903694956E-2</v>
       </c>
       <c r="AT1">
-        <f>(1-EXP(-((AT2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AT2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>8.0565722028919276E-2</v>
       </c>
       <c r="AU1">
-        <f>(1-EXP(-((AU2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AU2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>8.4197312252647025E-2</v>
       </c>
       <c r="AV1">
-        <f>(1-EXP(-((AV2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AV2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>8.7791023955795813E-2</v>
       </c>
       <c r="AW1">
-        <f>(1-EXP(-((AW2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AW2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>9.1335061238442886E-2</v>
       </c>
       <c r="AX1">
-        <f>(1-EXP(-((AX2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AX2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>9.4818083824283653E-2</v>
       </c>
       <c r="AY1">
-        <f>(1-EXP(-((AY2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AY2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>9.8229309507649534E-2</v>
       </c>
       <c r="AZ1">
-        <f>(1-EXP(-((AZ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((AZ2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.10155860955271043</v>
       </c>
       <c r="BA1">
-        <f>(1-EXP(-((BA2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BA2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.10479659555998135</v>
       </c>
       <c r="BB1">
-        <f>(1-EXP(-((BB2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BB2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.10793469645549059</v>
       </c>
       <c r="BC1">
-        <f>(1-EXP(-((BC2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BC2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.11096522443033115</v>
       </c>
       <c r="BD1">
-        <f>(1-EXP(-((BD2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BD2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.11388142885916275</v>
       </c>
       <c r="BE1">
-        <f>(1-EXP(-((BE2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BE2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.11667753745097514</v>
       </c>
       <c r="BF1">
-        <f>(1-EXP(-((BF2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BF2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.11934878412866376</v>
       </c>
       <c r="BG1">
-        <f>(1-EXP(-((BG2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BG2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.12189142338962897</v>
       </c>
       <c r="BH1">
-        <f>(1-EXP(-((BH2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BH2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.12430273116113988</v>
       </c>
       <c r="BI1">
-        <f>(1-EXP(-((BI2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BI2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.12658099242476617</v>
       </c>
       <c r="BJ1">
-        <f>(1-EXP(-((BJ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BJ2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.12872547613689861</v>
       </c>
       <c r="BK1">
-        <f>(1-EXP(-((BK2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BK2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.13073639821054656</v>
       </c>
       <c r="BL1">
-        <f>(1-EXP(-((BL2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BL2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.13261487354093182</v>
       </c>
       <c r="BM1">
-        <f>(1-EXP(-((BM2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BM2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.13436285824823427</v>
       </c>
       <c r="BN1">
-        <f>(1-EXP(-((BN2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BN2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.1359830834703562</v>
       </c>
       <c r="BO1">
-        <f>(1-EXP(-((BO2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BO2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.13747898216292775</v>
       </c>
       <c r="BP1">
-        <f>(1-EXP(-((BP2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BP2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.13885461045027209</v>
       </c>
       <c r="BQ1">
-        <f>(1-EXP(-((BQ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BQ2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.14011456511819612</v>
       </c>
       <c r="BR1">
-        <f>(1-EXP(-((BR2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BR2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.14126389884704021</v>
       </c>
       <c r="BS1">
-        <f>(1-EXP(-((BS2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BS2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.1423080347524181</v>
       </c>
       <c r="BT1">
-        <f>(1-EXP(-((BT2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BT2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.14325268173371089</v>
       </c>
       <c r="BU1">
-        <f>(1-EXP(-((BU2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BU2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.14410375202992939</v>
       </c>
       <c r="BV1">
-        <f>(1-EXP(-((BV2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BV2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.1448672822532501</v>
       </c>
       <c r="BW1">
-        <f>(1-EXP(-((BW2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BW2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.14554935901734684</v>
       </c>
       <c r="BX1">
-        <f>(1-EXP(-((BX2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BX2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.14615605010611638</v>
       </c>
       <c r="BY1">
-        <f>(1-EXP(-((BY2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BY2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.14669334194440264</v>
       </c>
       <c r="BZ1">
-        <f>(1-EXP(-((BZ2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((BZ2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.14716708394183772</v>
       </c>
       <c r="CA1">
-        <f>(1-EXP(-((CA2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((CA2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.14758294008979489</v>
       </c>
       <c r="CB1">
-        <f>(1-EXP(-((CB2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((CB2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.1479463480052261</v>
       </c>
       <c r="CC1">
-        <f>(1-EXP(-((CC2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((CC2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.14826248543885948</v>
       </c>
       <c r="CD1">
-        <f>(1-EXP(-((CD2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((CD2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.14853624410321731</v>
       </c>
       <c r="CE1">
-        <f>(1-EXP(-((CE2/About!$B$16-(About!$B$15-0.5))/About!$B$13)^About!$B$14))*About!$B$12</f>
+        <f>(1-EXP(-((CE2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
         <v>0.15</v>
       </c>
     </row>
     <row r="2" spans="1:83" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -6083,12 +6075,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2">
         <v>0.02</v>

</xml_diff>

<commit_message>
CCS electricity calibration edits
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF55D05-AAEC-4547-8908-FD5E1D83DFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C9E6D6-E9ED-400A-B5BE-DB8123CDB372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="6690" windowWidth="24240" windowHeight="13020" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
@@ -606,307 +606,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>1.3563306734076795E-6</c:v>
+                  <c:v>1.1302755611730664E-6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0850301995346534E-5</c:v>
+                  <c:v>9.041918329455445E-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.6616623765417522E-5</c:v>
+                  <c:v>3.0513853137847935E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.6780443051764905E-5</c:v>
+                  <c:v>7.2317035876470759E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6944632170386997E-4</c:v>
+                  <c:v>1.4120526808655831E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.926828338786713E-4</c:v>
+                  <c:v>2.4390236156555944E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.6450282648525794E-4</c:v>
+                  <c:v>3.8708568873771498E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.9283941201358503E-4</c:v>
+                  <c:v>5.7736617667798751E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.8551779614576844E-4</c:v>
+                  <c:v>8.2126483012147367E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.3502230815962135E-3</c:v>
+                  <c:v>1.1251859013301779E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.7944642344303095E-3</c:v>
+                  <c:v>1.4953868620252581E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.325534449188732E-3</c:v>
+                  <c:v>1.9379453743239433E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.9504682038741957E-3</c:v>
+                  <c:v>2.4587235032284965E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.6759953544767184E-3</c:v>
+                  <c:v>3.0633294620639323E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.5084926802983977E-3</c:v>
+                  <c:v>3.7570772335819985E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.4539333548070607E-3</c:v>
+                  <c:v>4.5449444623392177E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.5178348808602399E-3</c:v>
+                  <c:v>5.4315290673835337E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.7052060925004657E-3</c:v>
+                  <c:v>6.4210050770837218E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.0204938865930274E-3</c:v>
+                  <c:v>7.5170782388275237E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.0467530404697972E-2</c:v>
+                  <c:v>8.7229420039149769E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.2049481436979681E-2</c:v>
+                  <c:v>1.0041234530816401E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.3768796863832604E-2</c:v>
+                  <c:v>1.1473997386527171E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.5627163985386609E-2</c:v>
+                  <c:v>1.3022636654488842E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.7625464612310682E-2</c:v>
+                  <c:v>1.4687887176925568E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.9763736801589746E-2</c:v>
+                  <c:v>1.6469780667991457E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.2041142116558832E-2</c:v>
+                  <c:v>1.8367618430465693E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.4455939269979066E-2</c:v>
+                  <c:v>2.0379949391649221E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.7005464971113717E-2</c:v>
+                  <c:v>2.2504554142594765E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.9686122741700537E-2</c:v>
+                  <c:v>2.4738435618083782E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.249338039087727E-2</c:v>
+                  <c:v>2.7077816992397724E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.5421776745385977E-2</c:v>
+                  <c:v>2.951814728782165E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.8464938119114063E-2</c:v>
+                  <c:v>3.2054115099261718E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.1615604876098174E-2</c:v>
+                  <c:v>3.467967073008181E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4.4865668294935525E-2</c:v>
+                  <c:v>3.7388056912446274E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4.820621778208041E-2</c:v>
+                  <c:v>4.0171848151733677E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>5.1627598309274762E-2</c:v>
+                  <c:v>4.3022998591062303E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>5.5119477769415316E-2</c:v>
+                  <c:v>4.5932898141179429E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>5.8670923759033294E-2</c:v>
+                  <c:v>4.8892436465861083E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>6.2270489108216164E-2</c:v>
+                  <c:v>5.1892074256846804E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>6.5906305294534395E-2</c:v>
+                  <c:v>5.4921921078778663E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>6.9566182700893778E-2</c:v>
+                  <c:v>5.7971818917411488E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>7.3237716512875015E-2</c:v>
+                  <c:v>6.1031430427395852E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>7.6908396903694956E-2</c:v>
+                  <c:v>6.4090330753079128E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>8.0565722028919276E-2</c:v>
+                  <c:v>6.7138101690766061E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>8.4197312252647025E-2</c:v>
+                  <c:v>7.0164426877205852E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>8.7791023955795813E-2</c:v>
+                  <c:v>7.3159186629829842E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>9.1335061238442886E-2</c:v>
+                  <c:v>7.6112551032035736E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>9.4818083824283653E-2</c:v>
+                  <c:v>7.9015069853569708E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>9.8229309507649534E-2</c:v>
+                  <c:v>8.1857757923041286E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.10155860955271043</c:v>
+                  <c:v>8.4632174627258694E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.10479659555998135</c:v>
+                  <c:v>8.7330496299984461E-2</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.10793469645549059</c:v>
+                  <c:v>8.9945580379575493E-2</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.11096522443033115</c:v>
+                  <c:v>9.2471020358609296E-2</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.11388142885916275</c:v>
+                  <c:v>9.4901190715968961E-2</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.11667753745097514</c:v>
+                  <c:v>9.7231281209145953E-2</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.11934878412866376</c:v>
+                  <c:v>9.9457320107219804E-2</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.12189142338962897</c:v>
+                  <c:v>0.10157618615802415</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.12430273116113988</c:v>
+                  <c:v>0.1035856093009499</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.12658099242476617</c:v>
+                  <c:v>0.10548416035397182</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.12872547613689861</c:v>
+                  <c:v>0.10727123011408218</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.13073639821054656</c:v>
+                  <c:v>0.10894699850878881</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.13261487354093182</c:v>
+                  <c:v>0.11051239461744319</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.13436285824823427</c:v>
+                  <c:v>0.11196904854019522</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.1359830834703562</c:v>
+                  <c:v>0.11331923622529684</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.13747898216292775</c:v>
+                  <c:v>0.11456581846910648</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.13885461045027209</c:v>
+                  <c:v>0.11571217537522674</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.14011456511819612</c:v>
+                  <c:v>0.11676213759849677</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.14126389884704021</c:v>
+                  <c:v>0.11771991570586685</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.1423080347524181</c:v>
+                  <c:v>0.11859002896034841</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.14325268173371089</c:v>
+                  <c:v>0.11937723477809242</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.14410375202992939</c:v>
+                  <c:v>0.12008646002494117</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.1448672822532501</c:v>
+                  <c:v>0.12072273521104175</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.14554935901734684</c:v>
+                  <c:v>0.12129113251445571</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.14615605010611638</c:v>
+                  <c:v>0.12179670842176366</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.14669334194440264</c:v>
+                  <c:v>0.12224445162033554</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.14716708394183772</c:v>
+                  <c:v>0.12263923661819812</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.14758294008979489</c:v>
+                  <c:v>0.12298578340816241</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.1479463480052261</c:v>
+                  <c:v>0.12328862333768843</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.14826248543885948</c:v>
+                  <c:v>0.12355207119904957</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.14853624410321731</c:v>
+                  <c:v>0.12378020341934777</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.1487722105317654</c:v>
+                  <c:v>0.1239768421098045</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.14897465355692657</c:v>
+                  <c:v>0.12414554463077215</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.14914751789350353</c:v>
+                  <c:v>0.12428959824458628</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.14929442323616438</c:v>
+                  <c:v>0.12441201936347031</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.14941866822510363</c:v>
+                  <c:v>0.12451555685425303</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.14952323860205774</c:v>
+                  <c:v>0.12460269883504811</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.14961081886809813</c:v>
+                  <c:v>0.12467568239008178</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.14968380676304538</c:v>
+                  <c:v>0.12473650563587114</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.14974432991149983</c:v>
+                  <c:v>0.12478694159291652</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.14979426401963158</c:v>
+                  <c:v>0.12482855334969299</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.14983525205710502</c:v>
+                  <c:v>0.12486271004758752</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.14986872391689912</c:v>
+                  <c:v>0.12489060326408261</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.14989591610946901</c:v>
+                  <c:v>0.12491326342455751</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.14991789111400722</c:v>
+                  <c:v>0.12493157592833935</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.14993555607610648</c:v>
+                  <c:v>0.12494629673008874</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.14994968060581462</c:v>
+                  <c:v>0.12495806717151219</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.14996091349119239</c:v>
+                  <c:v>0.12496742790932699</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.14996979819869544</c:v>
+                  <c:v>0.1249748318322462</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.14997678708203718</c:v>
+                  <c:v>0.12498065590169766</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>0.14998225426504705</c:v>
+                  <c:v>0.12498521188753921</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>0.14998650720113471</c:v>
+                  <c:v>0.1249887560009456</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1324,124 +1324,124 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3563306734076795E-6</c:v>
+                  <c:v>1.1302755611730664E-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0850301995346534E-5</c:v>
+                  <c:v>9.041918329455445E-6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.6616623765417522E-5</c:v>
+                  <c:v>3.0513853137847935E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.6780443051764905E-5</c:v>
+                  <c:v>7.2317035876470759E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6944632170386997E-4</c:v>
+                  <c:v>1.4120526808655831E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.926828338786713E-4</c:v>
+                  <c:v>2.4390236156555944E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.6450282648525794E-4</c:v>
+                  <c:v>3.8708568873771498E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.9283941201358503E-4</c:v>
+                  <c:v>5.7736617667798751E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.8551779614576844E-4</c:v>
+                  <c:v>8.2126483012147367E-4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.3502230815962135E-3</c:v>
+                  <c:v>1.1251859013301779E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.7944642344303095E-3</c:v>
+                  <c:v>1.4953868620252581E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.325534449188732E-3</c:v>
+                  <c:v>1.9379453743239433E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.9504682038741957E-3</c:v>
+                  <c:v>2.4587235032284965E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.6759953544767184E-3</c:v>
+                  <c:v>3.0633294620639323E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.5084926802983977E-3</c:v>
+                  <c:v>3.7570772335819985E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.4539333548070607E-3</c:v>
+                  <c:v>4.5449444623392177E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.5178348808602399E-3</c:v>
+                  <c:v>5.4315290673835337E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.7052060925004657E-3</c:v>
+                  <c:v>6.4210050770837218E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9.0204938865930274E-3</c:v>
+                  <c:v>7.5170782388275237E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.0467530404697972E-2</c:v>
+                  <c:v>8.7229420039149769E-3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.2049481436979681E-2</c:v>
+                  <c:v>1.0041234530816401E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.3768796863832604E-2</c:v>
+                  <c:v>1.1473997386527171E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.5627163985386609E-2</c:v>
+                  <c:v>1.3022636654488842E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.7625464612310682E-2</c:v>
+                  <c:v>1.4687887176925568E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.9763736801589746E-2</c:v>
+                  <c:v>1.6469780667991457E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.2041142116558832E-2</c:v>
+                  <c:v>1.8367618430465693E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.4455939269979066E-2</c:v>
+                  <c:v>2.0379949391649221E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.7005464971113717E-2</c:v>
+                  <c:v>2.2504554142594765E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.9686122741700537E-2</c:v>
+                  <c:v>2.4738435618083782E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.249338039087727E-2</c:v>
+                  <c:v>2.7077816992397724E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.5421776745385977E-2</c:v>
+                  <c:v>2.951814728782165E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.8464938119114063E-2</c:v>
+                  <c:v>3.2054115099261718E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4.1615604876098174E-2</c:v>
+                  <c:v>3.467967073008181E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4.4865668294935525E-2</c:v>
+                  <c:v>3.7388056912446274E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.820621778208041E-2</c:v>
+                  <c:v>4.0171848151733677E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>5.1627598309274762E-2</c:v>
+                  <c:v>4.3022998591062303E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>5.5119477769415316E-2</c:v>
+                  <c:v>4.5932898141179429E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>5.8670923759033294E-2</c:v>
+                  <c:v>4.8892436465861083E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>6.2270489108216164E-2</c:v>
+                  <c:v>5.1892074256846804E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>6.5906305294534395E-2</c:v>
+                  <c:v>5.4921921078778663E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1859,124 +1859,124 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3563306734076795E-6</c:v>
+                  <c:v>1.1302755611730664E-6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0850301995346534E-5</c:v>
+                  <c:v>9.041918329455445E-6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.6616623765417522E-5</c:v>
+                  <c:v>3.0513853137847935E-5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.6780443051764905E-5</c:v>
+                  <c:v>7.2317035876470759E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6944632170386997E-4</c:v>
+                  <c:v>1.4120526808655831E-4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.926828338786713E-4</c:v>
+                  <c:v>2.4390236156555944E-4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.6450282648525794E-4</c:v>
+                  <c:v>3.8708568873771498E-4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.9283941201358503E-4</c:v>
+                  <c:v>5.7736617667798751E-4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.8551779614576844E-4</c:v>
+                  <c:v>8.2126483012147367E-4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.3502230815962135E-3</c:v>
+                  <c:v>1.1251859013301779E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.7944642344303095E-3</c:v>
+                  <c:v>1.4953868620252581E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.325534449188732E-3</c:v>
+                  <c:v>1.9379453743239433E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.9504682038741957E-3</c:v>
+                  <c:v>2.4587235032284965E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.6759953544767184E-3</c:v>
+                  <c:v>3.0633294620639323E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.5084926802983977E-3</c:v>
+                  <c:v>3.7570772335819985E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.4539333548070607E-3</c:v>
+                  <c:v>4.5449444623392177E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.5178348808602399E-3</c:v>
+                  <c:v>5.4315290673835337E-3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.7052060925004657E-3</c:v>
+                  <c:v>6.4210050770837218E-3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9.0204938865930274E-3</c:v>
+                  <c:v>7.5170782388275237E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.0467530404697972E-2</c:v>
+                  <c:v>8.7229420039149769E-3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>1.2049481436979681E-2</c:v>
+                  <c:v>1.0041234530816401E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.3768796863832604E-2</c:v>
+                  <c:v>1.1473997386527171E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.5627163985386609E-2</c:v>
+                  <c:v>1.3022636654488842E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.7625464612310682E-2</c:v>
+                  <c:v>1.4687887176925568E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.9763736801589746E-2</c:v>
+                  <c:v>1.6469780667991457E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.2041142116558832E-2</c:v>
+                  <c:v>1.8367618430465693E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.4455939269979066E-2</c:v>
+                  <c:v>2.0379949391649221E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.7005464971113717E-2</c:v>
+                  <c:v>2.2504554142594765E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.9686122741700537E-2</c:v>
+                  <c:v>2.4738435618083782E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.249338039087727E-2</c:v>
+                  <c:v>2.7077816992397724E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.5421776745385977E-2</c:v>
+                  <c:v>2.951814728782165E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.8464938119114063E-2</c:v>
+                  <c:v>3.2054115099261718E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4.1615604876098174E-2</c:v>
+                  <c:v>3.467967073008181E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4.4865668294935525E-2</c:v>
+                  <c:v>3.7388056912446274E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.820621778208041E-2</c:v>
+                  <c:v>4.0171848151733677E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>5.1627598309274762E-2</c:v>
+                  <c:v>4.3022998591062303E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>5.5119477769415316E-2</c:v>
+                  <c:v>4.5932898141179429E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>5.8670923759033294E-2</c:v>
+                  <c:v>4.8892436465861083E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>6.2270489108216164E-2</c:v>
+                  <c:v>5.1892074256846804E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>6.5906305294534395E-2</c:v>
+                  <c:v>5.4921921078778663E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4262,8 +4262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3D2DEE-686E-48A0-AC3D-0F54DEA5D0EC}">
   <dimension ref="A1:C120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4310,7 +4310,7 @@
         <v>37</v>
       </c>
       <c r="B11">
-        <v>0.15</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -4357,7 +4357,7 @@
     <row r="20" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B20">
         <f t="shared" ref="B20:B83" si="0">(1-EXP(-((C20/$B$15-($B$14-0.5))/$B$12)^$B$13))*$B$11</f>
-        <v>1.3563306734076795E-6</v>
+        <v>1.1302755611730664E-6</v>
       </c>
       <c r="C20">
         <f>C19+0.25</f>
@@ -4367,7 +4367,7 @@
     <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>1.0850301995346534E-5</v>
+        <v>9.041918329455445E-6</v>
       </c>
       <c r="C21">
         <f t="shared" ref="C21:C84" si="1">C20+0.25</f>
@@ -4377,7 +4377,7 @@
     <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>3.6616623765417522E-5</v>
+        <v>3.0513853137847935E-5</v>
       </c>
       <c r="C22">
         <f t="shared" si="1"/>
@@ -4387,7 +4387,7 @@
     <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>8.6780443051764905E-5</v>
+        <v>7.2317035876470759E-5</v>
       </c>
       <c r="C23">
         <f t="shared" si="1"/>
@@ -4397,7 +4397,7 @@
     <row r="24" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>1.6944632170386997E-4</v>
+        <v>1.4120526808655831E-4</v>
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
@@ -4407,7 +4407,7 @@
     <row r="25" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>2.926828338786713E-4</v>
+        <v>2.4390236156555944E-4</v>
       </c>
       <c r="C25">
         <f t="shared" si="1"/>
@@ -4417,7 +4417,7 @@
     <row r="26" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>4.6450282648525794E-4</v>
+        <v>3.8708568873771498E-4</v>
       </c>
       <c r="C26">
         <f t="shared" si="1"/>
@@ -4427,7 +4427,7 @@
     <row r="27" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>6.9283941201358503E-4</v>
+        <v>5.7736617667798751E-4</v>
       </c>
       <c r="C27">
         <f t="shared" si="1"/>
@@ -4437,7 +4437,7 @@
     <row r="28" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>9.8551779614576844E-4</v>
+        <v>8.2126483012147367E-4</v>
       </c>
       <c r="C28">
         <f t="shared" si="1"/>
@@ -4447,7 +4447,7 @@
     <row r="29" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>1.3502230815962135E-3</v>
+        <v>1.1251859013301779E-3</v>
       </c>
       <c r="C29">
         <f t="shared" si="1"/>
@@ -4457,7 +4457,7 @@
     <row r="30" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>1.7944642344303095E-3</v>
+        <v>1.4953868620252581E-3</v>
       </c>
       <c r="C30">
         <f t="shared" si="1"/>
@@ -4467,7 +4467,7 @@
     <row r="31" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>2.325534449188732E-3</v>
+        <v>1.9379453743239433E-3</v>
       </c>
       <c r="C31">
         <f t="shared" si="1"/>
@@ -4477,7 +4477,7 @@
     <row r="32" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>2.9504682038741957E-3</v>
+        <v>2.4587235032284965E-3</v>
       </c>
       <c r="C32">
         <f t="shared" si="1"/>
@@ -4487,7 +4487,7 @@
     <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B33">
         <f t="shared" si="0"/>
-        <v>3.6759953544767184E-3</v>
+        <v>3.0633294620639323E-3</v>
       </c>
       <c r="C33">
         <f t="shared" si="1"/>
@@ -4497,7 +4497,7 @@
     <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34">
         <f t="shared" si="0"/>
-        <v>4.5084926802983977E-3</v>
+        <v>3.7570772335819985E-3</v>
       </c>
       <c r="C34">
         <f t="shared" si="1"/>
@@ -4507,7 +4507,7 @@
     <row r="35" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B35">
         <f t="shared" si="0"/>
-        <v>5.4539333548070607E-3</v>
+        <v>4.5449444623392177E-3</v>
       </c>
       <c r="C35">
         <f t="shared" si="1"/>
@@ -4517,7 +4517,7 @@
     <row r="36" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B36">
         <f t="shared" si="0"/>
-        <v>6.5178348808602399E-3</v>
+        <v>5.4315290673835337E-3</v>
       </c>
       <c r="C36">
         <f t="shared" si="1"/>
@@ -4527,7 +4527,7 @@
     <row r="37" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B37">
         <f t="shared" si="0"/>
-        <v>7.7052060925004657E-3</v>
+        <v>6.4210050770837218E-3</v>
       </c>
       <c r="C37">
         <f t="shared" si="1"/>
@@ -4537,7 +4537,7 @@
     <row r="38" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B38">
         <f t="shared" si="0"/>
-        <v>9.0204938865930274E-3</v>
+        <v>7.5170782388275237E-3</v>
       </c>
       <c r="C38">
         <f t="shared" si="1"/>
@@ -4547,7 +4547,7 @@
     <row r="39" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B39">
         <f t="shared" si="0"/>
-        <v>1.0467530404697972E-2</v>
+        <v>8.7229420039149769E-3</v>
       </c>
       <c r="C39">
         <f t="shared" si="1"/>
@@ -4557,7 +4557,7 @@
     <row r="40" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B40">
         <f t="shared" si="0"/>
-        <v>1.2049481436979681E-2</v>
+        <v>1.0041234530816401E-2</v>
       </c>
       <c r="C40">
         <f t="shared" si="1"/>
@@ -4567,7 +4567,7 @@
     <row r="41" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B41">
         <f t="shared" si="0"/>
-        <v>1.3768796863832604E-2</v>
+        <v>1.1473997386527171E-2</v>
       </c>
       <c r="C41">
         <f t="shared" si="1"/>
@@ -4577,7 +4577,7 @@
     <row r="42" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B42">
         <f t="shared" si="0"/>
-        <v>1.5627163985386609E-2</v>
+        <v>1.3022636654488842E-2</v>
       </c>
       <c r="C42">
         <f t="shared" si="1"/>
@@ -4587,7 +4587,7 @@
     <row r="43" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B43">
         <f t="shared" si="0"/>
-        <v>1.7625464612310682E-2</v>
+        <v>1.4687887176925568E-2</v>
       </c>
       <c r="C43">
         <f t="shared" si="1"/>
@@ -4597,7 +4597,7 @@
     <row r="44" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B44">
         <f t="shared" si="0"/>
-        <v>1.9763736801589746E-2</v>
+        <v>1.6469780667991457E-2</v>
       </c>
       <c r="C44">
         <f t="shared" si="1"/>
@@ -4607,7 +4607,7 @@
     <row r="45" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B45">
         <f t="shared" si="0"/>
-        <v>2.2041142116558832E-2</v>
+        <v>1.8367618430465693E-2</v>
       </c>
       <c r="C45">
         <f t="shared" si="1"/>
@@ -4617,7 +4617,7 @@
     <row r="46" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B46">
         <f t="shared" si="0"/>
-        <v>2.4455939269979066E-2</v>
+        <v>2.0379949391649221E-2</v>
       </c>
       <c r="C46">
         <f t="shared" si="1"/>
@@ -4627,7 +4627,7 @@
     <row r="47" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B47">
         <f t="shared" si="0"/>
-        <v>2.7005464971113717E-2</v>
+        <v>2.2504554142594765E-2</v>
       </c>
       <c r="C47">
         <f t="shared" si="1"/>
@@ -4637,7 +4637,7 @@
     <row r="48" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B48">
         <f t="shared" si="0"/>
-        <v>2.9686122741700537E-2</v>
+        <v>2.4738435618083782E-2</v>
       </c>
       <c r="C48">
         <f t="shared" si="1"/>
@@ -4647,7 +4647,7 @@
     <row r="49" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B49">
         <f t="shared" si="0"/>
-        <v>3.249338039087727E-2</v>
+        <v>2.7077816992397724E-2</v>
       </c>
       <c r="C49">
         <f t="shared" si="1"/>
@@ -4657,7 +4657,7 @@
     <row r="50" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B50">
         <f t="shared" si="0"/>
-        <v>3.5421776745385977E-2</v>
+        <v>2.951814728782165E-2</v>
       </c>
       <c r="C50">
         <f t="shared" si="1"/>
@@ -4667,7 +4667,7 @@
     <row r="51" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B51">
         <f t="shared" si="0"/>
-        <v>3.8464938119114063E-2</v>
+        <v>3.2054115099261718E-2</v>
       </c>
       <c r="C51">
         <f t="shared" si="1"/>
@@ -4677,7 +4677,7 @@
     <row r="52" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B52">
         <f t="shared" si="0"/>
-        <v>4.1615604876098174E-2</v>
+        <v>3.467967073008181E-2</v>
       </c>
       <c r="C52">
         <f t="shared" si="1"/>
@@ -4687,7 +4687,7 @@
     <row r="53" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B53">
         <f t="shared" si="0"/>
-        <v>4.4865668294935525E-2</v>
+        <v>3.7388056912446274E-2</v>
       </c>
       <c r="C53">
         <f t="shared" si="1"/>
@@ -4697,7 +4697,7 @@
     <row r="54" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B54">
         <f t="shared" si="0"/>
-        <v>4.820621778208041E-2</v>
+        <v>4.0171848151733677E-2</v>
       </c>
       <c r="C54">
         <f t="shared" si="1"/>
@@ -4707,7 +4707,7 @@
     <row r="55" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B55">
         <f t="shared" si="0"/>
-        <v>5.1627598309274762E-2</v>
+        <v>4.3022998591062303E-2</v>
       </c>
       <c r="C55">
         <f t="shared" si="1"/>
@@ -4717,7 +4717,7 @@
     <row r="56" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B56">
         <f t="shared" si="0"/>
-        <v>5.5119477769415316E-2</v>
+        <v>4.5932898141179429E-2</v>
       </c>
       <c r="C56">
         <f t="shared" si="1"/>
@@ -4727,7 +4727,7 @@
     <row r="57" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B57">
         <f t="shared" si="0"/>
-        <v>5.8670923759033294E-2</v>
+        <v>4.8892436465861083E-2</v>
       </c>
       <c r="C57">
         <f t="shared" si="1"/>
@@ -4737,7 +4737,7 @@
     <row r="58" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B58">
         <f t="shared" si="0"/>
-        <v>6.2270489108216164E-2</v>
+        <v>5.1892074256846804E-2</v>
       </c>
       <c r="C58">
         <f t="shared" si="1"/>
@@ -4747,7 +4747,7 @@
     <row r="59" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B59">
         <f t="shared" si="0"/>
-        <v>6.5906305294534395E-2</v>
+        <v>5.4921921078778663E-2</v>
       </c>
       <c r="C59">
         <f t="shared" si="1"/>
@@ -4757,7 +4757,7 @@
     <row r="60" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B60">
         <f t="shared" si="0"/>
-        <v>6.9566182700893778E-2</v>
+        <v>5.7971818917411488E-2</v>
       </c>
       <c r="C60">
         <f t="shared" si="1"/>
@@ -4767,7 +4767,7 @@
     <row r="61" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B61">
         <f t="shared" si="0"/>
-        <v>7.3237716512875015E-2</v>
+        <v>6.1031430427395852E-2</v>
       </c>
       <c r="C61">
         <f t="shared" si="1"/>
@@ -4777,7 +4777,7 @@
     <row r="62" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B62">
         <f t="shared" si="0"/>
-        <v>7.6908396903694956E-2</v>
+        <v>6.4090330753079128E-2</v>
       </c>
       <c r="C62">
         <f t="shared" si="1"/>
@@ -4787,7 +4787,7 @@
     <row r="63" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B63">
         <f t="shared" si="0"/>
-        <v>8.0565722028919276E-2</v>
+        <v>6.7138101690766061E-2</v>
       </c>
       <c r="C63">
         <f t="shared" si="1"/>
@@ -4797,7 +4797,7 @@
     <row r="64" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B64">
         <f t="shared" si="0"/>
-        <v>8.4197312252647025E-2</v>
+        <v>7.0164426877205852E-2</v>
       </c>
       <c r="C64">
         <f t="shared" si="1"/>
@@ -4807,7 +4807,7 @@
     <row r="65" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B65">
         <f t="shared" si="0"/>
-        <v>8.7791023955795813E-2</v>
+        <v>7.3159186629829842E-2</v>
       </c>
       <c r="C65">
         <f t="shared" si="1"/>
@@ -4817,7 +4817,7 @@
     <row r="66" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B66">
         <f t="shared" si="0"/>
-        <v>9.1335061238442886E-2</v>
+        <v>7.6112551032035736E-2</v>
       </c>
       <c r="C66">
         <f t="shared" si="1"/>
@@ -4827,7 +4827,7 @@
     <row r="67" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B67">
         <f t="shared" si="0"/>
-        <v>9.4818083824283653E-2</v>
+        <v>7.9015069853569708E-2</v>
       </c>
       <c r="C67">
         <f t="shared" si="1"/>
@@ -4837,7 +4837,7 @@
     <row r="68" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B68">
         <f t="shared" si="0"/>
-        <v>9.8229309507649534E-2</v>
+        <v>8.1857757923041286E-2</v>
       </c>
       <c r="C68">
         <f t="shared" si="1"/>
@@ -4847,7 +4847,7 @@
     <row r="69" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B69">
         <f t="shared" si="0"/>
-        <v>0.10155860955271043</v>
+        <v>8.4632174627258694E-2</v>
       </c>
       <c r="C69">
         <f t="shared" si="1"/>
@@ -4857,7 +4857,7 @@
     <row r="70" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B70">
         <f t="shared" si="0"/>
-        <v>0.10479659555998135</v>
+        <v>8.7330496299984461E-2</v>
       </c>
       <c r="C70">
         <f t="shared" si="1"/>
@@ -4867,7 +4867,7 @@
     <row r="71" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B71">
         <f t="shared" si="0"/>
-        <v>0.10793469645549059</v>
+        <v>8.9945580379575493E-2</v>
       </c>
       <c r="C71">
         <f t="shared" si="1"/>
@@ -4877,7 +4877,7 @@
     <row r="72" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B72">
         <f t="shared" si="0"/>
-        <v>0.11096522443033115</v>
+        <v>9.2471020358609296E-2</v>
       </c>
       <c r="C72">
         <f t="shared" si="1"/>
@@ -4887,7 +4887,7 @@
     <row r="73" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B73">
         <f t="shared" si="0"/>
-        <v>0.11388142885916275</v>
+        <v>9.4901190715968961E-2</v>
       </c>
       <c r="C73">
         <f t="shared" si="1"/>
@@ -4897,7 +4897,7 @@
     <row r="74" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B74">
         <f t="shared" si="0"/>
-        <v>0.11667753745097514</v>
+        <v>9.7231281209145953E-2</v>
       </c>
       <c r="C74">
         <f t="shared" si="1"/>
@@ -4907,7 +4907,7 @@
     <row r="75" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B75">
         <f t="shared" si="0"/>
-        <v>0.11934878412866376</v>
+        <v>9.9457320107219804E-2</v>
       </c>
       <c r="C75">
         <f t="shared" si="1"/>
@@ -4917,7 +4917,7 @@
     <row r="76" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B76">
         <f t="shared" si="0"/>
-        <v>0.12189142338962897</v>
+        <v>0.10157618615802415</v>
       </c>
       <c r="C76">
         <f t="shared" si="1"/>
@@ -4927,7 +4927,7 @@
     <row r="77" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B77">
         <f t="shared" si="0"/>
-        <v>0.12430273116113988</v>
+        <v>0.1035856093009499</v>
       </c>
       <c r="C77">
         <f t="shared" si="1"/>
@@ -4937,7 +4937,7 @@
     <row r="78" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B78">
         <f t="shared" si="0"/>
-        <v>0.12658099242476617</v>
+        <v>0.10548416035397182</v>
       </c>
       <c r="C78">
         <f t="shared" si="1"/>
@@ -4947,7 +4947,7 @@
     <row r="79" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B79">
         <f t="shared" si="0"/>
-        <v>0.12872547613689861</v>
+        <v>0.10727123011408218</v>
       </c>
       <c r="C79">
         <f t="shared" si="1"/>
@@ -4957,7 +4957,7 @@
     <row r="80" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B80">
         <f t="shared" si="0"/>
-        <v>0.13073639821054656</v>
+        <v>0.10894699850878881</v>
       </c>
       <c r="C80">
         <f t="shared" si="1"/>
@@ -4967,7 +4967,7 @@
     <row r="81" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B81">
         <f t="shared" si="0"/>
-        <v>0.13261487354093182</v>
+        <v>0.11051239461744319</v>
       </c>
       <c r="C81">
         <f t="shared" si="1"/>
@@ -4977,7 +4977,7 @@
     <row r="82" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B82">
         <f t="shared" si="0"/>
-        <v>0.13436285824823427</v>
+        <v>0.11196904854019522</v>
       </c>
       <c r="C82">
         <f t="shared" si="1"/>
@@ -4987,7 +4987,7 @@
     <row r="83" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B83">
         <f t="shared" si="0"/>
-        <v>0.1359830834703562</v>
+        <v>0.11331923622529684</v>
       </c>
       <c r="C83">
         <f t="shared" si="1"/>
@@ -4997,7 +4997,7 @@
     <row r="84" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B84">
         <f t="shared" ref="B84:B120" si="2">(1-EXP(-((C84/$B$15-($B$14-0.5))/$B$12)^$B$13))*$B$11</f>
-        <v>0.13747898216292775</v>
+        <v>0.11456581846910648</v>
       </c>
       <c r="C84">
         <f t="shared" si="1"/>
@@ -5007,7 +5007,7 @@
     <row r="85" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B85">
         <f t="shared" si="2"/>
-        <v>0.13885461045027209</v>
+        <v>0.11571217537522674</v>
       </c>
       <c r="C85">
         <f t="shared" ref="C85:C120" si="3">C84+0.25</f>
@@ -5017,7 +5017,7 @@
     <row r="86" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B86">
         <f t="shared" si="2"/>
-        <v>0.14011456511819612</v>
+        <v>0.11676213759849677</v>
       </c>
       <c r="C86">
         <f t="shared" si="3"/>
@@ -5027,7 +5027,7 @@
     <row r="87" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B87">
         <f t="shared" si="2"/>
-        <v>0.14126389884704021</v>
+        <v>0.11771991570586685</v>
       </c>
       <c r="C87">
         <f t="shared" si="3"/>
@@ -5037,7 +5037,7 @@
     <row r="88" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B88">
         <f t="shared" si="2"/>
-        <v>0.1423080347524181</v>
+        <v>0.11859002896034841</v>
       </c>
       <c r="C88">
         <f t="shared" si="3"/>
@@ -5047,7 +5047,7 @@
     <row r="89" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B89">
         <f t="shared" si="2"/>
-        <v>0.14325268173371089</v>
+        <v>0.11937723477809242</v>
       </c>
       <c r="C89">
         <f t="shared" si="3"/>
@@ -5057,7 +5057,7 @@
     <row r="90" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B90">
         <f t="shared" si="2"/>
-        <v>0.14410375202992939</v>
+        <v>0.12008646002494117</v>
       </c>
       <c r="C90">
         <f t="shared" si="3"/>
@@ -5067,7 +5067,7 @@
     <row r="91" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B91">
         <f t="shared" si="2"/>
-        <v>0.1448672822532501</v>
+        <v>0.12072273521104175</v>
       </c>
       <c r="C91">
         <f t="shared" si="3"/>
@@ -5077,7 +5077,7 @@
     <row r="92" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B92">
         <f t="shared" si="2"/>
-        <v>0.14554935901734684</v>
+        <v>0.12129113251445571</v>
       </c>
       <c r="C92">
         <f t="shared" si="3"/>
@@ -5087,7 +5087,7 @@
     <row r="93" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B93">
         <f t="shared" si="2"/>
-        <v>0.14615605010611638</v>
+        <v>0.12179670842176366</v>
       </c>
       <c r="C93">
         <f t="shared" si="3"/>
@@ -5097,7 +5097,7 @@
     <row r="94" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B94">
         <f t="shared" si="2"/>
-        <v>0.14669334194440264</v>
+        <v>0.12224445162033554</v>
       </c>
       <c r="C94">
         <f t="shared" si="3"/>
@@ -5107,7 +5107,7 @@
     <row r="95" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B95">
         <f t="shared" si="2"/>
-        <v>0.14716708394183772</v>
+        <v>0.12263923661819812</v>
       </c>
       <c r="C95">
         <f t="shared" si="3"/>
@@ -5117,7 +5117,7 @@
     <row r="96" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B96">
         <f t="shared" si="2"/>
-        <v>0.14758294008979489</v>
+        <v>0.12298578340816241</v>
       </c>
       <c r="C96">
         <f t="shared" si="3"/>
@@ -5127,7 +5127,7 @@
     <row r="97" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B97">
         <f t="shared" si="2"/>
-        <v>0.1479463480052261</v>
+        <v>0.12328862333768843</v>
       </c>
       <c r="C97">
         <f t="shared" si="3"/>
@@ -5137,7 +5137,7 @@
     <row r="98" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B98">
         <f t="shared" si="2"/>
-        <v>0.14826248543885948</v>
+        <v>0.12355207119904957</v>
       </c>
       <c r="C98">
         <f t="shared" si="3"/>
@@ -5147,7 +5147,7 @@
     <row r="99" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B99">
         <f t="shared" si="2"/>
-        <v>0.14853624410321731</v>
+        <v>0.12378020341934777</v>
       </c>
       <c r="C99">
         <f t="shared" si="3"/>
@@ -5157,7 +5157,7 @@
     <row r="100" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B100">
         <f t="shared" si="2"/>
-        <v>0.1487722105317654</v>
+        <v>0.1239768421098045</v>
       </c>
       <c r="C100">
         <f t="shared" si="3"/>
@@ -5167,7 +5167,7 @@
     <row r="101" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B101">
         <f t="shared" si="2"/>
-        <v>0.14897465355692657</v>
+        <v>0.12414554463077215</v>
       </c>
       <c r="C101">
         <f t="shared" si="3"/>
@@ -5177,7 +5177,7 @@
     <row r="102" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B102">
         <f t="shared" si="2"/>
-        <v>0.14914751789350353</v>
+        <v>0.12428959824458628</v>
       </c>
       <c r="C102">
         <f t="shared" si="3"/>
@@ -5187,7 +5187,7 @@
     <row r="103" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B103">
         <f t="shared" si="2"/>
-        <v>0.14929442323616438</v>
+        <v>0.12441201936347031</v>
       </c>
       <c r="C103">
         <f t="shared" si="3"/>
@@ -5197,7 +5197,7 @@
     <row r="104" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B104">
         <f t="shared" si="2"/>
-        <v>0.14941866822510363</v>
+        <v>0.12451555685425303</v>
       </c>
       <c r="C104">
         <f t="shared" si="3"/>
@@ -5207,7 +5207,7 @@
     <row r="105" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B105">
         <f t="shared" si="2"/>
-        <v>0.14952323860205774</v>
+        <v>0.12460269883504811</v>
       </c>
       <c r="C105">
         <f t="shared" si="3"/>
@@ -5217,7 +5217,7 @@
     <row r="106" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B106">
         <f t="shared" si="2"/>
-        <v>0.14961081886809813</v>
+        <v>0.12467568239008178</v>
       </c>
       <c r="C106">
         <f t="shared" si="3"/>
@@ -5227,7 +5227,7 @@
     <row r="107" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B107">
         <f t="shared" si="2"/>
-        <v>0.14968380676304538</v>
+        <v>0.12473650563587114</v>
       </c>
       <c r="C107">
         <f t="shared" si="3"/>
@@ -5237,7 +5237,7 @@
     <row r="108" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B108">
         <f t="shared" si="2"/>
-        <v>0.14974432991149983</v>
+        <v>0.12478694159291652</v>
       </c>
       <c r="C108">
         <f t="shared" si="3"/>
@@ -5247,7 +5247,7 @@
     <row r="109" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B109">
         <f t="shared" si="2"/>
-        <v>0.14979426401963158</v>
+        <v>0.12482855334969299</v>
       </c>
       <c r="C109">
         <f t="shared" si="3"/>
@@ -5257,7 +5257,7 @@
     <row r="110" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B110">
         <f t="shared" si="2"/>
-        <v>0.14983525205710502</v>
+        <v>0.12486271004758752</v>
       </c>
       <c r="C110">
         <f t="shared" si="3"/>
@@ -5267,7 +5267,7 @@
     <row r="111" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B111">
         <f t="shared" si="2"/>
-        <v>0.14986872391689912</v>
+        <v>0.12489060326408261</v>
       </c>
       <c r="C111">
         <f t="shared" si="3"/>
@@ -5277,7 +5277,7 @@
     <row r="112" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B112">
         <f t="shared" si="2"/>
-        <v>0.14989591610946901</v>
+        <v>0.12491326342455751</v>
       </c>
       <c r="C112">
         <f t="shared" si="3"/>
@@ -5287,7 +5287,7 @@
     <row r="113" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B113">
         <f t="shared" si="2"/>
-        <v>0.14991789111400722</v>
+        <v>0.12493157592833935</v>
       </c>
       <c r="C113">
         <f t="shared" si="3"/>
@@ -5297,7 +5297,7 @@
     <row r="114" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B114">
         <f t="shared" si="2"/>
-        <v>0.14993555607610648</v>
+        <v>0.12494629673008874</v>
       </c>
       <c r="C114">
         <f t="shared" si="3"/>
@@ -5307,7 +5307,7 @@
     <row r="115" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B115">
         <f t="shared" si="2"/>
-        <v>0.14994968060581462</v>
+        <v>0.12495806717151219</v>
       </c>
       <c r="C115">
         <f t="shared" si="3"/>
@@ -5317,7 +5317,7 @@
     <row r="116" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B116">
         <f t="shared" si="2"/>
-        <v>0.14996091349119239</v>
+        <v>0.12496742790932699</v>
       </c>
       <c r="C116">
         <f t="shared" si="3"/>
@@ -5327,7 +5327,7 @@
     <row r="117" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B117">
         <f t="shared" si="2"/>
-        <v>0.14996979819869544</v>
+        <v>0.1249748318322462</v>
       </c>
       <c r="C117">
         <f t="shared" si="3"/>
@@ -5337,7 +5337,7 @@
     <row r="118" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B118">
         <f t="shared" si="2"/>
-        <v>0.14997678708203718</v>
+        <v>0.12498065590169766</v>
       </c>
       <c r="C118">
         <f t="shared" si="3"/>
@@ -5347,7 +5347,7 @@
     <row r="119" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B119">
         <f t="shared" si="2"/>
-        <v>0.14998225426504705</v>
+        <v>0.12498521188753921</v>
       </c>
       <c r="C119">
         <f t="shared" si="3"/>
@@ -5357,7 +5357,7 @@
     <row r="120" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B120">
         <f t="shared" si="2"/>
-        <v>0.14998650720113471</v>
+        <v>0.1249887560009456</v>
       </c>
       <c r="C120">
         <f t="shared" si="3"/>
@@ -5397,327 +5397,327 @@
       </c>
       <c r="C1">
         <f>(1-EXP(-((C2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>1.3563306734076795E-6</v>
+        <v>1.1302755611730664E-6</v>
       </c>
       <c r="D1">
         <f>(1-EXP(-((D2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>1.0850301995346534E-5</v>
+        <v>9.041918329455445E-6</v>
       </c>
       <c r="E1">
         <f>(1-EXP(-((E2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>3.6616623765417522E-5</v>
+        <v>3.0513853137847935E-5</v>
       </c>
       <c r="F1">
         <f>(1-EXP(-((F2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>8.6780443051764905E-5</v>
+        <v>7.2317035876470759E-5</v>
       </c>
       <c r="G1">
         <f>(1-EXP(-((G2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>1.6944632170386997E-4</v>
+        <v>1.4120526808655831E-4</v>
       </c>
       <c r="H1">
         <f>(1-EXP(-((H2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>2.926828338786713E-4</v>
+        <v>2.4390236156555944E-4</v>
       </c>
       <c r="I1">
         <f>(1-EXP(-((I2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>4.6450282648525794E-4</v>
+        <v>3.8708568873771498E-4</v>
       </c>
       <c r="J1">
         <f>(1-EXP(-((J2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>6.9283941201358503E-4</v>
+        <v>5.7736617667798751E-4</v>
       </c>
       <c r="K1">
         <f>(1-EXP(-((K2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>9.8551779614576844E-4</v>
+        <v>8.2126483012147367E-4</v>
       </c>
       <c r="L1">
         <f>(1-EXP(-((L2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>1.3502230815962135E-3</v>
+        <v>1.1251859013301779E-3</v>
       </c>
       <c r="M1">
         <f>(1-EXP(-((M2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>1.7944642344303095E-3</v>
+        <v>1.4953868620252581E-3</v>
       </c>
       <c r="N1">
         <f>(1-EXP(-((N2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>2.325534449188732E-3</v>
+        <v>1.9379453743239433E-3</v>
       </c>
       <c r="O1">
         <f>(1-EXP(-((O2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>2.9504682038741957E-3</v>
+        <v>2.4587235032284965E-3</v>
       </c>
       <c r="P1">
         <f>(1-EXP(-((P2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>3.6759953544767184E-3</v>
+        <v>3.0633294620639323E-3</v>
       </c>
       <c r="Q1">
         <f>(1-EXP(-((Q2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>4.5084926802983977E-3</v>
+        <v>3.7570772335819985E-3</v>
       </c>
       <c r="R1">
         <f>(1-EXP(-((R2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>5.4539333548070607E-3</v>
+        <v>4.5449444623392177E-3</v>
       </c>
       <c r="S1">
         <f>(1-EXP(-((S2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>6.5178348808602399E-3</v>
+        <v>5.4315290673835337E-3</v>
       </c>
       <c r="T1">
         <f>(1-EXP(-((T2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>7.7052060925004657E-3</v>
+        <v>6.4210050770837218E-3</v>
       </c>
       <c r="U1">
         <f>(1-EXP(-((U2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>9.0204938865930274E-3</v>
+        <v>7.5170782388275237E-3</v>
       </c>
       <c r="V1">
         <f>(1-EXP(-((V2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>1.0467530404697972E-2</v>
+        <v>8.7229420039149769E-3</v>
       </c>
       <c r="W1">
         <f>(1-EXP(-((W2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>1.2049481436979681E-2</v>
+        <v>1.0041234530816401E-2</v>
       </c>
       <c r="X1">
         <f>(1-EXP(-((X2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>1.3768796863832604E-2</v>
+        <v>1.1473997386527171E-2</v>
       </c>
       <c r="Y1">
         <f>(1-EXP(-((Y2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>1.5627163985386609E-2</v>
+        <v>1.3022636654488842E-2</v>
       </c>
       <c r="Z1">
         <f>(1-EXP(-((Z2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>1.7625464612310682E-2</v>
+        <v>1.4687887176925568E-2</v>
       </c>
       <c r="AA1">
         <f>(1-EXP(-((AA2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>1.9763736801589746E-2</v>
+        <v>1.6469780667991457E-2</v>
       </c>
       <c r="AB1">
         <f>(1-EXP(-((AB2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>2.2041142116558832E-2</v>
+        <v>1.8367618430465693E-2</v>
       </c>
       <c r="AC1">
         <f>(1-EXP(-((AC2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>2.4455939269979066E-2</v>
+        <v>2.0379949391649221E-2</v>
       </c>
       <c r="AD1">
         <f>(1-EXP(-((AD2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>2.7005464971113717E-2</v>
+        <v>2.2504554142594765E-2</v>
       </c>
       <c r="AE1">
         <f>(1-EXP(-((AE2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>2.9686122741700537E-2</v>
+        <v>2.4738435618083782E-2</v>
       </c>
       <c r="AF1">
         <f>(1-EXP(-((AF2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>3.249338039087727E-2</v>
+        <v>2.7077816992397724E-2</v>
       </c>
       <c r="AG1">
         <f>(1-EXP(-((AG2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>3.5421776745385977E-2</v>
+        <v>2.951814728782165E-2</v>
       </c>
       <c r="AH1">
         <f>(1-EXP(-((AH2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>3.8464938119114063E-2</v>
+        <v>3.2054115099261718E-2</v>
       </c>
       <c r="AI1">
         <f>(1-EXP(-((AI2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>4.1615604876098174E-2</v>
+        <v>3.467967073008181E-2</v>
       </c>
       <c r="AJ1">
         <f>(1-EXP(-((AJ2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>4.4865668294935525E-2</v>
+        <v>3.7388056912446274E-2</v>
       </c>
       <c r="AK1">
         <f>(1-EXP(-((AK2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>4.820621778208041E-2</v>
+        <v>4.0171848151733677E-2</v>
       </c>
       <c r="AL1">
         <f>(1-EXP(-((AL2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>5.1627598309274762E-2</v>
+        <v>4.3022998591062303E-2</v>
       </c>
       <c r="AM1">
         <f>(1-EXP(-((AM2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>5.5119477769415316E-2</v>
+        <v>4.5932898141179429E-2</v>
       </c>
       <c r="AN1">
         <f>(1-EXP(-((AN2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>5.8670923759033294E-2</v>
+        <v>4.8892436465861083E-2</v>
       </c>
       <c r="AO1">
         <f>(1-EXP(-((AO2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>6.2270489108216164E-2</v>
+        <v>5.1892074256846804E-2</v>
       </c>
       <c r="AP1">
         <f>(1-EXP(-((AP2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>6.5906305294534395E-2</v>
+        <v>5.4921921078778663E-2</v>
       </c>
       <c r="AQ1">
         <f>(1-EXP(-((AQ2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>6.9566182700893778E-2</v>
+        <v>5.7971818917411488E-2</v>
       </c>
       <c r="AR1">
         <f>(1-EXP(-((AR2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>7.3237716512875015E-2</v>
+        <v>6.1031430427395852E-2</v>
       </c>
       <c r="AS1">
         <f>(1-EXP(-((AS2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>7.6908396903694956E-2</v>
+        <v>6.4090330753079128E-2</v>
       </c>
       <c r="AT1">
         <f>(1-EXP(-((AT2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>8.0565722028919276E-2</v>
+        <v>6.7138101690766061E-2</v>
       </c>
       <c r="AU1">
         <f>(1-EXP(-((AU2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>8.4197312252647025E-2</v>
+        <v>7.0164426877205852E-2</v>
       </c>
       <c r="AV1">
         <f>(1-EXP(-((AV2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>8.7791023955795813E-2</v>
+        <v>7.3159186629829842E-2</v>
       </c>
       <c r="AW1">
         <f>(1-EXP(-((AW2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>9.1335061238442886E-2</v>
+        <v>7.6112551032035736E-2</v>
       </c>
       <c r="AX1">
         <f>(1-EXP(-((AX2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>9.4818083824283653E-2</v>
+        <v>7.9015069853569708E-2</v>
       </c>
       <c r="AY1">
         <f>(1-EXP(-((AY2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>9.8229309507649534E-2</v>
+        <v>8.1857757923041286E-2</v>
       </c>
       <c r="AZ1">
         <f>(1-EXP(-((AZ2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.10155860955271043</v>
+        <v>8.4632174627258694E-2</v>
       </c>
       <c r="BA1">
         <f>(1-EXP(-((BA2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.10479659555998135</v>
+        <v>8.7330496299984461E-2</v>
       </c>
       <c r="BB1">
         <f>(1-EXP(-((BB2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.10793469645549059</v>
+        <v>8.9945580379575493E-2</v>
       </c>
       <c r="BC1">
         <f>(1-EXP(-((BC2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.11096522443033115</v>
+        <v>9.2471020358609296E-2</v>
       </c>
       <c r="BD1">
         <f>(1-EXP(-((BD2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.11388142885916275</v>
+        <v>9.4901190715968961E-2</v>
       </c>
       <c r="BE1">
         <f>(1-EXP(-((BE2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.11667753745097514</v>
+        <v>9.7231281209145953E-2</v>
       </c>
       <c r="BF1">
         <f>(1-EXP(-((BF2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.11934878412866376</v>
+        <v>9.9457320107219804E-2</v>
       </c>
       <c r="BG1">
         <f>(1-EXP(-((BG2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.12189142338962897</v>
+        <v>0.10157618615802415</v>
       </c>
       <c r="BH1">
         <f>(1-EXP(-((BH2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.12430273116113988</v>
+        <v>0.1035856093009499</v>
       </c>
       <c r="BI1">
         <f>(1-EXP(-((BI2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.12658099242476617</v>
+        <v>0.10548416035397182</v>
       </c>
       <c r="BJ1">
         <f>(1-EXP(-((BJ2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.12872547613689861</v>
+        <v>0.10727123011408218</v>
       </c>
       <c r="BK1">
         <f>(1-EXP(-((BK2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.13073639821054656</v>
+        <v>0.10894699850878881</v>
       </c>
       <c r="BL1">
         <f>(1-EXP(-((BL2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.13261487354093182</v>
+        <v>0.11051239461744319</v>
       </c>
       <c r="BM1">
         <f>(1-EXP(-((BM2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.13436285824823427</v>
+        <v>0.11196904854019522</v>
       </c>
       <c r="BN1">
         <f>(1-EXP(-((BN2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.1359830834703562</v>
+        <v>0.11331923622529684</v>
       </c>
       <c r="BO1">
         <f>(1-EXP(-((BO2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.13747898216292775</v>
+        <v>0.11456581846910648</v>
       </c>
       <c r="BP1">
         <f>(1-EXP(-((BP2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.13885461045027209</v>
+        <v>0.11571217537522674</v>
       </c>
       <c r="BQ1">
         <f>(1-EXP(-((BQ2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.14011456511819612</v>
+        <v>0.11676213759849677</v>
       </c>
       <c r="BR1">
         <f>(1-EXP(-((BR2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.14126389884704021</v>
+        <v>0.11771991570586685</v>
       </c>
       <c r="BS1">
         <f>(1-EXP(-((BS2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.1423080347524181</v>
+        <v>0.11859002896034841</v>
       </c>
       <c r="BT1">
         <f>(1-EXP(-((BT2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.14325268173371089</v>
+        <v>0.11937723477809242</v>
       </c>
       <c r="BU1">
         <f>(1-EXP(-((BU2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.14410375202992939</v>
+        <v>0.12008646002494117</v>
       </c>
       <c r="BV1">
         <f>(1-EXP(-((BV2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.1448672822532501</v>
+        <v>0.12072273521104175</v>
       </c>
       <c r="BW1">
         <f>(1-EXP(-((BW2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.14554935901734684</v>
+        <v>0.12129113251445571</v>
       </c>
       <c r="BX1">
         <f>(1-EXP(-((BX2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.14615605010611638</v>
+        <v>0.12179670842176366</v>
       </c>
       <c r="BY1">
         <f>(1-EXP(-((BY2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.14669334194440264</v>
+        <v>0.12224445162033554</v>
       </c>
       <c r="BZ1">
         <f>(1-EXP(-((BZ2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.14716708394183772</v>
+        <v>0.12263923661819812</v>
       </c>
       <c r="CA1">
         <f>(1-EXP(-((CA2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.14758294008979489</v>
+        <v>0.12298578340816241</v>
       </c>
       <c r="CB1">
         <f>(1-EXP(-((CB2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.1479463480052261</v>
+        <v>0.12328862333768843</v>
       </c>
       <c r="CC1">
         <f>(1-EXP(-((CC2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.14826248543885948</v>
+        <v>0.12355207119904957</v>
       </c>
       <c r="CD1">
         <f>(1-EXP(-((CD2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.14853624410321731</v>
+        <v>0.12378020341934777</v>
       </c>
       <c r="CE1">
         <f>(1-EXP(-((CE2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
-        <v>0.15</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="2" spans="1:83" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Update to CSC assumption for onshore wind
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C9E6D6-E9ED-400A-B5BE-DB8123CDB372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94731181-DAE1-4C61-8902-F665038802D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="6690" windowWidth="24240" windowHeight="13020" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t xml:space="preserve">Source: </t>
   </si>
@@ -160,6 +160,18 @@
   <si>
     <t>Incremental Revenue</t>
   </si>
+  <si>
+    <t>Notes:</t>
+  </si>
+  <si>
+    <t>For the Share of Cost Effective Capacity Built in a Single Year, we use a value of 1 for all resources except wind,</t>
+  </si>
+  <si>
+    <t>which in recent years has faced unique siting constraints that have limited new capacity.</t>
+  </si>
+  <si>
+    <t>For onshore wind, we use a value of 0.75.</t>
+  </si>
 </sst>
 </file>
 
@@ -202,9 +214,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -289,7 +302,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>About!$C$20:$C$120</c:f>
+              <c:f>About!$C$24:$C$124</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
@@ -601,7 +614,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>About!$B$20:$B$120</c:f>
+              <c:f>About!$B$24:$B$124</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
@@ -3849,13 +3862,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>151130</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>138430</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3885,13 +3898,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>638175</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>5210175</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -4260,34 +4273,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3D2DEE-686E-48A0-AC3D-0F54DEA5D0EC}">
-  <dimension ref="A1:C120"/>
+  <dimension ref="A1:C124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="88.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="88.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -4295,1071 +4308,1094 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>37</v>
       </c>
-      <c r="B11">
+      <c r="B15">
         <v>0.125</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>35</v>
       </c>
-      <c r="B12">
+      <c r="B16">
         <v>0.6</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>36</v>
       </c>
-      <c r="B13">
+      <c r="B17">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>38</v>
       </c>
-      <c r="B14">
+      <c r="B18">
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>39</v>
       </c>
-      <c r="B15">
+      <c r="B19">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B19">
-        <f>(1-EXP(-((C19/$B$15-($B$14-0.5))/$B$12)^$B$13))*$B$11</f>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <f>(1-EXP(-((C23/$B$19-($B$18-0.5))/$B$16)^$B$17))*$B$15</f>
         <v>0</v>
       </c>
-      <c r="C19">
+      <c r="C23">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B20">
-        <f t="shared" ref="B20:B83" si="0">(1-EXP(-((C20/$B$15-($B$14-0.5))/$B$12)^$B$13))*$B$11</f>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <f t="shared" ref="B24:B87" si="0">(1-EXP(-((C24/$B$19-($B$18-0.5))/$B$16)^$B$17))*$B$15</f>
         <v>1.1302755611730664E-6</v>
       </c>
-      <c r="C20">
-        <f>C19+0.25</f>
+      <c r="C24">
+        <f>C23+0.25</f>
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B21">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25">
         <f t="shared" si="0"/>
         <v>9.041918329455445E-6</v>
       </c>
-      <c r="C21">
-        <f t="shared" ref="C21:C84" si="1">C20+0.25</f>
+      <c r="C25">
+        <f t="shared" ref="C25:C88" si="1">C24+0.25</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B22">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26">
         <f t="shared" si="0"/>
         <v>3.0513853137847935E-5</v>
       </c>
-      <c r="C22">
+      <c r="C26">
         <f t="shared" si="1"/>
         <v>0.75</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B23">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27">
         <f t="shared" si="0"/>
         <v>7.2317035876470759E-5</v>
       </c>
-      <c r="C23">
+      <c r="C27">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B24">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28">
         <f t="shared" si="0"/>
         <v>1.4120526808655831E-4</v>
       </c>
-      <c r="C24">
+      <c r="C28">
         <f t="shared" si="1"/>
         <v>1.25</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29">
         <f t="shared" si="0"/>
         <v>2.4390236156555944E-4</v>
       </c>
-      <c r="C25">
+      <c r="C29">
         <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B26">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30">
         <f t="shared" si="0"/>
         <v>3.8708568873771498E-4</v>
       </c>
-      <c r="C26">
+      <c r="C30">
         <f t="shared" si="1"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B27">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31">
         <f t="shared" si="0"/>
         <v>5.7736617667798751E-4</v>
       </c>
-      <c r="C27">
+      <c r="C31">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B28">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32">
         <f t="shared" si="0"/>
         <v>8.2126483012147367E-4</v>
       </c>
-      <c r="C28">
+      <c r="C32">
         <f t="shared" si="1"/>
         <v>2.25</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B29">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33">
         <f t="shared" si="0"/>
         <v>1.1251859013301779E-3</v>
       </c>
-      <c r="C29">
+      <c r="C33">
         <f t="shared" si="1"/>
         <v>2.5</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B30">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34">
         <f t="shared" si="0"/>
         <v>1.4953868620252581E-3</v>
       </c>
-      <c r="C30">
+      <c r="C34">
         <f t="shared" si="1"/>
         <v>2.75</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B31">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35">
         <f t="shared" si="0"/>
         <v>1.9379453743239433E-3</v>
       </c>
-      <c r="C31">
+      <c r="C35">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B32">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36">
         <f t="shared" si="0"/>
         <v>2.4587235032284965E-3</v>
       </c>
-      <c r="C32">
+      <c r="C36">
         <f t="shared" si="1"/>
         <v>3.25</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B33">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37">
         <f t="shared" si="0"/>
         <v>3.0633294620639323E-3</v>
       </c>
-      <c r="C33">
+      <c r="C37">
         <f t="shared" si="1"/>
         <v>3.5</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B34">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38">
         <f t="shared" si="0"/>
         <v>3.7570772335819985E-3</v>
       </c>
-      <c r="C34">
+      <c r="C38">
         <f t="shared" si="1"/>
         <v>3.75</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B35">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39">
         <f t="shared" si="0"/>
         <v>4.5449444623392177E-3</v>
       </c>
-      <c r="C35">
+      <c r="C39">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B36">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40">
         <f t="shared" si="0"/>
         <v>5.4315290673835337E-3</v>
       </c>
-      <c r="C36">
+      <c r="C40">
         <f t="shared" si="1"/>
         <v>4.25</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B37">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41">
         <f t="shared" si="0"/>
         <v>6.4210050770837218E-3</v>
       </c>
-      <c r="C37">
+      <c r="C41">
         <f t="shared" si="1"/>
         <v>4.5</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B38">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42">
         <f t="shared" si="0"/>
         <v>7.5170782388275237E-3</v>
       </c>
-      <c r="C38">
+      <c r="C42">
         <f t="shared" si="1"/>
         <v>4.75</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B39">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43">
         <f t="shared" si="0"/>
         <v>8.7229420039149769E-3</v>
       </c>
-      <c r="C39">
+      <c r="C43">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B40">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44">
         <f t="shared" si="0"/>
         <v>1.0041234530816401E-2</v>
       </c>
-      <c r="C40">
+      <c r="C44">
         <f t="shared" si="1"/>
         <v>5.25</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B41">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45">
         <f t="shared" si="0"/>
         <v>1.1473997386527171E-2</v>
       </c>
-      <c r="C41">
+      <c r="C45">
         <f t="shared" si="1"/>
         <v>5.5</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B42">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46">
         <f t="shared" si="0"/>
         <v>1.3022636654488842E-2</v>
       </c>
-      <c r="C42">
+      <c r="C46">
         <f t="shared" si="1"/>
         <v>5.75</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B43">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47">
         <f t="shared" si="0"/>
         <v>1.4687887176925568E-2</v>
       </c>
-      <c r="C43">
+      <c r="C47">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B44">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48">
         <f t="shared" si="0"/>
         <v>1.6469780667991457E-2</v>
       </c>
-      <c r="C44">
+      <c r="C48">
         <f t="shared" si="1"/>
         <v>6.25</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B45">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49">
         <f t="shared" si="0"/>
         <v>1.8367618430465693E-2</v>
       </c>
-      <c r="C45">
+      <c r="C49">
         <f t="shared" si="1"/>
         <v>6.5</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B46">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50">
         <f t="shared" si="0"/>
         <v>2.0379949391649221E-2</v>
       </c>
-      <c r="C46">
+      <c r="C50">
         <f t="shared" si="1"/>
         <v>6.75</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B47">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51">
         <f t="shared" si="0"/>
         <v>2.2504554142594765E-2</v>
       </c>
-      <c r="C47">
+      <c r="C51">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B48">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52">
         <f t="shared" si="0"/>
         <v>2.4738435618083782E-2</v>
       </c>
-      <c r="C48">
+      <c r="C52">
         <f t="shared" si="1"/>
         <v>7.25</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B49">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53">
         <f t="shared" si="0"/>
         <v>2.7077816992397724E-2</v>
       </c>
-      <c r="C49">
+      <c r="C53">
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B50">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54">
         <f t="shared" si="0"/>
         <v>2.951814728782165E-2</v>
       </c>
-      <c r="C50">
+      <c r="C54">
         <f t="shared" si="1"/>
         <v>7.75</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B51">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55">
         <f t="shared" si="0"/>
         <v>3.2054115099261718E-2</v>
       </c>
-      <c r="C51">
+      <c r="C55">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B52">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56">
         <f t="shared" si="0"/>
         <v>3.467967073008181E-2</v>
       </c>
-      <c r="C52">
+      <c r="C56">
         <f t="shared" si="1"/>
         <v>8.25</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B53">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57">
         <f t="shared" si="0"/>
         <v>3.7388056912446274E-2</v>
       </c>
-      <c r="C53">
+      <c r="C57">
         <f t="shared" si="1"/>
         <v>8.5</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B54">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58">
         <f t="shared" si="0"/>
         <v>4.0171848151733677E-2</v>
       </c>
-      <c r="C54">
+      <c r="C58">
         <f t="shared" si="1"/>
         <v>8.75</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B55">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59">
         <f t="shared" si="0"/>
         <v>4.3022998591062303E-2</v>
       </c>
-      <c r="C55">
+      <c r="C59">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B56">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60">
         <f t="shared" si="0"/>
         <v>4.5932898141179429E-2</v>
       </c>
-      <c r="C56">
+      <c r="C60">
         <f t="shared" si="1"/>
         <v>9.25</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B57">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61">
         <f t="shared" si="0"/>
         <v>4.8892436465861083E-2</v>
       </c>
-      <c r="C57">
+      <c r="C61">
         <f t="shared" si="1"/>
         <v>9.5</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B58">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62">
         <f t="shared" si="0"/>
         <v>5.1892074256846804E-2</v>
       </c>
-      <c r="C58">
+      <c r="C62">
         <f t="shared" si="1"/>
         <v>9.75</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B59">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63">
         <f t="shared" si="0"/>
         <v>5.4921921078778663E-2</v>
       </c>
-      <c r="C59">
+      <c r="C63">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B60">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64">
         <f t="shared" si="0"/>
         <v>5.7971818917411488E-2</v>
       </c>
-      <c r="C60">
+      <c r="C64">
         <f t="shared" si="1"/>
         <v>10.25</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B61">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65">
         <f t="shared" si="0"/>
         <v>6.1031430427395852E-2</v>
       </c>
-      <c r="C61">
+      <c r="C65">
         <f t="shared" si="1"/>
         <v>10.5</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B62">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66">
         <f t="shared" si="0"/>
         <v>6.4090330753079128E-2</v>
       </c>
-      <c r="C62">
+      <c r="C66">
         <f t="shared" si="1"/>
         <v>10.75</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B63">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67">
         <f t="shared" si="0"/>
         <v>6.7138101690766061E-2</v>
       </c>
-      <c r="C63">
+      <c r="C67">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B64">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68">
         <f t="shared" si="0"/>
         <v>7.0164426877205852E-2</v>
       </c>
-      <c r="C64">
+      <c r="C68">
         <f t="shared" si="1"/>
         <v>11.25</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B65">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B69">
         <f t="shared" si="0"/>
         <v>7.3159186629829842E-2</v>
       </c>
-      <c r="C65">
+      <c r="C69">
         <f t="shared" si="1"/>
         <v>11.5</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B66">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B70">
         <f t="shared" si="0"/>
         <v>7.6112551032035736E-2</v>
       </c>
-      <c r="C66">
+      <c r="C70">
         <f t="shared" si="1"/>
         <v>11.75</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B67">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B71">
         <f t="shared" si="0"/>
         <v>7.9015069853569708E-2</v>
       </c>
-      <c r="C67">
+      <c r="C71">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B68">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B72">
         <f t="shared" si="0"/>
         <v>8.1857757923041286E-2</v>
       </c>
-      <c r="C68">
+      <c r="C72">
         <f t="shared" si="1"/>
         <v>12.25</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B69">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B73">
         <f t="shared" si="0"/>
         <v>8.4632174627258694E-2</v>
       </c>
-      <c r="C69">
+      <c r="C73">
         <f t="shared" si="1"/>
         <v>12.5</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B70">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B74">
         <f t="shared" si="0"/>
         <v>8.7330496299984461E-2</v>
       </c>
-      <c r="C70">
+      <c r="C74">
         <f t="shared" si="1"/>
         <v>12.75</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B71">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B75">
         <f t="shared" si="0"/>
         <v>8.9945580379575493E-2</v>
       </c>
-      <c r="C71">
+      <c r="C75">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B72">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B76">
         <f t="shared" si="0"/>
         <v>9.2471020358609296E-2</v>
       </c>
-      <c r="C72">
+      <c r="C76">
         <f t="shared" si="1"/>
         <v>13.25</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B73">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B77">
         <f t="shared" si="0"/>
         <v>9.4901190715968961E-2</v>
       </c>
-      <c r="C73">
+      <c r="C77">
         <f t="shared" si="1"/>
         <v>13.5</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B74">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B78">
         <f t="shared" si="0"/>
         <v>9.7231281209145953E-2</v>
       </c>
-      <c r="C74">
+      <c r="C78">
         <f t="shared" si="1"/>
         <v>13.75</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B75">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B79">
         <f t="shared" si="0"/>
         <v>9.9457320107219804E-2</v>
       </c>
-      <c r="C75">
+      <c r="C79">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B76">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B80">
         <f t="shared" si="0"/>
         <v>0.10157618615802415</v>
       </c>
-      <c r="C76">
+      <c r="C80">
         <f t="shared" si="1"/>
         <v>14.25</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B77">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B81">
         <f t="shared" si="0"/>
         <v>0.1035856093009499</v>
       </c>
-      <c r="C77">
+      <c r="C81">
         <f t="shared" si="1"/>
         <v>14.5</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B78">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B82">
         <f t="shared" si="0"/>
         <v>0.10548416035397182</v>
       </c>
-      <c r="C78">
+      <c r="C82">
         <f t="shared" si="1"/>
         <v>14.75</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B79">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B83">
         <f t="shared" si="0"/>
         <v>0.10727123011408218</v>
       </c>
-      <c r="C79">
+      <c r="C83">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B80">
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B84">
         <f t="shared" si="0"/>
         <v>0.10894699850878881</v>
       </c>
-      <c r="C80">
+      <c r="C84">
         <f t="shared" si="1"/>
         <v>15.25</v>
       </c>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B81">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B85">
         <f t="shared" si="0"/>
         <v>0.11051239461744319</v>
       </c>
-      <c r="C81">
+      <c r="C85">
         <f t="shared" si="1"/>
         <v>15.5</v>
       </c>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B82">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B86">
         <f t="shared" si="0"/>
         <v>0.11196904854019522</v>
       </c>
-      <c r="C82">
+      <c r="C86">
         <f t="shared" si="1"/>
         <v>15.75</v>
       </c>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B83">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B87">
         <f t="shared" si="0"/>
         <v>0.11331923622529684</v>
       </c>
-      <c r="C83">
+      <c r="C87">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B84">
-        <f t="shared" ref="B84:B120" si="2">(1-EXP(-((C84/$B$15-($B$14-0.5))/$B$12)^$B$13))*$B$11</f>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B88">
+        <f t="shared" ref="B88:B124" si="2">(1-EXP(-((C88/$B$19-($B$18-0.5))/$B$16)^$B$17))*$B$15</f>
         <v>0.11456581846910648</v>
       </c>
-      <c r="C84">
+      <c r="C88">
         <f t="shared" si="1"/>
         <v>16.25</v>
       </c>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B85">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B89">
         <f t="shared" si="2"/>
         <v>0.11571217537522674</v>
       </c>
-      <c r="C85">
-        <f t="shared" ref="C85:C120" si="3">C84+0.25</f>
+      <c r="C89">
+        <f t="shared" ref="C89:C124" si="3">C88+0.25</f>
         <v>16.5</v>
       </c>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B86">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B90">
         <f t="shared" si="2"/>
         <v>0.11676213759849677</v>
       </c>
-      <c r="C86">
+      <c r="C90">
         <f t="shared" si="3"/>
         <v>16.75</v>
       </c>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B87">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B91">
         <f t="shared" si="2"/>
         <v>0.11771991570586685</v>
       </c>
-      <c r="C87">
+      <c r="C91">
         <f t="shared" si="3"/>
         <v>17</v>
       </c>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B88">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B92">
         <f t="shared" si="2"/>
         <v>0.11859002896034841</v>
       </c>
-      <c r="C88">
+      <c r="C92">
         <f t="shared" si="3"/>
         <v>17.25</v>
       </c>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B89">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B93">
         <f t="shared" si="2"/>
         <v>0.11937723477809242</v>
       </c>
-      <c r="C89">
+      <c r="C93">
         <f t="shared" si="3"/>
         <v>17.5</v>
       </c>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B90">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B94">
         <f t="shared" si="2"/>
         <v>0.12008646002494117</v>
       </c>
-      <c r="C90">
+      <c r="C94">
         <f t="shared" si="3"/>
         <v>17.75</v>
       </c>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B91">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B95">
         <f t="shared" si="2"/>
         <v>0.12072273521104175</v>
       </c>
-      <c r="C91">
+      <c r="C95">
         <f t="shared" si="3"/>
         <v>18</v>
       </c>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B92">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B96">
         <f t="shared" si="2"/>
         <v>0.12129113251445571</v>
       </c>
-      <c r="C92">
+      <c r="C96">
         <f t="shared" si="3"/>
         <v>18.25</v>
       </c>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B93">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B97">
         <f t="shared" si="2"/>
         <v>0.12179670842176366</v>
       </c>
-      <c r="C93">
+      <c r="C97">
         <f t="shared" si="3"/>
         <v>18.5</v>
       </c>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B94">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B98">
         <f t="shared" si="2"/>
         <v>0.12224445162033554</v>
       </c>
-      <c r="C94">
+      <c r="C98">
         <f t="shared" si="3"/>
         <v>18.75</v>
       </c>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B95">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B99">
         <f t="shared" si="2"/>
         <v>0.12263923661819812</v>
       </c>
-      <c r="C95">
+      <c r="C99">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B96">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B100">
         <f t="shared" si="2"/>
         <v>0.12298578340816241</v>
       </c>
-      <c r="C96">
+      <c r="C100">
         <f t="shared" si="3"/>
         <v>19.25</v>
       </c>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B97">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B101">
         <f t="shared" si="2"/>
         <v>0.12328862333768843</v>
       </c>
-      <c r="C97">
+      <c r="C101">
         <f t="shared" si="3"/>
         <v>19.5</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B98">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B102">
         <f t="shared" si="2"/>
         <v>0.12355207119904957</v>
       </c>
-      <c r="C98">
+      <c r="C102">
         <f t="shared" si="3"/>
         <v>19.75</v>
       </c>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B99">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B103">
         <f t="shared" si="2"/>
         <v>0.12378020341934777</v>
       </c>
-      <c r="C99">
+      <c r="C103">
         <f t="shared" si="3"/>
         <v>20</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B100">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B104">
         <f t="shared" si="2"/>
         <v>0.1239768421098045</v>
       </c>
-      <c r="C100">
+      <c r="C104">
         <f t="shared" si="3"/>
         <v>20.25</v>
       </c>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B101">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B105">
         <f t="shared" si="2"/>
         <v>0.12414554463077215</v>
       </c>
-      <c r="C101">
+      <c r="C105">
         <f t="shared" si="3"/>
         <v>20.5</v>
       </c>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B102">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B106">
         <f t="shared" si="2"/>
         <v>0.12428959824458628</v>
       </c>
-      <c r="C102">
+      <c r="C106">
         <f t="shared" si="3"/>
         <v>20.75</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B103">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B107">
         <f t="shared" si="2"/>
         <v>0.12441201936347031</v>
       </c>
-      <c r="C103">
+      <c r="C107">
         <f t="shared" si="3"/>
         <v>21</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B104">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B108">
         <f t="shared" si="2"/>
         <v>0.12451555685425303</v>
       </c>
-      <c r="C104">
+      <c r="C108">
         <f t="shared" si="3"/>
         <v>21.25</v>
       </c>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B105">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B109">
         <f t="shared" si="2"/>
         <v>0.12460269883504811</v>
       </c>
-      <c r="C105">
+      <c r="C109">
         <f t="shared" si="3"/>
         <v>21.5</v>
       </c>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B106">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B110">
         <f t="shared" si="2"/>
         <v>0.12467568239008178</v>
       </c>
-      <c r="C106">
+      <c r="C110">
         <f t="shared" si="3"/>
         <v>21.75</v>
       </c>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B107">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B111">
         <f t="shared" si="2"/>
         <v>0.12473650563587114</v>
       </c>
-      <c r="C107">
+      <c r="C111">
         <f t="shared" si="3"/>
         <v>22</v>
       </c>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B108">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B112">
         <f t="shared" si="2"/>
         <v>0.12478694159291652</v>
       </c>
-      <c r="C108">
+      <c r="C112">
         <f t="shared" si="3"/>
         <v>22.25</v>
       </c>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B109">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B113">
         <f t="shared" si="2"/>
         <v>0.12482855334969299</v>
       </c>
-      <c r="C109">
+      <c r="C113">
         <f t="shared" si="3"/>
         <v>22.5</v>
       </c>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B110">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B114">
         <f t="shared" si="2"/>
         <v>0.12486271004758752</v>
       </c>
-      <c r="C110">
+      <c r="C114">
         <f t="shared" si="3"/>
         <v>22.75</v>
       </c>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B111">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B115">
         <f t="shared" si="2"/>
         <v>0.12489060326408261</v>
       </c>
-      <c r="C111">
+      <c r="C115">
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B112">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B116">
         <f t="shared" si="2"/>
         <v>0.12491326342455751</v>
       </c>
-      <c r="C112">
+      <c r="C116">
         <f t="shared" si="3"/>
         <v>23.25</v>
       </c>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B113">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B117">
         <f t="shared" si="2"/>
         <v>0.12493157592833935</v>
       </c>
-      <c r="C113">
+      <c r="C117">
         <f t="shared" si="3"/>
         <v>23.5</v>
       </c>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B114">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B118">
         <f t="shared" si="2"/>
         <v>0.12494629673008874</v>
       </c>
-      <c r="C114">
+      <c r="C118">
         <f t="shared" si="3"/>
         <v>23.75</v>
       </c>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B115">
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B119">
         <f t="shared" si="2"/>
         <v>0.12495806717151219</v>
       </c>
-      <c r="C115">
+      <c r="C119">
         <f t="shared" si="3"/>
         <v>24</v>
       </c>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B116">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B120">
         <f t="shared" si="2"/>
         <v>0.12496742790932699</v>
       </c>
-      <c r="C116">
+      <c r="C120">
         <f t="shared" si="3"/>
         <v>24.25</v>
       </c>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B117">
+    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B121">
         <f t="shared" si="2"/>
         <v>0.1249748318322462</v>
       </c>
-      <c r="C117">
+      <c r="C121">
         <f t="shared" si="3"/>
         <v>24.5</v>
       </c>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B118">
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B122">
         <f t="shared" si="2"/>
         <v>0.12498065590169766</v>
       </c>
-      <c r="C118">
+      <c r="C122">
         <f t="shared" si="3"/>
         <v>24.75</v>
       </c>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B119">
+    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B123">
         <f t="shared" si="2"/>
         <v>0.12498521188753921</v>
       </c>
-      <c r="C119">
+      <c r="C123">
         <f t="shared" si="3"/>
         <v>25</v>
       </c>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B120">
+    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B124">
         <f t="shared" si="2"/>
         <v>0.1249887560009456</v>
       </c>
-      <c r="C120">
+      <c r="C124">
         <f t="shared" si="3"/>
         <v>25.25</v>
       </c>
@@ -5381,346 +5417,346 @@
       <selection activeCell="O5" sqref="O4:O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1">
-        <f>(1-EXP(-((B2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((B2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0</v>
       </c>
       <c r="C1">
-        <f>(1-EXP(-((C2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((C2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>1.1302755611730664E-6</v>
       </c>
       <c r="D1">
-        <f>(1-EXP(-((D2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((D2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>9.041918329455445E-6</v>
       </c>
       <c r="E1">
-        <f>(1-EXP(-((E2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((E2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>3.0513853137847935E-5</v>
       </c>
       <c r="F1">
-        <f>(1-EXP(-((F2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((F2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>7.2317035876470759E-5</v>
       </c>
       <c r="G1">
-        <f>(1-EXP(-((G2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((G2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>1.4120526808655831E-4</v>
       </c>
       <c r="H1">
-        <f>(1-EXP(-((H2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((H2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>2.4390236156555944E-4</v>
       </c>
       <c r="I1">
-        <f>(1-EXP(-((I2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((I2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>3.8708568873771498E-4</v>
       </c>
       <c r="J1">
-        <f>(1-EXP(-((J2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((J2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>5.7736617667798751E-4</v>
       </c>
       <c r="K1">
-        <f>(1-EXP(-((K2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((K2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>8.2126483012147367E-4</v>
       </c>
       <c r="L1">
-        <f>(1-EXP(-((L2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((L2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>1.1251859013301779E-3</v>
       </c>
       <c r="M1">
-        <f>(1-EXP(-((M2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((M2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>1.4953868620252581E-3</v>
       </c>
       <c r="N1">
-        <f>(1-EXP(-((N2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((N2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>1.9379453743239433E-3</v>
       </c>
       <c r="O1">
-        <f>(1-EXP(-((O2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((O2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>2.4587235032284965E-3</v>
       </c>
       <c r="P1">
-        <f>(1-EXP(-((P2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((P2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>3.0633294620639323E-3</v>
       </c>
       <c r="Q1">
-        <f>(1-EXP(-((Q2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((Q2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>3.7570772335819985E-3</v>
       </c>
       <c r="R1">
-        <f>(1-EXP(-((R2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((R2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>4.5449444623392177E-3</v>
       </c>
       <c r="S1">
-        <f>(1-EXP(-((S2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((S2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>5.4315290673835337E-3</v>
       </c>
       <c r="T1">
-        <f>(1-EXP(-((T2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((T2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>6.4210050770837218E-3</v>
       </c>
       <c r="U1">
-        <f>(1-EXP(-((U2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((U2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>7.5170782388275237E-3</v>
       </c>
       <c r="V1">
-        <f>(1-EXP(-((V2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((V2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>8.7229420039149769E-3</v>
       </c>
       <c r="W1">
-        <f>(1-EXP(-((W2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((W2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>1.0041234530816401E-2</v>
       </c>
       <c r="X1">
-        <f>(1-EXP(-((X2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((X2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>1.1473997386527171E-2</v>
       </c>
       <c r="Y1">
-        <f>(1-EXP(-((Y2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((Y2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>1.3022636654488842E-2</v>
       </c>
       <c r="Z1">
-        <f>(1-EXP(-((Z2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((Z2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>1.4687887176925568E-2</v>
       </c>
       <c r="AA1">
-        <f>(1-EXP(-((AA2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AA2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>1.6469780667991457E-2</v>
       </c>
       <c r="AB1">
-        <f>(1-EXP(-((AB2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AB2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>1.8367618430465693E-2</v>
       </c>
       <c r="AC1">
-        <f>(1-EXP(-((AC2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AC2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>2.0379949391649221E-2</v>
       </c>
       <c r="AD1">
-        <f>(1-EXP(-((AD2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AD2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>2.2504554142594765E-2</v>
       </c>
       <c r="AE1">
-        <f>(1-EXP(-((AE2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AE2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>2.4738435618083782E-2</v>
       </c>
       <c r="AF1">
-        <f>(1-EXP(-((AF2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AF2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>2.7077816992397724E-2</v>
       </c>
       <c r="AG1">
-        <f>(1-EXP(-((AG2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AG2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>2.951814728782165E-2</v>
       </c>
       <c r="AH1">
-        <f>(1-EXP(-((AH2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AH2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>3.2054115099261718E-2</v>
       </c>
       <c r="AI1">
-        <f>(1-EXP(-((AI2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AI2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>3.467967073008181E-2</v>
       </c>
       <c r="AJ1">
-        <f>(1-EXP(-((AJ2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AJ2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>3.7388056912446274E-2</v>
       </c>
       <c r="AK1">
-        <f>(1-EXP(-((AK2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AK2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>4.0171848151733677E-2</v>
       </c>
       <c r="AL1">
-        <f>(1-EXP(-((AL2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AL2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>4.3022998591062303E-2</v>
       </c>
       <c r="AM1">
-        <f>(1-EXP(-((AM2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AM2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>4.5932898141179429E-2</v>
       </c>
       <c r="AN1">
-        <f>(1-EXP(-((AN2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AN2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>4.8892436465861083E-2</v>
       </c>
       <c r="AO1">
-        <f>(1-EXP(-((AO2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AO2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>5.1892074256846804E-2</v>
       </c>
       <c r="AP1">
-        <f>(1-EXP(-((AP2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AP2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>5.4921921078778663E-2</v>
       </c>
       <c r="AQ1">
-        <f>(1-EXP(-((AQ2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AQ2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>5.7971818917411488E-2</v>
       </c>
       <c r="AR1">
-        <f>(1-EXP(-((AR2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AR2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>6.1031430427395852E-2</v>
       </c>
       <c r="AS1">
-        <f>(1-EXP(-((AS2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AS2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>6.4090330753079128E-2</v>
       </c>
       <c r="AT1">
-        <f>(1-EXP(-((AT2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AT2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>6.7138101690766061E-2</v>
       </c>
       <c r="AU1">
-        <f>(1-EXP(-((AU2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AU2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>7.0164426877205852E-2</v>
       </c>
       <c r="AV1">
-        <f>(1-EXP(-((AV2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AV2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>7.3159186629829842E-2</v>
       </c>
       <c r="AW1">
-        <f>(1-EXP(-((AW2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AW2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>7.6112551032035736E-2</v>
       </c>
       <c r="AX1">
-        <f>(1-EXP(-((AX2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AX2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>7.9015069853569708E-2</v>
       </c>
       <c r="AY1">
-        <f>(1-EXP(-((AY2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AY2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>8.1857757923041286E-2</v>
       </c>
       <c r="AZ1">
-        <f>(1-EXP(-((AZ2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((AZ2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>8.4632174627258694E-2</v>
       </c>
       <c r="BA1">
-        <f>(1-EXP(-((BA2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BA2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>8.7330496299984461E-2</v>
       </c>
       <c r="BB1">
-        <f>(1-EXP(-((BB2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BB2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>8.9945580379575493E-2</v>
       </c>
       <c r="BC1">
-        <f>(1-EXP(-((BC2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BC2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>9.2471020358609296E-2</v>
       </c>
       <c r="BD1">
-        <f>(1-EXP(-((BD2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BD2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>9.4901190715968961E-2</v>
       </c>
       <c r="BE1">
-        <f>(1-EXP(-((BE2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BE2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>9.7231281209145953E-2</v>
       </c>
       <c r="BF1">
-        <f>(1-EXP(-((BF2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BF2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>9.9457320107219804E-2</v>
       </c>
       <c r="BG1">
-        <f>(1-EXP(-((BG2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BG2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.10157618615802415</v>
       </c>
       <c r="BH1">
-        <f>(1-EXP(-((BH2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BH2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.1035856093009499</v>
       </c>
       <c r="BI1">
-        <f>(1-EXP(-((BI2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BI2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.10548416035397182</v>
       </c>
       <c r="BJ1">
-        <f>(1-EXP(-((BJ2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BJ2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.10727123011408218</v>
       </c>
       <c r="BK1">
-        <f>(1-EXP(-((BK2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BK2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.10894699850878881</v>
       </c>
       <c r="BL1">
-        <f>(1-EXP(-((BL2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BL2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.11051239461744319</v>
       </c>
       <c r="BM1">
-        <f>(1-EXP(-((BM2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BM2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.11196904854019522</v>
       </c>
       <c r="BN1">
-        <f>(1-EXP(-((BN2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BN2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.11331923622529684</v>
       </c>
       <c r="BO1">
-        <f>(1-EXP(-((BO2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BO2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.11456581846910648</v>
       </c>
       <c r="BP1">
-        <f>(1-EXP(-((BP2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BP2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.11571217537522674</v>
       </c>
       <c r="BQ1">
-        <f>(1-EXP(-((BQ2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BQ2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.11676213759849677</v>
       </c>
       <c r="BR1">
-        <f>(1-EXP(-((BR2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BR2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.11771991570586685</v>
       </c>
       <c r="BS1">
-        <f>(1-EXP(-((BS2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BS2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.11859002896034841</v>
       </c>
       <c r="BT1">
-        <f>(1-EXP(-((BT2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BT2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.11937723477809242</v>
       </c>
       <c r="BU1">
-        <f>(1-EXP(-((BU2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BU2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.12008646002494117</v>
       </c>
       <c r="BV1">
-        <f>(1-EXP(-((BV2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BV2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.12072273521104175</v>
       </c>
       <c r="BW1">
-        <f>(1-EXP(-((BW2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BW2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.12129113251445571</v>
       </c>
       <c r="BX1">
-        <f>(1-EXP(-((BX2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BX2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.12179670842176366</v>
       </c>
       <c r="BY1">
-        <f>(1-EXP(-((BY2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BY2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.12224445162033554</v>
       </c>
       <c r="BZ1">
-        <f>(1-EXP(-((BZ2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((BZ2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.12263923661819812</v>
       </c>
       <c r="CA1">
-        <f>(1-EXP(-((CA2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((CA2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.12298578340816241</v>
       </c>
       <c r="CB1">
-        <f>(1-EXP(-((CB2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((CB2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.12328862333768843</v>
       </c>
       <c r="CC1">
-        <f>(1-EXP(-((CC2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((CC2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.12355207119904957</v>
       </c>
       <c r="CD1">
-        <f>(1-EXP(-((CD2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((CD2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.12378020341934777</v>
       </c>
       <c r="CE1">
-        <f>(1-EXP(-((CE2/About!$B$15-(About!$B$14-0.5))/About!$B$12)^About!$B$13))*About!$B$11</f>
+        <f>(1-EXP(-((CE2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.125</v>
       </c>
     </row>
-    <row r="2" spans="1:83" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -6068,17 +6104,17 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
@@ -6099,15 +6135,15 @@
   <dimension ref="A1:AE25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+      <selection activeCell="B7" sqref="B7:AE7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -6202,7 +6238,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -6297,7 +6333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -6392,7 +6428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -6487,7 +6523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -6582,7 +6618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -6677,102 +6713,102 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="K7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="N7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="O7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="P7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="Q7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="R7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="S7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="T7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="U7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="V7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="W7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="X7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="Y7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="Z7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AA7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AB7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AC7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AD7">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AE7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -6867,7 +6903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -6962,7 +6998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -7057,7 +7093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -7152,7 +7188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -7247,7 +7283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -7342,7 +7378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -7437,7 +7473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -7532,7 +7568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -7627,7 +7663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -7722,7 +7758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -7817,7 +7853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -7912,7 +7948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -8007,7 +8043,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -8102,7 +8138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -8197,7 +8233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -8292,7 +8328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -8387,7 +8423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Extend CSCCCMvSoECBtY curve parameters
</commit_message>
<xml_diff>
--- a/InputData/elec/CSC/Capacity Supply Curve.xlsx
+++ b/InputData/elec/CSC/Capacity Supply Curve.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\CSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94731181-DAE1-4C61-8902-F665038802D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6367CB4D-9140-4286-9A37-2062052CD2A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{F87DB1D1-DC21-4EA7-B1DF-998EE56837F8}"/>
   </bookViews>
@@ -214,10 +214,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4314,17 +4313,17 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
         <v>44</v>
       </c>
     </row>
@@ -5411,10 +5410,10 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:CE2"/>
+  <dimension ref="A1:CF2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O4:O5"/>
+    <sheetView topLeftCell="BG1" workbookViewId="0">
+      <selection activeCell="CE1" sqref="CE1:CF1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5423,7 +5422,7 @@
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -5755,8 +5754,12 @@
         <f>(1-EXP(-((CE2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
         <v>0.125</v>
       </c>
-    </row>
-    <row r="2" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="CF1">
+        <f>(1-EXP(-((CF2/About!$B$19-(About!$B$18-0.5))/About!$B$16)^About!$B$17))*About!$B$15</f>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -6085,6 +6088,9 @@
       </c>
       <c r="CE2">
         <v>1000</v>
+      </c>
+      <c r="CF2">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>